<commit_message>
update xlsx text format
</commit_message>
<xml_diff>
--- a/config/i18n/i18n.xlsx
+++ b/config/i18n/i18n.xlsx
@@ -2698,18 +2698,13 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="13"/>
-      <color rgb="FF000000"/>
-      <name val="Helvetica"/>
     </font>
   </fonts>
   <fills count="2">
@@ -2732,7 +2727,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2741,7 +2736,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3065,7 +3059,7 @@
   <dimension ref="A1:G385"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A297" workbookViewId="0">
-      <selection activeCell="B322" sqref="B322"/>
+      <selection activeCell="B320" sqref="B320"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5852,8 +5846,8 @@
         <v>866</v>
       </c>
     </row>
-    <row r="320" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A320" s="4" t="s">
+    <row r="320" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A320" s="1" t="s">
         <v>861</v>
       </c>
       <c r="B320" s="1" t="s">

</xml_diff>

<commit_message>
fixed i18n translation key
</commit_message>
<xml_diff>
--- a/config/i18n/i18n.xlsx
+++ b/config/i18n/i18n.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28615"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28016"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vpp/work/sp-duh/config/i18n/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joaoramos/work/sp-duh/config/i18n/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -2691,9 +2691,6 @@
     <t>paid by employee</t>
   </si>
   <si>
-    <t>payment_mechanism_print_PC</t>
-  </si>
-  <si>
     <t>purchases_mission_map_receipt</t>
   </si>
   <si>
@@ -2728,6 +2725,9 @@
   </si>
   <si>
     <t>Payed on {0} the amount of {1} ({2}) for the settlement of the following documents:</t>
+  </si>
+  <si>
+    <t>payment_mechanism_print_PCL</t>
   </si>
 </sst>
 </file>
@@ -3095,7 +3095,7 @@
   <dimension ref="A1:G389"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A313" workbookViewId="0">
-      <selection activeCell="A324" sqref="A324"/>
+      <selection activeCell="A322" sqref="A322"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5895,7 +5895,7 @@
     </row>
     <row r="321" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A321" s="1" t="s">
-        <v>868</v>
+        <v>880</v>
       </c>
       <c r="B321" s="1" t="s">
         <v>864</v>
@@ -5906,13 +5906,13 @@
     </row>
     <row r="322" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A322" s="1" t="s">
+        <v>868</v>
+      </c>
+      <c r="B322" s="1" t="s">
         <v>869</v>
       </c>
-      <c r="B322" s="1" t="s">
+      <c r="C322" s="1" t="s">
         <v>870</v>
-      </c>
-      <c r="C322" s="1" t="s">
-        <v>871</v>
       </c>
     </row>
     <row r="323" spans="1:3" ht="48" x14ac:dyDescent="0.2">
@@ -5931,10 +5931,10 @@
         <v>676</v>
       </c>
       <c r="B324" s="1" t="s">
+        <v>874</v>
+      </c>
+      <c r="C324" s="1" t="s">
         <v>875</v>
-      </c>
-      <c r="C324" s="1" t="s">
-        <v>876</v>
       </c>
     </row>
     <row r="325" spans="1:3" ht="32" x14ac:dyDescent="0.2">
@@ -5942,10 +5942,10 @@
         <v>677</v>
       </c>
       <c r="B325" s="1" t="s">
+        <v>876</v>
+      </c>
+      <c r="C325" s="1" t="s">
         <v>877</v>
-      </c>
-      <c r="C325" s="1" t="s">
-        <v>878</v>
       </c>
     </row>
     <row r="326" spans="1:3" ht="32" x14ac:dyDescent="0.2">
@@ -5953,15 +5953,15 @@
         <v>858</v>
       </c>
       <c r="B326" s="1" t="s">
+        <v>878</v>
+      </c>
+      <c r="C326" s="1" t="s">
         <v>879</v>
-      </c>
-      <c r="C326" s="1" t="s">
-        <v>880</v>
       </c>
     </row>
     <row r="327" spans="1:3" ht="64" x14ac:dyDescent="0.2">
       <c r="A327" s="1" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
       <c r="B327" s="1" t="s">
         <v>853</v>
@@ -5972,7 +5972,7 @@
     </row>
     <row r="328" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A328" s="1" t="s">
-        <v>873</v>
+        <v>872</v>
       </c>
       <c r="B328" s="1" t="s">
         <v>855</v>
@@ -5983,7 +5983,7 @@
     </row>
     <row r="329" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A329" s="1" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
       <c r="B329" s="1" t="s">
         <v>859</v>

</xml_diff>

<commit_message>
Fix DSP description for printing
</commit_message>
<xml_diff>
--- a/config/i18n/i18n.xlsx
+++ b/config/i18n/i18n.xlsx
@@ -1,26 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28016"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joaoramos/work/sp-duh/config/i18n/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="25725"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19680" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
 </workbook>
@@ -2316,9 +2311,6 @@
   </si>
   <si>
     <t>document_type_DSP</t>
-  </si>
-  <si>
-    <t>Despesas de colaborador</t>
   </si>
   <si>
     <t>Employee expense</t>
@@ -2728,6 +2720,9 @@
   </si>
   <si>
     <t>payment_mechanism_print_PCL</t>
+  </si>
+  <si>
+    <t>Fatura de despesa</t>
   </si>
 </sst>
 </file>
@@ -2872,7 +2867,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic Light"/>
@@ -2907,7 +2902,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic"/>
@@ -3084,7 +3079,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -3094,18 +3089,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G389"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A313" workbookViewId="0">
-      <selection activeCell="A322" sqref="A322"/>
+    <sheetView tabSelected="1" topLeftCell="A329" workbookViewId="0">
+      <selection activeCell="B360" sqref="B360"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="41.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="44.33203125" style="1" customWidth="1"/>
     <col min="4" max="7" width="8" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" s="2" customFormat="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -3128,7 +3123,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -3136,7 +3131,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
@@ -3144,7 +3139,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7">
       <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
@@ -3152,7 +3147,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7">
       <c r="A5" s="1" t="s">
         <v>13</v>
       </c>
@@ -3160,7 +3155,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7">
       <c r="A6" s="1" t="s">
         <v>15</v>
       </c>
@@ -3168,7 +3163,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7">
       <c r="A7" s="1" t="s">
         <v>17</v>
       </c>
@@ -3176,7 +3171,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7">
       <c r="A8" s="1" t="s">
         <v>19</v>
       </c>
@@ -3184,7 +3179,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7">
       <c r="A9" s="1" t="s">
         <v>21</v>
       </c>
@@ -3192,7 +3187,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7">
       <c r="A10" s="1" t="s">
         <v>23</v>
       </c>
@@ -3200,7 +3195,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7">
       <c r="A11" s="1" t="s">
         <v>25</v>
       </c>
@@ -3208,7 +3203,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7">
       <c r="A12" s="1" t="s">
         <v>27</v>
       </c>
@@ -3216,7 +3211,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7">
       <c r="A13" s="1" t="s">
         <v>29</v>
       </c>
@@ -3224,7 +3219,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7">
       <c r="A14" s="1" t="s">
         <v>31</v>
       </c>
@@ -3232,7 +3227,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7">
       <c r="A15" s="1" t="s">
         <v>33</v>
       </c>
@@ -3240,7 +3235,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7">
       <c r="A16" s="1" t="s">
         <v>35</v>
       </c>
@@ -3248,7 +3243,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3">
       <c r="A17" s="1" t="s">
         <v>37</v>
       </c>
@@ -3256,7 +3251,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3">
       <c r="A18" s="1" t="s">
         <v>39</v>
       </c>
@@ -3264,7 +3259,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3">
       <c r="A19" s="1" t="s">
         <v>41</v>
       </c>
@@ -3272,7 +3267,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3">
       <c r="A20" s="1" t="s">
         <v>43</v>
       </c>
@@ -3280,7 +3275,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3">
       <c r="A21" s="1" t="s">
         <v>45</v>
       </c>
@@ -3288,7 +3283,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3">
       <c r="A22" s="1" t="s">
         <v>47</v>
       </c>
@@ -3296,7 +3291,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3">
       <c r="A23" s="1" t="s">
         <v>49</v>
       </c>
@@ -3304,7 +3299,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3">
       <c r="A24" s="1" t="s">
         <v>51</v>
       </c>
@@ -3312,7 +3307,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3">
       <c r="A25" s="1" t="s">
         <v>53</v>
       </c>
@@ -3320,7 +3315,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3">
       <c r="A26" s="1" t="s">
         <v>55</v>
       </c>
@@ -3328,7 +3323,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3">
       <c r="A27" s="1" t="s">
         <v>57</v>
       </c>
@@ -3336,7 +3331,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3">
       <c r="A28" s="1" t="s">
         <v>59</v>
       </c>
@@ -3344,7 +3339,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3">
       <c r="A29" s="1" t="s">
         <v>61</v>
       </c>
@@ -3352,7 +3347,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3">
       <c r="A30" s="1" t="s">
         <v>63</v>
       </c>
@@ -3360,7 +3355,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3">
       <c r="A31" s="1" t="s">
         <v>65</v>
       </c>
@@ -3368,7 +3363,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3">
       <c r="A32" s="1" t="s">
         <v>67</v>
       </c>
@@ -3376,7 +3371,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:3">
       <c r="A33" s="1" t="s">
         <v>69</v>
       </c>
@@ -3384,7 +3379,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:3">
       <c r="A34" s="1" t="s">
         <v>71</v>
       </c>
@@ -3392,7 +3387,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:3">
       <c r="A35" s="1" t="s">
         <v>73</v>
       </c>
@@ -3400,7 +3395,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:3">
       <c r="A36" s="1" t="s">
         <v>75</v>
       </c>
@@ -3408,7 +3403,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:3">
       <c r="A37" s="1" t="s">
         <v>77</v>
       </c>
@@ -3416,7 +3411,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:3">
       <c r="A38" s="1" t="s">
         <v>79</v>
       </c>
@@ -3424,7 +3419,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:3">
       <c r="A39" s="1" t="s">
         <v>81</v>
       </c>
@@ -3432,7 +3427,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:3">
       <c r="A40" s="1" t="s">
         <v>83</v>
       </c>
@@ -3440,7 +3435,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:3">
       <c r="A41" s="1" t="s">
         <v>85</v>
       </c>
@@ -3448,7 +3443,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:3">
       <c r="A42" s="1" t="s">
         <v>87</v>
       </c>
@@ -3456,7 +3451,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:3">
       <c r="A43" s="1" t="s">
         <v>89</v>
       </c>
@@ -3464,7 +3459,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:3">
       <c r="A44" s="1" t="s">
         <v>91</v>
       </c>
@@ -3472,7 +3467,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:3">
       <c r="A45" s="1" t="s">
         <v>93</v>
       </c>
@@ -3480,7 +3475,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:3">
       <c r="A46" s="1" t="s">
         <v>95</v>
       </c>
@@ -3488,7 +3483,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:3">
       <c r="A47" s="1" t="s">
         <v>97</v>
       </c>
@@ -3496,7 +3491,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:3">
       <c r="A48" s="1" t="s">
         <v>99</v>
       </c>
@@ -3504,7 +3499,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:3">
       <c r="A49" s="1" t="s">
         <v>101</v>
       </c>
@@ -3512,7 +3507,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:3">
       <c r="A50" s="1" t="s">
         <v>103</v>
       </c>
@@ -3520,7 +3515,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:3">
       <c r="A51" s="1" t="s">
         <v>105</v>
       </c>
@@ -3528,7 +3523,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:3">
       <c r="A52" s="1" t="s">
         <v>107</v>
       </c>
@@ -3536,7 +3531,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:3">
       <c r="A53" s="1" t="s">
         <v>109</v>
       </c>
@@ -3544,7 +3539,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:3">
       <c r="A54" s="1" t="s">
         <v>111</v>
       </c>
@@ -3552,7 +3547,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:3">
       <c r="A55" s="1" t="s">
         <v>113</v>
       </c>
@@ -3560,7 +3555,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:3">
       <c r="A56" s="1" t="s">
         <v>115</v>
       </c>
@@ -3568,7 +3563,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:3">
       <c r="A57" s="1" t="s">
         <v>117</v>
       </c>
@@ -3576,7 +3571,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:3">
       <c r="A58" s="1" t="s">
         <v>119</v>
       </c>
@@ -3584,7 +3579,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:3">
       <c r="A59" s="1" t="s">
         <v>121</v>
       </c>
@@ -3592,7 +3587,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:3">
       <c r="A60" s="1" t="s">
         <v>123</v>
       </c>
@@ -3600,7 +3595,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:3">
       <c r="A61" s="1" t="s">
         <v>125</v>
       </c>
@@ -3608,7 +3603,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:3">
       <c r="A62" s="1" t="s">
         <v>127</v>
       </c>
@@ -3616,7 +3611,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:3">
       <c r="A63" s="1" t="s">
         <v>129</v>
       </c>
@@ -3624,7 +3619,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:3">
       <c r="A64" s="1" t="s">
         <v>131</v>
       </c>
@@ -3632,7 +3627,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:3">
       <c r="A65" s="1" t="s">
         <v>133</v>
       </c>
@@ -3640,7 +3635,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:3">
       <c r="A66" s="1" t="s">
         <v>135</v>
       </c>
@@ -3648,7 +3643,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:3">
       <c r="A67" s="1" t="s">
         <v>137</v>
       </c>
@@ -3656,7 +3651,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:3">
       <c r="A68" s="1" t="s">
         <v>139</v>
       </c>
@@ -3664,7 +3659,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:3">
       <c r="A69" s="1" t="s">
         <v>141</v>
       </c>
@@ -3672,7 +3667,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:3">
       <c r="A70" s="1" t="s">
         <v>143</v>
       </c>
@@ -3680,7 +3675,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:3">
       <c r="A71" s="1" t="s">
         <v>145</v>
       </c>
@@ -3688,7 +3683,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:3">
       <c r="A72" s="1" t="s">
         <v>147</v>
       </c>
@@ -3696,7 +3691,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:3">
       <c r="A73" s="1" t="s">
         <v>149</v>
       </c>
@@ -3704,7 +3699,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:3">
       <c r="A74" s="1" t="s">
         <v>151</v>
       </c>
@@ -3712,7 +3707,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:3">
       <c r="A75" s="1" t="s">
         <v>153</v>
       </c>
@@ -3720,7 +3715,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:3">
       <c r="A76" s="1" t="s">
         <v>155</v>
       </c>
@@ -3728,7 +3723,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:3">
       <c r="A77" s="1" t="s">
         <v>157</v>
       </c>
@@ -3736,7 +3731,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:3">
       <c r="A78" s="1" t="s">
         <v>159</v>
       </c>
@@ -3744,7 +3739,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:3">
       <c r="A79" s="1" t="s">
         <v>161</v>
       </c>
@@ -3752,7 +3747,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:3">
       <c r="A80" s="1" t="s">
         <v>163</v>
       </c>
@@ -3760,7 +3755,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:3">
       <c r="A81" s="1" t="s">
         <v>165</v>
       </c>
@@ -3768,7 +3763,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:3">
       <c r="A82" s="1" t="s">
         <v>167</v>
       </c>
@@ -3776,7 +3771,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:3">
       <c r="A83" s="1" t="s">
         <v>169</v>
       </c>
@@ -3784,7 +3779,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:3">
       <c r="A84" s="1" t="s">
         <v>171</v>
       </c>
@@ -3792,7 +3787,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:3">
       <c r="A85" s="1" t="s">
         <v>173</v>
       </c>
@@ -3800,7 +3795,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:3">
       <c r="A86" s="1" t="s">
         <v>175</v>
       </c>
@@ -3808,7 +3803,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:3">
       <c r="A87" s="1" t="s">
         <v>177</v>
       </c>
@@ -3816,7 +3811,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:3">
       <c r="A88" s="1" t="s">
         <v>179</v>
       </c>
@@ -3824,7 +3819,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:3">
       <c r="A89" s="1" t="s">
         <v>181</v>
       </c>
@@ -3832,7 +3827,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:3">
       <c r="A90" s="1" t="s">
         <v>183</v>
       </c>
@@ -3840,7 +3835,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:3">
       <c r="A91" s="1" t="s">
         <v>185</v>
       </c>
@@ -3848,7 +3843,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:3">
       <c r="A92" s="1" t="s">
         <v>187</v>
       </c>
@@ -3856,7 +3851,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:3">
       <c r="A93" s="1" t="s">
         <v>189</v>
       </c>
@@ -3864,7 +3859,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:3">
       <c r="A94" s="1" t="s">
         <v>191</v>
       </c>
@@ -3872,7 +3867,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:3">
       <c r="A95" s="1" t="s">
         <v>193</v>
       </c>
@@ -3880,7 +3875,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:3">
       <c r="A96" s="1" t="s">
         <v>195</v>
       </c>
@@ -3888,7 +3883,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:3">
       <c r="A97" s="1" t="s">
         <v>197</v>
       </c>
@@ -3896,7 +3891,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:3">
       <c r="A98" s="1" t="s">
         <v>199</v>
       </c>
@@ -3904,7 +3899,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:3">
       <c r="A99" s="1" t="s">
         <v>201</v>
       </c>
@@ -3912,7 +3907,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:3">
       <c r="A100" s="1" t="s">
         <v>203</v>
       </c>
@@ -3920,7 +3915,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:3">
       <c r="A101" s="1" t="s">
         <v>205</v>
       </c>
@@ -3928,7 +3923,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:3">
       <c r="A102" s="1" t="s">
         <v>207</v>
       </c>
@@ -3936,7 +3931,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:3">
       <c r="A103" s="1" t="s">
         <v>209</v>
       </c>
@@ -3944,7 +3939,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:3">
       <c r="A104" s="1" t="s">
         <v>211</v>
       </c>
@@ -3952,7 +3947,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:3">
       <c r="A105" s="1" t="s">
         <v>213</v>
       </c>
@@ -3960,7 +3955,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:3">
       <c r="A106" s="1" t="s">
         <v>215</v>
       </c>
@@ -3968,7 +3963,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:3">
       <c r="A107" s="1" t="s">
         <v>217</v>
       </c>
@@ -3976,7 +3971,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:3">
       <c r="A108" s="1" t="s">
         <v>219</v>
       </c>
@@ -3984,7 +3979,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:3">
       <c r="A109" s="1" t="s">
         <v>221</v>
       </c>
@@ -3992,7 +3987,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:3">
       <c r="A110" s="1" t="s">
         <v>223</v>
       </c>
@@ -4000,7 +3995,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:3">
       <c r="A111" s="1" t="s">
         <v>225</v>
       </c>
@@ -4008,7 +4003,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:3">
       <c r="A112" s="1" t="s">
         <v>227</v>
       </c>
@@ -4016,7 +4011,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:3">
       <c r="A113" s="1" t="s">
         <v>229</v>
       </c>
@@ -4024,7 +4019,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:3">
       <c r="A114" s="1" t="s">
         <v>231</v>
       </c>
@@ -4032,7 +4027,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:3">
       <c r="A115" s="1" t="s">
         <v>233</v>
       </c>
@@ -4040,7 +4035,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:3">
       <c r="A116" s="1" t="s">
         <v>235</v>
       </c>
@@ -4048,7 +4043,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:3">
       <c r="A117" s="1" t="s">
         <v>237</v>
       </c>
@@ -4056,7 +4051,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:3">
       <c r="A118" s="1" t="s">
         <v>239</v>
       </c>
@@ -4064,7 +4059,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:3">
       <c r="A119" s="1" t="s">
         <v>241</v>
       </c>
@@ -4072,7 +4067,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:3">
       <c r="A120" s="1" t="s">
         <v>243</v>
       </c>
@@ -4080,7 +4075,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:3">
       <c r="A121" s="1" t="s">
         <v>245</v>
       </c>
@@ -4088,7 +4083,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:3">
       <c r="A122" s="1" t="s">
         <v>247</v>
       </c>
@@ -4096,7 +4091,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:3">
       <c r="A123" s="1" t="s">
         <v>249</v>
       </c>
@@ -4104,7 +4099,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:3">
       <c r="A124" s="1" t="s">
         <v>251</v>
       </c>
@@ -4112,7 +4107,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:3">
       <c r="A125" s="1" t="s">
         <v>253</v>
       </c>
@@ -4120,7 +4115,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:3">
       <c r="A126" s="1" t="s">
         <v>255</v>
       </c>
@@ -4128,7 +4123,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:3">
       <c r="A127" s="1" t="s">
         <v>257</v>
       </c>
@@ -4136,7 +4131,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:3">
       <c r="A128" s="1" t="s">
         <v>259</v>
       </c>
@@ -4144,7 +4139,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:3">
       <c r="A129" s="1" t="s">
         <v>261</v>
       </c>
@@ -4152,7 +4147,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:3">
       <c r="A130" s="1" t="s">
         <v>263</v>
       </c>
@@ -4160,7 +4155,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:3">
       <c r="A131" s="1" t="s">
         <v>265</v>
       </c>
@@ -4168,7 +4163,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:3">
       <c r="A132" s="1" t="s">
         <v>267</v>
       </c>
@@ -4176,7 +4171,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:3">
       <c r="A133" s="1" t="s">
         <v>269</v>
       </c>
@@ -4184,7 +4179,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:3">
       <c r="A134" s="1" t="s">
         <v>271</v>
       </c>
@@ -4192,7 +4187,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:3">
       <c r="A135" s="1" t="s">
         <v>273</v>
       </c>
@@ -4200,7 +4195,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:3">
       <c r="A136" s="1" t="s">
         <v>275</v>
       </c>
@@ -4208,7 +4203,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:3">
       <c r="A137" s="1" t="s">
         <v>277</v>
       </c>
@@ -4216,7 +4211,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:3">
       <c r="A138" s="1" t="s">
         <v>279</v>
       </c>
@@ -4224,7 +4219,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:3">
       <c r="A139" s="1" t="s">
         <v>281</v>
       </c>
@@ -4232,7 +4227,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:3">
       <c r="A140" s="1" t="s">
         <v>283</v>
       </c>
@@ -4240,7 +4235,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:3">
       <c r="A141" s="1" t="s">
         <v>285</v>
       </c>
@@ -4248,7 +4243,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:3">
       <c r="A142" s="1" t="s">
         <v>287</v>
       </c>
@@ -4256,7 +4251,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:3">
       <c r="A143" s="1" t="s">
         <v>289</v>
       </c>
@@ -4264,7 +4259,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:3">
       <c r="A144" s="1" t="s">
         <v>291</v>
       </c>
@@ -4272,7 +4267,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:3">
       <c r="A145" s="1" t="s">
         <v>293</v>
       </c>
@@ -4280,7 +4275,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:3">
       <c r="A146" s="1" t="s">
         <v>295</v>
       </c>
@@ -4288,7 +4283,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:3">
       <c r="A147" s="1" t="s">
         <v>297</v>
       </c>
@@ -4296,7 +4291,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:3">
       <c r="A148" s="1" t="s">
         <v>299</v>
       </c>
@@ -4304,7 +4299,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:3">
       <c r="A149" s="1" t="s">
         <v>301</v>
       </c>
@@ -4312,7 +4307,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:3">
       <c r="A150" s="1" t="s">
         <v>303</v>
       </c>
@@ -4320,7 +4315,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:3">
       <c r="A151" s="1" t="s">
         <v>305</v>
       </c>
@@ -4328,7 +4323,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:3">
       <c r="A152" s="1" t="s">
         <v>307</v>
       </c>
@@ -4336,7 +4331,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:3">
       <c r="A153" s="1" t="s">
         <v>309</v>
       </c>
@@ -4344,7 +4339,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:3">
       <c r="A154" s="1" t="s">
         <v>311</v>
       </c>
@@ -4352,7 +4347,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:3">
       <c r="A155" s="1" t="s">
         <v>313</v>
       </c>
@@ -4360,7 +4355,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:3">
       <c r="A156" s="1" t="s">
         <v>315</v>
       </c>
@@ -4368,7 +4363,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:3">
       <c r="A157" s="1" t="s">
         <v>317</v>
       </c>
@@ -4376,7 +4371,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="158" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:3">
       <c r="A158" s="1" t="s">
         <v>319</v>
       </c>
@@ -4384,7 +4379,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="159" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:3">
       <c r="A159" s="1" t="s">
         <v>321</v>
       </c>
@@ -4392,7 +4387,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="160" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:3">
       <c r="A160" s="1" t="s">
         <v>323</v>
       </c>
@@ -4400,7 +4395,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="161" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:3">
       <c r="A161" s="1" t="s">
         <v>325</v>
       </c>
@@ -4408,7 +4403,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="162" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:3">
       <c r="A162" s="1" t="s">
         <v>327</v>
       </c>
@@ -4416,7 +4411,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:3">
       <c r="A163" s="1" t="s">
         <v>329</v>
       </c>
@@ -4424,7 +4419,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="164" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:3">
       <c r="A164" s="1" t="s">
         <v>331</v>
       </c>
@@ -4432,7 +4427,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="165" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:3">
       <c r="A165" s="1" t="s">
         <v>333</v>
       </c>
@@ -4440,7 +4435,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="166" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:3">
       <c r="A166" s="1" t="s">
         <v>335</v>
       </c>
@@ -4448,7 +4443,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="167" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:3">
       <c r="A167" s="1" t="s">
         <v>337</v>
       </c>
@@ -4456,7 +4451,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="168" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:3">
       <c r="A168" s="1" t="s">
         <v>339</v>
       </c>
@@ -4464,7 +4459,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="169" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:3">
       <c r="A169" s="1" t="s">
         <v>341</v>
       </c>
@@ -4472,7 +4467,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="170" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:3">
       <c r="A170" s="1" t="s">
         <v>343</v>
       </c>
@@ -4480,7 +4475,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="171" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:3">
       <c r="A171" s="1" t="s">
         <v>345</v>
       </c>
@@ -4488,7 +4483,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="172" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:3">
       <c r="A172" s="1" t="s">
         <v>347</v>
       </c>
@@ -4496,7 +4491,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="173" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:3">
       <c r="A173" s="1" t="s">
         <v>349</v>
       </c>
@@ -4504,7 +4499,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="174" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:3">
       <c r="A174" s="1" t="s">
         <v>351</v>
       </c>
@@ -4512,7 +4507,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="175" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:3">
       <c r="A175" s="1" t="s">
         <v>353</v>
       </c>
@@ -4520,7 +4515,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="176" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:3">
       <c r="A176" s="1" t="s">
         <v>355</v>
       </c>
@@ -4528,7 +4523,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="177" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:3">
       <c r="A177" s="1" t="s">
         <v>357</v>
       </c>
@@ -4536,7 +4531,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="178" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:3">
       <c r="A178" s="1" t="s">
         <v>359</v>
       </c>
@@ -4544,7 +4539,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="179" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:3">
       <c r="A179" s="1" t="s">
         <v>361</v>
       </c>
@@ -4552,7 +4547,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="180" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:3">
       <c r="A180" s="1" t="s">
         <v>363</v>
       </c>
@@ -4560,7 +4555,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="181" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:3">
       <c r="A181" s="1" t="s">
         <v>365</v>
       </c>
@@ -4568,7 +4563,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="182" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:3">
       <c r="A182" s="1" t="s">
         <v>367</v>
       </c>
@@ -4576,7 +4571,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="183" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:3">
       <c r="A183" s="1" t="s">
         <v>369</v>
       </c>
@@ -4584,7 +4579,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="184" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:3">
       <c r="A184" s="1" t="s">
         <v>371</v>
       </c>
@@ -4592,7 +4587,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="185" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:3">
       <c r="A185" s="1" t="s">
         <v>373</v>
       </c>
@@ -4600,7 +4595,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="186" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:3">
       <c r="A186" s="1" t="s">
         <v>375</v>
       </c>
@@ -4608,7 +4603,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="187" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:3">
       <c r="A187" s="1" t="s">
         <v>377</v>
       </c>
@@ -4616,7 +4611,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="188" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:3">
       <c r="A188" s="1" t="s">
         <v>379</v>
       </c>
@@ -4624,7 +4619,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="189" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:3">
       <c r="A189" s="1" t="s">
         <v>381</v>
       </c>
@@ -4632,7 +4627,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="190" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:3">
       <c r="A190" s="1" t="s">
         <v>383</v>
       </c>
@@ -4640,7 +4635,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="191" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:3">
       <c r="A191" s="1" t="s">
         <v>385</v>
       </c>
@@ -4648,7 +4643,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="192" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:3">
       <c r="A192" s="1" t="s">
         <v>387</v>
       </c>
@@ -4656,7 +4651,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="193" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:3">
       <c r="A193" s="1" t="s">
         <v>389</v>
       </c>
@@ -4664,7 +4659,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="194" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:3">
       <c r="A194" s="1" t="s">
         <v>391</v>
       </c>
@@ -4672,7 +4667,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="195" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:3">
       <c r="A195" s="1" t="s">
         <v>393</v>
       </c>
@@ -4680,7 +4675,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="196" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:3">
       <c r="A196" s="1" t="s">
         <v>395</v>
       </c>
@@ -4688,7 +4683,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="197" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:3">
       <c r="A197" s="1" t="s">
         <v>397</v>
       </c>
@@ -4696,7 +4691,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="198" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:3">
       <c r="A198" s="1" t="s">
         <v>399</v>
       </c>
@@ -4704,7 +4699,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="199" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:3">
       <c r="A199" s="1" t="s">
         <v>401</v>
       </c>
@@ -4712,7 +4707,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="200" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:3">
       <c r="A200" s="1" t="s">
         <v>403</v>
       </c>
@@ -4720,7 +4715,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="201" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:3">
       <c r="A201" s="1" t="s">
         <v>405</v>
       </c>
@@ -4728,7 +4723,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="202" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:3">
       <c r="A202" s="1" t="s">
         <v>407</v>
       </c>
@@ -4736,7 +4731,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="203" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:3">
       <c r="A203" s="1" t="s">
         <v>409</v>
       </c>
@@ -4744,7 +4739,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="204" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:3">
       <c r="A204" s="1" t="s">
         <v>411</v>
       </c>
@@ -4752,7 +4747,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="205" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:3">
       <c r="A205" s="1" t="s">
         <v>413</v>
       </c>
@@ -4760,7 +4755,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="206" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:3">
       <c r="A206" s="1" t="s">
         <v>415</v>
       </c>
@@ -4768,7 +4763,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="207" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:3">
       <c r="A207" s="1" t="s">
         <v>417</v>
       </c>
@@ -4776,7 +4771,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="208" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:3">
       <c r="A208" s="1" t="s">
         <v>419</v>
       </c>
@@ -4784,7 +4779,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="209" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:3">
       <c r="A209" s="1" t="s">
         <v>421</v>
       </c>
@@ -4792,7 +4787,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="210" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:3">
       <c r="A210" s="1" t="s">
         <v>423</v>
       </c>
@@ -4800,7 +4795,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="211" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:3">
       <c r="A211" s="1" t="s">
         <v>425</v>
       </c>
@@ -4808,7 +4803,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="212" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:3">
       <c r="A212" s="1" t="s">
         <v>427</v>
       </c>
@@ -4816,7 +4811,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="213" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:3">
       <c r="A213" s="1" t="s">
         <v>429</v>
       </c>
@@ -4824,7 +4819,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="214" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:3">
       <c r="A214" s="1" t="s">
         <v>431</v>
       </c>
@@ -4832,7 +4827,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="215" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:3">
       <c r="A215" s="1" t="s">
         <v>433</v>
       </c>
@@ -4840,7 +4835,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="216" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:3">
       <c r="A216" s="1" t="s">
         <v>435</v>
       </c>
@@ -4848,7 +4843,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="217" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:3">
       <c r="A217" s="1" t="s">
         <v>437</v>
       </c>
@@ -4856,7 +4851,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="218" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:3">
       <c r="A218" s="1" t="s">
         <v>439</v>
       </c>
@@ -4864,7 +4859,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="219" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:3">
       <c r="A219" s="1" t="s">
         <v>441</v>
       </c>
@@ -4872,7 +4867,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="220" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:3">
       <c r="A220" s="1" t="s">
         <v>443</v>
       </c>
@@ -4880,7 +4875,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="221" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:3">
       <c r="A221" s="1" t="s">
         <v>445</v>
       </c>
@@ -4888,7 +4883,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="222" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:3">
       <c r="A222" s="1" t="s">
         <v>447</v>
       </c>
@@ -4896,7 +4891,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="223" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:3">
       <c r="A223" s="1" t="s">
         <v>449</v>
       </c>
@@ -4904,7 +4899,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="224" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:3">
       <c r="A224" s="1" t="s">
         <v>451</v>
       </c>
@@ -4912,7 +4907,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="225" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:3">
       <c r="A225" s="1" t="s">
         <v>453</v>
       </c>
@@ -4920,7 +4915,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="226" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:3">
       <c r="A226" s="1" t="s">
         <v>455</v>
       </c>
@@ -4928,7 +4923,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="227" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:3">
       <c r="A227" s="1" t="s">
         <v>457</v>
       </c>
@@ -4936,7 +4931,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="228" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:3">
       <c r="A228" s="1" t="s">
         <v>459</v>
       </c>
@@ -4944,7 +4939,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="229" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:3">
       <c r="A229" s="1" t="s">
         <v>461</v>
       </c>
@@ -4952,7 +4947,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="230" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:3">
       <c r="A230" s="1" t="s">
         <v>463</v>
       </c>
@@ -4960,7 +4955,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="231" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:3">
       <c r="A231" s="1" t="s">
         <v>465</v>
       </c>
@@ -4968,7 +4963,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="232" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:3">
       <c r="A232" s="1" t="s">
         <v>467</v>
       </c>
@@ -4976,7 +4971,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="233" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:3">
       <c r="A233" s="1" t="s">
         <v>468</v>
       </c>
@@ -4984,7 +4979,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="234" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:3">
       <c r="A234" s="1" t="s">
         <v>470</v>
       </c>
@@ -4992,7 +4987,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="235" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:3">
       <c r="A235" s="1" t="s">
         <v>472</v>
       </c>
@@ -5000,7 +4995,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="236" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:3">
       <c r="A236" s="1" t="s">
         <v>474</v>
       </c>
@@ -5008,7 +5003,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="237" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:3">
       <c r="A237" s="1" t="s">
         <v>476</v>
       </c>
@@ -5016,7 +5011,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="238" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:3">
       <c r="A238" s="1" t="s">
         <v>478</v>
       </c>
@@ -5024,7 +5019,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="239" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:3">
       <c r="A239" s="1" t="s">
         <v>480</v>
       </c>
@@ -5032,7 +5027,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="240" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:3">
       <c r="A240" s="1" t="s">
         <v>482</v>
       </c>
@@ -5040,7 +5035,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="241" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:3">
       <c r="A241" s="1" t="s">
         <v>484</v>
       </c>
@@ -5048,7 +5043,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="242" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:3">
       <c r="A242" s="1" t="s">
         <v>486</v>
       </c>
@@ -5056,7 +5051,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="243" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:3">
       <c r="A243" s="1" t="s">
         <v>488</v>
       </c>
@@ -5064,7 +5059,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="244" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:3">
       <c r="A244" s="1" t="s">
         <v>490</v>
       </c>
@@ -5072,7 +5067,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="245" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:3">
       <c r="A245" s="1" t="s">
         <v>492</v>
       </c>
@@ -5080,7 +5075,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="246" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="246" spans="1:3">
       <c r="A246" s="1" t="s">
         <v>494</v>
       </c>
@@ -5088,7 +5083,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="247" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="247" spans="1:3">
       <c r="A247" s="1" t="s">
         <v>496</v>
       </c>
@@ -5096,7 +5091,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="248" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="248" spans="1:3">
       <c r="A248" s="1" t="s">
         <v>502</v>
       </c>
@@ -5107,7 +5102,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="249" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="249" spans="1:3">
       <c r="A249" s="1" t="s">
         <v>505</v>
       </c>
@@ -5118,7 +5113,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="250" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="250" spans="1:3">
       <c r="A250" s="1" t="s">
         <v>508</v>
       </c>
@@ -5129,7 +5124,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="251" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="251" spans="1:3">
       <c r="A251" s="1" t="s">
         <v>509</v>
       </c>
@@ -5140,7 +5135,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="252" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="252" spans="1:3">
       <c r="A252" s="1" t="s">
         <v>510</v>
       </c>
@@ -5151,7 +5146,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="253" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="253" spans="1:3">
       <c r="A253" s="1" t="s">
         <v>513</v>
       </c>
@@ -5162,7 +5157,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="254" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="254" spans="1:3">
       <c r="A254" s="1" t="s">
         <v>516</v>
       </c>
@@ -5173,7 +5168,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="255" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="255" spans="1:3">
       <c r="A255" s="1" t="s">
         <v>519</v>
       </c>
@@ -5184,7 +5179,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="256" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+    <row r="256" spans="1:3" ht="32">
       <c r="A256" s="1" t="s">
         <v>498</v>
       </c>
@@ -5195,15 +5190,15 @@
         <v>500</v>
       </c>
     </row>
-    <row r="257" spans="1:3" ht="409" x14ac:dyDescent="0.2">
+    <row r="257" spans="1:3" ht="409">
       <c r="A257" s="1" t="s">
         <v>501</v>
       </c>
       <c r="B257" s="1" t="s">
-        <v>857</v>
-      </c>
-    </row>
-    <row r="258" spans="1:3" x14ac:dyDescent="0.2">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="258" spans="1:3">
       <c r="A258" s="1" t="s">
         <v>522</v>
       </c>
@@ -5214,7 +5209,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="259" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="259" spans="1:3">
       <c r="A259" s="1" t="s">
         <v>525</v>
       </c>
@@ -5222,7 +5217,7 @@
         <v>1662</v>
       </c>
     </row>
-    <row r="260" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="260" spans="1:3">
       <c r="A260" s="1" t="s">
         <v>526</v>
       </c>
@@ -5233,7 +5228,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="261" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="261" spans="1:3">
       <c r="A261" s="1" t="s">
         <v>529</v>
       </c>
@@ -5244,7 +5239,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="262" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="262" spans="1:3">
       <c r="A262" s="1" t="s">
         <v>532</v>
       </c>
@@ -5255,7 +5250,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="263" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="263" spans="1:3">
       <c r="A263" s="1" t="s">
         <v>535</v>
       </c>
@@ -5266,7 +5261,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="264" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="264" spans="1:3">
       <c r="A264" s="1" t="s">
         <v>538</v>
       </c>
@@ -5277,7 +5272,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="265" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="265" spans="1:3">
       <c r="A265" s="1" t="s">
         <v>541</v>
       </c>
@@ -5288,7 +5283,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="266" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="266" spans="1:3">
       <c r="A266" s="1" t="s">
         <v>544</v>
       </c>
@@ -5299,7 +5294,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="267" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="267" spans="1:3">
       <c r="A267" s="1" t="s">
         <v>547</v>
       </c>
@@ -5310,7 +5305,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="268" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="268" spans="1:3">
       <c r="A268" s="1" t="s">
         <v>550</v>
       </c>
@@ -5321,7 +5316,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="269" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="269" spans="1:3">
       <c r="A269" s="1" t="s">
         <v>553</v>
       </c>
@@ -5332,7 +5327,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="270" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="270" spans="1:3">
       <c r="A270" s="1" t="s">
         <v>556</v>
       </c>
@@ -5343,7 +5338,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="271" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="271" spans="1:3">
       <c r="A271" s="1" t="s">
         <v>559</v>
       </c>
@@ -5354,7 +5349,7 @@
         <v>561</v>
       </c>
     </row>
-    <row r="272" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="272" spans="1:3">
       <c r="A272" s="1" t="s">
         <v>562</v>
       </c>
@@ -5365,7 +5360,7 @@
         <v>564</v>
       </c>
     </row>
-    <row r="273" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="273" spans="1:3">
       <c r="A273" s="1" t="s">
         <v>565</v>
       </c>
@@ -5376,7 +5371,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="274" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="274" spans="1:3">
       <c r="A274" s="1" t="s">
         <v>568</v>
       </c>
@@ -5387,7 +5382,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="275" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="275" spans="1:3">
       <c r="A275" s="1" t="s">
         <v>571</v>
       </c>
@@ -5398,7 +5393,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="276" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="276" spans="1:3">
       <c r="A276" s="1" t="s">
         <v>574</v>
       </c>
@@ -5409,7 +5404,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="277" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="277" spans="1:3">
       <c r="A277" s="1" t="s">
         <v>577</v>
       </c>
@@ -5420,7 +5415,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="278" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="278" spans="1:3">
       <c r="A278" s="1" t="s">
         <v>580</v>
       </c>
@@ -5431,7 +5426,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="279" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="279" spans="1:3">
       <c r="A279" s="1" t="s">
         <v>583</v>
       </c>
@@ -5442,7 +5437,7 @@
         <v>585</v>
       </c>
     </row>
-    <row r="280" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="280" spans="1:3">
       <c r="A280" s="1" t="s">
         <v>586</v>
       </c>
@@ -5453,7 +5448,7 @@
         <v>588</v>
       </c>
     </row>
-    <row r="281" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="281" spans="1:3">
       <c r="A281" s="1" t="s">
         <v>589</v>
       </c>
@@ -5464,7 +5459,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="282" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="282" spans="1:3">
       <c r="A282" s="1" t="s">
         <v>592</v>
       </c>
@@ -5475,7 +5470,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="283" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="283" spans="1:3">
       <c r="A283" s="1" t="s">
         <v>595</v>
       </c>
@@ -5486,7 +5481,7 @@
         <v>597</v>
       </c>
     </row>
-    <row r="284" spans="1:3" ht="48" x14ac:dyDescent="0.2">
+    <row r="284" spans="1:3" ht="48">
       <c r="A284" s="1" t="s">
         <v>598</v>
       </c>
@@ -5497,7 +5492,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="285" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="285" spans="1:3">
       <c r="A285" s="1" t="s">
         <v>601</v>
       </c>
@@ -5508,7 +5503,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="286" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+    <row r="286" spans="1:3" ht="32">
       <c r="A286" s="1" t="s">
         <v>604</v>
       </c>
@@ -5519,7 +5514,7 @@
         <v>606</v>
       </c>
     </row>
-    <row r="287" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+    <row r="287" spans="1:3" ht="32">
       <c r="A287" s="1" t="s">
         <v>607</v>
       </c>
@@ -5530,7 +5525,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="288" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="288" spans="1:3">
       <c r="A288" s="1" t="s">
         <v>610</v>
       </c>
@@ -5541,7 +5536,7 @@
         <v>611</v>
       </c>
     </row>
-    <row r="289" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="289" spans="1:3">
       <c r="A289" s="1" t="s">
         <v>612</v>
       </c>
@@ -5552,7 +5547,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="290" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="290" spans="1:3">
       <c r="A290" s="1" t="s">
         <v>615</v>
       </c>
@@ -5563,7 +5558,7 @@
         <v>617</v>
       </c>
     </row>
-    <row r="291" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="291" spans="1:3">
       <c r="A291" s="1" t="s">
         <v>618</v>
       </c>
@@ -5574,7 +5569,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="292" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="292" spans="1:3">
       <c r="A292" s="1" t="s">
         <v>621</v>
       </c>
@@ -5585,7 +5580,7 @@
         <v>623</v>
       </c>
     </row>
-    <row r="293" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="293" spans="1:3">
       <c r="A293" s="1" t="s">
         <v>624</v>
       </c>
@@ -5596,7 +5591,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="294" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="294" spans="1:3">
       <c r="A294" s="1" t="s">
         <v>627</v>
       </c>
@@ -5607,7 +5602,7 @@
         <v>629</v>
       </c>
     </row>
-    <row r="295" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="295" spans="1:3">
       <c r="A295" s="1" t="s">
         <v>630</v>
       </c>
@@ -5618,7 +5613,7 @@
         <v>632</v>
       </c>
     </row>
-    <row r="296" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="296" spans="1:3">
       <c r="A296" s="1" t="s">
         <v>633</v>
       </c>
@@ -5629,7 +5624,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="297" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="297" spans="1:3">
       <c r="A297" s="1" t="s">
         <v>636</v>
       </c>
@@ -5640,7 +5635,7 @@
         <v>638</v>
       </c>
     </row>
-    <row r="298" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="298" spans="1:3">
       <c r="A298" s="1" t="s">
         <v>639</v>
       </c>
@@ -5651,7 +5646,7 @@
         <v>641</v>
       </c>
     </row>
-    <row r="299" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="299" spans="1:3">
       <c r="A299" s="1" t="s">
         <v>642</v>
       </c>
@@ -5662,7 +5657,7 @@
         <v>644</v>
       </c>
     </row>
-    <row r="300" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="300" spans="1:3">
       <c r="A300" s="1" t="s">
         <v>645</v>
       </c>
@@ -5673,7 +5668,7 @@
         <v>647</v>
       </c>
     </row>
-    <row r="301" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="301" spans="1:3">
       <c r="A301" s="1" t="s">
         <v>648</v>
       </c>
@@ -5684,7 +5679,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="302" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="302" spans="1:3">
       <c r="A302" s="1" t="s">
         <v>651</v>
       </c>
@@ -5695,7 +5690,7 @@
         <v>653</v>
       </c>
     </row>
-    <row r="303" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="303" spans="1:3">
       <c r="A303" s="1" t="s">
         <v>654</v>
       </c>
@@ -5706,7 +5701,7 @@
         <v>656</v>
       </c>
     </row>
-    <row r="304" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="304" spans="1:3">
       <c r="A304" s="1" t="s">
         <v>657</v>
       </c>
@@ -5717,7 +5712,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="305" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="305" spans="1:3">
       <c r="A305" s="1" t="s">
         <v>660</v>
       </c>
@@ -5728,7 +5723,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="306" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="306" spans="1:3">
       <c r="A306" s="1" t="s">
         <v>661</v>
       </c>
@@ -5739,7 +5734,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="307" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="307" spans="1:3">
       <c r="A307" s="1" t="s">
         <v>662</v>
       </c>
@@ -5750,7 +5745,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="308" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="308" spans="1:3">
       <c r="A308" s="1" t="s">
         <v>663</v>
       </c>
@@ -5761,7 +5756,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="309" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="309" spans="1:3">
       <c r="A309" s="1" t="s">
         <v>664</v>
       </c>
@@ -5772,7 +5767,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="310" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="310" spans="1:3">
       <c r="A310" s="1" t="s">
         <v>665</v>
       </c>
@@ -5783,7 +5778,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="311" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="311" spans="1:3">
       <c r="A311" s="1" t="s">
         <v>666</v>
       </c>
@@ -5794,7 +5789,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="312" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="312" spans="1:3">
       <c r="A312" s="1" t="s">
         <v>667</v>
       </c>
@@ -5805,7 +5800,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="313" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="313" spans="1:3">
       <c r="A313" s="1" t="s">
         <v>668</v>
       </c>
@@ -5816,7 +5811,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="314" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="314" spans="1:3">
       <c r="A314" s="1" t="s">
         <v>669</v>
       </c>
@@ -5827,7 +5822,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="315" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="315" spans="1:3">
       <c r="A315" s="1" t="s">
         <v>670</v>
       </c>
@@ -5838,7 +5833,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="316" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="316" spans="1:3">
       <c r="A316" s="1" t="s">
         <v>671</v>
       </c>
@@ -5849,7 +5844,7 @@
         <v>561</v>
       </c>
     </row>
-    <row r="317" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="317" spans="1:3">
       <c r="A317" s="1" t="s">
         <v>672</v>
       </c>
@@ -5860,7 +5855,7 @@
         <v>564</v>
       </c>
     </row>
-    <row r="318" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="318" spans="1:3">
       <c r="A318" s="1" t="s">
         <v>673</v>
       </c>
@@ -5871,128 +5866,128 @@
         <v>567</v>
       </c>
     </row>
-    <row r="319" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="319" spans="1:3">
       <c r="A319" s="1" t="s">
         <v>674</v>
       </c>
       <c r="B319" s="1" t="s">
+        <v>861</v>
+      </c>
+      <c r="C319" s="1" t="s">
+        <v>865</v>
+      </c>
+    </row>
+    <row r="320" spans="1:3">
+      <c r="A320" s="1" t="s">
+        <v>860</v>
+      </c>
+      <c r="B320" s="1" t="s">
         <v>862</v>
       </c>
-      <c r="C319" s="1" t="s">
+      <c r="C320" s="1" t="s">
         <v>866</v>
       </c>
     </row>
-    <row r="320" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A320" s="1" t="s">
-        <v>861</v>
-      </c>
-      <c r="B320" s="1" t="s">
+    <row r="321" spans="1:3">
+      <c r="A321" s="1" t="s">
+        <v>879</v>
+      </c>
+      <c r="B321" s="1" t="s">
         <v>863</v>
       </c>
-      <c r="C320" s="1" t="s">
+      <c r="C321" s="1" t="s">
+        <v>864</v>
+      </c>
+    </row>
+    <row r="322" spans="1:3">
+      <c r="A322" s="1" t="s">
         <v>867</v>
       </c>
-    </row>
-    <row r="321" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A321" s="1" t="s">
-        <v>880</v>
-      </c>
-      <c r="B321" s="1" t="s">
-        <v>864</v>
-      </c>
-      <c r="C321" s="1" t="s">
-        <v>865</v>
-      </c>
-    </row>
-    <row r="322" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A322" s="1" t="s">
+      <c r="B322" s="1" t="s">
         <v>868</v>
       </c>
-      <c r="B322" s="1" t="s">
+      <c r="C322" s="1" t="s">
         <v>869</v>
       </c>
-      <c r="C322" s="1" t="s">
-        <v>870</v>
-      </c>
-    </row>
-    <row r="323" spans="1:3" ht="48" x14ac:dyDescent="0.2">
+    </row>
+    <row r="323" spans="1:3" ht="48">
       <c r="A323" s="1" t="s">
         <v>675</v>
       </c>
       <c r="B323" s="1" t="s">
+        <v>850</v>
+      </c>
+      <c r="C323" s="1" t="s">
         <v>851</v>
       </c>
-      <c r="C323" s="1" t="s">
-        <v>852</v>
-      </c>
-    </row>
-    <row r="324" spans="1:3" ht="64" x14ac:dyDescent="0.2">
+    </row>
+    <row r="324" spans="1:3" ht="64">
       <c r="A324" s="1" t="s">
         <v>676</v>
       </c>
       <c r="B324" s="1" t="s">
+        <v>873</v>
+      </c>
+      <c r="C324" s="1" t="s">
         <v>874</v>
       </c>
-      <c r="C324" s="1" t="s">
-        <v>875</v>
-      </c>
-    </row>
-    <row r="325" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+    </row>
+    <row r="325" spans="1:3" ht="32">
       <c r="A325" s="1" t="s">
         <v>677</v>
       </c>
       <c r="B325" s="1" t="s">
+        <v>875</v>
+      </c>
+      <c r="C325" s="1" t="s">
         <v>876</v>
       </c>
-      <c r="C325" s="1" t="s">
+    </row>
+    <row r="326" spans="1:3" ht="32">
+      <c r="A326" s="1" t="s">
+        <v>857</v>
+      </c>
+      <c r="B326" s="1" t="s">
         <v>877</v>
       </c>
-    </row>
-    <row r="326" spans="1:3" ht="32" x14ac:dyDescent="0.2">
-      <c r="A326" s="1" t="s">
-        <v>858</v>
-      </c>
-      <c r="B326" s="1" t="s">
+      <c r="C326" s="1" t="s">
         <v>878</v>
       </c>
-      <c r="C326" s="1" t="s">
-        <v>879</v>
-      </c>
-    </row>
-    <row r="327" spans="1:3" ht="64" x14ac:dyDescent="0.2">
+    </row>
+    <row r="327" spans="1:3" ht="64">
       <c r="A327" s="1" t="s">
+        <v>870</v>
+      </c>
+      <c r="B327" s="1" t="s">
+        <v>852</v>
+      </c>
+      <c r="C327" s="1" t="s">
+        <v>853</v>
+      </c>
+    </row>
+    <row r="328" spans="1:3" ht="32">
+      <c r="A328" s="1" t="s">
         <v>871</v>
       </c>
-      <c r="B327" s="1" t="s">
-        <v>853</v>
-      </c>
-      <c r="C327" s="1" t="s">
+      <c r="B328" s="1" t="s">
         <v>854</v>
-      </c>
-    </row>
-    <row r="328" spans="1:3" ht="32" x14ac:dyDescent="0.2">
-      <c r="A328" s="1" t="s">
-        <v>872</v>
-      </c>
-      <c r="B328" s="1" t="s">
-        <v>855</v>
       </c>
       <c r="C328" s="1" t="s">
         <v>678</v>
       </c>
     </row>
-    <row r="329" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+    <row r="329" spans="1:3" ht="32">
       <c r="A329" s="1" t="s">
-        <v>873</v>
+        <v>872</v>
       </c>
       <c r="B329" s="1" t="s">
+        <v>858</v>
+      </c>
+      <c r="C329" s="1" t="s">
         <v>859</v>
       </c>
-      <c r="C329" s="1" t="s">
-        <v>860</v>
-      </c>
-    </row>
-    <row r="330" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="330" spans="1:3">
       <c r="A330" s="1" t="s">
         <v>679</v>
       </c>
@@ -6003,7 +5998,7 @@
         <v>681</v>
       </c>
     </row>
-    <row r="331" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="331" spans="1:3">
       <c r="A331" s="1" t="s">
         <v>682</v>
       </c>
@@ -6014,7 +6009,7 @@
         <v>684</v>
       </c>
     </row>
-    <row r="332" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="332" spans="1:3">
       <c r="A332" s="1" t="s">
         <v>685</v>
       </c>
@@ -6025,7 +6020,7 @@
         <v>687</v>
       </c>
     </row>
-    <row r="333" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="333" spans="1:3">
       <c r="A333" s="1" t="s">
         <v>688</v>
       </c>
@@ -6036,7 +6031,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="334" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="334" spans="1:3">
       <c r="A334" s="1" t="s">
         <v>691</v>
       </c>
@@ -6047,7 +6042,7 @@
         <v>693</v>
       </c>
     </row>
-    <row r="335" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="335" spans="1:3">
       <c r="A335" s="1" t="s">
         <v>694</v>
       </c>
@@ -6058,7 +6053,7 @@
         <v>696</v>
       </c>
     </row>
-    <row r="336" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="336" spans="1:3">
       <c r="A336" s="1" t="s">
         <v>697</v>
       </c>
@@ -6069,7 +6064,7 @@
         <v>699</v>
       </c>
     </row>
-    <row r="337" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="337" spans="1:3">
       <c r="A337" s="1" t="s">
         <v>700</v>
       </c>
@@ -6080,7 +6075,7 @@
         <v>699</v>
       </c>
     </row>
-    <row r="338" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="338" spans="1:3">
       <c r="A338" s="1" t="s">
         <v>702</v>
       </c>
@@ -6091,7 +6086,7 @@
         <v>704</v>
       </c>
     </row>
-    <row r="339" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="339" spans="1:3">
       <c r="A339" s="1" t="s">
         <v>705</v>
       </c>
@@ -6102,7 +6097,7 @@
         <v>707</v>
       </c>
     </row>
-    <row r="340" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="340" spans="1:3">
       <c r="A340" s="1" t="s">
         <v>708</v>
       </c>
@@ -6113,7 +6108,7 @@
         <v>710</v>
       </c>
     </row>
-    <row r="341" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="341" spans="1:3">
       <c r="A341" s="1" t="s">
         <v>711</v>
       </c>
@@ -6124,7 +6119,7 @@
         <v>713</v>
       </c>
     </row>
-    <row r="342" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="342" spans="1:3">
       <c r="A342" s="1" t="s">
         <v>714</v>
       </c>
@@ -6135,7 +6130,7 @@
         <v>716</v>
       </c>
     </row>
-    <row r="343" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="343" spans="1:3">
       <c r="A343" s="1" t="s">
         <v>717</v>
       </c>
@@ -6146,7 +6141,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="344" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="344" spans="1:3">
       <c r="A344" s="1" t="s">
         <v>720</v>
       </c>
@@ -6157,7 +6152,7 @@
         <v>722</v>
       </c>
     </row>
-    <row r="345" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="345" spans="1:3">
       <c r="A345" s="1" t="s">
         <v>723</v>
       </c>
@@ -6168,7 +6163,7 @@
         <v>725</v>
       </c>
     </row>
-    <row r="346" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="346" spans="1:3">
       <c r="A346" s="1" t="s">
         <v>726</v>
       </c>
@@ -6179,7 +6174,7 @@
         <v>687</v>
       </c>
     </row>
-    <row r="347" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="347" spans="1:3">
       <c r="A347" s="1" t="s">
         <v>728</v>
       </c>
@@ -6190,7 +6185,7 @@
         <v>730</v>
       </c>
     </row>
-    <row r="348" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="348" spans="1:3">
       <c r="A348" s="1" t="s">
         <v>731</v>
       </c>
@@ -6201,7 +6196,7 @@
         <v>733</v>
       </c>
     </row>
-    <row r="349" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="349" spans="1:3">
       <c r="A349" s="1" t="s">
         <v>734</v>
       </c>
@@ -6212,7 +6207,7 @@
         <v>736</v>
       </c>
     </row>
-    <row r="350" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="350" spans="1:3">
       <c r="A350" s="1" t="s">
         <v>737</v>
       </c>
@@ -6223,7 +6218,7 @@
         <v>739</v>
       </c>
     </row>
-    <row r="351" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="351" spans="1:3">
       <c r="A351" s="1" t="s">
         <v>740</v>
       </c>
@@ -6234,7 +6229,7 @@
         <v>742</v>
       </c>
     </row>
-    <row r="352" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="352" spans="1:3">
       <c r="A352" s="1" t="s">
         <v>743</v>
       </c>
@@ -6245,7 +6240,7 @@
         <v>745</v>
       </c>
     </row>
-    <row r="353" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="353" spans="1:3">
       <c r="A353" s="1" t="s">
         <v>746</v>
       </c>
@@ -6256,7 +6251,7 @@
         <v>748</v>
       </c>
     </row>
-    <row r="354" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="354" spans="1:3">
       <c r="A354" s="1" t="s">
         <v>749</v>
       </c>
@@ -6267,7 +6262,7 @@
         <v>751</v>
       </c>
     </row>
-    <row r="355" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="355" spans="1:3">
       <c r="A355" s="1" t="s">
         <v>752</v>
       </c>
@@ -6278,7 +6273,7 @@
         <v>699</v>
       </c>
     </row>
-    <row r="356" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="356" spans="1:3">
       <c r="A356" s="1" t="s">
         <v>754</v>
       </c>
@@ -6289,7 +6284,7 @@
         <v>696</v>
       </c>
     </row>
-    <row r="357" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="357" spans="1:3">
       <c r="A357" s="1" t="s">
         <v>756</v>
       </c>
@@ -6300,7 +6295,7 @@
         <v>758</v>
       </c>
     </row>
-    <row r="358" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="358" spans="1:3">
       <c r="A358" s="1" t="s">
         <v>759</v>
       </c>
@@ -6311,295 +6306,295 @@
         <v>761</v>
       </c>
     </row>
-    <row r="359" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="359" spans="1:3">
       <c r="A359" s="1" t="s">
         <v>762</v>
       </c>
       <c r="B359" s="1" t="s">
+        <v>880</v>
+      </c>
+      <c r="C359" s="1" t="s">
         <v>763</v>
       </c>
-      <c r="C359" s="1" t="s">
+    </row>
+    <row r="360" spans="1:3">
+      <c r="A360" s="1" t="s">
         <v>764</v>
       </c>
-    </row>
-    <row r="360" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A360" s="1" t="s">
+      <c r="B360" s="1" t="s">
         <v>765</v>
       </c>
-      <c r="B360" s="1" t="s">
+      <c r="C360" s="1" t="s">
         <v>766</v>
       </c>
-      <c r="C360" s="1" t="s">
+    </row>
+    <row r="361" spans="1:3">
+      <c r="A361" s="1" t="s">
         <v>767</v>
       </c>
-    </row>
-    <row r="361" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A361" s="1" t="s">
+      <c r="B361" s="1" t="s">
         <v>768</v>
       </c>
-      <c r="B361" s="1" t="s">
+      <c r="C361" s="1" t="s">
         <v>769</v>
       </c>
-      <c r="C361" s="1" t="s">
+    </row>
+    <row r="362" spans="1:3">
+      <c r="A362" s="1" t="s">
         <v>770</v>
       </c>
-    </row>
-    <row r="362" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A362" s="1" t="s">
+      <c r="B362" s="1" t="s">
         <v>771</v>
       </c>
-      <c r="B362" s="1" t="s">
+      <c r="C362" s="1" t="s">
         <v>772</v>
       </c>
-      <c r="C362" s="1" t="s">
+    </row>
+    <row r="363" spans="1:3">
+      <c r="A363" s="1" t="s">
         <v>773</v>
       </c>
-    </row>
-    <row r="363" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A363" s="1" t="s">
+      <c r="B363" s="1" t="s">
         <v>774</v>
       </c>
-      <c r="B363" s="1" t="s">
+      <c r="C363" s="1" t="s">
         <v>775</v>
       </c>
-      <c r="C363" s="1" t="s">
+    </row>
+    <row r="364" spans="1:3">
+      <c r="A364" s="1" t="s">
         <v>776</v>
       </c>
-    </row>
-    <row r="364" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A364" s="1" t="s">
+      <c r="B364" s="1" t="s">
         <v>777</v>
       </c>
-      <c r="B364" s="1" t="s">
+      <c r="C364" s="1" t="s">
         <v>778</v>
       </c>
-      <c r="C364" s="1" t="s">
+    </row>
+    <row r="365" spans="1:3">
+      <c r="A365" s="1" t="s">
         <v>779</v>
       </c>
-    </row>
-    <row r="365" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A365" s="1" t="s">
+      <c r="B365" s="1" t="s">
         <v>780</v>
       </c>
-      <c r="B365" s="1" t="s">
+      <c r="C365" s="1" t="s">
         <v>781</v>
       </c>
-      <c r="C365" s="1" t="s">
+    </row>
+    <row r="366" spans="1:3">
+      <c r="A366" s="1" t="s">
         <v>782</v>
       </c>
-    </row>
-    <row r="366" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A366" s="1" t="s">
+      <c r="B366" s="1" t="s">
         <v>783</v>
       </c>
-      <c r="B366" s="1" t="s">
+      <c r="C366" s="1" t="s">
         <v>784</v>
       </c>
-      <c r="C366" s="1" t="s">
+    </row>
+    <row r="367" spans="1:3">
+      <c r="A367" s="1" t="s">
         <v>785</v>
       </c>
-    </row>
-    <row r="367" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A367" s="1" t="s">
+      <c r="B367" s="1" t="s">
         <v>786</v>
       </c>
-      <c r="B367" s="1" t="s">
+      <c r="C367" s="1" t="s">
         <v>787</v>
       </c>
-      <c r="C367" s="1" t="s">
+    </row>
+    <row r="368" spans="1:3">
+      <c r="A368" s="1" t="s">
         <v>788</v>
       </c>
-    </row>
-    <row r="368" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A368" s="1" t="s">
+      <c r="B368" s="1" t="s">
         <v>789</v>
       </c>
-      <c r="B368" s="1" t="s">
+      <c r="C368" s="1" t="s">
         <v>790</v>
       </c>
-      <c r="C368" s="1" t="s">
+    </row>
+    <row r="369" spans="1:3">
+      <c r="A369" s="1" t="s">
         <v>791</v>
       </c>
-    </row>
-    <row r="369" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A369" s="1" t="s">
+      <c r="B369" s="1" t="s">
         <v>792</v>
       </c>
-      <c r="B369" s="1" t="s">
+      <c r="C369" s="1" t="s">
         <v>793</v>
       </c>
-      <c r="C369" s="1" t="s">
+    </row>
+    <row r="370" spans="1:3">
+      <c r="A370" s="1" t="s">
         <v>794</v>
       </c>
-    </row>
-    <row r="370" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A370" s="1" t="s">
+      <c r="B370" s="1" t="s">
         <v>795</v>
       </c>
-      <c r="B370" s="1" t="s">
+      <c r="C370" s="1" t="s">
         <v>796</v>
       </c>
-      <c r="C370" s="1" t="s">
+    </row>
+    <row r="371" spans="1:3">
+      <c r="A371" s="1" t="s">
         <v>797</v>
       </c>
-    </row>
-    <row r="371" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A371" s="1" t="s">
+      <c r="B371" s="1" t="s">
         <v>798</v>
       </c>
-      <c r="B371" s="1" t="s">
+      <c r="C371" s="1" t="s">
         <v>799</v>
       </c>
-      <c r="C371" s="1" t="s">
+    </row>
+    <row r="372" spans="1:3">
+      <c r="A372" s="1" t="s">
         <v>800</v>
       </c>
-    </row>
-    <row r="372" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A372" s="1" t="s">
+      <c r="B372" s="1" t="s">
         <v>801</v>
       </c>
-      <c r="B372" s="1" t="s">
+      <c r="C372" s="1" t="s">
         <v>802</v>
       </c>
-      <c r="C372" s="1" t="s">
+    </row>
+    <row r="373" spans="1:3">
+      <c r="A373" s="1" t="s">
         <v>803</v>
       </c>
-    </row>
-    <row r="373" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A373" s="1" t="s">
+      <c r="B373" s="1" t="s">
         <v>804</v>
       </c>
-      <c r="B373" s="1" t="s">
+      <c r="C373" s="1" t="s">
         <v>805</v>
       </c>
-      <c r="C373" s="1" t="s">
+    </row>
+    <row r="374" spans="1:3">
+      <c r="A374" s="1" t="s">
         <v>806</v>
       </c>
-    </row>
-    <row r="374" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A374" s="1" t="s">
+      <c r="B374" s="1" t="s">
         <v>807</v>
       </c>
-      <c r="B374" s="1" t="s">
+      <c r="C374" s="1" t="s">
         <v>808</v>
       </c>
-      <c r="C374" s="1" t="s">
+    </row>
+    <row r="375" spans="1:3">
+      <c r="A375" s="1" t="s">
         <v>809</v>
       </c>
-    </row>
-    <row r="375" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A375" s="1" t="s">
+      <c r="B375" s="1" t="s">
         <v>810</v>
       </c>
-      <c r="B375" s="1" t="s">
+      <c r="C375" s="1" t="s">
         <v>811</v>
       </c>
-      <c r="C375" s="1" t="s">
+    </row>
+    <row r="376" spans="1:3">
+      <c r="A376" s="1" t="s">
         <v>812</v>
       </c>
-    </row>
-    <row r="376" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A376" s="1" t="s">
+      <c r="B376" s="1" t="s">
         <v>813</v>
       </c>
-      <c r="B376" s="1" t="s">
+      <c r="C376" s="1" t="s">
         <v>814</v>
       </c>
-      <c r="C376" s="1" t="s">
+    </row>
+    <row r="377" spans="1:3">
+      <c r="A377" s="1" t="s">
         <v>815</v>
       </c>
-    </row>
-    <row r="377" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A377" s="1" t="s">
+      <c r="B377" s="1" t="s">
+        <v>855</v>
+      </c>
+      <c r="C377" s="1" t="s">
         <v>816</v>
       </c>
-      <c r="B377" s="1" t="s">
-        <v>856</v>
-      </c>
-      <c r="C377" s="1" t="s">
+    </row>
+    <row r="378" spans="1:3">
+      <c r="A378" s="1" t="s">
         <v>817</v>
       </c>
-    </row>
-    <row r="378" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A378" s="1" t="s">
+      <c r="B378" s="1" t="s">
         <v>818</v>
       </c>
-      <c r="B378" s="1" t="s">
+      <c r="C378" s="1" t="s">
         <v>819</v>
       </c>
-      <c r="C378" s="1" t="s">
+    </row>
+    <row r="379" spans="1:3">
+      <c r="A379" s="1" t="s">
         <v>820</v>
       </c>
-    </row>
-    <row r="379" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A379" s="1" t="s">
+      <c r="B379" s="1" t="s">
         <v>821</v>
       </c>
-      <c r="B379" s="1" t="s">
+      <c r="C379" s="1" t="s">
         <v>822</v>
       </c>
-      <c r="C379" s="1" t="s">
+    </row>
+    <row r="380" spans="1:3">
+      <c r="A380" s="1" t="s">
         <v>823</v>
       </c>
-    </row>
-    <row r="380" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A380" s="1" t="s">
+      <c r="B380" s="1" t="s">
         <v>824</v>
       </c>
-      <c r="B380" s="1" t="s">
+      <c r="C380" s="1" t="s">
         <v>825</v>
       </c>
-      <c r="C380" s="1" t="s">
+    </row>
+    <row r="381" spans="1:3">
+      <c r="A381" s="1" t="s">
         <v>826</v>
       </c>
-    </row>
-    <row r="381" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A381" s="1" t="s">
+      <c r="B381" s="1" t="s">
         <v>827</v>
       </c>
-      <c r="B381" s="1" t="s">
+      <c r="C381" s="1" t="s">
         <v>828</v>
       </c>
-      <c r="C381" s="1" t="s">
+    </row>
+    <row r="382" spans="1:3">
+      <c r="A382" s="1" t="s">
         <v>829</v>
       </c>
-    </row>
-    <row r="382" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A382" s="1" t="s">
+      <c r="B382" s="1" t="s">
         <v>830</v>
       </c>
-      <c r="B382" s="1" t="s">
+      <c r="C382" s="1" t="s">
+        <v>828</v>
+      </c>
+    </row>
+    <row r="383" spans="1:3">
+      <c r="A383" s="1" t="s">
         <v>831</v>
       </c>
-      <c r="C382" s="1" t="s">
-        <v>829</v>
-      </c>
-    </row>
-    <row r="383" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A383" s="1" t="s">
+      <c r="B383" s="1" t="s">
         <v>832</v>
       </c>
-      <c r="B383" s="1" t="s">
+      <c r="C383" s="1" t="s">
         <v>833</v>
       </c>
-      <c r="C383" s="1" t="s">
+    </row>
+    <row r="384" spans="1:3">
+      <c r="A384" s="1" t="s">
         <v>834</v>
       </c>
-    </row>
-    <row r="384" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A384" s="1" t="s">
+      <c r="B384" s="1" t="s">
         <v>835</v>
       </c>
-      <c r="B384" s="1" t="s">
+      <c r="C384" s="1" t="s">
         <v>836</v>
       </c>
-      <c r="C384" s="1" t="s">
+    </row>
+    <row r="385" spans="1:3">
+      <c r="A385" s="1" t="s">
         <v>837</v>
-      </c>
-    </row>
-    <row r="385" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A385" s="1" t="s">
-        <v>838</v>
       </c>
       <c r="B385" s="1" t="s">
         <v>622</v>
@@ -6608,48 +6603,48 @@
         <v>623</v>
       </c>
     </row>
-    <row r="386" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="386" spans="1:3">
       <c r="A386" s="1" t="s">
+        <v>838</v>
+      </c>
+      <c r="B386" s="1" t="s">
         <v>839</v>
       </c>
-      <c r="B386" s="1" t="s">
+      <c r="C386" s="1" t="s">
         <v>840</v>
       </c>
-      <c r="C386" s="1" t="s">
+    </row>
+    <row r="387" spans="1:3">
+      <c r="A387" s="1" t="s">
         <v>841</v>
       </c>
-    </row>
-    <row r="387" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A387" s="1" t="s">
+      <c r="B387" s="1" t="s">
         <v>842</v>
       </c>
-      <c r="B387" s="1" t="s">
+      <c r="C387" s="1" t="s">
         <v>843</v>
       </c>
-      <c r="C387" s="1" t="s">
+    </row>
+    <row r="388" spans="1:3">
+      <c r="A388" s="1" t="s">
         <v>844</v>
       </c>
-    </row>
-    <row r="388" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A388" s="1" t="s">
+      <c r="B388" s="1" t="s">
         <v>845</v>
       </c>
-      <c r="B388" s="1" t="s">
+      <c r="C388" s="1" t="s">
         <v>846</v>
       </c>
-      <c r="C388" s="1" t="s">
+    </row>
+    <row r="389" spans="1:3">
+      <c r="A389" s="1" t="s">
         <v>847</v>
       </c>
-    </row>
-    <row r="389" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A389" s="1" t="s">
+      <c r="B389" s="1" t="s">
         <v>848</v>
       </c>
-      <c r="B389" s="1" t="s">
+      <c r="C389" s="1" t="s">
         <v>849</v>
-      </c>
-      <c r="C389" s="1" t="s">
-        <v>850</v>
       </c>
     </row>
   </sheetData>
@@ -6657,5 +6652,10 @@
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add localization for the entity "supplier" (used in printing purchases)
</commit_message>
<xml_diff>
--- a/config/i18n/i18n.xlsx
+++ b/config/i18n/i18n.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="25725"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="29540" windowHeight="17820" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="922" uniqueCount="881">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="925" uniqueCount="882">
   <si>
     <t>key</t>
   </si>
@@ -2724,15 +2724,34 @@
   <si>
     <t>Fatura de despesa</t>
   </si>
+  <si>
+    <t>entity_supplier</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -2755,10 +2774,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2767,8 +2788,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="7">
@@ -2809,8 +2835,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="i18n" displayName="i18n" ref="A1:G389" totalsRowShown="0" headerRowDxfId="6">
-  <autoFilter ref="A1:G389"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="i18n" displayName="i18n" ref="A1:G390" totalsRowShown="0" headerRowDxfId="6">
+  <autoFilter ref="A1:G390"/>
   <tableColumns count="7">
     <tableColumn id="1" name="key"/>
     <tableColumn id="2" name="pt" dataDxfId="5"/>
@@ -3079,7 +3105,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -3087,10 +3113,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G389"/>
+  <dimension ref="A1:G390"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A329" workbookViewId="0">
-      <selection activeCell="B360" sqref="B360"/>
+    <sheetView tabSelected="1" topLeftCell="A358" workbookViewId="0">
+      <selection activeCell="A390" sqref="A390"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5179,7 +5205,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="256" spans="1:3" ht="32">
+    <row r="256" spans="1:3" ht="30">
       <c r="A256" s="1" t="s">
         <v>498</v>
       </c>
@@ -5470,7 +5496,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="283" spans="1:3">
+    <row r="283" spans="1:3" ht="30">
       <c r="A283" s="1" t="s">
         <v>595</v>
       </c>
@@ -5481,7 +5507,7 @@
         <v>597</v>
       </c>
     </row>
-    <row r="284" spans="1:3" ht="48">
+    <row r="284" spans="1:3" ht="45">
       <c r="A284" s="1" t="s">
         <v>598</v>
       </c>
@@ -5503,7 +5529,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="286" spans="1:3" ht="32">
+    <row r="286" spans="1:3" ht="30">
       <c r="A286" s="1" t="s">
         <v>604</v>
       </c>
@@ -5514,7 +5540,7 @@
         <v>606</v>
       </c>
     </row>
-    <row r="287" spans="1:3" ht="32">
+    <row r="287" spans="1:3" ht="30">
       <c r="A287" s="1" t="s">
         <v>607</v>
       </c>
@@ -5910,7 +5936,7 @@
         <v>869</v>
       </c>
     </row>
-    <row r="323" spans="1:3" ht="48">
+    <row r="323" spans="1:3" ht="45">
       <c r="A323" s="1" t="s">
         <v>675</v>
       </c>
@@ -5921,7 +5947,7 @@
         <v>851</v>
       </c>
     </row>
-    <row r="324" spans="1:3" ht="64">
+    <row r="324" spans="1:3" ht="60">
       <c r="A324" s="1" t="s">
         <v>676</v>
       </c>
@@ -5932,7 +5958,7 @@
         <v>874</v>
       </c>
     </row>
-    <row r="325" spans="1:3" ht="32">
+    <row r="325" spans="1:3" ht="30">
       <c r="A325" s="1" t="s">
         <v>677</v>
       </c>
@@ -5943,7 +5969,7 @@
         <v>876</v>
       </c>
     </row>
-    <row r="326" spans="1:3" ht="32">
+    <row r="326" spans="1:3" ht="30">
       <c r="A326" s="1" t="s">
         <v>857</v>
       </c>
@@ -5954,7 +5980,7 @@
         <v>878</v>
       </c>
     </row>
-    <row r="327" spans="1:3" ht="64">
+    <row r="327" spans="1:3" ht="60">
       <c r="A327" s="1" t="s">
         <v>870</v>
       </c>
@@ -5965,7 +5991,7 @@
         <v>853</v>
       </c>
     </row>
-    <row r="328" spans="1:3" ht="32">
+    <row r="328" spans="1:3" ht="30">
       <c r="A328" s="1" t="s">
         <v>871</v>
       </c>
@@ -5976,7 +6002,7 @@
         <v>678</v>
       </c>
     </row>
-    <row r="329" spans="1:3" ht="32">
+    <row r="329" spans="1:3" ht="30">
       <c r="A329" s="1" t="s">
         <v>872</v>
       </c>
@@ -6592,7 +6618,7 @@
         <v>836</v>
       </c>
     </row>
-    <row r="385" spans="1:3">
+    <row r="385" spans="1:7">
       <c r="A385" s="1" t="s">
         <v>837</v>
       </c>
@@ -6603,7 +6629,7 @@
         <v>623</v>
       </c>
     </row>
-    <row r="386" spans="1:3">
+    <row r="386" spans="1:7">
       <c r="A386" s="1" t="s">
         <v>838</v>
       </c>
@@ -6614,7 +6640,7 @@
         <v>840</v>
       </c>
     </row>
-    <row r="387" spans="1:3">
+    <row r="387" spans="1:7">
       <c r="A387" s="1" t="s">
         <v>841</v>
       </c>
@@ -6625,7 +6651,7 @@
         <v>843</v>
       </c>
     </row>
-    <row r="388" spans="1:3">
+    <row r="388" spans="1:7">
       <c r="A388" s="1" t="s">
         <v>844</v>
       </c>
@@ -6636,7 +6662,7 @@
         <v>846</v>
       </c>
     </row>
-    <row r="389" spans="1:3">
+    <row r="389" spans="1:7">
       <c r="A389" s="1" t="s">
         <v>847</v>
       </c>
@@ -6647,8 +6673,24 @@
         <v>849</v>
       </c>
     </row>
+    <row r="390" spans="1:7">
+      <c r="A390" s="1" t="s">
+        <v>881</v>
+      </c>
+      <c r="B390" s="1" t="s">
+        <v>658</v>
+      </c>
+      <c r="C390" s="1" t="s">
+        <v>659</v>
+      </c>
+      <c r="D390" s="4"/>
+      <c r="E390" s="4"/>
+      <c r="F390" s="4"/>
+      <c r="G390" s="4"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>

</xml_diff>

<commit_message>
Added localized resources for purchases (suppliers)
</commit_message>
<xml_diff>
--- a/config/i18n/i18n.xlsx
+++ b/config/i18n/i18n.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="25725"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="29540" windowHeight="17820" tabRatio="500"/>
+    <workbookView xWindow="780" yWindow="520" windowWidth="29540" windowHeight="17820" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="925" uniqueCount="882">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="931" uniqueCount="886">
   <si>
     <t>key</t>
   </si>
@@ -2727,6 +2727,18 @@
   <si>
     <t>entity_supplier</t>
   </si>
+  <si>
+    <t>unknown_pt_supplier</t>
+  </si>
+  <si>
+    <t>unknown_supplier</t>
+  </si>
+  <si>
+    <t>Fornecedor Indiferenciado</t>
+  </si>
+  <si>
+    <t>Unknown Supplier</t>
+  </si>
 </sst>
 </file>
 
@@ -2774,8 +2786,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
@@ -2792,9 +2808,13 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="7">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="7">
@@ -2835,8 +2855,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="i18n" displayName="i18n" ref="A1:G390" totalsRowShown="0" headerRowDxfId="6">
-  <autoFilter ref="A1:G390"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="i18n" displayName="i18n" ref="A1:G392" totalsRowShown="0" headerRowDxfId="6">
+  <autoFilter ref="A1:G392"/>
   <tableColumns count="7">
     <tableColumn id="1" name="key"/>
     <tableColumn id="2" name="pt" dataDxfId="5"/>
@@ -3105,7 +3125,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -3113,10 +3133,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G390"/>
+  <dimension ref="A1:G392"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A358" workbookViewId="0">
-      <selection activeCell="A390" sqref="A390"/>
+      <selection activeCell="D399" sqref="D399"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -6687,6 +6707,32 @@
       <c r="E390" s="4"/>
       <c r="F390" s="4"/>
       <c r="G390" s="4"/>
+    </row>
+    <row r="391" spans="1:7">
+      <c r="A391" s="1" t="s">
+        <v>882</v>
+      </c>
+      <c r="B391" s="1" t="s">
+        <v>884</v>
+      </c>
+      <c r="C391" s="1" t="s">
+        <v>885</v>
+      </c>
+    </row>
+    <row r="392" spans="1:7">
+      <c r="A392" s="1" t="s">
+        <v>883</v>
+      </c>
+      <c r="B392" s="1" t="s">
+        <v>830</v>
+      </c>
+      <c r="C392" s="1" t="s">
+        <v>885</v>
+      </c>
+      <c r="D392" s="4"/>
+      <c r="E392" s="4"/>
+      <c r="F392" s="4"/>
+      <c r="G392" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Report svat, first version
</commit_message>
<xml_diff>
--- a/config/i18n/i18n.xlsx
+++ b/config/i18n/i18n.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="500"/>
+    <workbookView xWindow="-1980" yWindow="-19600" windowWidth="28800" windowHeight="17540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="937" uniqueCount="892">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="991" uniqueCount="946">
   <si>
     <t>key</t>
   </si>
@@ -2745,15 +2745,9 @@
     <t>Unknown Supplier</t>
   </si>
   <si>
-    <t>against_nature</t>
-  </si>
-  <si>
     <t>Existem contas com saldo contra natura, que não permitem o correto preenchimento do Balanço. Verifique a(s) conta(s): {0}</t>
   </si>
   <si>
-    <t>not_expected_balance</t>
-  </si>
-  <si>
     <t>Existem contas com saldo não esperado que não permitem o correto preenchimento do Balanço. Verifique a(s) conta(s): {0}</t>
   </si>
   <si>
@@ -2761,6 +2755,174 @@
   </si>
   <si>
     <t>There are accounts with an unexpected balance that do not allow the correct completion of the Balance Sheet. Check the account (s): {0}</t>
+  </si>
+  <si>
+    <t>Existem contas com categoria no balanço por configurar: {0}</t>
+  </si>
+  <si>
+    <t>A conta {0} tem categorias no balanço por configurar.</t>
+  </si>
+  <si>
+    <t>Verifique as seguintes rubricas do Balanço uma vez que apresentam saldos contra natura: {0}</t>
+  </si>
+  <si>
+    <t>balance_against_nature</t>
+  </si>
+  <si>
+    <t>O RL apresentado foi obtido de forma aritmética, não sendo coincidente com o apresentado na conta 818 ({0}). Verifique por favor o lançamento de apuramento de resultados.</t>
+  </si>
+  <si>
+    <t>no_match_account_818</t>
+  </si>
+  <si>
+    <t>Account {0} has categories in the balance to be set up.</t>
+  </si>
+  <si>
+    <t>There are accounts with category in the balance to configure: {0}</t>
+  </si>
+  <si>
+    <t>The presented RL was obtained in arithmetic form, not coinciding with that presented in the account 818 ({0}). Please check the results.</t>
+  </si>
+  <si>
+    <t>Check the following balance sheet items as they show balances against nature: {0}</t>
+  </si>
+  <si>
+    <t>bs_categories_no_config</t>
+  </si>
+  <si>
+    <t>bs_account_no_config</t>
+  </si>
+  <si>
+    <t>Foi verificada a natureza do saldo de todas as contas e a sua concordância com a natureza esperada. Não foram encontradas quaisquer diferenças</t>
+  </si>
+  <si>
+    <t>The balance nature of all accounts and their concordance with the expected nature were verified. No differences found</t>
+  </si>
+  <si>
+    <t>rep_against_nature_ok</t>
+  </si>
+  <si>
+    <t>Foi verificada a natureza do saldo de todas as contas e a sua concordância com a natureza esperada. Identificaram-se as seguintes contas que apresentam um saldo contranatura e que deverão ser corrigidas para uma correta submissão do ficheiro SAF-T e construção das Demonstrações Financeiras: #Conta - Saldo (d) ou (c )</t>
+  </si>
+  <si>
+    <t>rep_against_nature_nok</t>
+  </si>
+  <si>
+    <t>The balance nature of all accounts and their concordance with the expected nature were verified. The following accounts that present a counter balance have been identified and should be corrected for a correct submission of the SAF-T file and construction of the Financial Statements: # Account - Balance (d) or (c)</t>
+  </si>
+  <si>
+    <t>rep_not_expected_balance_ok</t>
+  </si>
+  <si>
+    <t>rep_not_expected_balance_nok</t>
+  </si>
+  <si>
+    <t>Foi verificada a natureza do saldo a apresentar em cada rubrica do balanço e a sua concordância com a natureza esperada. Não foram encontradas quaisquer diferenças</t>
+  </si>
+  <si>
+    <t>Foi verificada a natureza do saldo a apresentar em cada rubrica do balanço e a sua concordância com a natureza esperada. As seguintes rubricas do Balanço apresentam um saldo não esperado e deverão ser corrigidas para uma correta submissão do ficheiro SAF-T e construção das Demonstrações Financeiras: Rubrica balanço: - Saldo (d) ou (c )</t>
+  </si>
+  <si>
+    <t>The nature of the balance was verified in each balance sheet item and its agreement with the expected nature. The following balance sheet items present an unexpired balance and should be corrected for a right submission of the SAF-T file and construction of the Financial Statements: Balance sheet item: Balance (d) or (c)</t>
+  </si>
+  <si>
+    <t>The nature of the balance was verified in each balance sheet item and its agreement with the expected nature. No differences found</t>
+  </si>
+  <si>
+    <t>bs_not_expected_balance_nok</t>
+  </si>
+  <si>
+    <t>bs_against_nature_nok</t>
+  </si>
+  <si>
+    <t>Foi efetuado um teste sobre a conta 219 - "Clientes - Perdas por imparidade acumuladas" e verificado que o saldo credor desta conta é igual ou  inferior à soma algébrica dos saldos das contas 211 a 217. Teste realizado com sucesso.</t>
+  </si>
+  <si>
+    <t>account_219_ok</t>
+  </si>
+  <si>
+    <t>account_219_nok</t>
+  </si>
+  <si>
+    <t>account_229_ok</t>
+  </si>
+  <si>
+    <t>account_229_nok</t>
+  </si>
+  <si>
+    <t>account_239_nok</t>
+  </si>
+  <si>
+    <t>account_239_ok</t>
+  </si>
+  <si>
+    <t>Foi efetuado um teste sobre a conta 229 - "Fornecedores - Perdas por imparidade acumuladas" e verificado que o saldo credor desta conta é inferior ou igual ao existente na conta 228 - "Fornecedores - Adiantamentos a fornecedores". Teste realizado com sucesso.</t>
+  </si>
+  <si>
+    <t>Foi efetuado um teste sobre a conta 239 - "Pessoal - Perdas por imparidade acumuladas" e verificado que esta conta, apresenta um saldo inferior ou igual à soma algébrica dos saldos das contas 232 e 238. Teste realizado com sucesso.</t>
+  </si>
+  <si>
+    <t>taxonomy_65_ok</t>
+  </si>
+  <si>
+    <t>taxonomy_65_nok</t>
+  </si>
+  <si>
+    <t>taxonomy_66_ok</t>
+  </si>
+  <si>
+    <t>taxonomy_66_nok</t>
+  </si>
+  <si>
+    <t>Foi efetuado um teste sobre a conta 239 - "Pessoal - Perdas por imparidade acumuladas - Adiantamentos - Aos órgãos sociais" (taxonomia 65) e verificado que esta conta, apresenta um saldo inferior ao saldo da conta 2321- "Pessoal - Adiantamentos - Aos órgãos sociais" (taxonomia 55)</t>
+  </si>
+  <si>
+    <t>Foi efetuado um teste sobre a conta 239 - "Pessoal - Perdas por imparidade acumuladas - Adiantamentos - Ao pessoal" (taxonomia 66) e verificado que esta conta, apresenta um saldo inferior ao saldo da conta 2322- "Pessoal - Adiantamentos - Ao pessoal" (taxonomia 56)</t>
+  </si>
+  <si>
+    <t>Foi efetuado um teste sobre a conta 219 - "Clientes - Perdas por imparidade acumuladas" e verificado que o saldo credor desta conta é superior à soma algébrica dos saldos das contas 211 a 217. Esta situação deve ser regularizada para uma correta submissão do ficheiro SAF-T.</t>
+  </si>
+  <si>
+    <t>Foi efetuado um teste sobre a conta 229 - "Fornecedores - Perdas por imparidade acumuladas" e verificado que o saldo credor desta conta é superior ao registado na conta 228 - "Fornecedores - Adiantamentos a fornecedores". Esta situação deve ser regularizada para uma correta submissão do ficheiro SAF-T.</t>
+  </si>
+  <si>
+    <t>Foi efetuado um teste sobre a conta 239 - "Pessoal - Perdas por imparidade acumuladas" e verificado que o saldo credor desta conta é superior à soma algébrica dos saldos das contas 232 e 238. Esta situação deve ser regularizada para uma correta submissão do ficheiro SAF-T.</t>
+  </si>
+  <si>
+    <t>Foi efetuado um teste sobre a conta 239 - "Pessoal - Perdas por imparidade acumuladas - Adiantamentos - Aos órgãos sociais" (taxonomia 65) e verificado que esta conta, apresenta um saldo superior ao saldo da conta 2321- "Pessoal - Adiantamentos - Aos órgãos sociais" (taxonomia 55). Esta situação deve ser regularizada para uma correta submissão do ficheiro SAF-T.</t>
+  </si>
+  <si>
+    <t>Foi efetuado um teste sobre a conta 239 - "Pessoal - Perdas por imparidade acumuladas - Adiantamentos - Ao pessoal" (taxonomia 66) e verificado que esta conta, apresenta um saldo superior ao saldo da conta 2322- "Pessoal - Adiantamentos - Ao pessoal" (taxonomia 56). Esta situação deve ser regularizada para uma correta submissão do ficheiro SAF-T.</t>
+  </si>
+  <si>
+    <t>A test was performed on account 219 - "Clientes - Perdas por imparidade acumuladas" and verified that the credit balance of this account is equal to or less than the algebraic sum of the balances of accounts 211 to 217. Test performed successfully.</t>
+  </si>
+  <si>
+    <t>A test was performed on account 219 - "Clientes - Perdas por imparidade acumuladas" and verified that the credit balance of this account is greater than the algebraic sum of the balances of accounts 211 to 217. This situation must be regularized for a correct submission of the file SAF-T.</t>
+  </si>
+  <si>
+    <t>A test was performed on account 229 - "Fornecedores - Perdas por imparidade acumuladas" and verified that the credit balance of this account is less than or equal to that in account 228 - "Suppliers - Advances to suppliers". Test performed successfully.</t>
+  </si>
+  <si>
+    <t>A test was performed on account 229 - "Fornecedores - Perdas por imparidade acumuladas" and verified that the credit balance of this account is greater than that recorded in account 228 - "Fornecedores - Adiantamentos a fornecedores". This situation must be regularized for a correct submission of the file SAF-T.</t>
+  </si>
+  <si>
+    <t>A test was performed on account 239 - "Pessoal - Perdas por imparidade acumuladas" and verified that this account has a balance less than or equal to the algebraic sum of the balances of accounts 232 and 238. Test performed successfully.</t>
+  </si>
+  <si>
+    <t>A test was performed on account 239 - "Pessoal - Perdas por imparidade acumuladas" and verified that the credit balance of this account is greater than the algebraic sum of the balances of accounts 232 and 238. This situation must be regularized for a correct submission of the file SAF-T.</t>
+  </si>
+  <si>
+    <t>A test was performed on account 239 - "Pessoal - Perdas por imparidade acumuladas - Adiantamentos - Aos órgãos sociais" (taxonomy 65) and verified that this account, has a balance lower than the balance of the account 2321 - "Pessoal - Adiantamentos - Aos órgãos sociais "(taxonomy 55)</t>
+  </si>
+  <si>
+    <t>A test was performed on account 239 - "Pessoal - Perdas por imparidade acumuladas - Adiantamentos - Aos órgãos sociais" (taxonomy 65) and verified that this account, has a balance higher than the balance of account 2321 - "Pessoal - Adiantamentos - Aos órgãos sociais"(taxonomy 55). This situation must be regularized for a correct submission of the file SAF-T.</t>
+  </si>
+  <si>
+    <t>A test was carried out on account 239 - "Pessoal - Perdas por imparidade acumuladas - Adiantamentos - Ao pessoal" (taxonomy 66) and verified that this account has a balance lower than the balance of account 2322 - "Pessoal - Adiantamentos - Ao pessoal" (taxonomy 56)</t>
+  </si>
+  <si>
+    <t>A test was performed on account 239 - "Pessoal - Perdas por imparidade acumuladas - Adiantamentos - Ao pessoal" (taxonomy 66) and verified that this account has a balance higher than the balance of account 2322 - "Pessoal - Adiantamentos - Ao pessoal" (taxonomy 56). This situation must be regularized for a correct submission of the file SAF-T.</t>
   </si>
 </sst>
 </file>
@@ -2878,8 +3040,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="i18n" displayName="i18n" ref="A1:G394" totalsRowShown="0" headerRowDxfId="6">
-  <autoFilter ref="A1:G394"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="i18n" displayName="i18n" ref="A1:G412" totalsRowShown="0" headerRowDxfId="6">
+  <autoFilter ref="A1:G412"/>
   <tableColumns count="7">
     <tableColumn id="1" name="key"/>
     <tableColumn id="2" name="pt" dataDxfId="5"/>
@@ -3156,10 +3318,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G394"/>
+  <dimension ref="A1:G412"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A371" workbookViewId="0">
-      <selection activeCell="A396" sqref="A396"/>
+    <sheetView tabSelected="1" topLeftCell="A407" workbookViewId="0">
+      <selection activeCell="A412" sqref="A412"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6759,13 +6921,13 @@
     </row>
     <row r="393" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A393" s="1" t="s">
+        <v>915</v>
+      </c>
+      <c r="B393" s="1" t="s">
         <v>886</v>
       </c>
-      <c r="B393" s="1" t="s">
-        <v>887</v>
-      </c>
       <c r="C393" s="1" t="s">
-        <v>890</v>
+        <v>888</v>
       </c>
       <c r="D393" s="4"/>
       <c r="E393" s="4"/>
@@ -6774,18 +6936,288 @@
     </row>
     <row r="394" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A394" s="1" t="s">
-        <v>888</v>
+        <v>904</v>
       </c>
       <c r="B394" s="1" t="s">
-        <v>889</v>
+        <v>902</v>
       </c>
       <c r="C394" s="1" t="s">
-        <v>891</v>
+        <v>903</v>
       </c>
       <c r="D394" s="4"/>
       <c r="E394" s="4"/>
       <c r="F394" s="4"/>
       <c r="G394" s="4"/>
+    </row>
+    <row r="395" spans="1:7" ht="112" x14ac:dyDescent="0.2">
+      <c r="A395" s="1" t="s">
+        <v>906</v>
+      </c>
+      <c r="B395" s="1" t="s">
+        <v>905</v>
+      </c>
+      <c r="C395" s="1" t="s">
+        <v>907</v>
+      </c>
+      <c r="D395" s="4"/>
+      <c r="E395" s="4"/>
+      <c r="F395" s="4"/>
+      <c r="G395" s="4"/>
+    </row>
+    <row r="396" spans="1:7" ht="48" x14ac:dyDescent="0.2">
+      <c r="A396" s="1" t="s">
+        <v>914</v>
+      </c>
+      <c r="B396" s="1" t="s">
+        <v>887</v>
+      </c>
+      <c r="C396" s="1" t="s">
+        <v>889</v>
+      </c>
+      <c r="D396" s="4"/>
+      <c r="E396" s="4"/>
+      <c r="F396" s="4"/>
+      <c r="G396" s="4"/>
+    </row>
+    <row r="397" spans="1:7" ht="64" x14ac:dyDescent="0.2">
+      <c r="A397" s="1" t="s">
+        <v>908</v>
+      </c>
+      <c r="B397" s="1" t="s">
+        <v>910</v>
+      </c>
+      <c r="C397" s="1" t="s">
+        <v>913</v>
+      </c>
+      <c r="D397" s="4"/>
+      <c r="E397" s="4"/>
+      <c r="F397" s="4"/>
+      <c r="G397" s="4"/>
+    </row>
+    <row r="398" spans="1:7" ht="112" x14ac:dyDescent="0.2">
+      <c r="A398" s="1" t="s">
+        <v>909</v>
+      </c>
+      <c r="B398" s="1" t="s">
+        <v>911</v>
+      </c>
+      <c r="C398" s="1" t="s">
+        <v>912</v>
+      </c>
+      <c r="D398" s="4"/>
+      <c r="E398" s="4"/>
+      <c r="F398" s="4"/>
+      <c r="G398" s="4"/>
+    </row>
+    <row r="399" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+      <c r="A399" s="1" t="s">
+        <v>900</v>
+      </c>
+      <c r="B399" s="1" t="s">
+        <v>891</v>
+      </c>
+      <c r="C399" s="1" t="s">
+        <v>896</v>
+      </c>
+      <c r="D399" s="4"/>
+      <c r="E399" s="4"/>
+      <c r="F399" s="4"/>
+      <c r="G399" s="4"/>
+    </row>
+    <row r="400" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+      <c r="A400" s="1" t="s">
+        <v>901</v>
+      </c>
+      <c r="B400" s="1" t="s">
+        <v>890</v>
+      </c>
+      <c r="C400" s="1" t="s">
+        <v>897</v>
+      </c>
+      <c r="D400" s="4"/>
+      <c r="E400" s="4"/>
+      <c r="F400" s="4"/>
+      <c r="G400" s="4"/>
+    </row>
+    <row r="401" spans="1:7" ht="64" x14ac:dyDescent="0.2">
+      <c r="A401" s="1" t="s">
+        <v>895</v>
+      </c>
+      <c r="B401" s="1" t="s">
+        <v>894</v>
+      </c>
+      <c r="C401" s="1" t="s">
+        <v>898</v>
+      </c>
+      <c r="D401" s="4"/>
+      <c r="E401" s="4"/>
+      <c r="F401" s="4"/>
+      <c r="G401" s="4"/>
+    </row>
+    <row r="402" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+      <c r="A402" s="1" t="s">
+        <v>893</v>
+      </c>
+      <c r="B402" s="1" t="s">
+        <v>892</v>
+      </c>
+      <c r="C402" s="1" t="s">
+        <v>899</v>
+      </c>
+      <c r="D402" s="4"/>
+      <c r="E402" s="4"/>
+      <c r="F402" s="4"/>
+      <c r="G402" s="4"/>
+    </row>
+    <row r="403" spans="1:7" ht="80" x14ac:dyDescent="0.2">
+      <c r="A403" s="1" t="s">
+        <v>917</v>
+      </c>
+      <c r="B403" s="1" t="s">
+        <v>916</v>
+      </c>
+      <c r="C403" s="1" t="s">
+        <v>936</v>
+      </c>
+      <c r="D403" s="4"/>
+      <c r="E403" s="4"/>
+      <c r="F403" s="4"/>
+      <c r="G403" s="4"/>
+    </row>
+    <row r="404" spans="1:7" ht="96" x14ac:dyDescent="0.2">
+      <c r="A404" s="1" t="s">
+        <v>918</v>
+      </c>
+      <c r="B404" s="1" t="s">
+        <v>931</v>
+      </c>
+      <c r="C404" s="1" t="s">
+        <v>937</v>
+      </c>
+      <c r="D404" s="4"/>
+      <c r="E404" s="4"/>
+      <c r="F404" s="4"/>
+      <c r="G404" s="4"/>
+    </row>
+    <row r="405" spans="1:7" ht="96" x14ac:dyDescent="0.2">
+      <c r="A405" s="1" t="s">
+        <v>919</v>
+      </c>
+      <c r="B405" s="1" t="s">
+        <v>923</v>
+      </c>
+      <c r="C405" s="1" t="s">
+        <v>938</v>
+      </c>
+      <c r="D405" s="4"/>
+      <c r="E405" s="4"/>
+      <c r="F405" s="4"/>
+      <c r="G405" s="4"/>
+    </row>
+    <row r="406" spans="1:7" ht="112" x14ac:dyDescent="0.2">
+      <c r="A406" s="1" t="s">
+        <v>920</v>
+      </c>
+      <c r="B406" s="1" t="s">
+        <v>932</v>
+      </c>
+      <c r="C406" s="1" t="s">
+        <v>939</v>
+      </c>
+      <c r="D406" s="4"/>
+      <c r="E406" s="4"/>
+      <c r="F406" s="4"/>
+      <c r="G406" s="4"/>
+    </row>
+    <row r="407" spans="1:7" ht="80" x14ac:dyDescent="0.2">
+      <c r="A407" s="1" t="s">
+        <v>922</v>
+      </c>
+      <c r="B407" s="1" t="s">
+        <v>924</v>
+      </c>
+      <c r="C407" s="1" t="s">
+        <v>940</v>
+      </c>
+      <c r="D407" s="4"/>
+      <c r="E407" s="4"/>
+      <c r="F407" s="4"/>
+      <c r="G407" s="4"/>
+    </row>
+    <row r="408" spans="1:7" ht="96" x14ac:dyDescent="0.2">
+      <c r="A408" s="1" t="s">
+        <v>921</v>
+      </c>
+      <c r="B408" s="1" t="s">
+        <v>933</v>
+      </c>
+      <c r="C408" s="1" t="s">
+        <v>941</v>
+      </c>
+      <c r="D408" s="4"/>
+      <c r="E408" s="4"/>
+      <c r="F408" s="4"/>
+      <c r="G408" s="4"/>
+    </row>
+    <row r="409" spans="1:7" ht="96" x14ac:dyDescent="0.2">
+      <c r="A409" s="1" t="s">
+        <v>925</v>
+      </c>
+      <c r="B409" s="1" t="s">
+        <v>929</v>
+      </c>
+      <c r="C409" s="1" t="s">
+        <v>942</v>
+      </c>
+      <c r="D409" s="4"/>
+      <c r="E409" s="4"/>
+      <c r="F409" s="4"/>
+      <c r="G409" s="4"/>
+    </row>
+    <row r="410" spans="1:7" ht="128" x14ac:dyDescent="0.2">
+      <c r="A410" s="1" t="s">
+        <v>926</v>
+      </c>
+      <c r="B410" s="1" t="s">
+        <v>934</v>
+      </c>
+      <c r="C410" s="1" t="s">
+        <v>943</v>
+      </c>
+      <c r="D410" s="4"/>
+      <c r="E410" s="4"/>
+      <c r="F410" s="4"/>
+      <c r="G410" s="4"/>
+    </row>
+    <row r="411" spans="1:7" ht="96" x14ac:dyDescent="0.2">
+      <c r="A411" s="1" t="s">
+        <v>927</v>
+      </c>
+      <c r="B411" s="1" t="s">
+        <v>930</v>
+      </c>
+      <c r="C411" s="1" t="s">
+        <v>944</v>
+      </c>
+      <c r="D411" s="4"/>
+      <c r="E411" s="4"/>
+      <c r="F411" s="4"/>
+      <c r="G411" s="4"/>
+    </row>
+    <row r="412" spans="1:7" ht="112" x14ac:dyDescent="0.2">
+      <c r="A412" s="1" t="s">
+        <v>928</v>
+      </c>
+      <c r="B412" s="1" t="s">
+        <v>935</v>
+      </c>
+      <c r="C412" s="1" t="s">
+        <v>945</v>
+      </c>
+      <c r="D412" s="4"/>
+      <c r="E412" s="4"/>
+      <c r="F412" s="4"/>
+      <c r="G412" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Each detail as a row, return json
</commit_message>
<xml_diff>
--- a/config/i18n/i18n.xlsx
+++ b/config/i18n/i18n.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-1980" yWindow="-19600" windowWidth="28800" windowHeight="17540" tabRatio="500"/>
+    <workbookView xWindow="-5080" yWindow="-21140" windowWidth="38400" windowHeight="21140" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2799,33 +2799,9 @@
     <t>The balance nature of all accounts and their concordance with the expected nature were verified. No differences found</t>
   </si>
   <si>
-    <t>rep_against_nature_ok</t>
-  </si>
-  <si>
-    <t>Foi verificada a natureza do saldo de todas as contas e a sua concordância com a natureza esperada. Identificaram-se as seguintes contas que apresentam um saldo contranatura e que deverão ser corrigidas para uma correta submissão do ficheiro SAF-T e construção das Demonstrações Financeiras: #Conta - Saldo (d) ou (c )</t>
-  </si>
-  <si>
-    <t>rep_against_nature_nok</t>
-  </si>
-  <si>
-    <t>The balance nature of all accounts and their concordance with the expected nature were verified. The following accounts that present a counter balance have been identified and should be corrected for a correct submission of the SAF-T file and construction of the Financial Statements: # Account - Balance (d) or (c)</t>
-  </si>
-  <si>
-    <t>rep_not_expected_balance_ok</t>
-  </si>
-  <si>
-    <t>rep_not_expected_balance_nok</t>
-  </si>
-  <si>
     <t>Foi verificada a natureza do saldo a apresentar em cada rubrica do balanço e a sua concordância com a natureza esperada. Não foram encontradas quaisquer diferenças</t>
   </si>
   <si>
-    <t>Foi verificada a natureza do saldo a apresentar em cada rubrica do balanço e a sua concordância com a natureza esperada. As seguintes rubricas do Balanço apresentam um saldo não esperado e deverão ser corrigidas para uma correta submissão do ficheiro SAF-T e construção das Demonstrações Financeiras: Rubrica balanço: - Saldo (d) ou (c )</t>
-  </si>
-  <si>
-    <t>The nature of the balance was verified in each balance sheet item and its agreement with the expected nature. The following balance sheet items present an unexpired balance and should be corrected for a right submission of the SAF-T file and construction of the Financial Statements: Balance sheet item: Balance (d) or (c)</t>
-  </si>
-  <si>
     <t>The nature of the balance was verified in each balance sheet item and its agreement with the expected nature. No differences found</t>
   </si>
   <si>
@@ -2923,6 +2899,30 @@
   </si>
   <si>
     <t>A test was performed on account 239 - "Pessoal - Perdas por imparidade acumuladas - Adiantamentos - Ao pessoal" (taxonomy 66) and verified that this account has a balance higher than the balance of account 2322 - "Pessoal - Adiantamentos - Ao pessoal" (taxonomy 56). This situation must be regularized for a correct submission of the file SAF-T.</t>
+  </si>
+  <si>
+    <t>Foi verificada a natureza do saldo de todas as contas e a sua concordância com a natureza esperada. Identificaram-se as seguintes contas que apresentam um saldo contranatura e que deverão ser corrigidas para uma correta submissão do ficheiro SAF-T e construção das Demonstrações Financeiras: {0}</t>
+  </si>
+  <si>
+    <t>Foi verificada a natureza do saldo a apresentar em cada rubrica do balanço e a sua concordância com a natureza esperada. As seguintes rubricas do Balanço apresentam um saldo não esperado e deverão ser corrigidas para uma correta submissão do ficheiro SAF-T e construção das Demonstrações Financeiras: {0}</t>
+  </si>
+  <si>
+    <t>The nature of the balance was verified in each balance sheet item and its agreement with the expected nature. The following balance sheet items present an unexpired balance and should be corrected for a right submission of the SAF-T file and construction of the Financial Statements: {0}</t>
+  </si>
+  <si>
+    <t>The balance nature of all accounts and their concordance with the expected nature were verified. The following accounts that present a counter balance have been identified and should be corrected for a correct submission of the SAF-T file and construction of the Financial Statements: {0}</t>
+  </si>
+  <si>
+    <t>rep_bs_against_nature_nok</t>
+  </si>
+  <si>
+    <t>rep_bs_against_nature_ok</t>
+  </si>
+  <si>
+    <t>do_not_allow_negatives_ok</t>
+  </si>
+  <si>
+    <t>do_not_allow_negatives_nok</t>
   </si>
 </sst>
 </file>
@@ -3320,8 +3320,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G412"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A407" workbookViewId="0">
-      <selection activeCell="A412" sqref="A412"/>
+    <sheetView tabSelected="1" topLeftCell="A385" workbookViewId="0">
+      <selection activeCell="A397" sqref="A397"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6921,7 +6921,7 @@
     </row>
     <row r="393" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A393" s="1" t="s">
-        <v>915</v>
+        <v>907</v>
       </c>
       <c r="B393" s="1" t="s">
         <v>886</v>
@@ -6936,7 +6936,7 @@
     </row>
     <row r="394" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A394" s="1" t="s">
-        <v>904</v>
+        <v>943</v>
       </c>
       <c r="B394" s="1" t="s">
         <v>902</v>
@@ -6949,15 +6949,15 @@
       <c r="F394" s="4"/>
       <c r="G394" s="4"/>
     </row>
-    <row r="395" spans="1:7" ht="112" x14ac:dyDescent="0.2">
+    <row r="395" spans="1:7" ht="96" x14ac:dyDescent="0.2">
       <c r="A395" s="1" t="s">
-        <v>906</v>
+        <v>942</v>
       </c>
       <c r="B395" s="1" t="s">
-        <v>905</v>
+        <v>938</v>
       </c>
       <c r="C395" s="1" t="s">
-        <v>907</v>
+        <v>941</v>
       </c>
       <c r="D395" s="4"/>
       <c r="E395" s="4"/>
@@ -6966,7 +6966,7 @@
     </row>
     <row r="396" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A396" s="1" t="s">
-        <v>914</v>
+        <v>906</v>
       </c>
       <c r="B396" s="1" t="s">
         <v>887</v>
@@ -6981,13 +6981,13 @@
     </row>
     <row r="397" spans="1:7" ht="64" x14ac:dyDescent="0.2">
       <c r="A397" s="1" t="s">
-        <v>908</v>
+        <v>944</v>
       </c>
       <c r="B397" s="1" t="s">
-        <v>910</v>
+        <v>904</v>
       </c>
       <c r="C397" s="1" t="s">
-        <v>913</v>
+        <v>905</v>
       </c>
       <c r="D397" s="4"/>
       <c r="E397" s="4"/>
@@ -6996,13 +6996,13 @@
     </row>
     <row r="398" spans="1:7" ht="112" x14ac:dyDescent="0.2">
       <c r="A398" s="1" t="s">
-        <v>909</v>
+        <v>945</v>
       </c>
       <c r="B398" s="1" t="s">
-        <v>911</v>
+        <v>939</v>
       </c>
       <c r="C398" s="1" t="s">
-        <v>912</v>
+        <v>940</v>
       </c>
       <c r="D398" s="4"/>
       <c r="E398" s="4"/>
@@ -7071,13 +7071,13 @@
     </row>
     <row r="403" spans="1:7" ht="80" x14ac:dyDescent="0.2">
       <c r="A403" s="1" t="s">
-        <v>917</v>
+        <v>909</v>
       </c>
       <c r="B403" s="1" t="s">
-        <v>916</v>
+        <v>908</v>
       </c>
       <c r="C403" s="1" t="s">
-        <v>936</v>
+        <v>928</v>
       </c>
       <c r="D403" s="4"/>
       <c r="E403" s="4"/>
@@ -7086,13 +7086,13 @@
     </row>
     <row r="404" spans="1:7" ht="96" x14ac:dyDescent="0.2">
       <c r="A404" s="1" t="s">
-        <v>918</v>
+        <v>910</v>
       </c>
       <c r="B404" s="1" t="s">
-        <v>931</v>
+        <v>923</v>
       </c>
       <c r="C404" s="1" t="s">
-        <v>937</v>
+        <v>929</v>
       </c>
       <c r="D404" s="4"/>
       <c r="E404" s="4"/>
@@ -7101,13 +7101,13 @@
     </row>
     <row r="405" spans="1:7" ht="96" x14ac:dyDescent="0.2">
       <c r="A405" s="1" t="s">
-        <v>919</v>
+        <v>911</v>
       </c>
       <c r="B405" s="1" t="s">
-        <v>923</v>
+        <v>915</v>
       </c>
       <c r="C405" s="1" t="s">
-        <v>938</v>
+        <v>930</v>
       </c>
       <c r="D405" s="4"/>
       <c r="E405" s="4"/>
@@ -7116,13 +7116,13 @@
     </row>
     <row r="406" spans="1:7" ht="112" x14ac:dyDescent="0.2">
       <c r="A406" s="1" t="s">
-        <v>920</v>
+        <v>912</v>
       </c>
       <c r="B406" s="1" t="s">
-        <v>932</v>
+        <v>924</v>
       </c>
       <c r="C406" s="1" t="s">
-        <v>939</v>
+        <v>931</v>
       </c>
       <c r="D406" s="4"/>
       <c r="E406" s="4"/>
@@ -7131,13 +7131,13 @@
     </row>
     <row r="407" spans="1:7" ht="80" x14ac:dyDescent="0.2">
       <c r="A407" s="1" t="s">
-        <v>922</v>
+        <v>914</v>
       </c>
       <c r="B407" s="1" t="s">
-        <v>924</v>
+        <v>916</v>
       </c>
       <c r="C407" s="1" t="s">
-        <v>940</v>
+        <v>932</v>
       </c>
       <c r="D407" s="4"/>
       <c r="E407" s="4"/>
@@ -7146,13 +7146,13 @@
     </row>
     <row r="408" spans="1:7" ht="96" x14ac:dyDescent="0.2">
       <c r="A408" s="1" t="s">
-        <v>921</v>
+        <v>913</v>
       </c>
       <c r="B408" s="1" t="s">
+        <v>925</v>
+      </c>
+      <c r="C408" s="1" t="s">
         <v>933</v>
-      </c>
-      <c r="C408" s="1" t="s">
-        <v>941</v>
       </c>
       <c r="D408" s="4"/>
       <c r="E408" s="4"/>
@@ -7161,13 +7161,13 @@
     </row>
     <row r="409" spans="1:7" ht="96" x14ac:dyDescent="0.2">
       <c r="A409" s="1" t="s">
-        <v>925</v>
+        <v>917</v>
       </c>
       <c r="B409" s="1" t="s">
-        <v>929</v>
+        <v>921</v>
       </c>
       <c r="C409" s="1" t="s">
-        <v>942</v>
+        <v>934</v>
       </c>
       <c r="D409" s="4"/>
       <c r="E409" s="4"/>
@@ -7176,13 +7176,13 @@
     </row>
     <row r="410" spans="1:7" ht="128" x14ac:dyDescent="0.2">
       <c r="A410" s="1" t="s">
+        <v>918</v>
+      </c>
+      <c r="B410" s="1" t="s">
         <v>926</v>
       </c>
-      <c r="B410" s="1" t="s">
-        <v>934</v>
-      </c>
       <c r="C410" s="1" t="s">
-        <v>943</v>
+        <v>935</v>
       </c>
       <c r="D410" s="4"/>
       <c r="E410" s="4"/>
@@ -7191,13 +7191,13 @@
     </row>
     <row r="411" spans="1:7" ht="96" x14ac:dyDescent="0.2">
       <c r="A411" s="1" t="s">
-        <v>927</v>
+        <v>919</v>
       </c>
       <c r="B411" s="1" t="s">
-        <v>930</v>
+        <v>922</v>
       </c>
       <c r="C411" s="1" t="s">
-        <v>944</v>
+        <v>936</v>
       </c>
       <c r="D411" s="4"/>
       <c r="E411" s="4"/>
@@ -7206,13 +7206,13 @@
     </row>
     <row r="412" spans="1:7" ht="112" x14ac:dyDescent="0.2">
       <c r="A412" s="1" t="s">
-        <v>928</v>
+        <v>920</v>
       </c>
       <c r="B412" s="1" t="s">
-        <v>935</v>
+        <v>927</v>
       </c>
       <c r="C412" s="1" t="s">
-        <v>945</v>
+        <v>937</v>
       </c>
       <c r="D412" s="4"/>
       <c r="E412" s="4"/>

</xml_diff>

<commit_message>
Revert "Each detail as a row, return json"
This reverts commit a7ec931b2ce60f05c0230bfa1a05139e495dab2a.
</commit_message>
<xml_diff>
--- a/config/i18n/i18n.xlsx
+++ b/config/i18n/i18n.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-5080" yWindow="-21140" windowWidth="38400" windowHeight="21140" tabRatio="500"/>
+    <workbookView xWindow="-1980" yWindow="-19600" windowWidth="28800" windowHeight="17540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2799,9 +2799,33 @@
     <t>The balance nature of all accounts and their concordance with the expected nature were verified. No differences found</t>
   </si>
   <si>
+    <t>rep_against_nature_ok</t>
+  </si>
+  <si>
+    <t>Foi verificada a natureza do saldo de todas as contas e a sua concordância com a natureza esperada. Identificaram-se as seguintes contas que apresentam um saldo contranatura e que deverão ser corrigidas para uma correta submissão do ficheiro SAF-T e construção das Demonstrações Financeiras: #Conta - Saldo (d) ou (c )</t>
+  </si>
+  <si>
+    <t>rep_against_nature_nok</t>
+  </si>
+  <si>
+    <t>The balance nature of all accounts and their concordance with the expected nature were verified. The following accounts that present a counter balance have been identified and should be corrected for a correct submission of the SAF-T file and construction of the Financial Statements: # Account - Balance (d) or (c)</t>
+  </si>
+  <si>
+    <t>rep_not_expected_balance_ok</t>
+  </si>
+  <si>
+    <t>rep_not_expected_balance_nok</t>
+  </si>
+  <si>
     <t>Foi verificada a natureza do saldo a apresentar em cada rubrica do balanço e a sua concordância com a natureza esperada. Não foram encontradas quaisquer diferenças</t>
   </si>
   <si>
+    <t>Foi verificada a natureza do saldo a apresentar em cada rubrica do balanço e a sua concordância com a natureza esperada. As seguintes rubricas do Balanço apresentam um saldo não esperado e deverão ser corrigidas para uma correta submissão do ficheiro SAF-T e construção das Demonstrações Financeiras: Rubrica balanço: - Saldo (d) ou (c )</t>
+  </si>
+  <si>
+    <t>The nature of the balance was verified in each balance sheet item and its agreement with the expected nature. The following balance sheet items present an unexpired balance and should be corrected for a right submission of the SAF-T file and construction of the Financial Statements: Balance sheet item: Balance (d) or (c)</t>
+  </si>
+  <si>
     <t>The nature of the balance was verified in each balance sheet item and its agreement with the expected nature. No differences found</t>
   </si>
   <si>
@@ -2899,30 +2923,6 @@
   </si>
   <si>
     <t>A test was performed on account 239 - "Pessoal - Perdas por imparidade acumuladas - Adiantamentos - Ao pessoal" (taxonomy 66) and verified that this account has a balance higher than the balance of account 2322 - "Pessoal - Adiantamentos - Ao pessoal" (taxonomy 56). This situation must be regularized for a correct submission of the file SAF-T.</t>
-  </si>
-  <si>
-    <t>Foi verificada a natureza do saldo de todas as contas e a sua concordância com a natureza esperada. Identificaram-se as seguintes contas que apresentam um saldo contranatura e que deverão ser corrigidas para uma correta submissão do ficheiro SAF-T e construção das Demonstrações Financeiras: {0}</t>
-  </si>
-  <si>
-    <t>Foi verificada a natureza do saldo a apresentar em cada rubrica do balanço e a sua concordância com a natureza esperada. As seguintes rubricas do Balanço apresentam um saldo não esperado e deverão ser corrigidas para uma correta submissão do ficheiro SAF-T e construção das Demonstrações Financeiras: {0}</t>
-  </si>
-  <si>
-    <t>The nature of the balance was verified in each balance sheet item and its agreement with the expected nature. The following balance sheet items present an unexpired balance and should be corrected for a right submission of the SAF-T file and construction of the Financial Statements: {0}</t>
-  </si>
-  <si>
-    <t>The balance nature of all accounts and their concordance with the expected nature were verified. The following accounts that present a counter balance have been identified and should be corrected for a correct submission of the SAF-T file and construction of the Financial Statements: {0}</t>
-  </si>
-  <si>
-    <t>rep_bs_against_nature_nok</t>
-  </si>
-  <si>
-    <t>rep_bs_against_nature_ok</t>
-  </si>
-  <si>
-    <t>do_not_allow_negatives_ok</t>
-  </si>
-  <si>
-    <t>do_not_allow_negatives_nok</t>
   </si>
 </sst>
 </file>
@@ -3320,8 +3320,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G412"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A385" workbookViewId="0">
-      <selection activeCell="A397" sqref="A397"/>
+    <sheetView tabSelected="1" topLeftCell="A407" workbookViewId="0">
+      <selection activeCell="A412" sqref="A412"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6921,7 +6921,7 @@
     </row>
     <row r="393" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A393" s="1" t="s">
-        <v>907</v>
+        <v>915</v>
       </c>
       <c r="B393" s="1" t="s">
         <v>886</v>
@@ -6936,7 +6936,7 @@
     </row>
     <row r="394" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A394" s="1" t="s">
-        <v>943</v>
+        <v>904</v>
       </c>
       <c r="B394" s="1" t="s">
         <v>902</v>
@@ -6949,15 +6949,15 @@
       <c r="F394" s="4"/>
       <c r="G394" s="4"/>
     </row>
-    <row r="395" spans="1:7" ht="96" x14ac:dyDescent="0.2">
+    <row r="395" spans="1:7" ht="112" x14ac:dyDescent="0.2">
       <c r="A395" s="1" t="s">
-        <v>942</v>
+        <v>906</v>
       </c>
       <c r="B395" s="1" t="s">
-        <v>938</v>
+        <v>905</v>
       </c>
       <c r="C395" s="1" t="s">
-        <v>941</v>
+        <v>907</v>
       </c>
       <c r="D395" s="4"/>
       <c r="E395" s="4"/>
@@ -6966,7 +6966,7 @@
     </row>
     <row r="396" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A396" s="1" t="s">
-        <v>906</v>
+        <v>914</v>
       </c>
       <c r="B396" s="1" t="s">
         <v>887</v>
@@ -6981,13 +6981,13 @@
     </row>
     <row r="397" spans="1:7" ht="64" x14ac:dyDescent="0.2">
       <c r="A397" s="1" t="s">
-        <v>944</v>
+        <v>908</v>
       </c>
       <c r="B397" s="1" t="s">
-        <v>904</v>
+        <v>910</v>
       </c>
       <c r="C397" s="1" t="s">
-        <v>905</v>
+        <v>913</v>
       </c>
       <c r="D397" s="4"/>
       <c r="E397" s="4"/>
@@ -6996,13 +6996,13 @@
     </row>
     <row r="398" spans="1:7" ht="112" x14ac:dyDescent="0.2">
       <c r="A398" s="1" t="s">
-        <v>945</v>
+        <v>909</v>
       </c>
       <c r="B398" s="1" t="s">
-        <v>939</v>
+        <v>911</v>
       </c>
       <c r="C398" s="1" t="s">
-        <v>940</v>
+        <v>912</v>
       </c>
       <c r="D398" s="4"/>
       <c r="E398" s="4"/>
@@ -7071,13 +7071,13 @@
     </row>
     <row r="403" spans="1:7" ht="80" x14ac:dyDescent="0.2">
       <c r="A403" s="1" t="s">
-        <v>909</v>
+        <v>917</v>
       </c>
       <c r="B403" s="1" t="s">
-        <v>908</v>
+        <v>916</v>
       </c>
       <c r="C403" s="1" t="s">
-        <v>928</v>
+        <v>936</v>
       </c>
       <c r="D403" s="4"/>
       <c r="E403" s="4"/>
@@ -7086,13 +7086,13 @@
     </row>
     <row r="404" spans="1:7" ht="96" x14ac:dyDescent="0.2">
       <c r="A404" s="1" t="s">
-        <v>910</v>
+        <v>918</v>
       </c>
       <c r="B404" s="1" t="s">
-        <v>923</v>
+        <v>931</v>
       </c>
       <c r="C404" s="1" t="s">
-        <v>929</v>
+        <v>937</v>
       </c>
       <c r="D404" s="4"/>
       <c r="E404" s="4"/>
@@ -7101,13 +7101,13 @@
     </row>
     <row r="405" spans="1:7" ht="96" x14ac:dyDescent="0.2">
       <c r="A405" s="1" t="s">
-        <v>911</v>
+        <v>919</v>
       </c>
       <c r="B405" s="1" t="s">
-        <v>915</v>
+        <v>923</v>
       </c>
       <c r="C405" s="1" t="s">
-        <v>930</v>
+        <v>938</v>
       </c>
       <c r="D405" s="4"/>
       <c r="E405" s="4"/>
@@ -7116,13 +7116,13 @@
     </row>
     <row r="406" spans="1:7" ht="112" x14ac:dyDescent="0.2">
       <c r="A406" s="1" t="s">
-        <v>912</v>
+        <v>920</v>
       </c>
       <c r="B406" s="1" t="s">
-        <v>924</v>
+        <v>932</v>
       </c>
       <c r="C406" s="1" t="s">
-        <v>931</v>
+        <v>939</v>
       </c>
       <c r="D406" s="4"/>
       <c r="E406" s="4"/>
@@ -7131,13 +7131,13 @@
     </row>
     <row r="407" spans="1:7" ht="80" x14ac:dyDescent="0.2">
       <c r="A407" s="1" t="s">
-        <v>914</v>
+        <v>922</v>
       </c>
       <c r="B407" s="1" t="s">
-        <v>916</v>
+        <v>924</v>
       </c>
       <c r="C407" s="1" t="s">
-        <v>932</v>
+        <v>940</v>
       </c>
       <c r="D407" s="4"/>
       <c r="E407" s="4"/>
@@ -7146,13 +7146,13 @@
     </row>
     <row r="408" spans="1:7" ht="96" x14ac:dyDescent="0.2">
       <c r="A408" s="1" t="s">
-        <v>913</v>
+        <v>921</v>
       </c>
       <c r="B408" s="1" t="s">
-        <v>925</v>
+        <v>933</v>
       </c>
       <c r="C408" s="1" t="s">
-        <v>933</v>
+        <v>941</v>
       </c>
       <c r="D408" s="4"/>
       <c r="E408" s="4"/>
@@ -7161,13 +7161,13 @@
     </row>
     <row r="409" spans="1:7" ht="96" x14ac:dyDescent="0.2">
       <c r="A409" s="1" t="s">
-        <v>917</v>
+        <v>925</v>
       </c>
       <c r="B409" s="1" t="s">
-        <v>921</v>
+        <v>929</v>
       </c>
       <c r="C409" s="1" t="s">
-        <v>934</v>
+        <v>942</v>
       </c>
       <c r="D409" s="4"/>
       <c r="E409" s="4"/>
@@ -7176,13 +7176,13 @@
     </row>
     <row r="410" spans="1:7" ht="128" x14ac:dyDescent="0.2">
       <c r="A410" s="1" t="s">
-        <v>918</v>
+        <v>926</v>
       </c>
       <c r="B410" s="1" t="s">
-        <v>926</v>
+        <v>934</v>
       </c>
       <c r="C410" s="1" t="s">
-        <v>935</v>
+        <v>943</v>
       </c>
       <c r="D410" s="4"/>
       <c r="E410" s="4"/>
@@ -7191,13 +7191,13 @@
     </row>
     <row r="411" spans="1:7" ht="96" x14ac:dyDescent="0.2">
       <c r="A411" s="1" t="s">
-        <v>919</v>
+        <v>927</v>
       </c>
       <c r="B411" s="1" t="s">
-        <v>922</v>
+        <v>930</v>
       </c>
       <c r="C411" s="1" t="s">
-        <v>936</v>
+        <v>944</v>
       </c>
       <c r="D411" s="4"/>
       <c r="E411" s="4"/>
@@ -7206,13 +7206,13 @@
     </row>
     <row r="412" spans="1:7" ht="112" x14ac:dyDescent="0.2">
       <c r="A412" s="1" t="s">
-        <v>920</v>
+        <v>928</v>
       </c>
       <c r="B412" s="1" t="s">
-        <v>927</v>
+        <v>935</v>
       </c>
       <c r="C412" s="1" t="s">
-        <v>937</v>
+        <v>945</v>
       </c>
       <c r="D412" s="4"/>
       <c r="E412" s="4"/>

</xml_diff>

<commit_message>
description changed in rules
</commit_message>
<xml_diff>
--- a/config/i18n/i18n.xlsx
+++ b/config/i18n/i18n.xlsx
@@ -2973,46 +2973,46 @@
     <t>taxonomy_66</t>
   </si>
   <si>
-    <t>Contas com saldo contra natura</t>
-  </si>
-  <si>
-    <t>Quando uma rubrica do balanço dá negativo e allow_negatives é falso</t>
-  </si>
-  <si>
-    <t>Conta 229 - "Fornecedores - Perdas por imparidade acumuladas"</t>
-  </si>
-  <si>
-    <t>Conta 219 - "Clientes - Perdas por imparidade acumuladas"</t>
-  </si>
-  <si>
-    <t>Conta 239 - "Pessoal - Perdas por imparidade acumuladas"</t>
-  </si>
-  <si>
-    <t>Conta 239 - "Pessoal - Perdas por imparidade acumuladas" - Taxonomia 65</t>
-  </si>
-  <si>
-    <t>Conta 239 - "Pessoal - Perdas por imparidade acumuladas" - Taxonomia 66</t>
-  </si>
-  <si>
-    <t>Accounts with unnatural balance</t>
-  </si>
-  <si>
-    <t>When a balance sheet item is negative and allow_negatives is false</t>
-  </si>
-  <si>
-    <t>Account 219</t>
-  </si>
-  <si>
-    <t>Account 229</t>
-  </si>
-  <si>
-    <t>Account 239</t>
-  </si>
-  <si>
-    <t>Account 239 - Taxonomy 65</t>
-  </si>
-  <si>
-    <t>Account 239 - Taxonomy 66</t>
+    <t>Teste à natureza do saldo das contas</t>
+  </si>
+  <si>
+    <t>Teste à natureza do saldo das rubricas do Balanço</t>
+  </si>
+  <si>
+    <t>Teste à conta 219- Clientes - Perdas por Imparidade</t>
+  </si>
+  <si>
+    <t>Teste à conta 229- Fornecedores - Perdas por Imparidade</t>
+  </si>
+  <si>
+    <t>Teste à conta 239- Pessoal - Perdas por Imparidade</t>
+  </si>
+  <si>
+    <t>Teste à conta 239- Pessoal - Perdas por imparidade acumuladas - Adiantamentos - Aos órgãos sociais</t>
+  </si>
+  <si>
+    <t>Teste à conta 239- Pessoal - Perdas por imparidade acumuladas - Adiantamentos - Ao pessoal</t>
+  </si>
+  <si>
+    <t>Test nature of the Balance Sheet items balance</t>
+  </si>
+  <si>
+    <t>Test nature of the account balance</t>
+  </si>
+  <si>
+    <t>Test account 219 - Customers - Losses due to Impairment</t>
+  </si>
+  <si>
+    <t>Test account 229- Suppliers - Losses due to Impairment</t>
+  </si>
+  <si>
+    <t>Test account 239- Personnel - Losses due to Impairment</t>
+  </si>
+  <si>
+    <t>Test account 239- Personnel - Accumulated impairment losses - Advances - To corporate bodies</t>
+  </si>
+  <si>
+    <t>Test account 239- Personnel - Accumulated impairment losses - Advances - To personnel</t>
   </si>
 </sst>
 </file>
@@ -3414,8 +3414,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G422"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A412" workbookViewId="0">
-      <selection activeCell="A421" sqref="A421"/>
+    <sheetView tabSelected="1" topLeftCell="A408" workbookViewId="0">
+      <selection activeCell="A422" sqref="A422"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7366,14 +7366,14 @@
         <v>962</v>
       </c>
       <c r="C416" s="1" t="s">
-        <v>969</v>
+        <v>970</v>
       </c>
       <c r="D416" s="4"/>
       <c r="E416" s="4"/>
       <c r="F416" s="4"/>
       <c r="G416" s="4"/>
     </row>
-    <row r="417" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+    <row r="417" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A417" s="1" t="s">
         <v>956</v>
       </c>
@@ -7381,7 +7381,7 @@
         <v>963</v>
       </c>
       <c r="C417" s="1" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
       <c r="D417" s="4"/>
       <c r="E417" s="4"/>
@@ -7393,7 +7393,7 @@
         <v>957</v>
       </c>
       <c r="B418" s="1" t="s">
-        <v>965</v>
+        <v>964</v>
       </c>
       <c r="C418" s="1" t="s">
         <v>971</v>
@@ -7408,7 +7408,7 @@
         <v>958</v>
       </c>
       <c r="B419" s="1" t="s">
-        <v>964</v>
+        <v>965</v>
       </c>
       <c r="C419" s="1" t="s">
         <v>972</v>

</xml_diff>

<commit_message>
Add SVAT titles to i18n
</commit_message>
<xml_diff>
--- a/config/i18n/i18n.xlsx
+++ b/config/i18n/i18n.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28109"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="29005"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/csantos/work/cw/sp-duh/config/i18n/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/krypton/Projects/cloudware/sp-duh/config/i18n/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-5080" yWindow="-21140" windowWidth="38400" windowHeight="21140" tabRatio="500"/>
+    <workbookView xWindow="7220" yWindow="-27280" windowWidth="38400" windowHeight="21140" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1033" uniqueCount="988">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1042" uniqueCount="997">
   <si>
     <t>key</t>
   </si>
@@ -3049,6 +3049,33 @@
   </si>
   <si>
     <t>{0} - Taxonomy {1}</t>
+  </si>
+  <si>
+    <t>svat_info</t>
+  </si>
+  <si>
+    <t>svat_error</t>
+  </si>
+  <si>
+    <t>svat_warn</t>
+  </si>
+  <si>
+    <t>Testes realizados com sucesso</t>
+  </si>
+  <si>
+    <t>Erros detetados</t>
+  </si>
+  <si>
+    <t>Avisos detetados</t>
+  </si>
+  <si>
+    <t>Success tests</t>
+  </si>
+  <si>
+    <t>Detected errors</t>
+  </si>
+  <si>
+    <t>Detected warnings</t>
   </si>
 </sst>
 </file>
@@ -3206,8 +3233,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="i18n" displayName="i18n" ref="A1:G426" totalsRowShown="0" headerRowDxfId="6">
-  <autoFilter ref="A1:G426"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="i18n" displayName="i18n" ref="A1:G429" totalsRowShown="0" headerRowDxfId="6">
+  <autoFilter ref="A1:G429"/>
   <tableColumns count="7">
     <tableColumn id="1" name="key"/>
     <tableColumn id="2" name="pt" dataDxfId="5"/>
@@ -3484,10 +3511,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G426"/>
+  <dimension ref="A1:G429"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A418" workbookViewId="0">
-      <selection activeCell="A426" sqref="A426"/>
+    <sheetView tabSelected="1" topLeftCell="A409" workbookViewId="0">
+      <selection activeCell="C430" sqref="C430"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7583,6 +7610,51 @@
         <v>984</v>
       </c>
     </row>
+    <row r="427" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A427" s="1" t="s">
+        <v>988</v>
+      </c>
+      <c r="B427" s="1" t="s">
+        <v>991</v>
+      </c>
+      <c r="C427" s="1" t="s">
+        <v>994</v>
+      </c>
+      <c r="D427" s="4"/>
+      <c r="E427" s="4"/>
+      <c r="F427" s="4"/>
+      <c r="G427" s="4"/>
+    </row>
+    <row r="428" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A428" s="1" t="s">
+        <v>989</v>
+      </c>
+      <c r="B428" s="1" t="s">
+        <v>992</v>
+      </c>
+      <c r="C428" s="1" t="s">
+        <v>995</v>
+      </c>
+      <c r="D428" s="4"/>
+      <c r="E428" s="4"/>
+      <c r="F428" s="4"/>
+      <c r="G428" s="4"/>
+    </row>
+    <row r="429" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A429" s="1" t="s">
+        <v>990</v>
+      </c>
+      <c r="B429" s="1" t="s">
+        <v>993</v>
+      </c>
+      <c r="C429" s="1" t="s">
+        <v>996</v>
+      </c>
+      <c r="D429" s="4"/>
+      <c r="E429" s="4"/>
+      <c r="F429" s="4"/>
+      <c r="G429" s="4"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
transaction_deleted must be considered 'Anulado' in pt
</commit_message>
<xml_diff>
--- a/config/i18n/i18n.xlsx
+++ b/config/i18n/i18n.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28109"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="29005"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/csantos/work/cw/sp-duh/config/i18n/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joana/work/sp-duh/config/i18n/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -3021,9 +3021,6 @@
     <t>transaction_deleted</t>
   </si>
   <si>
-    <t>Eliminado</t>
-  </si>
-  <si>
     <t>Finalizado</t>
   </si>
   <si>
@@ -3292,6 +3289,9 @@
   </si>
   <si>
     <t>Test taxonomy 70 NOK</t>
+  </si>
+  <si>
+    <t>Anulado</t>
   </si>
 </sst>
 </file>
@@ -3759,8 +3759,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G453"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A449" workbookViewId="0">
-      <selection activeCell="A453" sqref="A453"/>
+    <sheetView tabSelected="1" topLeftCell="A418" workbookViewId="0">
+      <selection activeCell="A426" sqref="A426"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6640,10 +6640,10 @@
         <v>867</v>
       </c>
       <c r="B328" s="1" t="s">
+        <v>994</v>
+      </c>
+      <c r="C328" s="1" t="s">
         <v>995</v>
-      </c>
-      <c r="C328" s="1" t="s">
-        <v>996</v>
       </c>
     </row>
     <row r="329" spans="1:3" ht="32" x14ac:dyDescent="0.2">
@@ -6651,10 +6651,10 @@
         <v>868</v>
       </c>
       <c r="B329" s="1" t="s">
+        <v>992</v>
+      </c>
+      <c r="C329" s="1" t="s">
         <v>993</v>
-      </c>
-      <c r="C329" s="1" t="s">
-        <v>994</v>
       </c>
     </row>
     <row r="330" spans="1:3" x14ac:dyDescent="0.2">
@@ -7810,13 +7810,13 @@
     </row>
     <row r="423" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A423" s="6" t="s">
+        <v>980</v>
+      </c>
+      <c r="B423" s="5" t="s">
         <v>981</v>
       </c>
-      <c r="B423" s="5" t="s">
+      <c r="C423" s="5" t="s">
         <v>982</v>
-      </c>
-      <c r="C423" s="5" t="s">
-        <v>983</v>
       </c>
       <c r="D423" s="4"/>
       <c r="E423" s="4"/>
@@ -7828,7 +7828,7 @@
         <v>972</v>
       </c>
       <c r="B424" s="1" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
       <c r="C424" s="1" t="s">
         <v>973</v>
@@ -7850,21 +7850,21 @@
         <v>977</v>
       </c>
       <c r="B426" s="1" t="s">
-        <v>978</v>
+        <v>1068</v>
       </c>
       <c r="C426" s="1" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
     </row>
     <row r="427" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A427" s="1" t="s">
-        <v>984</v>
+        <v>983</v>
       </c>
       <c r="B427" s="1" t="s">
-        <v>987</v>
+        <v>986</v>
       </c>
       <c r="C427" s="1" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
       <c r="D427" s="4"/>
       <c r="E427" s="4"/>
@@ -7873,13 +7873,13 @@
     </row>
     <row r="428" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A428" s="1" t="s">
-        <v>985</v>
+        <v>984</v>
       </c>
       <c r="B428" s="1" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
       <c r="C428" s="1" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="D428" s="4"/>
       <c r="E428" s="4"/>
@@ -7888,13 +7888,13 @@
     </row>
     <row r="429" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A429" s="1" t="s">
-        <v>986</v>
+        <v>985</v>
       </c>
       <c r="B429" s="1" t="s">
-        <v>989</v>
+        <v>988</v>
       </c>
       <c r="C429" s="1" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="D429" s="4"/>
       <c r="E429" s="4"/>
@@ -7903,13 +7903,13 @@
     </row>
     <row r="430" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A430" s="1" t="s">
+        <v>996</v>
+      </c>
+      <c r="B430" s="1" t="s">
         <v>997</v>
       </c>
-      <c r="B430" s="1" t="s">
+      <c r="C430" s="1" t="s">
         <v>998</v>
-      </c>
-      <c r="C430" s="1" t="s">
-        <v>999</v>
       </c>
       <c r="D430" s="4"/>
       <c r="E430" s="4"/>
@@ -7918,255 +7918,255 @@
     </row>
     <row r="431" spans="1:7" ht="160" x14ac:dyDescent="0.2">
       <c r="A431" s="1" t="s">
+        <v>999</v>
+      </c>
+      <c r="B431" s="1" t="s">
         <v>1000</v>
       </c>
-      <c r="B431" s="1" t="s">
+      <c r="C431" s="1" t="s">
         <v>1001</v>
-      </c>
-      <c r="C431" s="1" t="s">
-        <v>1002</v>
       </c>
     </row>
     <row r="432" spans="1:7" ht="176" x14ac:dyDescent="0.2">
       <c r="A432" s="1" t="s">
+        <v>1002</v>
+      </c>
+      <c r="B432" s="1" t="s">
         <v>1003</v>
       </c>
-      <c r="B432" s="1" t="s">
+      <c r="C432" s="1" t="s">
         <v>1004</v>
-      </c>
-      <c r="C432" s="1" t="s">
-        <v>1005</v>
       </c>
     </row>
     <row r="433" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A433" s="1" t="s">
+        <v>1005</v>
+      </c>
+      <c r="B433" s="1" t="s">
         <v>1006</v>
       </c>
-      <c r="B433" s="1" t="s">
+      <c r="C433" s="1" t="s">
         <v>1007</v>
-      </c>
-      <c r="C433" s="1" t="s">
-        <v>1008</v>
       </c>
     </row>
     <row r="434" spans="1:3" ht="96" x14ac:dyDescent="0.2">
       <c r="A434" s="1" t="s">
+        <v>1008</v>
+      </c>
+      <c r="B434" s="1" t="s">
         <v>1009</v>
       </c>
-      <c r="B434" s="1" t="s">
+      <c r="C434" s="1" t="s">
         <v>1010</v>
-      </c>
-      <c r="C434" s="1" t="s">
-        <v>1011</v>
       </c>
     </row>
     <row r="435" spans="1:3" ht="64" x14ac:dyDescent="0.2">
       <c r="A435" s="1" t="s">
+        <v>1011</v>
+      </c>
+      <c r="B435" s="1" t="s">
         <v>1012</v>
       </c>
-      <c r="B435" s="1" t="s">
+      <c r="C435" s="1" t="s">
         <v>1013</v>
-      </c>
-      <c r="C435" s="1" t="s">
-        <v>1014</v>
       </c>
     </row>
     <row r="436" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A436" s="1" t="s">
+        <v>1014</v>
+      </c>
+      <c r="B436" s="1" t="s">
         <v>1015</v>
       </c>
-      <c r="B436" s="1" t="s">
+      <c r="C436" s="1" t="s">
         <v>1016</v>
-      </c>
-      <c r="C436" s="1" t="s">
-        <v>1017</v>
       </c>
     </row>
     <row r="437" spans="1:3" ht="96" x14ac:dyDescent="0.2">
       <c r="A437" s="1" t="s">
+        <v>1017</v>
+      </c>
+      <c r="B437" s="1" t="s">
         <v>1018</v>
       </c>
-      <c r="B437" s="1" t="s">
+      <c r="C437" s="1" t="s">
         <v>1019</v>
-      </c>
-      <c r="C437" s="1" t="s">
-        <v>1020</v>
       </c>
     </row>
     <row r="438" spans="1:3" ht="128" x14ac:dyDescent="0.2">
       <c r="A438" s="1" t="s">
+        <v>1020</v>
+      </c>
+      <c r="B438" s="1" t="s">
         <v>1021</v>
       </c>
-      <c r="B438" s="1" t="s">
+      <c r="C438" s="7" t="s">
         <v>1022</v>
-      </c>
-      <c r="C438" s="7" t="s">
-        <v>1023</v>
       </c>
     </row>
     <row r="439" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A439" s="1" t="s">
+        <v>1023</v>
+      </c>
+      <c r="B439" s="1" t="s">
         <v>1024</v>
       </c>
-      <c r="B439" s="1" t="s">
+      <c r="C439" s="1" t="s">
         <v>1025</v>
-      </c>
-      <c r="C439" s="1" t="s">
-        <v>1026</v>
       </c>
     </row>
     <row r="440" spans="1:3" ht="64" x14ac:dyDescent="0.2">
       <c r="A440" s="1" t="s">
+        <v>1026</v>
+      </c>
+      <c r="B440" s="1" t="s">
         <v>1027</v>
       </c>
-      <c r="B440" s="1" t="s">
+      <c r="C440" s="1" t="s">
         <v>1028</v>
-      </c>
-      <c r="C440" s="1" t="s">
-        <v>1029</v>
       </c>
     </row>
     <row r="441" spans="1:3" ht="80" x14ac:dyDescent="0.2">
       <c r="A441" s="1" t="s">
+        <v>1029</v>
+      </c>
+      <c r="B441" s="1" t="s">
         <v>1030</v>
       </c>
-      <c r="B441" s="1" t="s">
+      <c r="C441" s="1" t="s">
         <v>1031</v>
-      </c>
-      <c r="C441" s="1" t="s">
-        <v>1032</v>
       </c>
     </row>
     <row r="442" spans="1:3" ht="48" x14ac:dyDescent="0.2">
       <c r="A442" s="1" t="s">
+        <v>1032</v>
+      </c>
+      <c r="B442" s="1" t="s">
         <v>1033</v>
       </c>
-      <c r="B442" s="1" t="s">
+      <c r="C442" s="1" t="s">
         <v>1034</v>
-      </c>
-      <c r="C442" s="1" t="s">
-        <v>1035</v>
       </c>
     </row>
     <row r="443" spans="1:3" ht="128" x14ac:dyDescent="0.2">
       <c r="A443" s="1" t="s">
+        <v>1035</v>
+      </c>
+      <c r="B443" s="1" t="s">
         <v>1036</v>
       </c>
-      <c r="B443" s="1" t="s">
+      <c r="C443" s="1" t="s">
         <v>1037</v>
-      </c>
-      <c r="C443" s="1" t="s">
-        <v>1038</v>
       </c>
     </row>
     <row r="444" spans="1:3" ht="144" x14ac:dyDescent="0.2">
       <c r="A444" s="1" t="s">
+        <v>1038</v>
+      </c>
+      <c r="B444" s="1" t="s">
         <v>1039</v>
       </c>
-      <c r="B444" s="1" t="s">
+      <c r="C444" s="1" t="s">
         <v>1040</v>
-      </c>
-      <c r="C444" s="1" t="s">
-        <v>1041</v>
       </c>
     </row>
     <row r="445" spans="1:3" ht="48" x14ac:dyDescent="0.2">
       <c r="A445" s="1" t="s">
+        <v>1041</v>
+      </c>
+      <c r="B445" s="1" t="s">
         <v>1042</v>
       </c>
-      <c r="B445" s="1" t="s">
+      <c r="C445" s="7" t="s">
         <v>1043</v>
-      </c>
-      <c r="C445" s="7" t="s">
-        <v>1044</v>
       </c>
     </row>
     <row r="446" spans="1:3" ht="128" x14ac:dyDescent="0.2">
       <c r="A446" s="1" t="s">
+        <v>1044</v>
+      </c>
+      <c r="B446" s="1" t="s">
         <v>1045</v>
       </c>
-      <c r="B446" s="1" t="s">
+      <c r="C446" s="7" t="s">
         <v>1046</v>
-      </c>
-      <c r="C446" s="7" t="s">
-        <v>1047</v>
       </c>
     </row>
     <row r="447" spans="1:3" ht="144" x14ac:dyDescent="0.2">
       <c r="A447" s="1" t="s">
+        <v>1047</v>
+      </c>
+      <c r="B447" s="1" t="s">
         <v>1048</v>
       </c>
-      <c r="B447" s="1" t="s">
+      <c r="C447" s="7" t="s">
         <v>1049</v>
-      </c>
-      <c r="C447" s="7" t="s">
-        <v>1050</v>
       </c>
     </row>
     <row r="448" spans="1:3" ht="48" x14ac:dyDescent="0.2">
       <c r="A448" s="1" t="s">
+        <v>1050</v>
+      </c>
+      <c r="B448" s="1" t="s">
         <v>1051</v>
       </c>
-      <c r="B448" s="1" t="s">
+      <c r="C448" s="7" t="s">
         <v>1052</v>
-      </c>
-      <c r="C448" s="7" t="s">
-        <v>1053</v>
       </c>
     </row>
     <row r="449" spans="1:3" ht="112" x14ac:dyDescent="0.2">
       <c r="A449" s="1" t="s">
+        <v>1053</v>
+      </c>
+      <c r="B449" s="1" t="s">
         <v>1054</v>
       </c>
-      <c r="B449" s="1" t="s">
+      <c r="C449" s="7" t="s">
         <v>1055</v>
-      </c>
-      <c r="C449" s="7" t="s">
-        <v>1056</v>
       </c>
     </row>
     <row r="450" spans="1:3" ht="128" x14ac:dyDescent="0.2">
       <c r="A450" s="1" t="s">
+        <v>1056</v>
+      </c>
+      <c r="B450" s="1" t="s">
         <v>1057</v>
       </c>
-      <c r="B450" s="1" t="s">
+      <c r="C450" s="7" t="s">
         <v>1058</v>
-      </c>
-      <c r="C450" s="7" t="s">
-        <v>1059</v>
       </c>
     </row>
     <row r="451" spans="1:3" ht="48" x14ac:dyDescent="0.2">
       <c r="A451" s="1" t="s">
+        <v>1059</v>
+      </c>
+      <c r="B451" s="1" t="s">
         <v>1060</v>
       </c>
-      <c r="B451" s="1" t="s">
+      <c r="C451" s="7" t="s">
         <v>1061</v>
-      </c>
-      <c r="C451" s="7" t="s">
-        <v>1062</v>
       </c>
     </row>
     <row r="452" spans="1:3" ht="128" x14ac:dyDescent="0.2">
       <c r="A452" s="1" t="s">
+        <v>1062</v>
+      </c>
+      <c r="B452" s="1" t="s">
         <v>1063</v>
       </c>
-      <c r="B452" s="1" t="s">
+      <c r="C452" s="7" t="s">
         <v>1064</v>
-      </c>
-      <c r="C452" s="7" t="s">
-        <v>1065</v>
       </c>
     </row>
     <row r="453" spans="1:3" ht="144" x14ac:dyDescent="0.2">
       <c r="A453" s="1" t="s">
+        <v>1065</v>
+      </c>
+      <c r="B453" s="1" t="s">
         <v>1066</v>
       </c>
-      <c r="B453" s="1" t="s">
+      <c r="C453" s="7" t="s">
         <v>1067</v>
-      </c>
-      <c r="C453" s="7" t="s">
-        <v>1068</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add messages for variable rules
</commit_message>
<xml_diff>
--- a/config/i18n/i18n.xlsx
+++ b/config/i18n/i18n.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="29005"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28109"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joana/work/sp-duh/config/i18n/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/csantos/work/cw/sp-duh/config/i18n/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1114" uniqueCount="1069">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1141" uniqueCount="1096">
   <si>
     <t>key</t>
   </si>
@@ -3292,6 +3292,87 @@
   </si>
   <si>
     <t>Anulado</t>
+  </si>
+  <si>
+    <t>account_219_var</t>
+  </si>
+  <si>
+    <t>account_219_var_ok</t>
+  </si>
+  <si>
+    <t>account_219_var_nok</t>
+  </si>
+  <si>
+    <t>Teste à conta 219- Clientes- Perdas por Imparidade, cliente a cliente</t>
+  </si>
+  <si>
+    <t>Foi efetuado um teste sobre a conta 219 - "Clientes - Perdas por imparidade acumuladas" e verificado que o saldo credor desta conta, cliente a cliente, é igual ou inferior à soma algébrica dos saldos das contas 211 a 217, de cada cliente. Teste realizado com sucesso.</t>
+  </si>
+  <si>
+    <t>Foi efetuado um teste sobre a conta 219 - "Clientes - Perdas por imparidade acumuladas" e verificado que o saldo credor desta conta, cliente a cliente, é superior à soma algébrica dos saldos das contas 211 a 217, para os seguintes clientes.</t>
+  </si>
+  <si>
+    <t>Test account 219 by client</t>
+  </si>
+  <si>
+    <t>Test account 219 by client OK</t>
+  </si>
+  <si>
+    <t>Test account 219 by client NOK</t>
+  </si>
+  <si>
+    <t>account_229_var</t>
+  </si>
+  <si>
+    <t>account_229_var_ok</t>
+  </si>
+  <si>
+    <t>account_229_var_nok</t>
+  </si>
+  <si>
+    <t>Foi efetuado um teste sobre a conta 229 - "Fornecedores - Perdas por imparidade acumuladas" e verificado que o saldo credor desta conta é, fornecedor e fornecedor, superior ao registado na conta 228 - "Fornecedores - Adiantamentos a fornecedores" para os seguintes fornecedores.</t>
+  </si>
+  <si>
+    <t>Test account 229 by supplier</t>
+  </si>
+  <si>
+    <t>Test account 229 by supplier OK</t>
+  </si>
+  <si>
+    <t>Test account 229 by supplier NOK</t>
+  </si>
+  <si>
+    <t>Test account 239 by employee</t>
+  </si>
+  <si>
+    <t>Test account 239 by employee OK</t>
+  </si>
+  <si>
+    <t>Test account 239 by employee NOK</t>
+  </si>
+  <si>
+    <t>account_239_var</t>
+  </si>
+  <si>
+    <t>account_239_var_ok</t>
+  </si>
+  <si>
+    <t>account_239_var_nok</t>
+  </si>
+  <si>
+    <t>Teste à conta 229- Fornecedores - Perdas por Imparidade, fornecedor a fornecedor</t>
+  </si>
+  <si>
+    <t>Foi efetuado um teste sobre a conta 229 - "Fornecedores - Perdas por imparidade acumuladas" e verificado que o saldo credor desta conta é, fornecedor a fornecedor, inferior ou igual ao saldo existente na conta 228 - "Fornecedores - Adiantamentos a fornecedores" de cada fornecedor. Teste realizado com sucesso.</t>
+  </si>
+  <si>
+    <t>Teste à conta 239- Pessoal - Perdas por Imparidade, colaborador a colaborador</t>
+  </si>
+  <si>
+    <t>Foi efetuado um teste sobre a conta 239 - "essoal - Perdas por Imparidade" e verificado que o saldo credor desta conta, colaborador a colaborador, é igual ou inferior à soma algébrica dos saldos das contas 232, 233, 234, 235, 236 e 238, de cada colaborador. Teste realizado com sucesso.</t>
+  </si>
+  <si>
+    <t>Foi efetuado um teste sobre a conta 239 - "essoal - Perdas por Imparidade" e verificado que o saldo credor desta conta, colaborador a colaborador, é igual ou superior à soma algébrica dos saldos das contas 232, 233, 234, 235, 236 e 238 para os seguintes colaboradores.</t>
   </si>
 </sst>
 </file>
@@ -3479,8 +3560,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="i18n" displayName="i18n" ref="A1:G453" totalsRowShown="0" headerRowDxfId="6">
-  <autoFilter ref="A1:G453"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="i18n" displayName="i18n" ref="A1:G462" totalsRowShown="0" headerRowDxfId="6">
+  <autoFilter ref="A1:G462"/>
   <tableColumns count="7">
     <tableColumn id="1" name="key"/>
     <tableColumn id="2" name="pt" dataDxfId="5"/>
@@ -3757,10 +3838,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G453"/>
+  <dimension ref="A1:G462"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A418" workbookViewId="0">
-      <selection activeCell="A426" sqref="A426"/>
+    <sheetView tabSelected="1" topLeftCell="A413" workbookViewId="0">
+      <selection activeCell="A413" sqref="A413"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7585,13 +7666,13 @@
     </row>
     <row r="408" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A408" s="1" t="s">
-        <v>954</v>
+        <v>1069</v>
       </c>
       <c r="B408" s="1" t="s">
-        <v>961</v>
+        <v>1072</v>
       </c>
       <c r="C408" s="1" t="s">
-        <v>968</v>
+        <v>1075</v>
       </c>
       <c r="D408" s="4"/>
       <c r="E408" s="4"/>
@@ -7600,28 +7681,28 @@
     </row>
     <row r="409" spans="1:7" ht="96" x14ac:dyDescent="0.2">
       <c r="A409" s="1" t="s">
-        <v>907</v>
+        <v>1070</v>
       </c>
       <c r="B409" s="1" t="s">
-        <v>911</v>
+        <v>1073</v>
       </c>
       <c r="C409" s="1" t="s">
-        <v>926</v>
+        <v>1076</v>
       </c>
       <c r="D409" s="4"/>
       <c r="E409" s="4"/>
       <c r="F409" s="4"/>
       <c r="G409" s="4"/>
     </row>
-    <row r="410" spans="1:7" ht="112" x14ac:dyDescent="0.2">
+    <row r="410" spans="1:7" ht="80" x14ac:dyDescent="0.2">
       <c r="A410" s="1" t="s">
-        <v>908</v>
+        <v>1071</v>
       </c>
       <c r="B410" s="1" t="s">
-        <v>920</v>
+        <v>1074</v>
       </c>
       <c r="C410" s="1" t="s">
-        <v>927</v>
+        <v>1077</v>
       </c>
       <c r="D410" s="4"/>
       <c r="E410" s="4"/>
@@ -7630,43 +7711,43 @@
     </row>
     <row r="411" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A411" s="1" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="B411" s="1" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="C411" s="1" t="s">
-        <v>969</v>
+        <v>968</v>
       </c>
       <c r="D411" s="4"/>
       <c r="E411" s="4"/>
       <c r="F411" s="4"/>
       <c r="G411" s="4"/>
     </row>
-    <row r="412" spans="1:7" ht="80" x14ac:dyDescent="0.2">
+    <row r="412" spans="1:7" ht="96" x14ac:dyDescent="0.2">
       <c r="A412" s="1" t="s">
-        <v>910</v>
+        <v>907</v>
       </c>
       <c r="B412" s="1" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
       <c r="C412" s="1" t="s">
-        <v>928</v>
+        <v>926</v>
       </c>
       <c r="D412" s="4"/>
       <c r="E412" s="4"/>
       <c r="F412" s="4"/>
       <c r="G412" s="4"/>
     </row>
-    <row r="413" spans="1:7" ht="96" x14ac:dyDescent="0.2">
+    <row r="413" spans="1:7" ht="112" x14ac:dyDescent="0.2">
       <c r="A413" s="1" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
       <c r="B413" s="1" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
       <c r="C413" s="1" t="s">
-        <v>929</v>
+        <v>927</v>
       </c>
       <c r="D413" s="4"/>
       <c r="E413" s="4"/>
@@ -7675,43 +7756,43 @@
     </row>
     <row r="414" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A414" s="1" t="s">
-        <v>956</v>
+        <v>1078</v>
       </c>
       <c r="B414" s="1" t="s">
-        <v>963</v>
+        <v>1091</v>
       </c>
       <c r="C414" s="1" t="s">
-        <v>970</v>
+        <v>1082</v>
       </c>
       <c r="D414" s="4"/>
       <c r="E414" s="4"/>
       <c r="F414" s="4"/>
       <c r="G414" s="4"/>
     </row>
-    <row r="415" spans="1:7" ht="96" x14ac:dyDescent="0.2">
+    <row r="415" spans="1:7" ht="112" x14ac:dyDescent="0.2">
       <c r="A415" s="1" t="s">
-        <v>913</v>
+        <v>1079</v>
       </c>
       <c r="B415" s="1" t="s">
-        <v>917</v>
+        <v>1092</v>
       </c>
       <c r="C415" s="1" t="s">
-        <v>930</v>
+        <v>1083</v>
       </c>
       <c r="D415" s="4"/>
       <c r="E415" s="4"/>
       <c r="F415" s="4"/>
       <c r="G415" s="4"/>
     </row>
-    <row r="416" spans="1:7" ht="128" x14ac:dyDescent="0.2">
+    <row r="416" spans="1:7" ht="96" x14ac:dyDescent="0.2">
       <c r="A416" s="1" t="s">
-        <v>914</v>
+        <v>1080</v>
       </c>
       <c r="B416" s="1" t="s">
-        <v>922</v>
+        <v>1081</v>
       </c>
       <c r="C416" s="1" t="s">
-        <v>931</v>
+        <v>1084</v>
       </c>
       <c r="D416" s="4"/>
       <c r="E416" s="4"/>
@@ -7720,166 +7801,178 @@
     </row>
     <row r="417" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A417" s="1" t="s">
-        <v>957</v>
+        <v>955</v>
       </c>
       <c r="B417" s="1" t="s">
-        <v>964</v>
+        <v>962</v>
       </c>
       <c r="C417" s="1" t="s">
-        <v>971</v>
+        <v>969</v>
       </c>
       <c r="D417" s="4"/>
       <c r="E417" s="4"/>
       <c r="F417" s="4"/>
       <c r="G417" s="4"/>
     </row>
-    <row r="418" spans="1:7" ht="96" x14ac:dyDescent="0.2">
+    <row r="418" spans="1:7" ht="80" x14ac:dyDescent="0.2">
       <c r="A418" s="1" t="s">
-        <v>915</v>
+        <v>910</v>
       </c>
       <c r="B418" s="1" t="s">
-        <v>918</v>
+        <v>912</v>
       </c>
       <c r="C418" s="1" t="s">
-        <v>932</v>
+        <v>928</v>
       </c>
       <c r="D418" s="4"/>
       <c r="E418" s="4"/>
       <c r="F418" s="4"/>
       <c r="G418" s="4"/>
     </row>
-    <row r="419" spans="1:7" ht="112" x14ac:dyDescent="0.2">
+    <row r="419" spans="1:7" ht="96" x14ac:dyDescent="0.2">
       <c r="A419" s="1" t="s">
-        <v>916</v>
+        <v>909</v>
       </c>
       <c r="B419" s="1" t="s">
-        <v>923</v>
+        <v>921</v>
       </c>
       <c r="C419" s="1" t="s">
-        <v>933</v>
+        <v>929</v>
       </c>
       <c r="D419" s="4"/>
       <c r="E419" s="4"/>
       <c r="F419" s="4"/>
       <c r="G419" s="4"/>
     </row>
-    <row r="420" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="420" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A420" s="1" t="s">
-        <v>942</v>
+        <v>1088</v>
       </c>
       <c r="B420" s="1" t="s">
-        <v>945</v>
+        <v>1093</v>
       </c>
       <c r="C420" s="1" t="s">
-        <v>948</v>
+        <v>1085</v>
       </c>
       <c r="D420" s="4"/>
       <c r="E420" s="4"/>
       <c r="F420" s="4"/>
       <c r="G420" s="4"/>
     </row>
-    <row r="421" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="421" spans="1:7" ht="96" x14ac:dyDescent="0.2">
       <c r="A421" s="1" t="s">
-        <v>943</v>
+        <v>1089</v>
       </c>
       <c r="B421" s="1" t="s">
-        <v>946</v>
+        <v>1094</v>
       </c>
       <c r="C421" s="1" t="s">
-        <v>949</v>
+        <v>1086</v>
       </c>
       <c r="D421" s="4"/>
       <c r="E421" s="4"/>
       <c r="F421" s="4"/>
       <c r="G421" s="4"/>
     </row>
-    <row r="422" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="422" spans="1:7" ht="96" x14ac:dyDescent="0.2">
       <c r="A422" s="1" t="s">
-        <v>944</v>
+        <v>1090</v>
       </c>
       <c r="B422" s="1" t="s">
-        <v>947</v>
+        <v>1095</v>
       </c>
       <c r="C422" s="1" t="s">
-        <v>950</v>
+        <v>1087</v>
       </c>
       <c r="D422" s="4"/>
       <c r="E422" s="4"/>
       <c r="F422" s="4"/>
       <c r="G422" s="4"/>
     </row>
-    <row r="423" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A423" s="6" t="s">
-        <v>980</v>
-      </c>
-      <c r="B423" s="5" t="s">
-        <v>981</v>
-      </c>
-      <c r="C423" s="5" t="s">
-        <v>982</v>
+    <row r="423" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+      <c r="A423" s="1" t="s">
+        <v>956</v>
+      </c>
+      <c r="B423" s="1" t="s">
+        <v>963</v>
+      </c>
+      <c r="C423" s="1" t="s">
+        <v>970</v>
       </c>
       <c r="D423" s="4"/>
       <c r="E423" s="4"/>
       <c r="F423" s="4"/>
       <c r="G423" s="4"/>
     </row>
-    <row r="424" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A424" t="s">
-        <v>972</v>
+    <row r="424" spans="1:7" ht="96" x14ac:dyDescent="0.2">
+      <c r="A424" s="1" t="s">
+        <v>913</v>
       </c>
       <c r="B424" s="1" t="s">
-        <v>978</v>
+        <v>917</v>
       </c>
       <c r="C424" s="1" t="s">
-        <v>973</v>
-      </c>
-    </row>
-    <row r="425" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A425" t="s">
-        <v>974</v>
+        <v>930</v>
+      </c>
+      <c r="D424" s="4"/>
+      <c r="E424" s="4"/>
+      <c r="F424" s="4"/>
+      <c r="G424" s="4"/>
+    </row>
+    <row r="425" spans="1:7" ht="128" x14ac:dyDescent="0.2">
+      <c r="A425" s="1" t="s">
+        <v>914</v>
       </c>
       <c r="B425" s="1" t="s">
-        <v>975</v>
+        <v>922</v>
       </c>
       <c r="C425" s="1" t="s">
-        <v>976</v>
-      </c>
-    </row>
-    <row r="426" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A426" t="s">
-        <v>977</v>
+        <v>931</v>
+      </c>
+      <c r="D425" s="4"/>
+      <c r="E425" s="4"/>
+      <c r="F425" s="4"/>
+      <c r="G425" s="4"/>
+    </row>
+    <row r="426" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+      <c r="A426" s="1" t="s">
+        <v>957</v>
       </c>
       <c r="B426" s="1" t="s">
-        <v>1068</v>
+        <v>964</v>
       </c>
       <c r="C426" s="1" t="s">
-        <v>979</v>
-      </c>
-    </row>
-    <row r="427" spans="1:7" x14ac:dyDescent="0.2">
+        <v>971</v>
+      </c>
+      <c r="D426" s="4"/>
+      <c r="E426" s="4"/>
+      <c r="F426" s="4"/>
+      <c r="G426" s="4"/>
+    </row>
+    <row r="427" spans="1:7" ht="96" x14ac:dyDescent="0.2">
       <c r="A427" s="1" t="s">
-        <v>983</v>
+        <v>915</v>
       </c>
       <c r="B427" s="1" t="s">
-        <v>986</v>
+        <v>918</v>
       </c>
       <c r="C427" s="1" t="s">
-        <v>989</v>
+        <v>932</v>
       </c>
       <c r="D427" s="4"/>
       <c r="E427" s="4"/>
       <c r="F427" s="4"/>
       <c r="G427" s="4"/>
     </row>
-    <row r="428" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="428" spans="1:7" ht="112" x14ac:dyDescent="0.2">
       <c r="A428" s="1" t="s">
-        <v>984</v>
+        <v>916</v>
       </c>
       <c r="B428" s="1" t="s">
-        <v>987</v>
+        <v>923</v>
       </c>
       <c r="C428" s="1" t="s">
-        <v>990</v>
+        <v>933</v>
       </c>
       <c r="D428" s="4"/>
       <c r="E428" s="4"/>
@@ -7888,284 +7981,407 @@
     </row>
     <row r="429" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A429" s="1" t="s">
-        <v>985</v>
+        <v>942</v>
       </c>
       <c r="B429" s="1" t="s">
-        <v>988</v>
+        <v>945</v>
       </c>
       <c r="C429" s="1" t="s">
-        <v>991</v>
+        <v>948</v>
       </c>
       <c r="D429" s="4"/>
       <c r="E429" s="4"/>
       <c r="F429" s="4"/>
       <c r="G429" s="4"/>
     </row>
-    <row r="430" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+    <row r="430" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A430" s="1" t="s">
-        <v>996</v>
+        <v>943</v>
       </c>
       <c r="B430" s="1" t="s">
-        <v>997</v>
+        <v>946</v>
       </c>
       <c r="C430" s="1" t="s">
-        <v>998</v>
+        <v>949</v>
       </c>
       <c r="D430" s="4"/>
       <c r="E430" s="4"/>
       <c r="F430" s="4"/>
       <c r="G430" s="4"/>
     </row>
-    <row r="431" spans="1:7" ht="160" x14ac:dyDescent="0.2">
+    <row r="431" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A431" s="1" t="s">
+        <v>944</v>
+      </c>
+      <c r="B431" s="1" t="s">
+        <v>947</v>
+      </c>
+      <c r="C431" s="1" t="s">
+        <v>950</v>
+      </c>
+      <c r="D431" s="4"/>
+      <c r="E431" s="4"/>
+      <c r="F431" s="4"/>
+      <c r="G431" s="4"/>
+    </row>
+    <row r="432" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A432" s="6" t="s">
+        <v>980</v>
+      </c>
+      <c r="B432" s="5" t="s">
+        <v>981</v>
+      </c>
+      <c r="C432" s="5" t="s">
+        <v>982</v>
+      </c>
+      <c r="D432" s="4"/>
+      <c r="E432" s="4"/>
+      <c r="F432" s="4"/>
+      <c r="G432" s="4"/>
+    </row>
+    <row r="433" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A433" t="s">
+        <v>972</v>
+      </c>
+      <c r="B433" s="1" t="s">
+        <v>978</v>
+      </c>
+      <c r="C433" s="1" t="s">
+        <v>973</v>
+      </c>
+    </row>
+    <row r="434" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A434" t="s">
+        <v>974</v>
+      </c>
+      <c r="B434" s="1" t="s">
+        <v>975</v>
+      </c>
+      <c r="C434" s="1" t="s">
+        <v>976</v>
+      </c>
+    </row>
+    <row r="435" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A435" t="s">
+        <v>977</v>
+      </c>
+      <c r="B435" s="1" t="s">
+        <v>1068</v>
+      </c>
+      <c r="C435" s="1" t="s">
+        <v>979</v>
+      </c>
+    </row>
+    <row r="436" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A436" s="1" t="s">
+        <v>983</v>
+      </c>
+      <c r="B436" s="1" t="s">
+        <v>986</v>
+      </c>
+      <c r="C436" s="1" t="s">
+        <v>989</v>
+      </c>
+      <c r="D436" s="4"/>
+      <c r="E436" s="4"/>
+      <c r="F436" s="4"/>
+      <c r="G436" s="4"/>
+    </row>
+    <row r="437" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A437" s="1" t="s">
+        <v>984</v>
+      </c>
+      <c r="B437" s="1" t="s">
+        <v>987</v>
+      </c>
+      <c r="C437" s="1" t="s">
+        <v>990</v>
+      </c>
+      <c r="D437" s="4"/>
+      <c r="E437" s="4"/>
+      <c r="F437" s="4"/>
+      <c r="G437" s="4"/>
+    </row>
+    <row r="438" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A438" s="1" t="s">
+        <v>985</v>
+      </c>
+      <c r="B438" s="1" t="s">
+        <v>988</v>
+      </c>
+      <c r="C438" s="1" t="s">
+        <v>991</v>
+      </c>
+      <c r="D438" s="4"/>
+      <c r="E438" s="4"/>
+      <c r="F438" s="4"/>
+      <c r="G438" s="4"/>
+    </row>
+    <row r="439" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+      <c r="A439" s="1" t="s">
+        <v>996</v>
+      </c>
+      <c r="B439" s="1" t="s">
+        <v>997</v>
+      </c>
+      <c r="C439" s="1" t="s">
+        <v>998</v>
+      </c>
+      <c r="D439" s="4"/>
+      <c r="E439" s="4"/>
+      <c r="F439" s="4"/>
+      <c r="G439" s="4"/>
+    </row>
+    <row r="440" spans="1:7" ht="160" x14ac:dyDescent="0.2">
+      <c r="A440" s="1" t="s">
         <v>999</v>
       </c>
-      <c r="B431" s="1" t="s">
+      <c r="B440" s="1" t="s">
         <v>1000</v>
       </c>
-      <c r="C431" s="1" t="s">
+      <c r="C440" s="1" t="s">
         <v>1001</v>
       </c>
     </row>
-    <row r="432" spans="1:7" ht="176" x14ac:dyDescent="0.2">
-      <c r="A432" s="1" t="s">
+    <row r="441" spans="1:7" ht="176" x14ac:dyDescent="0.2">
+      <c r="A441" s="1" t="s">
         <v>1002</v>
       </c>
-      <c r="B432" s="1" t="s">
+      <c r="B441" s="1" t="s">
         <v>1003</v>
       </c>
-      <c r="C432" s="1" t="s">
+      <c r="C441" s="1" t="s">
         <v>1004</v>
       </c>
     </row>
-    <row r="433" spans="1:3" ht="32" x14ac:dyDescent="0.2">
-      <c r="A433" s="1" t="s">
+    <row r="442" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+      <c r="A442" s="1" t="s">
         <v>1005</v>
       </c>
-      <c r="B433" s="1" t="s">
+      <c r="B442" s="1" t="s">
         <v>1006</v>
       </c>
-      <c r="C433" s="1" t="s">
+      <c r="C442" s="1" t="s">
         <v>1007</v>
       </c>
     </row>
-    <row r="434" spans="1:3" ht="96" x14ac:dyDescent="0.2">
-      <c r="A434" s="1" t="s">
+    <row r="443" spans="1:7" ht="96" x14ac:dyDescent="0.2">
+      <c r="A443" s="1" t="s">
         <v>1008</v>
       </c>
-      <c r="B434" s="1" t="s">
+      <c r="B443" s="1" t="s">
         <v>1009</v>
       </c>
-      <c r="C434" s="1" t="s">
+      <c r="C443" s="1" t="s">
         <v>1010</v>
       </c>
     </row>
-    <row r="435" spans="1:3" ht="64" x14ac:dyDescent="0.2">
-      <c r="A435" s="1" t="s">
+    <row r="444" spans="1:7" ht="64" x14ac:dyDescent="0.2">
+      <c r="A444" s="1" t="s">
         <v>1011</v>
       </c>
-      <c r="B435" s="1" t="s">
+      <c r="B444" s="1" t="s">
         <v>1012</v>
       </c>
-      <c r="C435" s="1" t="s">
+      <c r="C444" s="1" t="s">
         <v>1013</v>
       </c>
     </row>
-    <row r="436" spans="1:3" ht="32" x14ac:dyDescent="0.2">
-      <c r="A436" s="1" t="s">
+    <row r="445" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+      <c r="A445" s="1" t="s">
         <v>1014</v>
       </c>
-      <c r="B436" s="1" t="s">
+      <c r="B445" s="1" t="s">
         <v>1015</v>
       </c>
-      <c r="C436" s="1" t="s">
+      <c r="C445" s="1" t="s">
         <v>1016</v>
       </c>
     </row>
-    <row r="437" spans="1:3" ht="96" x14ac:dyDescent="0.2">
-      <c r="A437" s="1" t="s">
+    <row r="446" spans="1:7" ht="96" x14ac:dyDescent="0.2">
+      <c r="A446" s="1" t="s">
         <v>1017</v>
       </c>
-      <c r="B437" s="1" t="s">
+      <c r="B446" s="1" t="s">
         <v>1018</v>
       </c>
-      <c r="C437" s="1" t="s">
+      <c r="C446" s="1" t="s">
         <v>1019</v>
       </c>
     </row>
-    <row r="438" spans="1:3" ht="128" x14ac:dyDescent="0.2">
-      <c r="A438" s="1" t="s">
+    <row r="447" spans="1:7" ht="128" x14ac:dyDescent="0.2">
+      <c r="A447" s="1" t="s">
         <v>1020</v>
       </c>
-      <c r="B438" s="1" t="s">
+      <c r="B447" s="1" t="s">
         <v>1021</v>
       </c>
-      <c r="C438" s="7" t="s">
+      <c r="C447" s="7" t="s">
         <v>1022</v>
       </c>
     </row>
-    <row r="439" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A439" s="1" t="s">
+    <row r="448" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A448" s="1" t="s">
         <v>1023</v>
       </c>
-      <c r="B439" s="1" t="s">
+      <c r="B448" s="1" t="s">
         <v>1024</v>
       </c>
-      <c r="C439" s="1" t="s">
+      <c r="C448" s="1" t="s">
         <v>1025</v>
       </c>
     </row>
-    <row r="440" spans="1:3" ht="64" x14ac:dyDescent="0.2">
-      <c r="A440" s="1" t="s">
+    <row r="449" spans="1:3" ht="64" x14ac:dyDescent="0.2">
+      <c r="A449" s="1" t="s">
         <v>1026</v>
       </c>
-      <c r="B440" s="1" t="s">
+      <c r="B449" s="1" t="s">
         <v>1027</v>
       </c>
-      <c r="C440" s="1" t="s">
+      <c r="C449" s="1" t="s">
         <v>1028</v>
       </c>
     </row>
-    <row r="441" spans="1:3" ht="80" x14ac:dyDescent="0.2">
-      <c r="A441" s="1" t="s">
+    <row r="450" spans="1:3" ht="80" x14ac:dyDescent="0.2">
+      <c r="A450" s="1" t="s">
         <v>1029</v>
       </c>
-      <c r="B441" s="1" t="s">
+      <c r="B450" s="1" t="s">
         <v>1030</v>
       </c>
-      <c r="C441" s="1" t="s">
+      <c r="C450" s="1" t="s">
         <v>1031</v>
-      </c>
-    </row>
-    <row r="442" spans="1:3" ht="48" x14ac:dyDescent="0.2">
-      <c r="A442" s="1" t="s">
-        <v>1032</v>
-      </c>
-      <c r="B442" s="1" t="s">
-        <v>1033</v>
-      </c>
-      <c r="C442" s="1" t="s">
-        <v>1034</v>
-      </c>
-    </row>
-    <row r="443" spans="1:3" ht="128" x14ac:dyDescent="0.2">
-      <c r="A443" s="1" t="s">
-        <v>1035</v>
-      </c>
-      <c r="B443" s="1" t="s">
-        <v>1036</v>
-      </c>
-      <c r="C443" s="1" t="s">
-        <v>1037</v>
-      </c>
-    </row>
-    <row r="444" spans="1:3" ht="144" x14ac:dyDescent="0.2">
-      <c r="A444" s="1" t="s">
-        <v>1038</v>
-      </c>
-      <c r="B444" s="1" t="s">
-        <v>1039</v>
-      </c>
-      <c r="C444" s="1" t="s">
-        <v>1040</v>
-      </c>
-    </row>
-    <row r="445" spans="1:3" ht="48" x14ac:dyDescent="0.2">
-      <c r="A445" s="1" t="s">
-        <v>1041</v>
-      </c>
-      <c r="B445" s="1" t="s">
-        <v>1042</v>
-      </c>
-      <c r="C445" s="7" t="s">
-        <v>1043</v>
-      </c>
-    </row>
-    <row r="446" spans="1:3" ht="128" x14ac:dyDescent="0.2">
-      <c r="A446" s="1" t="s">
-        <v>1044</v>
-      </c>
-      <c r="B446" s="1" t="s">
-        <v>1045</v>
-      </c>
-      <c r="C446" s="7" t="s">
-        <v>1046</v>
-      </c>
-    </row>
-    <row r="447" spans="1:3" ht="144" x14ac:dyDescent="0.2">
-      <c r="A447" s="1" t="s">
-        <v>1047</v>
-      </c>
-      <c r="B447" s="1" t="s">
-        <v>1048</v>
-      </c>
-      <c r="C447" s="7" t="s">
-        <v>1049</v>
-      </c>
-    </row>
-    <row r="448" spans="1:3" ht="48" x14ac:dyDescent="0.2">
-      <c r="A448" s="1" t="s">
-        <v>1050</v>
-      </c>
-      <c r="B448" s="1" t="s">
-        <v>1051</v>
-      </c>
-      <c r="C448" s="7" t="s">
-        <v>1052</v>
-      </c>
-    </row>
-    <row r="449" spans="1:3" ht="112" x14ac:dyDescent="0.2">
-      <c r="A449" s="1" t="s">
-        <v>1053</v>
-      </c>
-      <c r="B449" s="1" t="s">
-        <v>1054</v>
-      </c>
-      <c r="C449" s="7" t="s">
-        <v>1055</v>
-      </c>
-    </row>
-    <row r="450" spans="1:3" ht="128" x14ac:dyDescent="0.2">
-      <c r="A450" s="1" t="s">
-        <v>1056</v>
-      </c>
-      <c r="B450" s="1" t="s">
-        <v>1057</v>
-      </c>
-      <c r="C450" s="7" t="s">
-        <v>1058</v>
       </c>
     </row>
     <row r="451" spans="1:3" ht="48" x14ac:dyDescent="0.2">
       <c r="A451" s="1" t="s">
-        <v>1059</v>
+        <v>1032</v>
       </c>
       <c r="B451" s="1" t="s">
-        <v>1060</v>
-      </c>
-      <c r="C451" s="7" t="s">
-        <v>1061</v>
+        <v>1033</v>
+      </c>
+      <c r="C451" s="1" t="s">
+        <v>1034</v>
       </c>
     </row>
     <row r="452" spans="1:3" ht="128" x14ac:dyDescent="0.2">
       <c r="A452" s="1" t="s">
-        <v>1062</v>
+        <v>1035</v>
       </c>
       <c r="B452" s="1" t="s">
-        <v>1063</v>
-      </c>
-      <c r="C452" s="7" t="s">
-        <v>1064</v>
+        <v>1036</v>
+      </c>
+      <c r="C452" s="1" t="s">
+        <v>1037</v>
       </c>
     </row>
     <row r="453" spans="1:3" ht="144" x14ac:dyDescent="0.2">
       <c r="A453" s="1" t="s">
+        <v>1038</v>
+      </c>
+      <c r="B453" s="1" t="s">
+        <v>1039</v>
+      </c>
+      <c r="C453" s="1" t="s">
+        <v>1040</v>
+      </c>
+    </row>
+    <row r="454" spans="1:3" ht="48" x14ac:dyDescent="0.2">
+      <c r="A454" s="1" t="s">
+        <v>1041</v>
+      </c>
+      <c r="B454" s="1" t="s">
+        <v>1042</v>
+      </c>
+      <c r="C454" s="7" t="s">
+        <v>1043</v>
+      </c>
+    </row>
+    <row r="455" spans="1:3" ht="128" x14ac:dyDescent="0.2">
+      <c r="A455" s="1" t="s">
+        <v>1044</v>
+      </c>
+      <c r="B455" s="1" t="s">
+        <v>1045</v>
+      </c>
+      <c r="C455" s="7" t="s">
+        <v>1046</v>
+      </c>
+    </row>
+    <row r="456" spans="1:3" ht="144" x14ac:dyDescent="0.2">
+      <c r="A456" s="1" t="s">
+        <v>1047</v>
+      </c>
+      <c r="B456" s="1" t="s">
+        <v>1048</v>
+      </c>
+      <c r="C456" s="7" t="s">
+        <v>1049</v>
+      </c>
+    </row>
+    <row r="457" spans="1:3" ht="48" x14ac:dyDescent="0.2">
+      <c r="A457" s="1" t="s">
+        <v>1050</v>
+      </c>
+      <c r="B457" s="1" t="s">
+        <v>1051</v>
+      </c>
+      <c r="C457" s="7" t="s">
+        <v>1052</v>
+      </c>
+    </row>
+    <row r="458" spans="1:3" ht="112" x14ac:dyDescent="0.2">
+      <c r="A458" s="1" t="s">
+        <v>1053</v>
+      </c>
+      <c r="B458" s="1" t="s">
+        <v>1054</v>
+      </c>
+      <c r="C458" s="7" t="s">
+        <v>1055</v>
+      </c>
+    </row>
+    <row r="459" spans="1:3" ht="128" x14ac:dyDescent="0.2">
+      <c r="A459" s="1" t="s">
+        <v>1056</v>
+      </c>
+      <c r="B459" s="1" t="s">
+        <v>1057</v>
+      </c>
+      <c r="C459" s="7" t="s">
+        <v>1058</v>
+      </c>
+    </row>
+    <row r="460" spans="1:3" ht="48" x14ac:dyDescent="0.2">
+      <c r="A460" s="1" t="s">
+        <v>1059</v>
+      </c>
+      <c r="B460" s="1" t="s">
+        <v>1060</v>
+      </c>
+      <c r="C460" s="7" t="s">
+        <v>1061</v>
+      </c>
+    </row>
+    <row r="461" spans="1:3" ht="128" x14ac:dyDescent="0.2">
+      <c r="A461" s="1" t="s">
+        <v>1062</v>
+      </c>
+      <c r="B461" s="1" t="s">
+        <v>1063</v>
+      </c>
+      <c r="C461" s="7" t="s">
+        <v>1064</v>
+      </c>
+    </row>
+    <row r="462" spans="1:3" ht="144" x14ac:dyDescent="0.2">
+      <c r="A462" s="1" t="s">
         <v>1065</v>
       </c>
-      <c r="B453" s="1" t="s">
+      <c r="B462" s="1" t="s">
         <v>1066</v>
       </c>
-      <c r="C453" s="7" t="s">
+      <c r="C462" s="7" t="s">
         <v>1067</v>
       </c>
     </row>

</xml_diff>

<commit_message>
"Fix" (the customer is always right, anyway, part II) en localised texts for sales document types descriptions: ALL document type descriptions were rolled-back to their previous (toconline's billing.en.yml) versions
</commit_message>
<xml_diff>
--- a/config/i18n/i18n.xlsx
+++ b/config/i18n/i18n.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="25725"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="500"/>
+    <workbookView xWindow="3420" yWindow="700" windowWidth="28800" windowHeight="17540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1186" uniqueCount="1141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1186" uniqueCount="1144">
   <si>
     <t>key</t>
   </si>
@@ -2088,18 +2088,12 @@
     <t>Fatura-recibo</t>
   </si>
   <si>
-    <t>Invoice-Receipt</t>
-  </si>
-  <si>
     <t>document_type_GC</t>
   </si>
   <si>
     <t>Guia de consignação</t>
   </si>
   <si>
-    <t xml:space="preserve">Consignment movement of goods </t>
-  </si>
-  <si>
     <t>document_type_GD</t>
   </si>
   <si>
@@ -2130,9 +2124,6 @@
     <t>Guia de movimentação de ativos próprios</t>
   </si>
   <si>
-    <t>Movement of fixed assets</t>
-  </si>
-  <si>
     <t>document_type_NC</t>
   </si>
   <si>
@@ -2166,25 +2157,16 @@
     <t>Saldos iniciais</t>
   </si>
   <si>
-    <t>Initial balance</t>
-  </si>
-  <si>
     <t>document_type_NLC</t>
   </si>
   <si>
     <t>Nota de lançamento a crédito</t>
   </si>
   <si>
-    <t>Current account credit ajustment</t>
-  </si>
-  <si>
     <t>document_type_NLD</t>
   </si>
   <si>
     <t>Nota de lançamento a débito</t>
-  </si>
-  <si>
-    <t>Current account debit ajustment</t>
   </si>
   <si>
     <t>document_type_VCF</t>
@@ -3503,6 +3485,33 @@
   </si>
   <si>
     <t>Proforma Invoice</t>
+  </si>
+  <si>
+    <t>Receipt-Invoice</t>
+  </si>
+  <si>
+    <t>Consignment Shipments</t>
+  </si>
+  <si>
+    <t>Devolution Guide</t>
+  </si>
+  <si>
+    <t>Delivery note</t>
+  </si>
+  <si>
+    <t>Transport Guide</t>
+  </si>
+  <si>
+    <t>Guide movement of own assets</t>
+  </si>
+  <si>
+    <t>Initial balances</t>
+  </si>
+  <si>
+    <t>Credit release note</t>
+  </si>
+  <si>
+    <t>Debit release note</t>
   </si>
 </sst>
 </file>
@@ -3963,7 +3972,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -3973,8 +3982,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G477"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A329" workbookViewId="0">
-      <selection activeCell="C331" sqref="C331"/>
+    <sheetView tabSelected="1" topLeftCell="A327" workbookViewId="0">
+      <selection activeCell="C333" sqref="C333"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -6063,7 +6072,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="256" spans="1:3" ht="32">
+    <row r="256" spans="1:3" ht="30">
       <c r="A256" s="1" t="s">
         <v>498</v>
       </c>
@@ -6079,7 +6088,7 @@
         <v>501</v>
       </c>
       <c r="B257" s="1" t="s">
-        <v>852</v>
+        <v>846</v>
       </c>
     </row>
     <row r="258" spans="1:3">
@@ -6354,7 +6363,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="283" spans="1:3">
+    <row r="283" spans="1:3" ht="30">
       <c r="A283" s="1" t="s">
         <v>595</v>
       </c>
@@ -6365,7 +6374,7 @@
         <v>597</v>
       </c>
     </row>
-    <row r="284" spans="1:3" ht="48">
+    <row r="284" spans="1:3" ht="45">
       <c r="A284" s="1" t="s">
         <v>598</v>
       </c>
@@ -6387,7 +6396,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="286" spans="1:3" ht="32">
+    <row r="286" spans="1:3" ht="30">
       <c r="A286" s="1" t="s">
         <v>604</v>
       </c>
@@ -6398,7 +6407,7 @@
         <v>606</v>
       </c>
     </row>
-    <row r="287" spans="1:3" ht="32">
+    <row r="287" spans="1:3" ht="30">
       <c r="A287" s="1" t="s">
         <v>607</v>
       </c>
@@ -6755,120 +6764,120 @@
         <v>674</v>
       </c>
       <c r="B319" s="1" t="s">
-        <v>855</v>
+        <v>849</v>
       </c>
       <c r="C319" s="1" t="s">
-        <v>859</v>
+        <v>853</v>
       </c>
     </row>
     <row r="320" spans="1:3">
       <c r="A320" s="1" t="s">
+        <v>848</v>
+      </c>
+      <c r="B320" s="1" t="s">
+        <v>850</v>
+      </c>
+      <c r="C320" s="1" t="s">
         <v>854</v>
-      </c>
-      <c r="B320" s="1" t="s">
-        <v>856</v>
-      </c>
-      <c r="C320" s="1" t="s">
-        <v>860</v>
       </c>
     </row>
     <row r="321" spans="1:3">
       <c r="A321" s="1" t="s">
-        <v>873</v>
+        <v>867</v>
       </c>
       <c r="B321" s="1" t="s">
-        <v>857</v>
+        <v>851</v>
       </c>
       <c r="C321" s="1" t="s">
-        <v>858</v>
+        <v>852</v>
       </c>
     </row>
     <row r="322" spans="1:3">
       <c r="A322" s="1" t="s">
-        <v>861</v>
+        <v>855</v>
       </c>
       <c r="B322" s="1" t="s">
-        <v>862</v>
+        <v>856</v>
       </c>
       <c r="C322" s="1" t="s">
-        <v>863</v>
-      </c>
-    </row>
-    <row r="323" spans="1:3" ht="48">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="323" spans="1:3" ht="45">
       <c r="A323" s="1" t="s">
         <v>675</v>
       </c>
       <c r="B323" s="1" t="s">
-        <v>847</v>
+        <v>841</v>
       </c>
       <c r="C323" s="1" t="s">
-        <v>848</v>
-      </c>
-    </row>
-    <row r="324" spans="1:3" ht="64">
+        <v>842</v>
+      </c>
+    </row>
+    <row r="324" spans="1:3" ht="60">
       <c r="A324" s="1" t="s">
         <v>676</v>
       </c>
       <c r="B324" s="1" t="s">
-        <v>867</v>
+        <v>861</v>
       </c>
       <c r="C324" s="1" t="s">
-        <v>868</v>
-      </c>
-    </row>
-    <row r="325" spans="1:3" ht="32">
+        <v>862</v>
+      </c>
+    </row>
+    <row r="325" spans="1:3" ht="30">
       <c r="A325" s="1" t="s">
         <v>677</v>
       </c>
       <c r="B325" s="1" t="s">
-        <v>869</v>
+        <v>863</v>
       </c>
       <c r="C325" s="1" t="s">
-        <v>870</v>
-      </c>
-    </row>
-    <row r="326" spans="1:3" ht="32">
+        <v>864</v>
+      </c>
+    </row>
+    <row r="326" spans="1:3" ht="30">
       <c r="A326" s="1" t="s">
-        <v>853</v>
+        <v>847</v>
       </c>
       <c r="B326" s="1" t="s">
-        <v>871</v>
+        <v>865</v>
       </c>
       <c r="C326" s="1" t="s">
-        <v>872</v>
-      </c>
-    </row>
-    <row r="327" spans="1:3" ht="64">
+        <v>866</v>
+      </c>
+    </row>
+    <row r="327" spans="1:3" ht="60">
       <c r="A327" s="1" t="s">
-        <v>864</v>
+        <v>858</v>
       </c>
       <c r="B327" s="1" t="s">
-        <v>849</v>
+        <v>843</v>
       </c>
       <c r="C327" s="1" t="s">
-        <v>850</v>
-      </c>
-    </row>
-    <row r="328" spans="1:3" ht="32">
+        <v>844</v>
+      </c>
+    </row>
+    <row r="328" spans="1:3" ht="30">
       <c r="A328" s="1" t="s">
-        <v>865</v>
+        <v>859</v>
       </c>
       <c r="B328" s="1" t="s">
-        <v>992</v>
+        <v>986</v>
       </c>
       <c r="C328" s="1" t="s">
-        <v>993</v>
-      </c>
-    </row>
-    <row r="329" spans="1:3" ht="32">
+        <v>987</v>
+      </c>
+    </row>
+    <row r="329" spans="1:3" ht="30">
       <c r="A329" s="1" t="s">
-        <v>866</v>
+        <v>860</v>
       </c>
       <c r="B329" s="1" t="s">
-        <v>990</v>
+        <v>984</v>
       </c>
       <c r="C329" s="1" t="s">
-        <v>991</v>
+        <v>985</v>
       </c>
     </row>
     <row r="330" spans="1:3">
@@ -6879,7 +6888,7 @@
         <v>679</v>
       </c>
       <c r="C330" s="1" t="s">
-        <v>1140</v>
+        <v>1134</v>
       </c>
     </row>
     <row r="331" spans="1:3">
@@ -6912,147 +6921,147 @@
         <v>687</v>
       </c>
       <c r="C333" s="1" t="s">
-        <v>688</v>
+        <v>1135</v>
       </c>
     </row>
     <row r="334" spans="1:3">
       <c r="A334" s="1" t="s">
+        <v>688</v>
+      </c>
+      <c r="B334" s="1" t="s">
         <v>689</v>
       </c>
-      <c r="B334" s="1" t="s">
-        <v>690</v>
-      </c>
       <c r="C334" s="1" t="s">
-        <v>691</v>
+        <v>1136</v>
       </c>
     </row>
     <row r="335" spans="1:3">
       <c r="A335" s="1" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="B335" s="1" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
       <c r="C335" s="1" t="s">
-        <v>694</v>
+        <v>1137</v>
       </c>
     </row>
     <row r="336" spans="1:3">
       <c r="A336" s="1" t="s">
-        <v>695</v>
+        <v>693</v>
       </c>
       <c r="B336" s="1" t="s">
-        <v>696</v>
+        <v>694</v>
       </c>
       <c r="C336" s="1" t="s">
-        <v>697</v>
+        <v>1138</v>
       </c>
     </row>
     <row r="337" spans="1:3">
       <c r="A337" s="1" t="s">
-        <v>698</v>
+        <v>696</v>
       </c>
       <c r="B337" s="1" t="s">
-        <v>699</v>
+        <v>697</v>
       </c>
       <c r="C337" s="1" t="s">
-        <v>697</v>
+        <v>1139</v>
       </c>
     </row>
     <row r="338" spans="1:3">
       <c r="A338" s="1" t="s">
-        <v>700</v>
+        <v>698</v>
       </c>
       <c r="B338" s="1" t="s">
-        <v>701</v>
+        <v>699</v>
       </c>
       <c r="C338" s="1" t="s">
-        <v>702</v>
+        <v>1140</v>
       </c>
     </row>
     <row r="339" spans="1:3">
       <c r="A339" s="1" t="s">
-        <v>703</v>
+        <v>700</v>
       </c>
       <c r="B339" s="1" t="s">
-        <v>704</v>
+        <v>701</v>
       </c>
       <c r="C339" s="1" t="s">
-        <v>705</v>
+        <v>702</v>
       </c>
     </row>
     <row r="340" spans="1:3">
       <c r="A340" s="1" t="s">
-        <v>706</v>
+        <v>703</v>
       </c>
       <c r="B340" s="1" t="s">
-        <v>707</v>
+        <v>704</v>
       </c>
       <c r="C340" s="1" t="s">
-        <v>708</v>
+        <v>705</v>
       </c>
     </row>
     <row r="341" spans="1:3">
       <c r="A341" s="1" t="s">
-        <v>709</v>
+        <v>706</v>
       </c>
       <c r="B341" s="1" t="s">
-        <v>710</v>
+        <v>707</v>
       </c>
       <c r="C341" s="1" t="s">
-        <v>711</v>
+        <v>708</v>
       </c>
     </row>
     <row r="342" spans="1:3">
       <c r="A342" s="1" t="s">
-        <v>712</v>
+        <v>709</v>
       </c>
       <c r="B342" s="1" t="s">
-        <v>713</v>
+        <v>710</v>
       </c>
       <c r="C342" s="1" t="s">
-        <v>714</v>
+        <v>1141</v>
       </c>
     </row>
     <row r="343" spans="1:3">
       <c r="A343" s="1" t="s">
-        <v>715</v>
+        <v>711</v>
       </c>
       <c r="B343" s="1" t="s">
-        <v>716</v>
+        <v>712</v>
       </c>
       <c r="C343" s="1" t="s">
-        <v>717</v>
+        <v>1142</v>
       </c>
     </row>
     <row r="344" spans="1:3">
       <c r="A344" s="1" t="s">
-        <v>718</v>
+        <v>713</v>
       </c>
       <c r="B344" s="1" t="s">
-        <v>719</v>
+        <v>714</v>
       </c>
       <c r="C344" s="1" t="s">
-        <v>720</v>
+        <v>1143</v>
       </c>
     </row>
     <row r="345" spans="1:3">
       <c r="A345" s="1" t="s">
-        <v>721</v>
+        <v>715</v>
       </c>
       <c r="B345" s="1" t="s">
-        <v>722</v>
+        <v>716</v>
       </c>
       <c r="C345" s="1" t="s">
-        <v>723</v>
+        <v>717</v>
       </c>
     </row>
     <row r="346" spans="1:3">
       <c r="A346" s="1" t="s">
-        <v>724</v>
+        <v>718</v>
       </c>
       <c r="B346" s="1" t="s">
-        <v>725</v>
+        <v>719</v>
       </c>
       <c r="C346" s="1" t="s">
         <v>685</v>
@@ -7060,425 +7069,425 @@
     </row>
     <row r="347" spans="1:3">
       <c r="A347" s="1" t="s">
-        <v>726</v>
+        <v>720</v>
       </c>
       <c r="B347" s="1" t="s">
-        <v>727</v>
+        <v>721</v>
       </c>
       <c r="C347" s="1" t="s">
-        <v>728</v>
+        <v>722</v>
       </c>
     </row>
     <row r="348" spans="1:3">
       <c r="A348" s="1" t="s">
-        <v>729</v>
+        <v>723</v>
       </c>
       <c r="B348" s="1" t="s">
-        <v>730</v>
+        <v>724</v>
       </c>
       <c r="C348" s="1" t="s">
-        <v>731</v>
+        <v>725</v>
       </c>
     </row>
     <row r="349" spans="1:3">
       <c r="A349" s="1" t="s">
-        <v>732</v>
+        <v>726</v>
       </c>
       <c r="B349" s="1" t="s">
-        <v>733</v>
+        <v>727</v>
       </c>
       <c r="C349" s="1" t="s">
-        <v>734</v>
+        <v>728</v>
       </c>
     </row>
     <row r="350" spans="1:3">
       <c r="A350" s="1" t="s">
-        <v>735</v>
+        <v>729</v>
       </c>
       <c r="B350" s="1" t="s">
-        <v>736</v>
+        <v>730</v>
       </c>
       <c r="C350" s="1" t="s">
-        <v>1139</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="351" spans="1:3">
       <c r="A351" s="1" t="s">
-        <v>737</v>
+        <v>731</v>
       </c>
       <c r="B351" s="1" t="s">
-        <v>738</v>
+        <v>732</v>
       </c>
       <c r="C351" s="1" t="s">
-        <v>739</v>
+        <v>733</v>
       </c>
     </row>
     <row r="352" spans="1:3">
       <c r="A352" s="1" t="s">
-        <v>740</v>
+        <v>734</v>
       </c>
       <c r="B352" s="1" t="s">
-        <v>741</v>
+        <v>735</v>
       </c>
       <c r="C352" s="1" t="s">
-        <v>742</v>
+        <v>736</v>
       </c>
     </row>
     <row r="353" spans="1:3">
       <c r="A353" s="1" t="s">
-        <v>743</v>
+        <v>737</v>
       </c>
       <c r="B353" s="1" t="s">
-        <v>744</v>
+        <v>738</v>
       </c>
       <c r="C353" s="1" t="s">
-        <v>745</v>
+        <v>739</v>
       </c>
     </row>
     <row r="354" spans="1:3">
       <c r="A354" s="1" t="s">
-        <v>746</v>
+        <v>740</v>
       </c>
       <c r="B354" s="1" t="s">
-        <v>747</v>
+        <v>741</v>
       </c>
       <c r="C354" s="1" t="s">
-        <v>748</v>
+        <v>742</v>
       </c>
     </row>
     <row r="355" spans="1:3">
       <c r="A355" s="1" t="s">
-        <v>749</v>
+        <v>743</v>
       </c>
       <c r="B355" s="1" t="s">
-        <v>750</v>
+        <v>744</v>
       </c>
       <c r="C355" s="1" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
     </row>
     <row r="356" spans="1:3">
       <c r="A356" s="1" t="s">
-        <v>751</v>
+        <v>745</v>
       </c>
       <c r="B356" s="1" t="s">
-        <v>752</v>
+        <v>746</v>
       </c>
       <c r="C356" s="1" t="s">
-        <v>694</v>
+        <v>692</v>
       </c>
     </row>
     <row r="357" spans="1:3">
       <c r="A357" s="1" t="s">
-        <v>753</v>
+        <v>747</v>
       </c>
       <c r="B357" s="1" t="s">
-        <v>754</v>
+        <v>748</v>
       </c>
       <c r="C357" s="1" t="s">
-        <v>755</v>
+        <v>749</v>
       </c>
     </row>
     <row r="358" spans="1:3">
       <c r="A358" s="1" t="s">
-        <v>756</v>
+        <v>750</v>
       </c>
       <c r="B358" s="1" t="s">
-        <v>757</v>
+        <v>751</v>
       </c>
       <c r="C358" s="1" t="s">
-        <v>758</v>
+        <v>752</v>
       </c>
     </row>
     <row r="359" spans="1:3">
       <c r="A359" s="1" t="s">
-        <v>759</v>
+        <v>753</v>
       </c>
       <c r="B359" s="1" t="s">
-        <v>874</v>
+        <v>868</v>
       </c>
       <c r="C359" s="1" t="s">
-        <v>760</v>
+        <v>754</v>
       </c>
     </row>
     <row r="360" spans="1:3">
       <c r="A360" s="1" t="s">
-        <v>761</v>
+        <v>755</v>
       </c>
       <c r="B360" s="1" t="s">
-        <v>762</v>
+        <v>756</v>
       </c>
       <c r="C360" s="1" t="s">
-        <v>763</v>
+        <v>757</v>
       </c>
     </row>
     <row r="361" spans="1:3">
       <c r="A361" s="1" t="s">
-        <v>764</v>
+        <v>758</v>
       </c>
       <c r="B361" s="1" t="s">
-        <v>765</v>
+        <v>759</v>
       </c>
       <c r="C361" s="1" t="s">
-        <v>766</v>
+        <v>760</v>
       </c>
     </row>
     <row r="362" spans="1:3">
       <c r="A362" s="1" t="s">
-        <v>767</v>
+        <v>761</v>
       </c>
       <c r="B362" s="1" t="s">
-        <v>768</v>
+        <v>762</v>
       </c>
       <c r="C362" s="1" t="s">
-        <v>769</v>
+        <v>763</v>
       </c>
     </row>
     <row r="363" spans="1:3">
       <c r="A363" s="1" t="s">
-        <v>770</v>
+        <v>764</v>
       </c>
       <c r="B363" s="1" t="s">
-        <v>771</v>
+        <v>765</v>
       </c>
       <c r="C363" s="1" t="s">
-        <v>772</v>
+        <v>766</v>
       </c>
     </row>
     <row r="364" spans="1:3">
       <c r="A364" s="1" t="s">
-        <v>773</v>
+        <v>767</v>
       </c>
       <c r="B364" s="1" t="s">
-        <v>774</v>
+        <v>768</v>
       </c>
       <c r="C364" s="1" t="s">
-        <v>775</v>
+        <v>769</v>
       </c>
     </row>
     <row r="365" spans="1:3">
       <c r="A365" s="1" t="s">
-        <v>776</v>
+        <v>770</v>
       </c>
       <c r="B365" s="1" t="s">
-        <v>777</v>
+        <v>771</v>
       </c>
       <c r="C365" s="1" t="s">
-        <v>778</v>
+        <v>772</v>
       </c>
     </row>
     <row r="366" spans="1:3">
       <c r="A366" s="1" t="s">
-        <v>779</v>
+        <v>773</v>
       </c>
       <c r="B366" s="1" t="s">
-        <v>780</v>
+        <v>774</v>
       </c>
       <c r="C366" s="1" t="s">
-        <v>781</v>
+        <v>775</v>
       </c>
     </row>
     <row r="367" spans="1:3">
       <c r="A367" s="1" t="s">
-        <v>782</v>
+        <v>776</v>
       </c>
       <c r="B367" s="1" t="s">
-        <v>783</v>
+        <v>777</v>
       </c>
       <c r="C367" s="1" t="s">
-        <v>784</v>
+        <v>778</v>
       </c>
     </row>
     <row r="368" spans="1:3">
       <c r="A368" s="1" t="s">
-        <v>785</v>
+        <v>779</v>
       </c>
       <c r="B368" s="1" t="s">
-        <v>786</v>
+        <v>780</v>
       </c>
       <c r="C368" s="1" t="s">
-        <v>787</v>
+        <v>781</v>
       </c>
     </row>
     <row r="369" spans="1:3">
       <c r="A369" s="1" t="s">
-        <v>788</v>
+        <v>782</v>
       </c>
       <c r="B369" s="1" t="s">
-        <v>789</v>
+        <v>783</v>
       </c>
       <c r="C369" s="1" t="s">
-        <v>790</v>
+        <v>784</v>
       </c>
     </row>
     <row r="370" spans="1:3">
       <c r="A370" s="1" t="s">
-        <v>791</v>
+        <v>785</v>
       </c>
       <c r="B370" s="1" t="s">
-        <v>792</v>
+        <v>786</v>
       </c>
       <c r="C370" s="1" t="s">
-        <v>793</v>
+        <v>787</v>
       </c>
     </row>
     <row r="371" spans="1:3">
       <c r="A371" s="1" t="s">
-        <v>794</v>
+        <v>788</v>
       </c>
       <c r="B371" s="1" t="s">
-        <v>795</v>
+        <v>789</v>
       </c>
       <c r="C371" s="1" t="s">
-        <v>796</v>
+        <v>790</v>
       </c>
     </row>
     <row r="372" spans="1:3">
       <c r="A372" s="1" t="s">
-        <v>797</v>
+        <v>791</v>
       </c>
       <c r="B372" s="1" t="s">
-        <v>798</v>
+        <v>792</v>
       </c>
       <c r="C372" s="1" t="s">
-        <v>799</v>
+        <v>793</v>
       </c>
     </row>
     <row r="373" spans="1:3">
       <c r="A373" s="1" t="s">
-        <v>800</v>
+        <v>794</v>
       </c>
       <c r="B373" s="1" t="s">
-        <v>801</v>
+        <v>795</v>
       </c>
       <c r="C373" s="1" t="s">
-        <v>802</v>
+        <v>796</v>
       </c>
     </row>
     <row r="374" spans="1:3">
       <c r="A374" s="1" t="s">
-        <v>803</v>
+        <v>797</v>
       </c>
       <c r="B374" s="1" t="s">
-        <v>804</v>
+        <v>798</v>
       </c>
       <c r="C374" s="1" t="s">
-        <v>805</v>
+        <v>799</v>
       </c>
     </row>
     <row r="375" spans="1:3">
       <c r="A375" s="1" t="s">
-        <v>806</v>
+        <v>800</v>
       </c>
       <c r="B375" s="1" t="s">
-        <v>807</v>
+        <v>801</v>
       </c>
       <c r="C375" s="1" t="s">
-        <v>808</v>
+        <v>802</v>
       </c>
     </row>
     <row r="376" spans="1:3">
       <c r="A376" s="1" t="s">
-        <v>809</v>
+        <v>803</v>
       </c>
       <c r="B376" s="1" t="s">
-        <v>810</v>
+        <v>804</v>
       </c>
       <c r="C376" s="1" t="s">
-        <v>811</v>
+        <v>805</v>
       </c>
     </row>
     <row r="377" spans="1:3">
       <c r="A377" s="1" t="s">
-        <v>812</v>
+        <v>806</v>
       </c>
       <c r="B377" s="1" t="s">
-        <v>851</v>
+        <v>845</v>
       </c>
       <c r="C377" s="1" t="s">
-        <v>813</v>
+        <v>807</v>
       </c>
     </row>
     <row r="378" spans="1:3">
       <c r="A378" s="1" t="s">
-        <v>814</v>
+        <v>808</v>
       </c>
       <c r="B378" s="1" t="s">
-        <v>815</v>
+        <v>809</v>
       </c>
       <c r="C378" s="1" t="s">
-        <v>816</v>
+        <v>810</v>
       </c>
     </row>
     <row r="379" spans="1:3">
       <c r="A379" s="1" t="s">
-        <v>817</v>
+        <v>811</v>
       </c>
       <c r="B379" s="1" t="s">
-        <v>818</v>
+        <v>812</v>
       </c>
       <c r="C379" s="1" t="s">
-        <v>819</v>
+        <v>813</v>
       </c>
     </row>
     <row r="380" spans="1:3">
       <c r="A380" s="1" t="s">
-        <v>820</v>
+        <v>814</v>
       </c>
       <c r="B380" s="1" t="s">
-        <v>821</v>
+        <v>815</v>
       </c>
       <c r="C380" s="1" t="s">
-        <v>822</v>
+        <v>816</v>
       </c>
     </row>
     <row r="381" spans="1:3">
       <c r="A381" s="1" t="s">
-        <v>823</v>
+        <v>817</v>
       </c>
       <c r="B381" s="1" t="s">
-        <v>824</v>
+        <v>818</v>
       </c>
       <c r="C381" s="1" t="s">
-        <v>825</v>
+        <v>819</v>
       </c>
     </row>
     <row r="382" spans="1:3">
       <c r="A382" s="1" t="s">
-        <v>826</v>
+        <v>820</v>
       </c>
       <c r="B382" s="1" t="s">
-        <v>827</v>
+        <v>821</v>
       </c>
       <c r="C382" s="1" t="s">
-        <v>825</v>
+        <v>819</v>
       </c>
     </row>
     <row r="383" spans="1:3">
       <c r="A383" s="1" t="s">
-        <v>828</v>
+        <v>822</v>
       </c>
       <c r="B383" s="1" t="s">
-        <v>829</v>
+        <v>823</v>
       </c>
       <c r="C383" s="1" t="s">
-        <v>830</v>
+        <v>824</v>
       </c>
     </row>
     <row r="384" spans="1:3">
       <c r="A384" s="1" t="s">
-        <v>831</v>
+        <v>825</v>
       </c>
       <c r="B384" s="1" t="s">
-        <v>832</v>
+        <v>826</v>
       </c>
       <c r="C384" s="1" t="s">
-        <v>833</v>
+        <v>827</v>
       </c>
     </row>
     <row r="385" spans="1:7">
       <c r="A385" s="1" t="s">
-        <v>834</v>
+        <v>828</v>
       </c>
       <c r="B385" s="1" t="s">
         <v>622</v>
@@ -7489,51 +7498,51 @@
     </row>
     <row r="386" spans="1:7">
       <c r="A386" s="1" t="s">
-        <v>835</v>
+        <v>829</v>
       </c>
       <c r="B386" s="1" t="s">
-        <v>836</v>
+        <v>830</v>
       </c>
       <c r="C386" s="1" t="s">
-        <v>837</v>
+        <v>831</v>
       </c>
     </row>
     <row r="387" spans="1:7">
       <c r="A387" s="1" t="s">
-        <v>838</v>
+        <v>832</v>
       </c>
       <c r="B387" s="1" t="s">
-        <v>839</v>
+        <v>833</v>
       </c>
       <c r="C387" s="1" t="s">
-        <v>840</v>
+        <v>834</v>
       </c>
     </row>
     <row r="388" spans="1:7">
       <c r="A388" s="1" t="s">
-        <v>841</v>
+        <v>835</v>
       </c>
       <c r="B388" s="1" t="s">
-        <v>842</v>
+        <v>836</v>
       </c>
       <c r="C388" s="1" t="s">
-        <v>843</v>
+        <v>837</v>
       </c>
     </row>
     <row r="389" spans="1:7">
       <c r="A389" s="1" t="s">
-        <v>844</v>
+        <v>838</v>
       </c>
       <c r="B389" s="1" t="s">
-        <v>845</v>
+        <v>839</v>
       </c>
       <c r="C389" s="1" t="s">
-        <v>846</v>
+        <v>840</v>
       </c>
     </row>
     <row r="390" spans="1:7">
       <c r="A390" s="1" t="s">
-        <v>875</v>
+        <v>869</v>
       </c>
       <c r="B390" s="1" t="s">
         <v>658</v>
@@ -7548,24 +7557,24 @@
     </row>
     <row r="391" spans="1:7">
       <c r="A391" s="1" t="s">
-        <v>876</v>
+        <v>870</v>
       </c>
       <c r="B391" s="1" t="s">
-        <v>878</v>
+        <v>872</v>
       </c>
       <c r="C391" s="1" t="s">
-        <v>879</v>
+        <v>873</v>
       </c>
     </row>
     <row r="392" spans="1:7">
       <c r="A392" s="1" t="s">
-        <v>877</v>
+        <v>871</v>
       </c>
       <c r="B392" s="1" t="s">
-        <v>827</v>
+        <v>821</v>
       </c>
       <c r="C392" s="1" t="s">
-        <v>879</v>
+        <v>873</v>
       </c>
       <c r="D392" s="4"/>
       <c r="E392" s="4"/>
@@ -7574,88 +7583,88 @@
     </row>
     <row r="393" spans="1:7">
       <c r="A393" s="1" t="s">
-        <v>949</v>
+        <v>943</v>
       </c>
       <c r="B393" s="1" t="s">
-        <v>956</v>
+        <v>950</v>
       </c>
       <c r="C393" s="1" t="s">
-        <v>964</v>
+        <v>958</v>
       </c>
       <c r="D393" s="4"/>
       <c r="E393" s="4"/>
       <c r="F393" s="4"/>
       <c r="G393" s="4"/>
     </row>
-    <row r="394" spans="1:7" ht="32">
+    <row r="394" spans="1:7" ht="30">
       <c r="A394" s="1" t="s">
+        <v>881</v>
+      </c>
+      <c r="B394" s="1" t="s">
+        <v>880</v>
+      </c>
+      <c r="C394" s="1" t="s">
         <v>887</v>
-      </c>
-      <c r="B394" s="1" t="s">
-        <v>886</v>
-      </c>
-      <c r="C394" s="1" t="s">
-        <v>893</v>
       </c>
       <c r="D394" s="4"/>
       <c r="E394" s="4"/>
       <c r="F394" s="4"/>
       <c r="G394" s="4"/>
     </row>
-    <row r="395" spans="1:7" ht="48">
+    <row r="395" spans="1:7" ht="45">
       <c r="A395" s="1" t="s">
-        <v>901</v>
+        <v>895</v>
       </c>
       <c r="B395" s="1" t="s">
-        <v>880</v>
+        <v>874</v>
       </c>
       <c r="C395" s="1" t="s">
-        <v>882</v>
+        <v>876</v>
       </c>
       <c r="D395" s="4"/>
       <c r="E395" s="4"/>
       <c r="F395" s="4"/>
       <c r="G395" s="4"/>
     </row>
-    <row r="396" spans="1:7" ht="48">
+    <row r="396" spans="1:7" ht="45">
       <c r="A396" s="1" t="s">
-        <v>932</v>
+        <v>926</v>
       </c>
       <c r="B396" s="1" t="s">
-        <v>896</v>
+        <v>890</v>
       </c>
       <c r="C396" s="1" t="s">
-        <v>897</v>
+        <v>891</v>
       </c>
       <c r="D396" s="4"/>
       <c r="E396" s="4"/>
       <c r="F396" s="4"/>
       <c r="G396" s="4"/>
     </row>
-    <row r="397" spans="1:7" ht="96">
+    <row r="397" spans="1:7" ht="105">
       <c r="A397" s="1" t="s">
-        <v>933</v>
+        <v>927</v>
       </c>
       <c r="B397" s="1" t="s">
-        <v>936</v>
+        <v>930</v>
       </c>
       <c r="C397" s="1" t="s">
-        <v>937</v>
+        <v>931</v>
       </c>
       <c r="D397" s="4"/>
       <c r="E397" s="4"/>
       <c r="F397" s="4"/>
       <c r="G397" s="4"/>
     </row>
-    <row r="398" spans="1:7" ht="48">
+    <row r="398" spans="1:7" ht="45">
       <c r="A398" s="1" t="s">
-        <v>900</v>
+        <v>894</v>
       </c>
       <c r="B398" s="1" t="s">
-        <v>881</v>
+        <v>875</v>
       </c>
       <c r="C398" s="1" t="s">
-        <v>883</v>
+        <v>877</v>
       </c>
       <c r="D398" s="4"/>
       <c r="E398" s="4"/>
@@ -7664,448 +7673,448 @@
     </row>
     <row r="399" spans="1:7">
       <c r="A399" s="1" t="s">
-        <v>950</v>
+        <v>944</v>
       </c>
       <c r="B399" s="1" t="s">
+        <v>951</v>
+      </c>
+      <c r="C399" s="1" t="s">
         <v>957</v>
-      </c>
-      <c r="C399" s="1" t="s">
-        <v>963</v>
       </c>
       <c r="D399" s="4"/>
       <c r="E399" s="4"/>
       <c r="F399" s="4"/>
       <c r="G399" s="4"/>
     </row>
-    <row r="400" spans="1:7" ht="64">
+    <row r="400" spans="1:7" ht="60">
       <c r="A400" s="1" t="s">
-        <v>934</v>
+        <v>928</v>
       </c>
       <c r="B400" s="1" t="s">
-        <v>898</v>
+        <v>892</v>
       </c>
       <c r="C400" s="1" t="s">
-        <v>899</v>
+        <v>893</v>
       </c>
       <c r="D400" s="4"/>
       <c r="E400" s="4"/>
       <c r="F400" s="4"/>
       <c r="G400" s="4"/>
     </row>
-    <row r="401" spans="1:7" ht="96">
+    <row r="401" spans="1:7" ht="90">
       <c r="A401" s="1" t="s">
-        <v>935</v>
+        <v>929</v>
       </c>
       <c r="B401" s="1" t="s">
-        <v>938</v>
+        <v>932</v>
       </c>
       <c r="C401" s="1" t="s">
-        <v>939</v>
+        <v>933</v>
       </c>
       <c r="D401" s="4"/>
       <c r="E401" s="4"/>
       <c r="F401" s="4"/>
       <c r="G401" s="4"/>
     </row>
-    <row r="402" spans="1:7" ht="32">
+    <row r="402" spans="1:7" ht="30">
       <c r="A402" s="1" t="s">
-        <v>894</v>
+        <v>888</v>
       </c>
       <c r="B402" s="1" t="s">
-        <v>885</v>
+        <v>879</v>
       </c>
       <c r="C402" s="1" t="s">
-        <v>890</v>
+        <v>884</v>
       </c>
       <c r="D402" s="4"/>
       <c r="E402" s="4"/>
       <c r="F402" s="4"/>
       <c r="G402" s="4"/>
     </row>
-    <row r="403" spans="1:7" ht="32">
+    <row r="403" spans="1:7" ht="30">
       <c r="A403" s="1" t="s">
-        <v>895</v>
+        <v>889</v>
       </c>
       <c r="B403" s="1" t="s">
-        <v>884</v>
+        <v>878</v>
       </c>
       <c r="C403" s="1" t="s">
-        <v>891</v>
+        <v>885</v>
       </c>
       <c r="D403" s="4"/>
       <c r="E403" s="4"/>
       <c r="F403" s="4"/>
       <c r="G403" s="4"/>
     </row>
-    <row r="404" spans="1:7" ht="64">
+    <row r="404" spans="1:7" ht="60">
       <c r="A404" s="1" t="s">
-        <v>889</v>
+        <v>883</v>
       </c>
       <c r="B404" s="1" t="s">
-        <v>888</v>
+        <v>882</v>
       </c>
       <c r="C404" s="1" t="s">
-        <v>892</v>
+        <v>886</v>
       </c>
       <c r="D404" s="4"/>
       <c r="E404" s="4"/>
       <c r="F404" s="4"/>
       <c r="G404" s="4"/>
     </row>
-    <row r="405" spans="1:7" ht="32">
+    <row r="405" spans="1:7" ht="30">
       <c r="A405" s="1" t="s">
-        <v>951</v>
+        <v>945</v>
       </c>
       <c r="B405" s="1" t="s">
-        <v>958</v>
+        <v>952</v>
       </c>
       <c r="C405" s="1" t="s">
-        <v>965</v>
+        <v>959</v>
       </c>
       <c r="D405" s="4"/>
       <c r="E405" s="4"/>
       <c r="F405" s="4"/>
       <c r="G405" s="4"/>
     </row>
-    <row r="406" spans="1:7" ht="80">
+    <row r="406" spans="1:7" ht="75">
       <c r="A406" s="1" t="s">
-        <v>903</v>
+        <v>897</v>
       </c>
       <c r="B406" s="1" t="s">
-        <v>902</v>
+        <v>896</v>
       </c>
       <c r="C406" s="1" t="s">
-        <v>922</v>
+        <v>916</v>
       </c>
       <c r="D406" s="4"/>
       <c r="E406" s="4"/>
       <c r="F406" s="4"/>
       <c r="G406" s="4"/>
     </row>
-    <row r="407" spans="1:7" ht="96">
+    <row r="407" spans="1:7" ht="90">
       <c r="A407" s="1" t="s">
-        <v>904</v>
+        <v>898</v>
       </c>
       <c r="B407" s="1" t="s">
+        <v>911</v>
+      </c>
+      <c r="C407" s="1" t="s">
         <v>917</v>
-      </c>
-      <c r="C407" s="1" t="s">
-        <v>923</v>
       </c>
       <c r="D407" s="4"/>
       <c r="E407" s="4"/>
       <c r="F407" s="4"/>
       <c r="G407" s="4"/>
     </row>
-    <row r="408" spans="1:7" ht="32">
+    <row r="408" spans="1:7" ht="30">
       <c r="A408" s="1" t="s">
+        <v>1061</v>
+      </c>
+      <c r="B408" s="1" t="s">
+        <v>1064</v>
+      </c>
+      <c r="C408" s="1" t="s">
         <v>1067</v>
-      </c>
-      <c r="B408" s="1" t="s">
-        <v>1070</v>
-      </c>
-      <c r="C408" s="1" t="s">
-        <v>1073</v>
       </c>
       <c r="D408" s="4"/>
       <c r="E408" s="4"/>
       <c r="F408" s="4"/>
       <c r="G408" s="4"/>
     </row>
-    <row r="409" spans="1:7" ht="96">
+    <row r="409" spans="1:7" ht="90">
       <c r="A409" s="1" t="s">
+        <v>1062</v>
+      </c>
+      <c r="B409" s="1" t="s">
+        <v>1065</v>
+      </c>
+      <c r="C409" s="1" t="s">
         <v>1068</v>
-      </c>
-      <c r="B409" s="1" t="s">
-        <v>1071</v>
-      </c>
-      <c r="C409" s="1" t="s">
-        <v>1074</v>
       </c>
       <c r="D409" s="4"/>
       <c r="E409" s="4"/>
       <c r="F409" s="4"/>
       <c r="G409" s="4"/>
     </row>
-    <row r="410" spans="1:7" ht="80">
+    <row r="410" spans="1:7" ht="75">
       <c r="A410" s="1" t="s">
+        <v>1063</v>
+      </c>
+      <c r="B410" s="1" t="s">
+        <v>1066</v>
+      </c>
+      <c r="C410" s="1" t="s">
         <v>1069</v>
-      </c>
-      <c r="B410" s="1" t="s">
-        <v>1072</v>
-      </c>
-      <c r="C410" s="1" t="s">
-        <v>1075</v>
       </c>
       <c r="D410" s="4"/>
       <c r="E410" s="4"/>
       <c r="F410" s="4"/>
       <c r="G410" s="4"/>
     </row>
-    <row r="411" spans="1:7" ht="32">
+    <row r="411" spans="1:7" ht="30">
       <c r="A411" s="1" t="s">
-        <v>952</v>
+        <v>946</v>
       </c>
       <c r="B411" s="1" t="s">
-        <v>959</v>
+        <v>953</v>
       </c>
       <c r="C411" s="1" t="s">
-        <v>966</v>
+        <v>960</v>
       </c>
       <c r="D411" s="4"/>
       <c r="E411" s="4"/>
       <c r="F411" s="4"/>
       <c r="G411" s="4"/>
     </row>
-    <row r="412" spans="1:7" ht="96">
+    <row r="412" spans="1:7" ht="90">
       <c r="A412" s="1" t="s">
-        <v>905</v>
+        <v>899</v>
       </c>
       <c r="B412" s="1" t="s">
-        <v>909</v>
+        <v>903</v>
       </c>
       <c r="C412" s="1" t="s">
-        <v>924</v>
+        <v>918</v>
       </c>
       <c r="D412" s="4"/>
       <c r="E412" s="4"/>
       <c r="F412" s="4"/>
       <c r="G412" s="4"/>
     </row>
-    <row r="413" spans="1:7" ht="112">
+    <row r="413" spans="1:7" ht="105">
       <c r="A413" s="1" t="s">
-        <v>906</v>
+        <v>900</v>
       </c>
       <c r="B413" s="1" t="s">
-        <v>918</v>
+        <v>912</v>
       </c>
       <c r="C413" s="1" t="s">
-        <v>925</v>
+        <v>919</v>
       </c>
       <c r="D413" s="4"/>
       <c r="E413" s="4"/>
       <c r="F413" s="4"/>
       <c r="G413" s="4"/>
     </row>
-    <row r="414" spans="1:7" ht="32">
+    <row r="414" spans="1:7" ht="30">
       <c r="A414" s="1" t="s">
-        <v>1076</v>
+        <v>1070</v>
       </c>
       <c r="B414" s="1" t="s">
-        <v>1089</v>
+        <v>1083</v>
       </c>
       <c r="C414" s="1" t="s">
-        <v>1080</v>
+        <v>1074</v>
       </c>
       <c r="D414" s="4"/>
       <c r="E414" s="4"/>
       <c r="F414" s="4"/>
       <c r="G414" s="4"/>
     </row>
-    <row r="415" spans="1:7" ht="112">
+    <row r="415" spans="1:7" ht="105">
       <c r="A415" s="1" t="s">
-        <v>1077</v>
+        <v>1071</v>
       </c>
       <c r="B415" s="1" t="s">
-        <v>1090</v>
+        <v>1084</v>
       </c>
       <c r="C415" s="1" t="s">
-        <v>1081</v>
+        <v>1075</v>
       </c>
       <c r="D415" s="4"/>
       <c r="E415" s="4"/>
       <c r="F415" s="4"/>
       <c r="G415" s="4"/>
     </row>
-    <row r="416" spans="1:7" ht="96">
+    <row r="416" spans="1:7" ht="90">
       <c r="A416" s="1" t="s">
-        <v>1078</v>
+        <v>1072</v>
       </c>
       <c r="B416" s="1" t="s">
-        <v>1079</v>
+        <v>1073</v>
       </c>
       <c r="C416" s="1" t="s">
-        <v>1082</v>
+        <v>1076</v>
       </c>
       <c r="D416" s="4"/>
       <c r="E416" s="4"/>
       <c r="F416" s="4"/>
       <c r="G416" s="4"/>
     </row>
-    <row r="417" spans="1:7" ht="32">
+    <row r="417" spans="1:7" ht="30">
       <c r="A417" s="1" t="s">
-        <v>953</v>
+        <v>947</v>
       </c>
       <c r="B417" s="1" t="s">
-        <v>960</v>
+        <v>954</v>
       </c>
       <c r="C417" s="1" t="s">
-        <v>967</v>
+        <v>961</v>
       </c>
       <c r="D417" s="4"/>
       <c r="E417" s="4"/>
       <c r="F417" s="4"/>
       <c r="G417" s="4"/>
     </row>
-    <row r="418" spans="1:7" ht="80">
+    <row r="418" spans="1:7" ht="75">
       <c r="A418" s="1" t="s">
-        <v>908</v>
+        <v>902</v>
       </c>
       <c r="B418" s="1" t="s">
-        <v>910</v>
+        <v>904</v>
       </c>
       <c r="C418" s="1" t="s">
-        <v>926</v>
+        <v>920</v>
       </c>
       <c r="D418" s="4"/>
       <c r="E418" s="4"/>
       <c r="F418" s="4"/>
       <c r="G418" s="4"/>
     </row>
-    <row r="419" spans="1:7" ht="96">
+    <row r="419" spans="1:7" ht="90">
       <c r="A419" s="1" t="s">
-        <v>907</v>
+        <v>901</v>
       </c>
       <c r="B419" s="1" t="s">
-        <v>919</v>
+        <v>913</v>
       </c>
       <c r="C419" s="1" t="s">
-        <v>927</v>
+        <v>921</v>
       </c>
       <c r="D419" s="4"/>
       <c r="E419" s="4"/>
       <c r="F419" s="4"/>
       <c r="G419" s="4"/>
     </row>
-    <row r="420" spans="1:7" ht="32">
+    <row r="420" spans="1:7" ht="30">
       <c r="A420" s="1" t="s">
-        <v>1086</v>
+        <v>1080</v>
       </c>
       <c r="B420" s="1" t="s">
-        <v>1091</v>
+        <v>1085</v>
       </c>
       <c r="C420" s="1" t="s">
-        <v>1083</v>
+        <v>1077</v>
       </c>
       <c r="D420" s="4"/>
       <c r="E420" s="4"/>
       <c r="F420" s="4"/>
       <c r="G420" s="4"/>
     </row>
-    <row r="421" spans="1:7" ht="96">
+    <row r="421" spans="1:7" ht="90">
       <c r="A421" s="1" t="s">
-        <v>1087</v>
+        <v>1081</v>
       </c>
       <c r="B421" s="1" t="s">
-        <v>1092</v>
+        <v>1086</v>
       </c>
       <c r="C421" s="1" t="s">
-        <v>1084</v>
+        <v>1078</v>
       </c>
       <c r="D421" s="4"/>
       <c r="E421" s="4"/>
       <c r="F421" s="4"/>
       <c r="G421" s="4"/>
     </row>
-    <row r="422" spans="1:7" ht="96">
+    <row r="422" spans="1:7" ht="90">
       <c r="A422" s="1" t="s">
-        <v>1088</v>
+        <v>1082</v>
       </c>
       <c r="B422" s="1" t="s">
-        <v>1093</v>
+        <v>1087</v>
       </c>
       <c r="C422" s="1" t="s">
-        <v>1085</v>
+        <v>1079</v>
       </c>
       <c r="D422" s="4"/>
       <c r="E422" s="4"/>
       <c r="F422" s="4"/>
       <c r="G422" s="4"/>
     </row>
-    <row r="423" spans="1:7" ht="32">
+    <row r="423" spans="1:7" ht="30">
       <c r="A423" s="1" t="s">
-        <v>954</v>
+        <v>948</v>
       </c>
       <c r="B423" s="1" t="s">
-        <v>961</v>
+        <v>955</v>
       </c>
       <c r="C423" s="1" t="s">
-        <v>968</v>
+        <v>962</v>
       </c>
       <c r="D423" s="4"/>
       <c r="E423" s="4"/>
       <c r="F423" s="4"/>
       <c r="G423" s="4"/>
     </row>
-    <row r="424" spans="1:7" ht="96">
+    <row r="424" spans="1:7" ht="90">
       <c r="A424" s="1" t="s">
-        <v>911</v>
+        <v>905</v>
       </c>
       <c r="B424" s="1" t="s">
-        <v>915</v>
+        <v>909</v>
       </c>
       <c r="C424" s="1" t="s">
-        <v>928</v>
+        <v>922</v>
       </c>
       <c r="D424" s="4"/>
       <c r="E424" s="4"/>
       <c r="F424" s="4"/>
       <c r="G424" s="4"/>
     </row>
-    <row r="425" spans="1:7" ht="128">
+    <row r="425" spans="1:7" ht="120">
       <c r="A425" s="1" t="s">
-        <v>912</v>
+        <v>906</v>
       </c>
       <c r="B425" s="1" t="s">
-        <v>920</v>
+        <v>914</v>
       </c>
       <c r="C425" s="1" t="s">
-        <v>929</v>
+        <v>923</v>
       </c>
       <c r="D425" s="4"/>
       <c r="E425" s="4"/>
       <c r="F425" s="4"/>
       <c r="G425" s="4"/>
     </row>
-    <row r="426" spans="1:7" ht="32">
+    <row r="426" spans="1:7" ht="30">
       <c r="A426" s="1" t="s">
-        <v>955</v>
+        <v>949</v>
       </c>
       <c r="B426" s="1" t="s">
-        <v>962</v>
+        <v>956</v>
       </c>
       <c r="C426" s="1" t="s">
-        <v>969</v>
+        <v>963</v>
       </c>
       <c r="D426" s="4"/>
       <c r="E426" s="4"/>
       <c r="F426" s="4"/>
       <c r="G426" s="4"/>
     </row>
-    <row r="427" spans="1:7" ht="96">
+    <row r="427" spans="1:7" ht="90">
       <c r="A427" s="1" t="s">
-        <v>913</v>
+        <v>907</v>
       </c>
       <c r="B427" s="1" t="s">
-        <v>916</v>
+        <v>910</v>
       </c>
       <c r="C427" s="1" t="s">
-        <v>930</v>
+        <v>924</v>
       </c>
       <c r="D427" s="4"/>
       <c r="E427" s="4"/>
       <c r="F427" s="4"/>
       <c r="G427" s="4"/>
     </row>
-    <row r="428" spans="1:7" ht="112">
+    <row r="428" spans="1:7" ht="105">
       <c r="A428" s="1" t="s">
-        <v>914</v>
+        <v>908</v>
       </c>
       <c r="B428" s="1" t="s">
-        <v>921</v>
+        <v>915</v>
       </c>
       <c r="C428" s="1" t="s">
-        <v>931</v>
+        <v>925</v>
       </c>
       <c r="D428" s="4"/>
       <c r="E428" s="4"/>
@@ -8114,13 +8123,13 @@
     </row>
     <row r="429" spans="1:7">
       <c r="A429" s="1" t="s">
+        <v>934</v>
+      </c>
+      <c r="B429" s="1" t="s">
+        <v>937</v>
+      </c>
+      <c r="C429" s="1" t="s">
         <v>940</v>
-      </c>
-      <c r="B429" s="1" t="s">
-        <v>943</v>
-      </c>
-      <c r="C429" s="1" t="s">
-        <v>946</v>
       </c>
       <c r="D429" s="4"/>
       <c r="E429" s="4"/>
@@ -8129,13 +8138,13 @@
     </row>
     <row r="430" spans="1:7">
       <c r="A430" s="1" t="s">
+        <v>935</v>
+      </c>
+      <c r="B430" s="1" t="s">
+        <v>938</v>
+      </c>
+      <c r="C430" s="1" t="s">
         <v>941</v>
-      </c>
-      <c r="B430" s="1" t="s">
-        <v>944</v>
-      </c>
-      <c r="C430" s="1" t="s">
-        <v>947</v>
       </c>
       <c r="D430" s="4"/>
       <c r="E430" s="4"/>
@@ -8144,13 +8153,13 @@
     </row>
     <row r="431" spans="1:7">
       <c r="A431" s="1" t="s">
+        <v>936</v>
+      </c>
+      <c r="B431" s="1" t="s">
+        <v>939</v>
+      </c>
+      <c r="C431" s="1" t="s">
         <v>942</v>
-      </c>
-      <c r="B431" s="1" t="s">
-        <v>945</v>
-      </c>
-      <c r="C431" s="1" t="s">
-        <v>948</v>
       </c>
       <c r="D431" s="4"/>
       <c r="E431" s="4"/>
@@ -8159,13 +8168,13 @@
     </row>
     <row r="432" spans="1:7">
       <c r="A432" s="6" t="s">
-        <v>978</v>
+        <v>972</v>
       </c>
       <c r="B432" s="5" t="s">
-        <v>979</v>
+        <v>973</v>
       </c>
       <c r="C432" s="5" t="s">
-        <v>980</v>
+        <v>974</v>
       </c>
       <c r="D432" s="4"/>
       <c r="E432" s="4"/>
@@ -8174,46 +8183,46 @@
     </row>
     <row r="433" spans="1:7">
       <c r="A433" t="s">
+        <v>964</v>
+      </c>
+      <c r="B433" s="1" t="s">
         <v>970</v>
       </c>
-      <c r="B433" s="1" t="s">
-        <v>976</v>
-      </c>
       <c r="C433" s="1" t="s">
-        <v>971</v>
+        <v>965</v>
       </c>
     </row>
     <row r="434" spans="1:7">
       <c r="A434" t="s">
-        <v>972</v>
+        <v>966</v>
       </c>
       <c r="B434" s="1" t="s">
-        <v>973</v>
+        <v>967</v>
       </c>
       <c r="C434" s="1" t="s">
-        <v>974</v>
+        <v>968</v>
       </c>
     </row>
     <row r="435" spans="1:7">
       <c r="A435" t="s">
-        <v>975</v>
+        <v>969</v>
       </c>
       <c r="B435" s="1" t="s">
-        <v>1066</v>
+        <v>1060</v>
       </c>
       <c r="C435" s="1" t="s">
-        <v>977</v>
+        <v>971</v>
       </c>
     </row>
     <row r="436" spans="1:7">
       <c r="A436" s="1" t="s">
+        <v>975</v>
+      </c>
+      <c r="B436" s="1" t="s">
+        <v>978</v>
+      </c>
+      <c r="C436" s="1" t="s">
         <v>981</v>
-      </c>
-      <c r="B436" s="1" t="s">
-        <v>984</v>
-      </c>
-      <c r="C436" s="1" t="s">
-        <v>987</v>
       </c>
       <c r="D436" s="4"/>
       <c r="E436" s="4"/>
@@ -8222,13 +8231,13 @@
     </row>
     <row r="437" spans="1:7">
       <c r="A437" s="1" t="s">
+        <v>976</v>
+      </c>
+      <c r="B437" s="1" t="s">
+        <v>979</v>
+      </c>
+      <c r="C437" s="1" t="s">
         <v>982</v>
-      </c>
-      <c r="B437" s="1" t="s">
-        <v>985</v>
-      </c>
-      <c r="C437" s="1" t="s">
-        <v>988</v>
       </c>
       <c r="D437" s="4"/>
       <c r="E437" s="4"/>
@@ -8237,450 +8246,450 @@
     </row>
     <row r="438" spans="1:7">
       <c r="A438" s="1" t="s">
+        <v>977</v>
+      </c>
+      <c r="B438" s="1" t="s">
+        <v>980</v>
+      </c>
+      <c r="C438" s="1" t="s">
         <v>983</v>
-      </c>
-      <c r="B438" s="1" t="s">
-        <v>986</v>
-      </c>
-      <c r="C438" s="1" t="s">
-        <v>989</v>
       </c>
       <c r="D438" s="4"/>
       <c r="E438" s="4"/>
       <c r="F438" s="4"/>
       <c r="G438" s="4"/>
     </row>
-    <row r="439" spans="1:7" ht="32">
+    <row r="439" spans="1:7" ht="30">
       <c r="A439" s="1" t="s">
-        <v>994</v>
+        <v>988</v>
       </c>
       <c r="B439" s="1" t="s">
-        <v>995</v>
+        <v>989</v>
       </c>
       <c r="C439" s="1" t="s">
-        <v>996</v>
+        <v>990</v>
       </c>
       <c r="D439" s="4"/>
       <c r="E439" s="4"/>
       <c r="F439" s="4"/>
       <c r="G439" s="4"/>
     </row>
-    <row r="440" spans="1:7" ht="160">
+    <row r="440" spans="1:7" ht="150">
       <c r="A440" s="1" t="s">
+        <v>991</v>
+      </c>
+      <c r="B440" s="1" t="s">
+        <v>992</v>
+      </c>
+      <c r="C440" s="1" t="s">
+        <v>993</v>
+      </c>
+    </row>
+    <row r="441" spans="1:7" ht="165">
+      <c r="A441" s="1" t="s">
+        <v>994</v>
+      </c>
+      <c r="B441" s="1" t="s">
+        <v>995</v>
+      </c>
+      <c r="C441" s="1" t="s">
+        <v>996</v>
+      </c>
+    </row>
+    <row r="442" spans="1:7" ht="30">
+      <c r="A442" s="1" t="s">
         <v>997</v>
       </c>
-      <c r="B440" s="1" t="s">
+      <c r="B442" s="1" t="s">
         <v>998</v>
       </c>
-      <c r="C440" s="1" t="s">
+      <c r="C442" s="1" t="s">
         <v>999</v>
       </c>
     </row>
-    <row r="441" spans="1:7" ht="176">
-      <c r="A441" s="1" t="s">
+    <row r="443" spans="1:7" ht="90">
+      <c r="A443" s="1" t="s">
         <v>1000</v>
       </c>
-      <c r="B441" s="1" t="s">
+      <c r="B443" s="1" t="s">
         <v>1001</v>
       </c>
-      <c r="C441" s="1" t="s">
+      <c r="C443" s="1" t="s">
         <v>1002</v>
       </c>
     </row>
-    <row r="442" spans="1:7" ht="32">
-      <c r="A442" s="1" t="s">
+    <row r="444" spans="1:7" ht="60">
+      <c r="A444" s="1" t="s">
         <v>1003</v>
       </c>
-      <c r="B442" s="1" t="s">
+      <c r="B444" s="1" t="s">
         <v>1004</v>
       </c>
-      <c r="C442" s="1" t="s">
+      <c r="C444" s="1" t="s">
         <v>1005</v>
       </c>
     </row>
-    <row r="443" spans="1:7" ht="96">
-      <c r="A443" s="1" t="s">
+    <row r="445" spans="1:7" ht="30">
+      <c r="A445" s="1" t="s">
         <v>1006</v>
       </c>
-      <c r="B443" s="1" t="s">
+      <c r="B445" s="1" t="s">
         <v>1007</v>
       </c>
-      <c r="C443" s="1" t="s">
+      <c r="C445" s="1" t="s">
         <v>1008</v>
       </c>
     </row>
-    <row r="444" spans="1:7" ht="64">
-      <c r="A444" s="1" t="s">
+    <row r="446" spans="1:7" ht="90">
+      <c r="A446" s="1" t="s">
         <v>1009</v>
       </c>
-      <c r="B444" s="1" t="s">
+      <c r="B446" s="1" t="s">
         <v>1010</v>
       </c>
-      <c r="C444" s="1" t="s">
+      <c r="C446" s="1" t="s">
         <v>1011</v>
       </c>
     </row>
-    <row r="445" spans="1:7" ht="32">
-      <c r="A445" s="1" t="s">
+    <row r="447" spans="1:7" ht="120">
+      <c r="A447" s="1" t="s">
         <v>1012</v>
       </c>
-      <c r="B445" s="1" t="s">
+      <c r="B447" s="1" t="s">
         <v>1013</v>
       </c>
-      <c r="C445" s="1" t="s">
+      <c r="C447" s="7" t="s">
         <v>1014</v>
-      </c>
-    </row>
-    <row r="446" spans="1:7" ht="96">
-      <c r="A446" s="1" t="s">
-        <v>1015</v>
-      </c>
-      <c r="B446" s="1" t="s">
-        <v>1016</v>
-      </c>
-      <c r="C446" s="1" t="s">
-        <v>1017</v>
-      </c>
-    </row>
-    <row r="447" spans="1:7" ht="128">
-      <c r="A447" s="1" t="s">
-        <v>1018</v>
-      </c>
-      <c r="B447" s="1" t="s">
-        <v>1019</v>
-      </c>
-      <c r="C447" s="7" t="s">
-        <v>1020</v>
       </c>
     </row>
     <row r="448" spans="1:7">
       <c r="A448" s="1" t="s">
+        <v>1015</v>
+      </c>
+      <c r="B448" s="1" t="s">
+        <v>1016</v>
+      </c>
+      <c r="C448" s="1" t="s">
+        <v>1017</v>
+      </c>
+    </row>
+    <row r="449" spans="1:3" ht="60">
+      <c r="A449" s="1" t="s">
+        <v>1018</v>
+      </c>
+      <c r="B449" s="1" t="s">
+        <v>1019</v>
+      </c>
+      <c r="C449" s="1" t="s">
+        <v>1020</v>
+      </c>
+    </row>
+    <row r="450" spans="1:3" ht="75">
+      <c r="A450" s="1" t="s">
         <v>1021</v>
       </c>
-      <c r="B448" s="1" t="s">
+      <c r="B450" s="1" t="s">
         <v>1022</v>
       </c>
-      <c r="C448" s="1" t="s">
+      <c r="C450" s="1" t="s">
         <v>1023</v>
       </c>
     </row>
-    <row r="449" spans="1:3" ht="64">
-      <c r="A449" s="1" t="s">
+    <row r="451" spans="1:3" ht="45">
+      <c r="A451" s="1" t="s">
         <v>1024</v>
       </c>
-      <c r="B449" s="1" t="s">
+      <c r="B451" s="1" t="s">
         <v>1025</v>
       </c>
-      <c r="C449" s="1" t="s">
+      <c r="C451" s="1" t="s">
         <v>1026</v>
       </c>
     </row>
-    <row r="450" spans="1:3" ht="80">
-      <c r="A450" s="1" t="s">
+    <row r="452" spans="1:3" ht="120">
+      <c r="A452" s="1" t="s">
         <v>1027</v>
       </c>
-      <c r="B450" s="1" t="s">
+      <c r="B452" s="1" t="s">
         <v>1028</v>
       </c>
-      <c r="C450" s="1" t="s">
+      <c r="C452" s="1" t="s">
         <v>1029</v>
       </c>
     </row>
-    <row r="451" spans="1:3" ht="48">
-      <c r="A451" s="1" t="s">
+    <row r="453" spans="1:3" ht="135">
+      <c r="A453" s="1" t="s">
         <v>1030</v>
       </c>
-      <c r="B451" s="1" t="s">
+      <c r="B453" s="1" t="s">
         <v>1031</v>
       </c>
-      <c r="C451" s="1" t="s">
+      <c r="C453" s="1" t="s">
         <v>1032</v>
       </c>
     </row>
-    <row r="452" spans="1:3" ht="128">
-      <c r="A452" s="1" t="s">
+    <row r="454" spans="1:3" ht="45">
+      <c r="A454" s="1" t="s">
         <v>1033</v>
       </c>
-      <c r="B452" s="1" t="s">
+      <c r="B454" s="1" t="s">
         <v>1034</v>
       </c>
-      <c r="C452" s="1" t="s">
+      <c r="C454" s="7" t="s">
         <v>1035</v>
       </c>
     </row>
-    <row r="453" spans="1:3" ht="144">
-      <c r="A453" s="1" t="s">
+    <row r="455" spans="1:3" ht="120">
+      <c r="A455" s="1" t="s">
         <v>1036</v>
       </c>
-      <c r="B453" s="1" t="s">
+      <c r="B455" s="1" t="s">
         <v>1037</v>
       </c>
-      <c r="C453" s="1" t="s">
+      <c r="C455" s="7" t="s">
         <v>1038</v>
       </c>
     </row>
-    <row r="454" spans="1:3" ht="48">
-      <c r="A454" s="1" t="s">
+    <row r="456" spans="1:3" ht="135">
+      <c r="A456" s="1" t="s">
         <v>1039</v>
       </c>
-      <c r="B454" s="1" t="s">
+      <c r="B456" s="1" t="s">
         <v>1040</v>
       </c>
-      <c r="C454" s="7" t="s">
+      <c r="C456" s="7" t="s">
         <v>1041</v>
       </c>
     </row>
-    <row r="455" spans="1:3" ht="128">
-      <c r="A455" s="1" t="s">
+    <row r="457" spans="1:3" ht="45">
+      <c r="A457" s="1" t="s">
         <v>1042</v>
       </c>
-      <c r="B455" s="1" t="s">
+      <c r="B457" s="1" t="s">
         <v>1043</v>
       </c>
-      <c r="C455" s="7" t="s">
+      <c r="C457" s="7" t="s">
         <v>1044</v>
       </c>
     </row>
-    <row r="456" spans="1:3" ht="144">
-      <c r="A456" s="1" t="s">
+    <row r="458" spans="1:3" ht="105">
+      <c r="A458" s="1" t="s">
         <v>1045</v>
       </c>
-      <c r="B456" s="1" t="s">
+      <c r="B458" s="1" t="s">
         <v>1046</v>
       </c>
-      <c r="C456" s="7" t="s">
+      <c r="C458" s="7" t="s">
         <v>1047</v>
       </c>
     </row>
-    <row r="457" spans="1:3" ht="48">
-      <c r="A457" s="1" t="s">
+    <row r="459" spans="1:3" ht="120">
+      <c r="A459" s="1" t="s">
         <v>1048</v>
       </c>
-      <c r="B457" s="1" t="s">
+      <c r="B459" s="1" t="s">
         <v>1049</v>
       </c>
-      <c r="C457" s="7" t="s">
+      <c r="C459" s="7" t="s">
         <v>1050</v>
       </c>
     </row>
-    <row r="458" spans="1:3" ht="112">
-      <c r="A458" s="1" t="s">
+    <row r="460" spans="1:3" ht="45">
+      <c r="A460" s="1" t="s">
         <v>1051</v>
       </c>
-      <c r="B458" s="1" t="s">
+      <c r="B460" s="1" t="s">
         <v>1052</v>
       </c>
-      <c r="C458" s="7" t="s">
+      <c r="C460" s="7" t="s">
         <v>1053</v>
       </c>
     </row>
-    <row r="459" spans="1:3" ht="128">
-      <c r="A459" s="1" t="s">
+    <row r="461" spans="1:3" ht="120">
+      <c r="A461" s="1" t="s">
         <v>1054</v>
       </c>
-      <c r="B459" s="1" t="s">
+      <c r="B461" s="1" t="s">
         <v>1055</v>
       </c>
-      <c r="C459" s="7" t="s">
+      <c r="C461" s="7" t="s">
         <v>1056</v>
       </c>
     </row>
-    <row r="460" spans="1:3" ht="48">
-      <c r="A460" s="1" t="s">
+    <row r="462" spans="1:3" ht="135">
+      <c r="A462" s="1" t="s">
         <v>1057</v>
       </c>
-      <c r="B460" s="1" t="s">
+      <c r="B462" s="1" t="s">
         <v>1058</v>
       </c>
-      <c r="C460" s="7" t="s">
+      <c r="C462" s="7" t="s">
         <v>1059</v>
-      </c>
-    </row>
-    <row r="461" spans="1:3" ht="128">
-      <c r="A461" s="1" t="s">
-        <v>1060</v>
-      </c>
-      <c r="B461" s="1" t="s">
-        <v>1061</v>
-      </c>
-      <c r="C461" s="7" t="s">
-        <v>1062</v>
-      </c>
-    </row>
-    <row r="462" spans="1:3" ht="144">
-      <c r="A462" s="1" t="s">
-        <v>1063</v>
-      </c>
-      <c r="B462" s="1" t="s">
-        <v>1064</v>
-      </c>
-      <c r="C462" s="7" t="s">
-        <v>1065</v>
       </c>
     </row>
     <row r="463" spans="1:3">
       <c r="A463" s="1" t="s">
-        <v>1094</v>
+        <v>1088</v>
       </c>
       <c r="B463" s="1" t="s">
-        <v>1106</v>
+        <v>1100</v>
       </c>
       <c r="C463" s="8" t="s">
-        <v>1107</v>
+        <v>1101</v>
       </c>
     </row>
     <row r="464" spans="1:3">
       <c r="A464" s="1" t="s">
-        <v>1095</v>
+        <v>1089</v>
       </c>
       <c r="B464" s="1" t="s">
-        <v>1119</v>
+        <v>1113</v>
       </c>
       <c r="C464" s="8" t="s">
-        <v>1108</v>
+        <v>1102</v>
       </c>
     </row>
     <row r="465" spans="1:3">
       <c r="A465" s="1" t="s">
-        <v>1096</v>
+        <v>1090</v>
       </c>
       <c r="B465" s="1" t="s">
-        <v>1120</v>
+        <v>1114</v>
       </c>
       <c r="C465" s="8" t="s">
-        <v>1109</v>
+        <v>1103</v>
       </c>
     </row>
     <row r="466" spans="1:3">
       <c r="A466" s="1" t="s">
-        <v>1097</v>
+        <v>1091</v>
       </c>
       <c r="B466" s="1" t="s">
-        <v>1121</v>
+        <v>1115</v>
       </c>
       <c r="C466" s="8" t="s">
-        <v>1110</v>
+        <v>1104</v>
       </c>
     </row>
     <row r="467" spans="1:3">
       <c r="A467" s="1" t="s">
-        <v>1098</v>
+        <v>1092</v>
       </c>
       <c r="B467" s="1" t="s">
-        <v>1122</v>
+        <v>1116</v>
       </c>
       <c r="C467" s="8" t="s">
-        <v>1111</v>
+        <v>1105</v>
       </c>
     </row>
     <row r="468" spans="1:3">
       <c r="A468" s="1" t="s">
-        <v>1099</v>
+        <v>1093</v>
       </c>
       <c r="B468" s="1" t="s">
-        <v>1123</v>
+        <v>1117</v>
       </c>
       <c r="C468" s="8" t="s">
-        <v>1112</v>
+        <v>1106</v>
       </c>
     </row>
     <row r="469" spans="1:3">
       <c r="A469" s="1" t="s">
-        <v>1100</v>
+        <v>1094</v>
       </c>
       <c r="B469" s="1" t="s">
-        <v>1124</v>
+        <v>1118</v>
       </c>
       <c r="C469" s="8" t="s">
-        <v>1113</v>
+        <v>1107</v>
       </c>
     </row>
     <row r="470" spans="1:3">
       <c r="A470" s="1" t="s">
-        <v>1101</v>
+        <v>1095</v>
       </c>
       <c r="B470" s="1" t="s">
-        <v>1125</v>
+        <v>1119</v>
       </c>
       <c r="C470" s="8" t="s">
-        <v>1114</v>
+        <v>1108</v>
       </c>
     </row>
     <row r="471" spans="1:3">
       <c r="A471" s="1" t="s">
-        <v>1102</v>
+        <v>1096</v>
       </c>
       <c r="B471" s="1" t="s">
-        <v>1126</v>
+        <v>1120</v>
       </c>
       <c r="C471" s="8" t="s">
-        <v>1115</v>
+        <v>1109</v>
       </c>
     </row>
     <row r="472" spans="1:3">
       <c r="A472" s="1" t="s">
-        <v>1103</v>
+        <v>1097</v>
       </c>
       <c r="B472" s="1" t="s">
-        <v>1127</v>
+        <v>1121</v>
       </c>
       <c r="C472" s="8" t="s">
-        <v>1116</v>
+        <v>1110</v>
       </c>
     </row>
     <row r="473" spans="1:3">
       <c r="A473" s="1" t="s">
-        <v>1104</v>
+        <v>1098</v>
       </c>
       <c r="B473" s="1" t="s">
-        <v>1128</v>
+        <v>1122</v>
       </c>
       <c r="C473" s="8" t="s">
-        <v>1117</v>
+        <v>1111</v>
       </c>
     </row>
     <row r="474" spans="1:3">
       <c r="A474" s="1" t="s">
-        <v>1105</v>
+        <v>1099</v>
       </c>
       <c r="B474" s="1" t="s">
-        <v>1129</v>
+        <v>1123</v>
       </c>
       <c r="C474" s="8" t="s">
-        <v>1118</v>
+        <v>1112</v>
       </c>
     </row>
     <row r="475" spans="1:3">
       <c r="A475" s="1" t="s">
+        <v>1124</v>
+      </c>
+      <c r="B475" s="1" t="s">
+        <v>1127</v>
+      </c>
+      <c r="C475" s="1" t="s">
+        <v>1128</v>
+      </c>
+    </row>
+    <row r="476" spans="1:3" ht="45">
+      <c r="A476" s="1" t="s">
+        <v>1125</v>
+      </c>
+      <c r="B476" s="1" t="s">
+        <v>1131</v>
+      </c>
+      <c r="C476" s="8" t="s">
+        <v>1129</v>
+      </c>
+    </row>
+    <row r="477" spans="1:3" ht="45">
+      <c r="A477" s="1" t="s">
+        <v>1126</v>
+      </c>
+      <c r="B477" s="1" t="s">
+        <v>1132</v>
+      </c>
+      <c r="C477" s="8" t="s">
         <v>1130</v>
-      </c>
-      <c r="B475" s="1" t="s">
-        <v>1133</v>
-      </c>
-      <c r="C475" s="1" t="s">
-        <v>1134</v>
-      </c>
-    </row>
-    <row r="476" spans="1:3" ht="48">
-      <c r="A476" s="1" t="s">
-        <v>1131</v>
-      </c>
-      <c r="B476" s="1" t="s">
-        <v>1137</v>
-      </c>
-      <c r="C476" s="8" t="s">
-        <v>1135</v>
-      </c>
-    </row>
-    <row r="477" spans="1:3" ht="48">
-      <c r="A477" s="1" t="s">
-        <v>1132</v>
-      </c>
-      <c r="B477" s="1" t="s">
-        <v>1138</v>
-      </c>
-      <c r="C477" s="8" t="s">
-        <v>1136</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
rules 36 and 37
</commit_message>
<xml_diff>
--- a/config/i18n/i18n.xlsx
+++ b/config/i18n/i18n.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-1360" yWindow="-18900" windowWidth="28800" windowHeight="17540" tabRatio="500"/>
+    <workbookView xWindow="-5080" yWindow="-21140" windowWidth="38400" windowHeight="21140" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1244" uniqueCount="1196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1256" uniqueCount="1208">
   <si>
     <t>key</t>
   </si>
@@ -3612,9 +3612,6 @@
     <t>Teste ao lançamento de apuramento de resultado líquido</t>
   </si>
   <si>
-    <t>Os movimentos de apuramento de resultado líquido  devem ser efetuado em diário próprio, para uma correta identificação no ficheiro SAF-T (PT). Teste realizado com sucesso.</t>
-  </si>
-  <si>
     <t>Verificamos que não existe nenhum movimento de apuramento de resultado líquido, ou se existir não está registado no diário correto. Por favor verifique se deve fazer este movimento ou se deve registar o mesmo no diário correto de apuramento de resultados. Alertamos para a FAQ 15-2887, que refere que em entidades com atividade, este movimento tem sempre de existir, ainda que tenha valor "0,00" (zero)</t>
   </si>
   <si>
@@ -3627,9 +3624,6 @@
     <t>Os saldos de abertura devem ser coincidentes com os saldos finais do exercício anterior. Comparamos os saldos de abertura do exercício com o exercício do ano anterior maracdo como principal e encontramos diferenças ao nível das seguintes contas:</t>
   </si>
   <si>
-    <t>Verificamos que existe um movimento de apuramento de resultado antes de impostos:</t>
-  </si>
-  <si>
     <t>O movimento de apuramento de resultado líquido tem de ser efetuado em diário próprio, para uma correta identificação no ficheiro SAF-T (PT). Verificamos que os seguintes lançamentos estão registados em diário tipificado como apuramento e movimentam contas não expectáveis:</t>
   </si>
   <si>
@@ -3673,6 +3667,48 @@
   </si>
   <si>
     <t>Verificamos que o movimento de aplicação de resultados foi registado em {0}. Verifique se não deverá efetuar esse registo até à data de 31 de Março, ou 31 de Maio para contas com MEP.</t>
+  </si>
+  <si>
+    <t>Teste à conta 811- "Resultado antes de imposto"</t>
+  </si>
+  <si>
+    <t>svat_t36</t>
+  </si>
+  <si>
+    <t>svat_t36_ok</t>
+  </si>
+  <si>
+    <t>svat_t36_nok</t>
+  </si>
+  <si>
+    <t>svat_t37</t>
+  </si>
+  <si>
+    <t>svat_t37_ok</t>
+  </si>
+  <si>
+    <t>svat_t37_nok</t>
+  </si>
+  <si>
+    <t>A conta 811- "Resultado antes de imposto" deve ser movimentada apenas em diário apropriado de apuramento de resultados. Teste realizado com sucesso.</t>
+  </si>
+  <si>
+    <t>A conta 811- "Resultado antes de imposto" deve ser movimentada apenas em diário apropriado de apuramento de resultados. Verificamos os seguintes lançamentos que movimentam a conta 811 e não estão registados em diário de Apuramento de Resultados:</t>
+  </si>
+  <si>
+    <t>Teste à conta 818- "Resultado líquido"</t>
+  </si>
+  <si>
+    <t>A conta 818 - "Resultado Líquido" deve ser movimentada apenas em diário apropriado de apuramento de resultados. Teste realizado com sucesso</t>
+  </si>
+  <si>
+    <t>A conta 818 - "Resultado Líquido" deve ser movimentada apenas em diário apropriado de apuramento de resultados. Verificamos os seguintes lançamentos que movimentam a conta 818 e não estão registados em diário de Apuramento de Resultados</t>
+  </si>
+  <si>
+    <t>Verificamos que existem os seguintes movimentos de apuramento de resultado antes de impostos: Diario Num Diario e data</t>
+  </si>
+  <si>
+    <t>Os movimentos de apuramento de resultado líquido  devem ser efetuados em diário próprio, para uma correta identificação no ficheiro SAF-T (PT). Teste realizado com sucesso.</t>
   </si>
 </sst>
 </file>
@@ -3863,8 +3899,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="i18n" displayName="i18n" ref="A1:G505" totalsRowShown="0" headerRowDxfId="6">
-  <autoFilter ref="A1:G505"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="i18n" displayName="i18n" ref="A1:G511" totalsRowShown="0" headerRowDxfId="6">
+  <autoFilter ref="A1:G511"/>
   <tableColumns count="7">
     <tableColumn id="1" name="key"/>
     <tableColumn id="2" name="pt" dataDxfId="5"/>
@@ -4141,10 +4177,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G505"/>
+  <dimension ref="A1:G511"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A489" workbookViewId="0">
-      <selection activeCell="B495" sqref="B495"/>
+    <sheetView tabSelected="1" topLeftCell="A498" workbookViewId="0">
+      <selection activeCell="B511" sqref="B511"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8893,12 +8929,12 @@
       </c>
       <c r="C481" s="8"/>
     </row>
-    <row r="482" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+    <row r="482" spans="1:3" ht="48" x14ac:dyDescent="0.2">
       <c r="A482" s="1" t="s">
         <v>1147</v>
       </c>
       <c r="B482" s="1" t="s">
-        <v>1180</v>
+        <v>1206</v>
       </c>
       <c r="C482" s="8"/>
     </row>
@@ -8925,7 +8961,7 @@
         <v>1148</v>
       </c>
       <c r="B485" s="1" t="s">
-        <v>1175</v>
+        <v>1207</v>
       </c>
       <c r="C485" s="8"/>
     </row>
@@ -8934,7 +8970,7 @@
         <v>1153</v>
       </c>
       <c r="B486" s="1" t="s">
-        <v>1181</v>
+        <v>1179</v>
       </c>
       <c r="C486" s="8"/>
     </row>
@@ -8952,7 +8988,7 @@
         <v>1149</v>
       </c>
       <c r="B488" s="1" t="s">
-        <v>1182</v>
+        <v>1180</v>
       </c>
       <c r="C488" s="8"/>
     </row>
@@ -8961,7 +8997,7 @@
         <v>1154</v>
       </c>
       <c r="B489" s="1" t="s">
-        <v>1176</v>
+        <v>1175</v>
       </c>
       <c r="C489" s="8"/>
     </row>
@@ -8970,7 +9006,7 @@
         <v>1166</v>
       </c>
       <c r="B490" s="1" t="s">
-        <v>1183</v>
+        <v>1181</v>
       </c>
       <c r="C490" s="8"/>
     </row>
@@ -8979,7 +9015,7 @@
         <v>1150</v>
       </c>
       <c r="B491" s="1" t="s">
-        <v>1184</v>
+        <v>1182</v>
       </c>
       <c r="C491" s="8"/>
     </row>
@@ -8988,7 +9024,7 @@
         <v>1155</v>
       </c>
       <c r="B492" s="1" t="s">
-        <v>1177</v>
+        <v>1176</v>
       </c>
       <c r="C492" s="8"/>
     </row>
@@ -8997,7 +9033,7 @@
         <v>1167</v>
       </c>
       <c r="B493" s="1" t="s">
-        <v>1183</v>
+        <v>1181</v>
       </c>
       <c r="C493" s="8"/>
     </row>
@@ -9006,7 +9042,7 @@
         <v>1151</v>
       </c>
       <c r="B494" s="1" t="s">
-        <v>1192</v>
+        <v>1190</v>
       </c>
       <c r="C494" s="8"/>
     </row>
@@ -9015,7 +9051,7 @@
         <v>1156</v>
       </c>
       <c r="B495" s="1" t="s">
-        <v>1195</v>
+        <v>1193</v>
       </c>
       <c r="C495" s="8"/>
     </row>
@@ -9024,7 +9060,7 @@
         <v>1168</v>
       </c>
       <c r="B496" s="1" t="s">
-        <v>1185</v>
+        <v>1183</v>
       </c>
       <c r="C496" s="8"/>
     </row>
@@ -9033,7 +9069,7 @@
         <v>1157</v>
       </c>
       <c r="B497" s="1" t="s">
-        <v>1193</v>
+        <v>1191</v>
       </c>
       <c r="C497" s="8"/>
     </row>
@@ -9042,7 +9078,7 @@
         <v>1158</v>
       </c>
       <c r="B498" s="1" t="s">
-        <v>1186</v>
+        <v>1184</v>
       </c>
       <c r="C498" s="8"/>
     </row>
@@ -9051,7 +9087,7 @@
         <v>1169</v>
       </c>
       <c r="B499" s="1" t="s">
-        <v>1185</v>
+        <v>1183</v>
       </c>
       <c r="C499" s="8"/>
     </row>
@@ -9060,25 +9096,25 @@
         <v>1159</v>
       </c>
       <c r="B500" s="1" t="s">
-        <v>1194</v>
+        <v>1192</v>
       </c>
       <c r="C500" s="8"/>
     </row>
     <row r="501" spans="1:3" ht="48" x14ac:dyDescent="0.2">
       <c r="A501" s="1" t="s">
+        <v>1186</v>
+      </c>
+      <c r="B501" s="1" t="s">
         <v>1188</v>
-      </c>
-      <c r="B501" s="1" t="s">
-        <v>1190</v>
       </c>
       <c r="C501" s="8"/>
     </row>
     <row r="502" spans="1:3" ht="80" x14ac:dyDescent="0.2">
       <c r="A502" s="1" t="s">
+        <v>1187</v>
+      </c>
+      <c r="B502" s="1" t="s">
         <v>1189</v>
-      </c>
-      <c r="B502" s="1" t="s">
-        <v>1191</v>
       </c>
       <c r="C502" s="8"/>
     </row>
@@ -9087,7 +9123,7 @@
         <v>1170</v>
       </c>
       <c r="B503" s="1" t="s">
-        <v>1187</v>
+        <v>1185</v>
       </c>
       <c r="C503" s="8"/>
     </row>
@@ -9096,7 +9132,7 @@
         <v>1160</v>
       </c>
       <c r="B504" s="1" t="s">
-        <v>1178</v>
+        <v>1177</v>
       </c>
       <c r="C504" s="8"/>
     </row>
@@ -9105,9 +9141,63 @@
         <v>1161</v>
       </c>
       <c r="B505" s="1" t="s">
-        <v>1179</v>
+        <v>1178</v>
       </c>
       <c r="C505" s="8"/>
+    </row>
+    <row r="506" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A506" s="1" t="s">
+        <v>1195</v>
+      </c>
+      <c r="B506" s="1" t="s">
+        <v>1194</v>
+      </c>
+      <c r="C506" s="8"/>
+    </row>
+    <row r="507" spans="1:3" ht="64" x14ac:dyDescent="0.2">
+      <c r="A507" s="1" t="s">
+        <v>1196</v>
+      </c>
+      <c r="B507" s="1" t="s">
+        <v>1201</v>
+      </c>
+      <c r="C507" s="8"/>
+    </row>
+    <row r="508" spans="1:3" ht="96" x14ac:dyDescent="0.2">
+      <c r="A508" s="1" t="s">
+        <v>1197</v>
+      </c>
+      <c r="B508" s="1" t="s">
+        <v>1202</v>
+      </c>
+      <c r="C508" s="8"/>
+    </row>
+    <row r="509" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A509" s="1" t="s">
+        <v>1198</v>
+      </c>
+      <c r="B509" s="1" t="s">
+        <v>1203</v>
+      </c>
+      <c r="C509" s="8"/>
+    </row>
+    <row r="510" spans="1:3" ht="64" x14ac:dyDescent="0.2">
+      <c r="A510" s="1" t="s">
+        <v>1199</v>
+      </c>
+      <c r="B510" s="1" t="s">
+        <v>1204</v>
+      </c>
+      <c r="C510" s="8"/>
+    </row>
+    <row r="511" spans="1:3" ht="96" x14ac:dyDescent="0.2">
+      <c r="A511" s="1" t="s">
+        <v>1200</v>
+      </c>
+      <c r="B511" s="1" t="s">
+        <v>1205</v>
+      </c>
+      <c r="C511" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
changes in rule 29
</commit_message>
<xml_diff>
--- a/config/i18n/i18n.xlsx
+++ b/config/i18n/i18n.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1274" uniqueCount="1226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1276" uniqueCount="1228">
   <si>
     <t>key</t>
   </si>
@@ -3618,12 +3618,6 @@
     <t>Verificamos que não existe nenhum movimento de aplicação de resultados. Confirme por favor se não deverá efetuar esse movimento. Alertamos para a FAQ 14-2886, que refere que em entidades com atividade, este movimento tem sempre de existir, ainda que tenha valor "0,00" (zero)</t>
   </si>
   <si>
-    <t>Os saldos de abertura devem ser coincidentes com os saldos finais do exercício anterior. Comparamos os saldos de abertura do exercício com o exercício do ano anterior maracdo como principal. Sem exceções</t>
-  </si>
-  <si>
-    <t>Os saldos de abertura devem ser coincidentes com os saldos finais do exercício anterior. Comparamos os saldos de abertura do exercício com o exercício do ano anterior maracdo como principal e encontramos diferenças ao nível das seguintes contas:</t>
-  </si>
-  <si>
     <t>O movimento de apuramento de resultado líquido tem de ser efetuado em diário próprio, para uma correta identificação no ficheiro SAF-T (PT). Verificamos que os seguintes lançamentos estão registados em diário tipificado como apuramento e movimentam contas não expectáveis:</t>
   </si>
   <si>
@@ -3763,6 +3757,18 @@
   </si>
   <si>
     <t>Verificamos que existem os seguintes movimentos que estão em aberto. Deverá finalizar ou anular os mesmos:</t>
+  </si>
+  <si>
+    <t>svat_t29_ok_no_py</t>
+  </si>
+  <si>
+    <t>Os saldos de abertura devem ser coincidentes com os saldos finais do exercício anterior. Comparamos os saldos de abertura do exercício com o exercício do ano anterior marcado como principal. Sem exceções</t>
+  </si>
+  <si>
+    <t>Os saldos de abertura devem ser coincidentes com os saldos finais do exercício anterior. Não nos foi possível efetuar este teste uma vez que não existe exercício do ano {0} no TOConline.</t>
+  </si>
+  <si>
+    <t>Os saldos de abertura devem ser coincidentes com os saldos finais do exercício anterior. Comparamos os saldos de abertura do exercício com o exercício do ano anterior marcado como principal "{0}" e encontramos diferenças ao nível das seguintes contas:</t>
   </si>
 </sst>
 </file>
@@ -3953,8 +3959,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="i18n" displayName="i18n" ref="A1:G520" totalsRowShown="0" headerRowDxfId="6">
-  <autoFilter ref="A1:G520"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="i18n" displayName="i18n" ref="A1:G521" totalsRowShown="0" headerRowDxfId="6">
+  <autoFilter ref="A1:G521"/>
   <tableColumns count="7">
     <tableColumn id="1" name="key"/>
     <tableColumn id="2" name="pt" dataDxfId="5"/>
@@ -4231,10 +4237,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G520"/>
+  <dimension ref="A1:G521"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A508" workbookViewId="0">
-      <selection activeCell="A520" sqref="A520"/>
+    <sheetView tabSelected="1" topLeftCell="A498" workbookViewId="0">
+      <selection activeCell="C502" sqref="C502"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8988,7 +8994,7 @@
         <v>1147</v>
       </c>
       <c r="B482" s="1" t="s">
-        <v>1206</v>
+        <v>1204</v>
       </c>
       <c r="C482" s="8"/>
     </row>
@@ -9015,7 +9021,7 @@
         <v>1148</v>
       </c>
       <c r="B485" s="1" t="s">
-        <v>1207</v>
+        <v>1205</v>
       </c>
       <c r="C485" s="8"/>
     </row>
@@ -9024,7 +9030,7 @@
         <v>1153</v>
       </c>
       <c r="B486" s="1" t="s">
-        <v>1179</v>
+        <v>1177</v>
       </c>
       <c r="C486" s="8"/>
     </row>
@@ -9042,7 +9048,7 @@
         <v>1149</v>
       </c>
       <c r="B488" s="1" t="s">
-        <v>1180</v>
+        <v>1178</v>
       </c>
       <c r="C488" s="8"/>
     </row>
@@ -9060,7 +9066,7 @@
         <v>1166</v>
       </c>
       <c r="B490" s="1" t="s">
-        <v>1181</v>
+        <v>1179</v>
       </c>
       <c r="C490" s="8"/>
     </row>
@@ -9069,7 +9075,7 @@
         <v>1150</v>
       </c>
       <c r="B491" s="1" t="s">
-        <v>1182</v>
+        <v>1180</v>
       </c>
       <c r="C491" s="8"/>
     </row>
@@ -9087,7 +9093,7 @@
         <v>1167</v>
       </c>
       <c r="B493" s="1" t="s">
-        <v>1181</v>
+        <v>1179</v>
       </c>
       <c r="C493" s="8"/>
     </row>
@@ -9096,7 +9102,7 @@
         <v>1151</v>
       </c>
       <c r="B494" s="1" t="s">
-        <v>1190</v>
+        <v>1188</v>
       </c>
       <c r="C494" s="8"/>
     </row>
@@ -9105,7 +9111,7 @@
         <v>1156</v>
       </c>
       <c r="B495" s="1" t="s">
-        <v>1193</v>
+        <v>1191</v>
       </c>
       <c r="C495" s="8"/>
     </row>
@@ -9114,7 +9120,7 @@
         <v>1168</v>
       </c>
       <c r="B496" s="1" t="s">
-        <v>1183</v>
+        <v>1181</v>
       </c>
       <c r="C496" s="8"/>
     </row>
@@ -9123,7 +9129,7 @@
         <v>1157</v>
       </c>
       <c r="B497" s="1" t="s">
-        <v>1191</v>
+        <v>1189</v>
       </c>
       <c r="C497" s="8"/>
     </row>
@@ -9132,7 +9138,7 @@
         <v>1158</v>
       </c>
       <c r="B498" s="1" t="s">
-        <v>1184</v>
+        <v>1182</v>
       </c>
       <c r="C498" s="8"/>
     </row>
@@ -9141,7 +9147,7 @@
         <v>1169</v>
       </c>
       <c r="B499" s="1" t="s">
-        <v>1183</v>
+        <v>1181</v>
       </c>
       <c r="C499" s="8"/>
     </row>
@@ -9150,25 +9156,25 @@
         <v>1159</v>
       </c>
       <c r="B500" s="1" t="s">
-        <v>1192</v>
+        <v>1190</v>
       </c>
       <c r="C500" s="8"/>
     </row>
     <row r="501" spans="1:3" ht="48" x14ac:dyDescent="0.2">
       <c r="A501" s="1" t="s">
+        <v>1184</v>
+      </c>
+      <c r="B501" s="1" t="s">
         <v>1186</v>
-      </c>
-      <c r="B501" s="1" t="s">
-        <v>1188</v>
       </c>
       <c r="C501" s="8"/>
     </row>
     <row r="502" spans="1:3" ht="80" x14ac:dyDescent="0.2">
       <c r="A502" s="1" t="s">
+        <v>1185</v>
+      </c>
+      <c r="B502" s="1" t="s">
         <v>1187</v>
-      </c>
-      <c r="B502" s="1" t="s">
-        <v>1189</v>
       </c>
       <c r="C502" s="8"/>
     </row>
@@ -9177,7 +9183,7 @@
         <v>1170</v>
       </c>
       <c r="B503" s="1" t="s">
-        <v>1185</v>
+        <v>1183</v>
       </c>
       <c r="C503" s="8"/>
     </row>
@@ -9186,153 +9192,162 @@
         <v>1160</v>
       </c>
       <c r="B504" s="1" t="s">
-        <v>1177</v>
+        <v>1225</v>
       </c>
       <c r="C504" s="8"/>
     </row>
-    <row r="505" spans="1:3" ht="80" x14ac:dyDescent="0.2">
+    <row r="505" spans="1:3" ht="64" x14ac:dyDescent="0.2">
       <c r="A505" s="1" t="s">
+        <v>1224</v>
+      </c>
+      <c r="B505" s="1" t="s">
+        <v>1226</v>
+      </c>
+      <c r="C505" s="8"/>
+    </row>
+    <row r="506" spans="1:3" ht="96" x14ac:dyDescent="0.2">
+      <c r="A506" s="1" t="s">
         <v>1161</v>
       </c>
-      <c r="B505" s="1" t="s">
-        <v>1178</v>
-      </c>
-      <c r="C505" s="8"/>
-    </row>
-    <row r="506" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A506" s="1" t="s">
+      <c r="B506" s="1" t="s">
+        <v>1227</v>
+      </c>
+      <c r="C506" s="8"/>
+    </row>
+    <row r="507" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A507" s="1" t="s">
+        <v>1193</v>
+      </c>
+      <c r="B507" s="1" t="s">
+        <v>1192</v>
+      </c>
+      <c r="C507" s="8"/>
+    </row>
+    <row r="508" spans="1:3" ht="64" x14ac:dyDescent="0.2">
+      <c r="A508" s="1" t="s">
+        <v>1194</v>
+      </c>
+      <c r="B508" s="1" t="s">
+        <v>1199</v>
+      </c>
+      <c r="C508" s="8"/>
+    </row>
+    <row r="509" spans="1:3" ht="96" x14ac:dyDescent="0.2">
+      <c r="A509" s="1" t="s">
         <v>1195</v>
       </c>
-      <c r="B506" s="1" t="s">
-        <v>1194</v>
-      </c>
-      <c r="C506" s="8"/>
-    </row>
-    <row r="507" spans="1:3" ht="64" x14ac:dyDescent="0.2">
-      <c r="A507" s="1" t="s">
+      <c r="B509" s="1" t="s">
+        <v>1200</v>
+      </c>
+      <c r="C509" s="8"/>
+    </row>
+    <row r="510" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A510" s="1" t="s">
         <v>1196</v>
       </c>
-      <c r="B507" s="1" t="s">
+      <c r="B510" s="1" t="s">
         <v>1201</v>
       </c>
-      <c r="C507" s="8"/>
-    </row>
-    <row r="508" spans="1:3" ht="96" x14ac:dyDescent="0.2">
-      <c r="A508" s="1" t="s">
+      <c r="C510" s="8"/>
+    </row>
+    <row r="511" spans="1:3" ht="64" x14ac:dyDescent="0.2">
+      <c r="A511" s="1" t="s">
         <v>1197</v>
       </c>
-      <c r="B508" s="1" t="s">
+      <c r="B511" s="1" t="s">
         <v>1202</v>
       </c>
-      <c r="C508" s="8"/>
-    </row>
-    <row r="509" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A509" s="1" t="s">
+      <c r="C511" s="8"/>
+    </row>
+    <row r="512" spans="1:3" ht="96" x14ac:dyDescent="0.2">
+      <c r="A512" s="1" t="s">
         <v>1198</v>
       </c>
-      <c r="B509" s="1" t="s">
+      <c r="B512" s="1" t="s">
         <v>1203</v>
       </c>
-      <c r="C509" s="8"/>
-    </row>
-    <row r="510" spans="1:3" ht="64" x14ac:dyDescent="0.2">
-      <c r="A510" s="1" t="s">
-        <v>1199</v>
-      </c>
-      <c r="B510" s="1" t="s">
-        <v>1204</v>
-      </c>
-      <c r="C510" s="8"/>
-    </row>
-    <row r="511" spans="1:3" ht="96" x14ac:dyDescent="0.2">
-      <c r="A511" s="1" t="s">
-        <v>1200</v>
-      </c>
-      <c r="B511" s="1" t="s">
-        <v>1205</v>
-      </c>
-      <c r="C511" s="8"/>
-    </row>
-    <row r="512" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A512" s="1" t="s">
+      <c r="C512" s="8"/>
+    </row>
+    <row r="513" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A513" s="1" t="s">
+        <v>1206</v>
+      </c>
+      <c r="B513" s="1" t="s">
+        <v>1215</v>
+      </c>
+      <c r="C513" s="8"/>
+    </row>
+    <row r="514" spans="1:3" ht="48" x14ac:dyDescent="0.2">
+      <c r="A514" s="1" t="s">
+        <v>1207</v>
+      </c>
+      <c r="B514" s="1" t="s">
+        <v>1216</v>
+      </c>
+      <c r="C514" s="8"/>
+    </row>
+    <row r="515" spans="1:3" ht="64" x14ac:dyDescent="0.2">
+      <c r="A515" s="1" t="s">
         <v>1208</v>
       </c>
-      <c r="B512" s="1" t="s">
+      <c r="B515" s="1" t="s">
         <v>1217</v>
       </c>
-      <c r="C512" s="8"/>
-    </row>
-    <row r="513" spans="1:3" ht="48" x14ac:dyDescent="0.2">
-      <c r="A513" s="1" t="s">
+      <c r="C515" s="8"/>
+    </row>
+    <row r="516" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A516" s="1" t="s">
         <v>1209</v>
       </c>
-      <c r="B513" s="1" t="s">
+      <c r="B516" s="1" t="s">
         <v>1218</v>
       </c>
-      <c r="C513" s="8"/>
-    </row>
-    <row r="514" spans="1:3" ht="64" x14ac:dyDescent="0.2">
-      <c r="A514" s="1" t="s">
+      <c r="C516" s="8"/>
+    </row>
+    <row r="517" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+      <c r="A517" s="1" t="s">
         <v>1210</v>
       </c>
-      <c r="B514" s="1" t="s">
+      <c r="B517" s="1" t="s">
         <v>1219</v>
       </c>
-      <c r="C514" s="8"/>
-    </row>
-    <row r="515" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A515" s="1" t="s">
+      <c r="C517" s="8"/>
+    </row>
+    <row r="518" spans="1:3" ht="48" x14ac:dyDescent="0.2">
+      <c r="A518" s="1" t="s">
         <v>1211</v>
       </c>
-      <c r="B515" s="1" t="s">
+      <c r="B518" s="1" t="s">
         <v>1220</v>
       </c>
-      <c r="C515" s="8"/>
-    </row>
-    <row r="516" spans="1:3" ht="32" x14ac:dyDescent="0.2">
-      <c r="A516" s="1" t="s">
+      <c r="C518" s="8"/>
+    </row>
+    <row r="519" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A519" s="1" t="s">
         <v>1212</v>
       </c>
-      <c r="B516" s="1" t="s">
+      <c r="B519" s="1" t="s">
         <v>1221</v>
       </c>
-      <c r="C516" s="8"/>
-    </row>
-    <row r="517" spans="1:3" ht="48" x14ac:dyDescent="0.2">
-      <c r="A517" s="1" t="s">
+      <c r="C519" s="8"/>
+    </row>
+    <row r="520" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+      <c r="A520" s="1" t="s">
         <v>1213</v>
       </c>
-      <c r="B517" s="1" t="s">
+      <c r="B520" s="1" t="s">
         <v>1222</v>
       </c>
-      <c r="C517" s="8"/>
-    </row>
-    <row r="518" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A518" s="1" t="s">
+      <c r="C520" s="8"/>
+    </row>
+    <row r="521" spans="1:3" ht="48" x14ac:dyDescent="0.2">
+      <c r="A521" s="1" t="s">
         <v>1214</v>
       </c>
-      <c r="B518" s="1" t="s">
+      <c r="B521" s="1" t="s">
         <v>1223</v>
       </c>
-      <c r="C518" s="8"/>
-    </row>
-    <row r="519" spans="1:3" ht="32" x14ac:dyDescent="0.2">
-      <c r="A519" s="1" t="s">
-        <v>1215</v>
-      </c>
-      <c r="B519" s="1" t="s">
-        <v>1224</v>
-      </c>
-      <c r="C519" s="8"/>
-    </row>
-    <row r="520" spans="1:3" ht="48" x14ac:dyDescent="0.2">
-      <c r="A520" s="1" t="s">
-        <v>1216</v>
-      </c>
-      <c r="B520" s="1" t="s">
-        <v>1225</v>
-      </c>
-      <c r="C520" s="8"/>
+      <c r="C521" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
svat rules 30 to 35
</commit_message>
<xml_diff>
--- a/config/i18n/i18n.xlsx
+++ b/config/i18n/i18n.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1276" uniqueCount="1228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1312" uniqueCount="1263">
   <si>
     <t>key</t>
   </si>
@@ -3769,6 +3769,111 @@
   </si>
   <si>
     <t>Os saldos de abertura devem ser coincidentes com os saldos finais do exercício anterior. Comparamos os saldos de abertura do exercício com o exercício do ano anterior marcado como principal "{0}" e encontramos diferenças ao nível das seguintes contas:</t>
+  </si>
+  <si>
+    <t>svat_t30</t>
+  </si>
+  <si>
+    <t>svat_t30_ok</t>
+  </si>
+  <si>
+    <t>svat_t30_nok</t>
+  </si>
+  <si>
+    <t>svat_t31</t>
+  </si>
+  <si>
+    <t>svat_t31_ok</t>
+  </si>
+  <si>
+    <t>svat_t31_nok</t>
+  </si>
+  <si>
+    <t>svat_t32</t>
+  </si>
+  <si>
+    <t>svat_t32_ok</t>
+  </si>
+  <si>
+    <t>svat_t32_nok</t>
+  </si>
+  <si>
+    <t>svat_t35</t>
+  </si>
+  <si>
+    <t>svat_t35_ok</t>
+  </si>
+  <si>
+    <t>svat_t35_nok</t>
+  </si>
+  <si>
+    <t>Teste à utilização da conta 261- "Acionistas - Acionistas com subscrição"</t>
+  </si>
+  <si>
+    <t>Teste à utilização da conta 262- "Sócios - Quotas não liberadas"</t>
+  </si>
+  <si>
+    <t>A conta 261 deve ser utilizada exclusivamente por sociedades anónimas e comandita por ações. Sem exceções.</t>
+  </si>
+  <si>
+    <t>A conta 261 deve ser utilizada exclusivamente por sociedades anónimas e comandita por ações. Verifique o 'tipo de sociedade' na ficha da empresa ou os movimentos nas seguintes contas:</t>
+  </si>
+  <si>
+    <t>A conta 262 deve ser utilizada exclusivamente por sociedades anónimas e comandita por ações. Sem exceções.</t>
+  </si>
+  <si>
+    <t>A conta 262 deve ser utilizada exclusivamente por sociedades anónimas e comandita por ações. Verifique o 'tipo de sociedade' na ficha da empresa ou os movimentos nas seguintes contas:</t>
+  </si>
+  <si>
+    <t>Teste à utilização da conta 263-"Adiantamentos por conta de lucros"</t>
+  </si>
+  <si>
+    <t>A conta 263 não deve ser utilizada por sociedades anónimas. Sem exceções.</t>
+  </si>
+  <si>
+    <t>A conta 263 não deve ser utilizada por sociedades anónimas. Nas sociedades anónimas, os adiantamentos devem estar representados no saldo devedor da conta 89 - "Dividendos antecipados". Verifique o saldo das contas:</t>
+  </si>
+  <si>
+    <t>Teste à conta 269-  "Acionistas/sócios - Perdas por imparidade acumuladas"</t>
+  </si>
+  <si>
+    <t>Foi efetuado um teste sobre a conta 269 - "Acionistas/sócios - Perdas por imparidade acumuladas"e verificado que o saldo credor desta conta, entidade a entidade, é igual ou  superior à soma algébrica dos saldos das contas 261;262;263;266;267 e 268, para as seguintes entidades:</t>
+  </si>
+  <si>
+    <t>Representação dos impostos diferidos no Ativo e no Passivo</t>
+  </si>
+  <si>
+    <t>Verificamos que apenas tem saldo numa sub-conta da conta 274- "Impostos Diferidos". Se eventualmente efetuou compensação de saldos entre as contas 2741 e 2742, recomendamos verificar se essa compensação é adequada tendo em conta os parágrafos 68 a 69 da NCRF 25.</t>
+  </si>
+  <si>
+    <t>Verificamos que tem saldos nas contas 2741 -'Ativos por impostos diferidos' e 2742-'Passivos por impostos diferidos'. Sugerimos rever se não deverá efetuar compensação de saldos de acordo com os parágrafos 68 a 69 da NCRF 25.</t>
+  </si>
+  <si>
+    <t>account_269</t>
+  </si>
+  <si>
+    <t>account_269_var</t>
+  </si>
+  <si>
+    <t>account_269_ok</t>
+  </si>
+  <si>
+    <t>account_269_nok</t>
+  </si>
+  <si>
+    <t>account_269_var_ok</t>
+  </si>
+  <si>
+    <t>account_269_var_nok</t>
+  </si>
+  <si>
+    <t>Foi efetuado um teste sobre a conta 269 - "Acionistas/sócios - Perdas por imparidade acumuladas"e verificado que o saldo credor desta conta é igual ou  inferior à soma algébrica dos saldos das contas 261;262;263;266;267 e 268. Teste realizado com sucesso.</t>
+  </si>
+  <si>
+    <t>Foi efetuado um teste sobre a conta 269 - "Acionistas/sócios - Perdas por imparidade acumuladas"e verificado que o saldo credor desta conta, entidade a entidade, é igual ou  inferior à soma algébrica dos saldos das contas 261;262;263;266;267 e 268. Teste realizado com sucesso.</t>
+  </si>
+  <si>
+    <t>Foi efetuado um teste sobre a conta 269 - "Acionistas/sócios - Perdas por imparidade acumuladas"e verificado que o saldo credor desta conta é igual ou  superior à soma algébrica dos saldos das contas 261;262;263;266;267 e 268. Esta situação deve ser regularizada para uma correta submissão do ficheiro SAF-T.</t>
   </si>
 </sst>
 </file>
@@ -3959,8 +4064,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="i18n" displayName="i18n" ref="A1:G521" totalsRowShown="0" headerRowDxfId="6">
-  <autoFilter ref="A1:G521"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="i18n" displayName="i18n" ref="A1:G539" totalsRowShown="0" headerRowDxfId="6">
+  <autoFilter ref="A1:G539"/>
   <tableColumns count="7">
     <tableColumn id="1" name="key"/>
     <tableColumn id="2" name="pt" dataDxfId="5"/>
@@ -4237,10 +4342,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G521"/>
+  <dimension ref="A1:G539"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A498" workbookViewId="0">
-      <selection activeCell="C502" sqref="C502"/>
+    <sheetView tabSelected="1" topLeftCell="A517" workbookViewId="0">
+      <selection activeCell="A520" sqref="A520"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9214,140 +9319,302 @@
       </c>
       <c r="C506" s="8"/>
     </row>
-    <row r="507" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="507" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A507" s="1" t="s">
+        <v>1228</v>
+      </c>
+      <c r="B507" s="1" t="s">
+        <v>1240</v>
+      </c>
+      <c r="C507" s="8"/>
+    </row>
+    <row r="508" spans="1:3" ht="48" x14ac:dyDescent="0.2">
+      <c r="A508" s="1" t="s">
+        <v>1229</v>
+      </c>
+      <c r="B508" s="1" t="s">
+        <v>1242</v>
+      </c>
+      <c r="C508" s="8"/>
+    </row>
+    <row r="509" spans="1:3" ht="64" x14ac:dyDescent="0.2">
+      <c r="A509" s="1" t="s">
+        <v>1230</v>
+      </c>
+      <c r="B509" s="1" t="s">
+        <v>1243</v>
+      </c>
+      <c r="C509" s="8"/>
+    </row>
+    <row r="510" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+      <c r="A510" s="1" t="s">
+        <v>1231</v>
+      </c>
+      <c r="B510" s="1" t="s">
+        <v>1241</v>
+      </c>
+      <c r="C510" s="8"/>
+    </row>
+    <row r="511" spans="1:3" ht="48" x14ac:dyDescent="0.2">
+      <c r="A511" s="1" t="s">
+        <v>1232</v>
+      </c>
+      <c r="B511" s="1" t="s">
+        <v>1244</v>
+      </c>
+      <c r="C511" s="8"/>
+    </row>
+    <row r="512" spans="1:3" ht="64" x14ac:dyDescent="0.2">
+      <c r="A512" s="1" t="s">
+        <v>1233</v>
+      </c>
+      <c r="B512" s="1" t="s">
+        <v>1245</v>
+      </c>
+      <c r="C512" s="8"/>
+    </row>
+    <row r="513" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+      <c r="A513" s="1" t="s">
+        <v>1234</v>
+      </c>
+      <c r="B513" s="1" t="s">
+        <v>1246</v>
+      </c>
+      <c r="C513" s="8"/>
+    </row>
+    <row r="514" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+      <c r="A514" s="1" t="s">
+        <v>1235</v>
+      </c>
+      <c r="B514" s="1" t="s">
+        <v>1247</v>
+      </c>
+      <c r="C514" s="8"/>
+    </row>
+    <row r="515" spans="1:3" ht="80" x14ac:dyDescent="0.2">
+      <c r="A515" s="1" t="s">
+        <v>1236</v>
+      </c>
+      <c r="B515" s="1" t="s">
+        <v>1248</v>
+      </c>
+      <c r="C515" s="8"/>
+    </row>
+    <row r="516" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+      <c r="A516" s="1" t="s">
+        <v>1254</v>
+      </c>
+      <c r="B516" s="1" t="s">
+        <v>1249</v>
+      </c>
+      <c r="C516" s="8"/>
+    </row>
+    <row r="517" spans="1:3" ht="96" x14ac:dyDescent="0.2">
+      <c r="A517" s="1" t="s">
+        <v>1256</v>
+      </c>
+      <c r="B517" s="1" t="s">
+        <v>1260</v>
+      </c>
+      <c r="C517" s="8"/>
+    </row>
+    <row r="518" spans="1:3" ht="112" x14ac:dyDescent="0.2">
+      <c r="A518" s="1" t="s">
+        <v>1257</v>
+      </c>
+      <c r="B518" s="1" t="s">
+        <v>1262</v>
+      </c>
+      <c r="C518" s="8"/>
+    </row>
+    <row r="519" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+      <c r="A519" s="1" t="s">
+        <v>1255</v>
+      </c>
+      <c r="B519" s="1" t="s">
+        <v>1249</v>
+      </c>
+      <c r="C519" s="8"/>
+    </row>
+    <row r="520" spans="1:3" ht="112" x14ac:dyDescent="0.2">
+      <c r="A520" s="1" t="s">
+        <v>1258</v>
+      </c>
+      <c r="B520" s="1" t="s">
+        <v>1261</v>
+      </c>
+      <c r="C520" s="8"/>
+    </row>
+    <row r="521" spans="1:3" ht="112" x14ac:dyDescent="0.2">
+      <c r="A521" s="1" t="s">
+        <v>1259</v>
+      </c>
+      <c r="B521" s="1" t="s">
+        <v>1250</v>
+      </c>
+      <c r="C521" s="8"/>
+    </row>
+    <row r="522" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+      <c r="A522" s="1" t="s">
+        <v>1237</v>
+      </c>
+      <c r="B522" s="1" t="s">
+        <v>1251</v>
+      </c>
+      <c r="C522" s="8"/>
+    </row>
+    <row r="523" spans="1:3" ht="96" x14ac:dyDescent="0.2">
+      <c r="A523" s="1" t="s">
+        <v>1238</v>
+      </c>
+      <c r="B523" s="1" t="s">
+        <v>1252</v>
+      </c>
+      <c r="C523" s="8"/>
+    </row>
+    <row r="524" spans="1:3" ht="80" x14ac:dyDescent="0.2">
+      <c r="A524" s="1" t="s">
+        <v>1239</v>
+      </c>
+      <c r="B524" s="1" t="s">
+        <v>1253</v>
+      </c>
+      <c r="C524" s="8"/>
+    </row>
+    <row r="525" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A525" s="1" t="s">
         <v>1193</v>
       </c>
-      <c r="B507" s="1" t="s">
+      <c r="B525" s="1" t="s">
         <v>1192</v>
       </c>
-      <c r="C507" s="8"/>
-    </row>
-    <row r="508" spans="1:3" ht="64" x14ac:dyDescent="0.2">
-      <c r="A508" s="1" t="s">
+      <c r="C525" s="8"/>
+    </row>
+    <row r="526" spans="1:3" ht="64" x14ac:dyDescent="0.2">
+      <c r="A526" s="1" t="s">
         <v>1194</v>
       </c>
-      <c r="B508" s="1" t="s">
+      <c r="B526" s="1" t="s">
         <v>1199</v>
       </c>
-      <c r="C508" s="8"/>
-    </row>
-    <row r="509" spans="1:3" ht="96" x14ac:dyDescent="0.2">
-      <c r="A509" s="1" t="s">
+      <c r="C526" s="8"/>
+    </row>
+    <row r="527" spans="1:3" ht="96" x14ac:dyDescent="0.2">
+      <c r="A527" s="1" t="s">
         <v>1195</v>
       </c>
-      <c r="B509" s="1" t="s">
+      <c r="B527" s="1" t="s">
         <v>1200</v>
       </c>
-      <c r="C509" s="8"/>
-    </row>
-    <row r="510" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A510" s="1" t="s">
+      <c r="C527" s="8"/>
+    </row>
+    <row r="528" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A528" s="1" t="s">
         <v>1196</v>
       </c>
-      <c r="B510" s="1" t="s">
+      <c r="B528" s="1" t="s">
         <v>1201</v>
       </c>
-      <c r="C510" s="8"/>
-    </row>
-    <row r="511" spans="1:3" ht="64" x14ac:dyDescent="0.2">
-      <c r="A511" s="1" t="s">
+      <c r="C528" s="8"/>
+    </row>
+    <row r="529" spans="1:3" ht="64" x14ac:dyDescent="0.2">
+      <c r="A529" s="1" t="s">
         <v>1197</v>
       </c>
-      <c r="B511" s="1" t="s">
+      <c r="B529" s="1" t="s">
         <v>1202</v>
       </c>
-      <c r="C511" s="8"/>
-    </row>
-    <row r="512" spans="1:3" ht="96" x14ac:dyDescent="0.2">
-      <c r="A512" s="1" t="s">
+      <c r="C529" s="8"/>
+    </row>
+    <row r="530" spans="1:3" ht="96" x14ac:dyDescent="0.2">
+      <c r="A530" s="1" t="s">
         <v>1198</v>
       </c>
-      <c r="B512" s="1" t="s">
+      <c r="B530" s="1" t="s">
         <v>1203</v>
       </c>
-      <c r="C512" s="8"/>
-    </row>
-    <row r="513" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A513" s="1" t="s">
+      <c r="C530" s="8"/>
+    </row>
+    <row r="531" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A531" s="1" t="s">
         <v>1206</v>
       </c>
-      <c r="B513" s="1" t="s">
+      <c r="B531" s="1" t="s">
         <v>1215</v>
       </c>
-      <c r="C513" s="8"/>
-    </row>
-    <row r="514" spans="1:3" ht="48" x14ac:dyDescent="0.2">
-      <c r="A514" s="1" t="s">
+      <c r="C531" s="8"/>
+    </row>
+    <row r="532" spans="1:3" ht="48" x14ac:dyDescent="0.2">
+      <c r="A532" s="1" t="s">
         <v>1207</v>
       </c>
-      <c r="B514" s="1" t="s">
+      <c r="B532" s="1" t="s">
         <v>1216</v>
       </c>
-      <c r="C514" s="8"/>
-    </row>
-    <row r="515" spans="1:3" ht="64" x14ac:dyDescent="0.2">
-      <c r="A515" s="1" t="s">
+      <c r="C532" s="8"/>
+    </row>
+    <row r="533" spans="1:3" ht="64" x14ac:dyDescent="0.2">
+      <c r="A533" s="1" t="s">
         <v>1208</v>
       </c>
-      <c r="B515" s="1" t="s">
+      <c r="B533" s="1" t="s">
         <v>1217</v>
       </c>
-      <c r="C515" s="8"/>
-    </row>
-    <row r="516" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A516" s="1" t="s">
+      <c r="C533" s="8"/>
+    </row>
+    <row r="534" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A534" s="1" t="s">
         <v>1209</v>
       </c>
-      <c r="B516" s="1" t="s">
+      <c r="B534" s="1" t="s">
         <v>1218</v>
       </c>
-      <c r="C516" s="8"/>
-    </row>
-    <row r="517" spans="1:3" ht="32" x14ac:dyDescent="0.2">
-      <c r="A517" s="1" t="s">
+      <c r="C534" s="8"/>
+    </row>
+    <row r="535" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+      <c r="A535" s="1" t="s">
         <v>1210</v>
       </c>
-      <c r="B517" s="1" t="s">
+      <c r="B535" s="1" t="s">
         <v>1219</v>
       </c>
-      <c r="C517" s="8"/>
-    </row>
-    <row r="518" spans="1:3" ht="48" x14ac:dyDescent="0.2">
-      <c r="A518" s="1" t="s">
+      <c r="C535" s="8"/>
+    </row>
+    <row r="536" spans="1:3" ht="48" x14ac:dyDescent="0.2">
+      <c r="A536" s="1" t="s">
         <v>1211</v>
       </c>
-      <c r="B518" s="1" t="s">
+      <c r="B536" s="1" t="s">
         <v>1220</v>
       </c>
-      <c r="C518" s="8"/>
-    </row>
-    <row r="519" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A519" s="1" t="s">
+      <c r="C536" s="8"/>
+    </row>
+    <row r="537" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A537" s="1" t="s">
         <v>1212</v>
       </c>
-      <c r="B519" s="1" t="s">
+      <c r="B537" s="1" t="s">
         <v>1221</v>
       </c>
-      <c r="C519" s="8"/>
-    </row>
-    <row r="520" spans="1:3" ht="32" x14ac:dyDescent="0.2">
-      <c r="A520" s="1" t="s">
+      <c r="C537" s="8"/>
+    </row>
+    <row r="538" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+      <c r="A538" s="1" t="s">
         <v>1213</v>
       </c>
-      <c r="B520" s="1" t="s">
+      <c r="B538" s="1" t="s">
         <v>1222</v>
       </c>
-      <c r="C520" s="8"/>
-    </row>
-    <row r="521" spans="1:3" ht="48" x14ac:dyDescent="0.2">
-      <c r="A521" s="1" t="s">
+      <c r="C538" s="8"/>
+    </row>
+    <row r="539" spans="1:3" ht="48" x14ac:dyDescent="0.2">
+      <c r="A539" s="1" t="s">
         <v>1214</v>
       </c>
-      <c r="B521" s="1" t="s">
+      <c r="B539" s="1" t="s">
         <v>1223</v>
       </c>
-      <c r="C521" s="8"/>
+      <c r="C539" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Fix retention message (en) for sales documents
</commit_message>
<xml_diff>
--- a/config/i18n/i18n.xlsx
+++ b/config/i18n/i18n.xlsx
@@ -2548,9 +2548,6 @@
   </si>
   <si>
     <t xml:space="preserve">Sobre o valor dos serviços incide retenção na fonte em sede de {0} à taxa de {1} no montante de {2}. O montante do documento a pagar será de {3}. {4} </t>
-  </si>
-  <si>
-    <t>{0} withholding rate will be applied on the billed services in the amount of {1}. The payable amount will be {2}.</t>
   </si>
   <si>
     <t>Recebemos nesta data {0} a quantia de {1} para a liquidação do documento {2} de {3}. O valor do recebido já é líquido de retenção na fonte à taxa de {4} no montante de {5}. {6}</t>
@@ -3903,6 +3900,9 @@
   <si>
     <t>Void</t>
   </si>
+  <si>
+    <t>{1} withholding rate will be applied on the billed services in the amount of {2}. The payable amount will be {3}.</t>
+  </si>
 </sst>
 </file>
 
@@ -3914,7 +3914,6 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -4367,7 +4366,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -4377,8 +4376,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G544"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A535" workbookViewId="0">
-      <selection activeCell="C543" sqref="C543"/>
+    <sheetView tabSelected="1" topLeftCell="A302" workbookViewId="0">
+      <selection activeCell="C323" sqref="C323"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -6467,7 +6466,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="256" spans="1:3" ht="32">
+    <row r="256" spans="1:3" ht="30">
       <c r="A256" s="1" t="s">
         <v>498</v>
       </c>
@@ -6483,7 +6482,7 @@
         <v>501</v>
       </c>
       <c r="B257" s="1" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
     </row>
     <row r="258" spans="1:3">
@@ -6758,7 +6757,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="283" spans="1:3">
+    <row r="283" spans="1:3" ht="30">
       <c r="A283" s="1" t="s">
         <v>595</v>
       </c>
@@ -6769,7 +6768,7 @@
         <v>597</v>
       </c>
     </row>
-    <row r="284" spans="1:3" ht="48">
+    <row r="284" spans="1:3" ht="45">
       <c r="A284" s="1" t="s">
         <v>598</v>
       </c>
@@ -6791,7 +6790,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="286" spans="1:3" ht="32">
+    <row r="286" spans="1:3" ht="30">
       <c r="A286" s="1" t="s">
         <v>604</v>
       </c>
@@ -6802,7 +6801,7 @@
         <v>606</v>
       </c>
     </row>
-    <row r="287" spans="1:3" ht="32">
+    <row r="287" spans="1:3" ht="30">
       <c r="A287" s="1" t="s">
         <v>607</v>
       </c>
@@ -7159,46 +7158,46 @@
         <v>674</v>
       </c>
       <c r="B319" s="1" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="C319" s="1" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
     </row>
     <row r="320" spans="1:3">
       <c r="A320" s="1" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
       <c r="B320" s="1" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
       <c r="C320" s="1" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
     </row>
     <row r="321" spans="1:3">
       <c r="A321" s="1" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
       <c r="B321" s="1" t="s">
+        <v>850</v>
+      </c>
+      <c r="C321" s="1" t="s">
         <v>851</v>
-      </c>
-      <c r="C321" s="1" t="s">
-        <v>852</v>
       </c>
     </row>
     <row r="322" spans="1:3">
       <c r="A322" s="1" t="s">
+        <v>854</v>
+      </c>
+      <c r="B322" s="1" t="s">
         <v>855</v>
       </c>
-      <c r="B322" s="1" t="s">
+      <c r="C322" s="1" t="s">
         <v>856</v>
       </c>
-      <c r="C322" s="1" t="s">
-        <v>857</v>
-      </c>
-    </row>
-    <row r="323" spans="1:3" ht="48">
+    </row>
+    <row r="323" spans="1:3" ht="45">
       <c r="A323" s="1" t="s">
         <v>675</v>
       </c>
@@ -7206,73 +7205,73 @@
         <v>841</v>
       </c>
       <c r="C323" s="1" t="s">
-        <v>842</v>
-      </c>
-    </row>
-    <row r="324" spans="1:3" ht="64">
+        <v>1273</v>
+      </c>
+    </row>
+    <row r="324" spans="1:3" ht="60">
       <c r="A324" s="1" t="s">
         <v>676</v>
       </c>
       <c r="B324" s="1" t="s">
+        <v>860</v>
+      </c>
+      <c r="C324" s="1" t="s">
         <v>861</v>
       </c>
-      <c r="C324" s="1" t="s">
-        <v>862</v>
-      </c>
-    </row>
-    <row r="325" spans="1:3" ht="32">
+    </row>
+    <row r="325" spans="1:3" ht="30">
       <c r="A325" s="1" t="s">
         <v>677</v>
       </c>
       <c r="B325" s="1" t="s">
+        <v>862</v>
+      </c>
+      <c r="C325" s="1" t="s">
         <v>863</v>
       </c>
-      <c r="C325" s="1" t="s">
+    </row>
+    <row r="326" spans="1:3" ht="30">
+      <c r="A326" s="1" t="s">
+        <v>846</v>
+      </c>
+      <c r="B326" s="1" t="s">
         <v>864</v>
       </c>
-    </row>
-    <row r="326" spans="1:3" ht="32">
-      <c r="A326" s="1" t="s">
-        <v>847</v>
-      </c>
-      <c r="B326" s="1" t="s">
+      <c r="C326" s="1" t="s">
         <v>865</v>
       </c>
-      <c r="C326" s="1" t="s">
-        <v>866</v>
-      </c>
-    </row>
-    <row r="327" spans="1:3" ht="64">
+    </row>
+    <row r="327" spans="1:3" ht="60">
       <c r="A327" s="1" t="s">
+        <v>857</v>
+      </c>
+      <c r="B327" s="1" t="s">
+        <v>842</v>
+      </c>
+      <c r="C327" s="1" t="s">
+        <v>843</v>
+      </c>
+    </row>
+    <row r="328" spans="1:3" ht="30">
+      <c r="A328" s="1" t="s">
         <v>858</v>
       </c>
-      <c r="B327" s="1" t="s">
-        <v>843</v>
-      </c>
-      <c r="C327" s="1" t="s">
-        <v>844</v>
-      </c>
-    </row>
-    <row r="328" spans="1:3" ht="32">
-      <c r="A328" s="1" t="s">
+      <c r="B328" s="1" t="s">
+        <v>985</v>
+      </c>
+      <c r="C328" s="1" t="s">
+        <v>986</v>
+      </c>
+    </row>
+    <row r="329" spans="1:3" ht="30">
+      <c r="A329" s="1" t="s">
         <v>859</v>
       </c>
-      <c r="B328" s="1" t="s">
-        <v>986</v>
-      </c>
-      <c r="C328" s="1" t="s">
-        <v>987</v>
-      </c>
-    </row>
-    <row r="329" spans="1:3" ht="32">
-      <c r="A329" s="1" t="s">
-        <v>860</v>
-      </c>
       <c r="B329" s="1" t="s">
+        <v>983</v>
+      </c>
+      <c r="C329" s="1" t="s">
         <v>984</v>
-      </c>
-      <c r="C329" s="1" t="s">
-        <v>985</v>
       </c>
     </row>
     <row r="330" spans="1:3">
@@ -7283,7 +7282,7 @@
         <v>679</v>
       </c>
       <c r="C330" s="1" t="s">
-        <v>1134</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="331" spans="1:3">
@@ -7316,7 +7315,7 @@
         <v>687</v>
       </c>
       <c r="C333" s="1" t="s">
-        <v>1135</v>
+        <v>1134</v>
       </c>
     </row>
     <row r="334" spans="1:3">
@@ -7327,7 +7326,7 @@
         <v>689</v>
       </c>
       <c r="C334" s="1" t="s">
-        <v>1136</v>
+        <v>1135</v>
       </c>
     </row>
     <row r="335" spans="1:3">
@@ -7338,7 +7337,7 @@
         <v>691</v>
       </c>
       <c r="C335" s="1" t="s">
-        <v>1137</v>
+        <v>1136</v>
       </c>
     </row>
     <row r="336" spans="1:3">
@@ -7349,7 +7348,7 @@
         <v>694</v>
       </c>
       <c r="C336" s="1" t="s">
-        <v>1138</v>
+        <v>1137</v>
       </c>
     </row>
     <row r="337" spans="1:3">
@@ -7360,7 +7359,7 @@
         <v>697</v>
       </c>
       <c r="C337" s="1" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
     </row>
     <row r="338" spans="1:3">
@@ -7371,7 +7370,7 @@
         <v>699</v>
       </c>
       <c r="C338" s="1" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
     </row>
     <row r="339" spans="1:3">
@@ -7415,7 +7414,7 @@
         <v>710</v>
       </c>
       <c r="C342" s="1" t="s">
-        <v>1141</v>
+        <v>1140</v>
       </c>
     </row>
     <row r="343" spans="1:3">
@@ -7426,7 +7425,7 @@
         <v>712</v>
       </c>
       <c r="C343" s="1" t="s">
-        <v>1142</v>
+        <v>1141</v>
       </c>
     </row>
     <row r="344" spans="1:3">
@@ -7437,7 +7436,7 @@
         <v>714</v>
       </c>
       <c r="C344" s="1" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
     </row>
     <row r="345" spans="1:3">
@@ -7503,7 +7502,7 @@
         <v>730</v>
       </c>
       <c r="C350" s="1" t="s">
-        <v>1133</v>
+        <v>1132</v>
       </c>
     </row>
     <row r="351" spans="1:3">
@@ -7599,7 +7598,7 @@
         <v>753</v>
       </c>
       <c r="B359" s="1" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="C359" s="1" t="s">
         <v>754</v>
@@ -7797,7 +7796,7 @@
         <v>806</v>
       </c>
       <c r="B377" s="1" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="C377" s="1" t="s">
         <v>807</v>
@@ -7937,7 +7936,7 @@
     </row>
     <row r="390" spans="1:7">
       <c r="A390" s="1" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
       <c r="B390" s="1" t="s">
         <v>658</v>
@@ -7952,24 +7951,24 @@
     </row>
     <row r="391" spans="1:7">
       <c r="A391" s="1" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
       <c r="B391" s="1" t="s">
+        <v>871</v>
+      </c>
+      <c r="C391" s="1" t="s">
         <v>872</v>
-      </c>
-      <c r="C391" s="1" t="s">
-        <v>873</v>
       </c>
     </row>
     <row r="392" spans="1:7">
       <c r="A392" s="1" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
       <c r="B392" s="1" t="s">
         <v>821</v>
       </c>
       <c r="C392" s="1" t="s">
-        <v>873</v>
+        <v>872</v>
       </c>
       <c r="D392" s="4"/>
       <c r="E392" s="4"/>
@@ -7978,88 +7977,88 @@
     </row>
     <row r="393" spans="1:7">
       <c r="A393" s="1" t="s">
-        <v>943</v>
+        <v>942</v>
       </c>
       <c r="B393" s="1" t="s">
-        <v>950</v>
+        <v>949</v>
       </c>
       <c r="C393" s="1" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="D393" s="4"/>
       <c r="E393" s="4"/>
       <c r="F393" s="4"/>
       <c r="G393" s="4"/>
     </row>
-    <row r="394" spans="1:7" ht="32">
+    <row r="394" spans="1:7" ht="30">
       <c r="A394" s="1" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
       <c r="B394" s="1" t="s">
-        <v>880</v>
+        <v>879</v>
       </c>
       <c r="C394" s="1" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
       <c r="D394" s="4"/>
       <c r="E394" s="4"/>
       <c r="F394" s="4"/>
       <c r="G394" s="4"/>
     </row>
-    <row r="395" spans="1:7" ht="48">
+    <row r="395" spans="1:7" ht="45">
       <c r="A395" s="1" t="s">
-        <v>895</v>
+        <v>894</v>
       </c>
       <c r="B395" s="1" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
       <c r="C395" s="1" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
       <c r="D395" s="4"/>
       <c r="E395" s="4"/>
       <c r="F395" s="4"/>
       <c r="G395" s="4"/>
     </row>
-    <row r="396" spans="1:7" ht="48">
+    <row r="396" spans="1:7" ht="45">
       <c r="A396" s="1" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
       <c r="B396" s="1" t="s">
+        <v>889</v>
+      </c>
+      <c r="C396" s="1" t="s">
         <v>890</v>
-      </c>
-      <c r="C396" s="1" t="s">
-        <v>891</v>
       </c>
       <c r="D396" s="4"/>
       <c r="E396" s="4"/>
       <c r="F396" s="4"/>
       <c r="G396" s="4"/>
     </row>
-    <row r="397" spans="1:7" ht="96">
+    <row r="397" spans="1:7" ht="105">
       <c r="A397" s="1" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="B397" s="1" t="s">
+        <v>929</v>
+      </c>
+      <c r="C397" s="1" t="s">
         <v>930</v>
-      </c>
-      <c r="C397" s="1" t="s">
-        <v>931</v>
       </c>
       <c r="D397" s="4"/>
       <c r="E397" s="4"/>
       <c r="F397" s="4"/>
       <c r="G397" s="4"/>
     </row>
-    <row r="398" spans="1:7" ht="48">
+    <row r="398" spans="1:7" ht="45">
       <c r="A398" s="1" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
       <c r="B398" s="1" t="s">
-        <v>875</v>
+        <v>874</v>
       </c>
       <c r="C398" s="1" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
       <c r="D398" s="4"/>
       <c r="E398" s="4"/>
@@ -8068,448 +8067,448 @@
     </row>
     <row r="399" spans="1:7">
       <c r="A399" s="1" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
       <c r="B399" s="1" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
       <c r="C399" s="1" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="D399" s="4"/>
       <c r="E399" s="4"/>
       <c r="F399" s="4"/>
       <c r="G399" s="4"/>
     </row>
-    <row r="400" spans="1:7" ht="64">
+    <row r="400" spans="1:7" ht="60">
       <c r="A400" s="1" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
       <c r="B400" s="1" t="s">
+        <v>891</v>
+      </c>
+      <c r="C400" s="1" t="s">
         <v>892</v>
-      </c>
-      <c r="C400" s="1" t="s">
-        <v>893</v>
       </c>
       <c r="D400" s="4"/>
       <c r="E400" s="4"/>
       <c r="F400" s="4"/>
       <c r="G400" s="4"/>
     </row>
-    <row r="401" spans="1:7" ht="96">
+    <row r="401" spans="1:7" ht="90">
       <c r="A401" s="1" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
       <c r="B401" s="1" t="s">
+        <v>931</v>
+      </c>
+      <c r="C401" s="1" t="s">
         <v>932</v>
-      </c>
-      <c r="C401" s="1" t="s">
-        <v>933</v>
       </c>
       <c r="D401" s="4"/>
       <c r="E401" s="4"/>
       <c r="F401" s="4"/>
       <c r="G401" s="4"/>
     </row>
-    <row r="402" spans="1:7" ht="32">
+    <row r="402" spans="1:7" ht="30">
       <c r="A402" s="1" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
       <c r="B402" s="1" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="C402" s="1" t="s">
-        <v>884</v>
+        <v>883</v>
       </c>
       <c r="D402" s="4"/>
       <c r="E402" s="4"/>
       <c r="F402" s="4"/>
       <c r="G402" s="4"/>
     </row>
-    <row r="403" spans="1:7" ht="32">
+    <row r="403" spans="1:7" ht="30">
       <c r="A403" s="1" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
       <c r="B403" s="1" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="C403" s="1" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
       <c r="D403" s="4"/>
       <c r="E403" s="4"/>
       <c r="F403" s="4"/>
       <c r="G403" s="4"/>
     </row>
-    <row r="404" spans="1:7" ht="64">
+    <row r="404" spans="1:7" ht="60">
       <c r="A404" s="1" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
       <c r="B404" s="1" t="s">
-        <v>882</v>
+        <v>881</v>
       </c>
       <c r="C404" s="1" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="D404" s="4"/>
       <c r="E404" s="4"/>
       <c r="F404" s="4"/>
       <c r="G404" s="4"/>
     </row>
-    <row r="405" spans="1:7" ht="32">
+    <row r="405" spans="1:7" ht="30">
       <c r="A405" s="1" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
       <c r="B405" s="1" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
       <c r="C405" s="1" t="s">
-        <v>959</v>
+        <v>958</v>
       </c>
       <c r="D405" s="4"/>
       <c r="E405" s="4"/>
       <c r="F405" s="4"/>
       <c r="G405" s="4"/>
     </row>
-    <row r="406" spans="1:7" ht="80">
+    <row r="406" spans="1:7" ht="75">
       <c r="A406" s="1" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="B406" s="1" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
       <c r="C406" s="1" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="D406" s="4"/>
       <c r="E406" s="4"/>
       <c r="F406" s="4"/>
       <c r="G406" s="4"/>
     </row>
-    <row r="407" spans="1:7" ht="96">
+    <row r="407" spans="1:7" ht="90">
       <c r="A407" s="1" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
       <c r="B407" s="1" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
       <c r="C407" s="1" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
       <c r="D407" s="4"/>
       <c r="E407" s="4"/>
       <c r="F407" s="4"/>
       <c r="G407" s="4"/>
     </row>
-    <row r="408" spans="1:7" ht="32">
+    <row r="408" spans="1:7" ht="30">
       <c r="A408" s="1" t="s">
-        <v>1061</v>
+        <v>1060</v>
       </c>
       <c r="B408" s="1" t="s">
-        <v>1064</v>
+        <v>1063</v>
       </c>
       <c r="C408" s="1" t="s">
-        <v>1067</v>
+        <v>1066</v>
       </c>
       <c r="D408" s="4"/>
       <c r="E408" s="4"/>
       <c r="F408" s="4"/>
       <c r="G408" s="4"/>
     </row>
-    <row r="409" spans="1:7" ht="96">
+    <row r="409" spans="1:7" ht="90">
       <c r="A409" s="1" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
       <c r="B409" s="1" t="s">
-        <v>1065</v>
+        <v>1064</v>
       </c>
       <c r="C409" s="1" t="s">
-        <v>1068</v>
+        <v>1067</v>
       </c>
       <c r="D409" s="4"/>
       <c r="E409" s="4"/>
       <c r="F409" s="4"/>
       <c r="G409" s="4"/>
     </row>
-    <row r="410" spans="1:7" ht="80">
+    <row r="410" spans="1:7" ht="75">
       <c r="A410" s="1" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
       <c r="B410" s="1" t="s">
-        <v>1066</v>
+        <v>1065</v>
       </c>
       <c r="C410" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
       <c r="D410" s="4"/>
       <c r="E410" s="4"/>
       <c r="F410" s="4"/>
       <c r="G410" s="4"/>
     </row>
-    <row r="411" spans="1:7" ht="32">
+    <row r="411" spans="1:7" ht="30">
       <c r="A411" s="1" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="B411" s="1" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
       <c r="C411" s="1" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="D411" s="4"/>
       <c r="E411" s="4"/>
       <c r="F411" s="4"/>
       <c r="G411" s="4"/>
     </row>
-    <row r="412" spans="1:7" ht="96">
+    <row r="412" spans="1:7" ht="90">
       <c r="A412" s="1" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
       <c r="B412" s="1" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
       <c r="C412" s="1" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
       <c r="D412" s="4"/>
       <c r="E412" s="4"/>
       <c r="F412" s="4"/>
       <c r="G412" s="4"/>
     </row>
-    <row r="413" spans="1:7" ht="112">
+    <row r="413" spans="1:7" ht="105">
       <c r="A413" s="1" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
       <c r="B413" s="1" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
       <c r="C413" s="1" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
       <c r="D413" s="4"/>
       <c r="E413" s="4"/>
       <c r="F413" s="4"/>
       <c r="G413" s="4"/>
     </row>
-    <row r="414" spans="1:7" ht="32">
+    <row r="414" spans="1:7" ht="30">
       <c r="A414" s="1" t="s">
-        <v>1070</v>
+        <v>1069</v>
       </c>
       <c r="B414" s="1" t="s">
-        <v>1083</v>
+        <v>1082</v>
       </c>
       <c r="C414" s="1" t="s">
-        <v>1074</v>
+        <v>1073</v>
       </c>
       <c r="D414" s="4"/>
       <c r="E414" s="4"/>
       <c r="F414" s="4"/>
       <c r="G414" s="4"/>
     </row>
-    <row r="415" spans="1:7" ht="112">
+    <row r="415" spans="1:7" ht="105">
       <c r="A415" s="1" t="s">
-        <v>1071</v>
+        <v>1070</v>
       </c>
       <c r="B415" s="1" t="s">
-        <v>1084</v>
+        <v>1083</v>
       </c>
       <c r="C415" s="1" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
       <c r="D415" s="4"/>
       <c r="E415" s="4"/>
       <c r="F415" s="4"/>
       <c r="G415" s="4"/>
     </row>
-    <row r="416" spans="1:7" ht="96">
+    <row r="416" spans="1:7" ht="90">
       <c r="A416" s="1" t="s">
+        <v>1071</v>
+      </c>
+      <c r="B416" s="1" t="s">
         <v>1072</v>
       </c>
-      <c r="B416" s="1" t="s">
-        <v>1073</v>
-      </c>
       <c r="C416" s="1" t="s">
-        <v>1076</v>
+        <v>1075</v>
       </c>
       <c r="D416" s="4"/>
       <c r="E416" s="4"/>
       <c r="F416" s="4"/>
       <c r="G416" s="4"/>
     </row>
-    <row r="417" spans="1:7" ht="32">
+    <row r="417" spans="1:7" ht="30">
       <c r="A417" s="1" t="s">
-        <v>947</v>
+        <v>946</v>
       </c>
       <c r="B417" s="1" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="C417" s="1" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="D417" s="4"/>
       <c r="E417" s="4"/>
       <c r="F417" s="4"/>
       <c r="G417" s="4"/>
     </row>
-    <row r="418" spans="1:7" ht="80">
+    <row r="418" spans="1:7" ht="75">
       <c r="A418" s="1" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="B418" s="1" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="C418" s="1" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
       <c r="D418" s="4"/>
       <c r="E418" s="4"/>
       <c r="F418" s="4"/>
       <c r="G418" s="4"/>
     </row>
-    <row r="419" spans="1:7" ht="96">
+    <row r="419" spans="1:7" ht="90">
       <c r="A419" s="1" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
       <c r="B419" s="1" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="C419" s="1" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
       <c r="D419" s="4"/>
       <c r="E419" s="4"/>
       <c r="F419" s="4"/>
       <c r="G419" s="4"/>
     </row>
-    <row r="420" spans="1:7" ht="32">
+    <row r="420" spans="1:7" ht="30">
       <c r="A420" s="1" t="s">
-        <v>1080</v>
+        <v>1079</v>
       </c>
       <c r="B420" s="1" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
       <c r="C420" s="1" t="s">
-        <v>1077</v>
+        <v>1076</v>
       </c>
       <c r="D420" s="4"/>
       <c r="E420" s="4"/>
       <c r="F420" s="4"/>
       <c r="G420" s="4"/>
     </row>
-    <row r="421" spans="1:7" ht="96">
+    <row r="421" spans="1:7" ht="90">
       <c r="A421" s="1" t="s">
-        <v>1081</v>
+        <v>1080</v>
       </c>
       <c r="B421" s="1" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
       <c r="C421" s="1" t="s">
-        <v>1078</v>
+        <v>1077</v>
       </c>
       <c r="D421" s="4"/>
       <c r="E421" s="4"/>
       <c r="F421" s="4"/>
       <c r="G421" s="4"/>
     </row>
-    <row r="422" spans="1:7" ht="96">
+    <row r="422" spans="1:7" ht="90">
       <c r="A422" s="1" t="s">
-        <v>1082</v>
+        <v>1081</v>
       </c>
       <c r="B422" s="1" t="s">
-        <v>1087</v>
+        <v>1086</v>
       </c>
       <c r="C422" s="1" t="s">
-        <v>1079</v>
+        <v>1078</v>
       </c>
       <c r="D422" s="4"/>
       <c r="E422" s="4"/>
       <c r="F422" s="4"/>
       <c r="G422" s="4"/>
     </row>
-    <row r="423" spans="1:7" ht="32">
+    <row r="423" spans="1:7" ht="30">
       <c r="A423" s="1" t="s">
-        <v>948</v>
+        <v>947</v>
       </c>
       <c r="B423" s="1" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="C423" s="1" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="D423" s="4"/>
       <c r="E423" s="4"/>
       <c r="F423" s="4"/>
       <c r="G423" s="4"/>
     </row>
-    <row r="424" spans="1:7" ht="96">
+    <row r="424" spans="1:7" ht="90">
       <c r="A424" s="1" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="B424" s="1" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
       <c r="C424" s="1" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D424" s="4"/>
       <c r="E424" s="4"/>
       <c r="F424" s="4"/>
       <c r="G424" s="4"/>
     </row>
-    <row r="425" spans="1:7" ht="128">
+    <row r="425" spans="1:7" ht="120">
       <c r="A425" s="1" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="B425" s="1" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="C425" s="1" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D425" s="4"/>
       <c r="E425" s="4"/>
       <c r="F425" s="4"/>
       <c r="G425" s="4"/>
     </row>
-    <row r="426" spans="1:7" ht="32">
+    <row r="426" spans="1:7" ht="30">
       <c r="A426" s="1" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
       <c r="B426" s="1" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
       <c r="C426" s="1" t="s">
-        <v>963</v>
+        <v>962</v>
       </c>
       <c r="D426" s="4"/>
       <c r="E426" s="4"/>
       <c r="F426" s="4"/>
       <c r="G426" s="4"/>
     </row>
-    <row r="427" spans="1:7" ht="96">
+    <row r="427" spans="1:7" ht="90">
       <c r="A427" s="1" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
       <c r="B427" s="1" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
       <c r="C427" s="1" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
       <c r="D427" s="4"/>
       <c r="E427" s="4"/>
       <c r="F427" s="4"/>
       <c r="G427" s="4"/>
     </row>
-    <row r="428" spans="1:7" ht="112">
+    <row r="428" spans="1:7" ht="105">
       <c r="A428" s="1" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
       <c r="B428" s="1" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="C428" s="1" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
       <c r="D428" s="4"/>
       <c r="E428" s="4"/>
@@ -8518,13 +8517,13 @@
     </row>
     <row r="429" spans="1:7">
       <c r="A429" s="1" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
       <c r="B429" s="1" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
       <c r="C429" s="1" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
       <c r="D429" s="4"/>
       <c r="E429" s="4"/>
@@ -8533,13 +8532,13 @@
     </row>
     <row r="430" spans="1:7">
       <c r="A430" s="1" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
       <c r="B430" s="1" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
       <c r="C430" s="1" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
       <c r="D430" s="4"/>
       <c r="E430" s="4"/>
@@ -8548,13 +8547,13 @@
     </row>
     <row r="431" spans="1:7">
       <c r="A431" s="1" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
       <c r="B431" s="1" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
       <c r="C431" s="1" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
       <c r="D431" s="4"/>
       <c r="E431" s="4"/>
@@ -8563,13 +8562,13 @@
     </row>
     <row r="432" spans="1:7">
       <c r="A432" s="6" t="s">
+        <v>971</v>
+      </c>
+      <c r="B432" s="5" t="s">
         <v>972</v>
       </c>
-      <c r="B432" s="5" t="s">
+      <c r="C432" s="5" t="s">
         <v>973</v>
-      </c>
-      <c r="C432" s="5" t="s">
-        <v>974</v>
       </c>
       <c r="D432" s="4"/>
       <c r="E432" s="4"/>
@@ -8578,46 +8577,46 @@
     </row>
     <row r="433" spans="1:7">
       <c r="A433" t="s">
+        <v>963</v>
+      </c>
+      <c r="B433" s="1" t="s">
+        <v>969</v>
+      </c>
+      <c r="C433" s="1" t="s">
         <v>964</v>
-      </c>
-      <c r="B433" s="1" t="s">
-        <v>970</v>
-      </c>
-      <c r="C433" s="1" t="s">
-        <v>965</v>
       </c>
     </row>
     <row r="434" spans="1:7">
       <c r="A434" t="s">
+        <v>965</v>
+      </c>
+      <c r="B434" s="1" t="s">
         <v>966</v>
       </c>
-      <c r="B434" s="1" t="s">
+      <c r="C434" s="1" t="s">
         <v>967</v>
-      </c>
-      <c r="C434" s="1" t="s">
-        <v>968</v>
       </c>
     </row>
     <row r="435" spans="1:7">
       <c r="A435" t="s">
-        <v>969</v>
+        <v>968</v>
       </c>
       <c r="B435" s="1" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
       <c r="C435" s="1" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
     </row>
     <row r="436" spans="1:7">
       <c r="A436" s="1" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
       <c r="B436" s="1" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
       <c r="C436" s="1" t="s">
-        <v>981</v>
+        <v>980</v>
       </c>
       <c r="D436" s="4"/>
       <c r="E436" s="4"/>
@@ -8626,13 +8625,13 @@
     </row>
     <row r="437" spans="1:7">
       <c r="A437" s="1" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
       <c r="B437" s="1" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
       <c r="C437" s="1" t="s">
-        <v>982</v>
+        <v>981</v>
       </c>
       <c r="D437" s="4"/>
       <c r="E437" s="4"/>
@@ -8641,1067 +8640,1067 @@
     </row>
     <row r="438" spans="1:7">
       <c r="A438" s="1" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
       <c r="B438" s="1" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
       <c r="C438" s="1" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
       <c r="D438" s="4"/>
       <c r="E438" s="4"/>
       <c r="F438" s="4"/>
       <c r="G438" s="4"/>
     </row>
-    <row r="439" spans="1:7" ht="32">
+    <row r="439" spans="1:7" ht="30">
       <c r="A439" s="1" t="s">
+        <v>987</v>
+      </c>
+      <c r="B439" s="1" t="s">
         <v>988</v>
       </c>
-      <c r="B439" s="1" t="s">
+      <c r="C439" s="1" t="s">
         <v>989</v>
-      </c>
-      <c r="C439" s="1" t="s">
-        <v>990</v>
       </c>
       <c r="D439" s="4"/>
       <c r="E439" s="4"/>
       <c r="F439" s="4"/>
       <c r="G439" s="4"/>
     </row>
-    <row r="440" spans="1:7" ht="160">
+    <row r="440" spans="1:7" ht="150">
       <c r="A440" s="1" t="s">
+        <v>990</v>
+      </c>
+      <c r="B440" s="1" t="s">
         <v>991</v>
       </c>
-      <c r="B440" s="1" t="s">
+      <c r="C440" s="1" t="s">
         <v>992</v>
       </c>
-      <c r="C440" s="1" t="s">
+    </row>
+    <row r="441" spans="1:7" ht="165">
+      <c r="A441" s="1" t="s">
         <v>993</v>
       </c>
-    </row>
-    <row r="441" spans="1:7" ht="176">
-      <c r="A441" s="1" t="s">
+      <c r="B441" s="1" t="s">
         <v>994</v>
       </c>
-      <c r="B441" s="1" t="s">
+      <c r="C441" s="1" t="s">
         <v>995</v>
       </c>
-      <c r="C441" s="1" t="s">
+    </row>
+    <row r="442" spans="1:7" ht="30">
+      <c r="A442" s="1" t="s">
         <v>996</v>
       </c>
-    </row>
-    <row r="442" spans="1:7" ht="32">
-      <c r="A442" s="1" t="s">
+      <c r="B442" s="1" t="s">
         <v>997</v>
       </c>
-      <c r="B442" s="1" t="s">
+      <c r="C442" s="1" t="s">
         <v>998</v>
       </c>
-      <c r="C442" s="1" t="s">
+    </row>
+    <row r="443" spans="1:7" ht="90">
+      <c r="A443" s="1" t="s">
         <v>999</v>
       </c>
-    </row>
-    <row r="443" spans="1:7" ht="96">
-      <c r="A443" s="1" t="s">
+      <c r="B443" s="1" t="s">
         <v>1000</v>
       </c>
-      <c r="B443" s="1" t="s">
+      <c r="C443" s="1" t="s">
         <v>1001</v>
       </c>
-      <c r="C443" s="1" t="s">
+    </row>
+    <row r="444" spans="1:7" ht="60">
+      <c r="A444" s="1" t="s">
         <v>1002</v>
       </c>
-    </row>
-    <row r="444" spans="1:7" ht="64">
-      <c r="A444" s="1" t="s">
+      <c r="B444" s="1" t="s">
         <v>1003</v>
       </c>
-      <c r="B444" s="1" t="s">
+      <c r="C444" s="1" t="s">
         <v>1004</v>
       </c>
-      <c r="C444" s="1" t="s">
+    </row>
+    <row r="445" spans="1:7" ht="30">
+      <c r="A445" s="1" t="s">
         <v>1005</v>
       </c>
-    </row>
-    <row r="445" spans="1:7" ht="32">
-      <c r="A445" s="1" t="s">
+      <c r="B445" s="1" t="s">
         <v>1006</v>
       </c>
-      <c r="B445" s="1" t="s">
+      <c r="C445" s="1" t="s">
         <v>1007</v>
       </c>
-      <c r="C445" s="1" t="s">
+    </row>
+    <row r="446" spans="1:7" ht="90">
+      <c r="A446" s="1" t="s">
         <v>1008</v>
       </c>
-    </row>
-    <row r="446" spans="1:7" ht="96">
-      <c r="A446" s="1" t="s">
+      <c r="B446" s="1" t="s">
         <v>1009</v>
       </c>
-      <c r="B446" s="1" t="s">
+      <c r="C446" s="1" t="s">
         <v>1010</v>
       </c>
-      <c r="C446" s="1" t="s">
+    </row>
+    <row r="447" spans="1:7" ht="120">
+      <c r="A447" s="1" t="s">
         <v>1011</v>
       </c>
-    </row>
-    <row r="447" spans="1:7" ht="128">
-      <c r="A447" s="1" t="s">
+      <c r="B447" s="1" t="s">
         <v>1012</v>
       </c>
-      <c r="B447" s="1" t="s">
+      <c r="C447" s="7" t="s">
         <v>1013</v>
-      </c>
-      <c r="C447" s="7" t="s">
-        <v>1014</v>
       </c>
     </row>
     <row r="448" spans="1:7">
       <c r="A448" s="1" t="s">
+        <v>1014</v>
+      </c>
+      <c r="B448" s="1" t="s">
         <v>1015</v>
       </c>
-      <c r="B448" s="1" t="s">
+      <c r="C448" s="1" t="s">
         <v>1016</v>
       </c>
-      <c r="C448" s="1" t="s">
+    </row>
+    <row r="449" spans="1:3" ht="60">
+      <c r="A449" s="1" t="s">
         <v>1017</v>
       </c>
-    </row>
-    <row r="449" spans="1:3" ht="64">
-      <c r="A449" s="1" t="s">
+      <c r="B449" s="1" t="s">
         <v>1018</v>
       </c>
-      <c r="B449" s="1" t="s">
+      <c r="C449" s="1" t="s">
         <v>1019</v>
       </c>
-      <c r="C449" s="1" t="s">
+    </row>
+    <row r="450" spans="1:3" ht="75">
+      <c r="A450" s="1" t="s">
         <v>1020</v>
       </c>
-    </row>
-    <row r="450" spans="1:3" ht="80">
-      <c r="A450" s="1" t="s">
+      <c r="B450" s="1" t="s">
         <v>1021</v>
       </c>
-      <c r="B450" s="1" t="s">
+      <c r="C450" s="1" t="s">
         <v>1022</v>
       </c>
-      <c r="C450" s="1" t="s">
+    </row>
+    <row r="451" spans="1:3" ht="45">
+      <c r="A451" s="1" t="s">
         <v>1023</v>
       </c>
-    </row>
-    <row r="451" spans="1:3" ht="48">
-      <c r="A451" s="1" t="s">
+      <c r="B451" s="1" t="s">
         <v>1024</v>
       </c>
-      <c r="B451" s="1" t="s">
+      <c r="C451" s="1" t="s">
         <v>1025</v>
       </c>
-      <c r="C451" s="1" t="s">
+    </row>
+    <row r="452" spans="1:3" ht="120">
+      <c r="A452" s="1" t="s">
         <v>1026</v>
       </c>
-    </row>
-    <row r="452" spans="1:3" ht="128">
-      <c r="A452" s="1" t="s">
+      <c r="B452" s="1" t="s">
         <v>1027</v>
       </c>
-      <c r="B452" s="1" t="s">
+      <c r="C452" s="1" t="s">
         <v>1028</v>
       </c>
-      <c r="C452" s="1" t="s">
+    </row>
+    <row r="453" spans="1:3" ht="135">
+      <c r="A453" s="1" t="s">
         <v>1029</v>
       </c>
-    </row>
-    <row r="453" spans="1:3" ht="144">
-      <c r="A453" s="1" t="s">
+      <c r="B453" s="1" t="s">
         <v>1030</v>
       </c>
-      <c r="B453" s="1" t="s">
+      <c r="C453" s="1" t="s">
         <v>1031</v>
       </c>
-      <c r="C453" s="1" t="s">
+    </row>
+    <row r="454" spans="1:3" ht="45">
+      <c r="A454" s="1" t="s">
         <v>1032</v>
       </c>
-    </row>
-    <row r="454" spans="1:3" ht="48">
-      <c r="A454" s="1" t="s">
+      <c r="B454" s="1" t="s">
         <v>1033</v>
       </c>
-      <c r="B454" s="1" t="s">
+      <c r="C454" s="7" t="s">
         <v>1034</v>
       </c>
-      <c r="C454" s="7" t="s">
+    </row>
+    <row r="455" spans="1:3" ht="120">
+      <c r="A455" s="1" t="s">
         <v>1035</v>
       </c>
-    </row>
-    <row r="455" spans="1:3" ht="128">
-      <c r="A455" s="1" t="s">
+      <c r="B455" s="1" t="s">
         <v>1036</v>
       </c>
-      <c r="B455" s="1" t="s">
+      <c r="C455" s="7" t="s">
         <v>1037</v>
       </c>
-      <c r="C455" s="7" t="s">
+    </row>
+    <row r="456" spans="1:3" ht="135">
+      <c r="A456" s="1" t="s">
         <v>1038</v>
       </c>
-    </row>
-    <row r="456" spans="1:3" ht="144">
-      <c r="A456" s="1" t="s">
+      <c r="B456" s="1" t="s">
         <v>1039</v>
       </c>
-      <c r="B456" s="1" t="s">
+      <c r="C456" s="7" t="s">
         <v>1040</v>
       </c>
-      <c r="C456" s="7" t="s">
+    </row>
+    <row r="457" spans="1:3" ht="45">
+      <c r="A457" s="1" t="s">
         <v>1041</v>
       </c>
-    </row>
-    <row r="457" spans="1:3" ht="48">
-      <c r="A457" s="1" t="s">
+      <c r="B457" s="1" t="s">
         <v>1042</v>
       </c>
-      <c r="B457" s="1" t="s">
+      <c r="C457" s="7" t="s">
         <v>1043</v>
       </c>
-      <c r="C457" s="7" t="s">
+    </row>
+    <row r="458" spans="1:3" ht="105">
+      <c r="A458" s="1" t="s">
         <v>1044</v>
       </c>
-    </row>
-    <row r="458" spans="1:3" ht="112">
-      <c r="A458" s="1" t="s">
+      <c r="B458" s="1" t="s">
         <v>1045</v>
       </c>
-      <c r="B458" s="1" t="s">
+      <c r="C458" s="7" t="s">
         <v>1046</v>
       </c>
-      <c r="C458" s="7" t="s">
+    </row>
+    <row r="459" spans="1:3" ht="120">
+      <c r="A459" s="1" t="s">
         <v>1047</v>
       </c>
-    </row>
-    <row r="459" spans="1:3" ht="128">
-      <c r="A459" s="1" t="s">
+      <c r="B459" s="1" t="s">
         <v>1048</v>
       </c>
-      <c r="B459" s="1" t="s">
+      <c r="C459" s="7" t="s">
         <v>1049</v>
       </c>
-      <c r="C459" s="7" t="s">
+    </row>
+    <row r="460" spans="1:3" ht="45">
+      <c r="A460" s="1" t="s">
         <v>1050</v>
       </c>
-    </row>
-    <row r="460" spans="1:3" ht="48">
-      <c r="A460" s="1" t="s">
+      <c r="B460" s="1" t="s">
         <v>1051</v>
       </c>
-      <c r="B460" s="1" t="s">
+      <c r="C460" s="7" t="s">
         <v>1052</v>
       </c>
-      <c r="C460" s="7" t="s">
+    </row>
+    <row r="461" spans="1:3" ht="120">
+      <c r="A461" s="1" t="s">
         <v>1053</v>
       </c>
-    </row>
-    <row r="461" spans="1:3" ht="128">
-      <c r="A461" s="1" t="s">
+      <c r="B461" s="1" t="s">
         <v>1054</v>
       </c>
-      <c r="B461" s="1" t="s">
+      <c r="C461" s="7" t="s">
         <v>1055</v>
       </c>
-      <c r="C461" s="7" t="s">
+    </row>
+    <row r="462" spans="1:3" ht="135">
+      <c r="A462" s="1" t="s">
         <v>1056</v>
       </c>
-    </row>
-    <row r="462" spans="1:3" ht="144">
-      <c r="A462" s="1" t="s">
+      <c r="B462" s="1" t="s">
         <v>1057</v>
       </c>
-      <c r="B462" s="1" t="s">
+      <c r="C462" s="7" t="s">
         <v>1058</v>
-      </c>
-      <c r="C462" s="7" t="s">
-        <v>1059</v>
       </c>
     </row>
     <row r="463" spans="1:3">
       <c r="A463" s="1" t="s">
-        <v>1088</v>
+        <v>1087</v>
       </c>
       <c r="B463" s="1" t="s">
+        <v>1099</v>
+      </c>
+      <c r="C463" s="8" t="s">
         <v>1100</v>
-      </c>
-      <c r="C463" s="8" t="s">
-        <v>1101</v>
       </c>
     </row>
     <row r="464" spans="1:3">
       <c r="A464" s="1" t="s">
-        <v>1089</v>
+        <v>1088</v>
       </c>
       <c r="B464" s="1" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
       <c r="C464" s="8" t="s">
-        <v>1102</v>
+        <v>1101</v>
       </c>
     </row>
     <row r="465" spans="1:3">
       <c r="A465" s="1" t="s">
-        <v>1090</v>
+        <v>1089</v>
       </c>
       <c r="B465" s="1" t="s">
-        <v>1114</v>
+        <v>1113</v>
       </c>
       <c r="C465" s="8" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
     </row>
     <row r="466" spans="1:3">
       <c r="A466" s="1" t="s">
-        <v>1091</v>
+        <v>1090</v>
       </c>
       <c r="B466" s="1" t="s">
-        <v>1115</v>
+        <v>1114</v>
       </c>
       <c r="C466" s="8" t="s">
-        <v>1104</v>
+        <v>1103</v>
       </c>
     </row>
     <row r="467" spans="1:3">
       <c r="A467" s="1" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
       <c r="B467" s="1" t="s">
-        <v>1116</v>
+        <v>1115</v>
       </c>
       <c r="C467" s="8" t="s">
-        <v>1105</v>
+        <v>1104</v>
       </c>
     </row>
     <row r="468" spans="1:3">
       <c r="A468" s="1" t="s">
-        <v>1093</v>
+        <v>1092</v>
       </c>
       <c r="B468" s="1" t="s">
-        <v>1117</v>
+        <v>1116</v>
       </c>
       <c r="C468" s="8" t="s">
-        <v>1106</v>
+        <v>1105</v>
       </c>
     </row>
     <row r="469" spans="1:3">
       <c r="A469" s="1" t="s">
-        <v>1094</v>
+        <v>1093</v>
       </c>
       <c r="B469" s="1" t="s">
-        <v>1118</v>
+        <v>1117</v>
       </c>
       <c r="C469" s="8" t="s">
-        <v>1107</v>
+        <v>1106</v>
       </c>
     </row>
     <row r="470" spans="1:3">
       <c r="A470" s="1" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
       <c r="B470" s="1" t="s">
-        <v>1119</v>
+        <v>1118</v>
       </c>
       <c r="C470" s="8" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
     </row>
     <row r="471" spans="1:3">
       <c r="A471" s="1" t="s">
-        <v>1096</v>
+        <v>1095</v>
       </c>
       <c r="B471" s="1" t="s">
-        <v>1120</v>
+        <v>1119</v>
       </c>
       <c r="C471" s="8" t="s">
-        <v>1109</v>
+        <v>1108</v>
       </c>
     </row>
     <row r="472" spans="1:3">
       <c r="A472" s="1" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
       <c r="B472" s="1" t="s">
-        <v>1121</v>
+        <v>1120</v>
       </c>
       <c r="C472" s="8" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
     </row>
     <row r="473" spans="1:3">
       <c r="A473" s="1" t="s">
-        <v>1098</v>
+        <v>1097</v>
       </c>
       <c r="B473" s="1" t="s">
-        <v>1122</v>
+        <v>1121</v>
       </c>
       <c r="C473" s="8" t="s">
-        <v>1111</v>
+        <v>1110</v>
       </c>
     </row>
     <row r="474" spans="1:3">
       <c r="A474" s="1" t="s">
-        <v>1099</v>
+        <v>1098</v>
       </c>
       <c r="B474" s="1" t="s">
-        <v>1123</v>
+        <v>1122</v>
       </c>
       <c r="C474" s="8" t="s">
-        <v>1112</v>
+        <v>1111</v>
       </c>
     </row>
     <row r="475" spans="1:3">
       <c r="A475" s="1" t="s">
+        <v>1123</v>
+      </c>
+      <c r="B475" s="1" t="s">
+        <v>1126</v>
+      </c>
+      <c r="C475" s="1" t="s">
+        <v>1127</v>
+      </c>
+    </row>
+    <row r="476" spans="1:3" ht="45">
+      <c r="A476" s="1" t="s">
         <v>1124</v>
       </c>
-      <c r="B475" s="1" t="s">
-        <v>1127</v>
-      </c>
-      <c r="C475" s="1" t="s">
+      <c r="B476" s="1" t="s">
+        <v>1130</v>
+      </c>
+      <c r="C476" s="8" t="s">
         <v>1128</v>
       </c>
     </row>
-    <row r="476" spans="1:3" ht="48">
-      <c r="A476" s="1" t="s">
+    <row r="477" spans="1:3" ht="45">
+      <c r="A477" s="1" t="s">
         <v>1125</v>
       </c>
-      <c r="B476" s="1" t="s">
+      <c r="B477" s="1" t="s">
         <v>1131</v>
       </c>
-      <c r="C476" s="8" t="s">
+      <c r="C477" s="8" t="s">
         <v>1129</v>
       </c>
     </row>
-    <row r="477" spans="1:3" ht="48">
-      <c r="A477" s="1" t="s">
-        <v>1126</v>
-      </c>
-      <c r="B477" s="1" t="s">
-        <v>1132</v>
-      </c>
-      <c r="C477" s="8" t="s">
-        <v>1130</v>
-      </c>
-    </row>
-    <row r="478" spans="1:3" ht="32">
+    <row r="478" spans="1:3" ht="30">
       <c r="A478" s="1" t="s">
+        <v>1143</v>
+      </c>
+      <c r="B478" s="1" t="s">
+        <v>1170</v>
+      </c>
+      <c r="C478" s="8"/>
+    </row>
+    <row r="479" spans="1:3" ht="60">
+      <c r="A479" s="1" t="s">
         <v>1144</v>
       </c>
-      <c r="B478" s="1" t="s">
+      <c r="B479" s="1" t="s">
+        <v>1161</v>
+      </c>
+      <c r="C479" s="8" t="s">
+        <v>1128</v>
+      </c>
+    </row>
+    <row r="480" spans="1:3" ht="90">
+      <c r="A480" s="1" t="s">
+        <v>1145</v>
+      </c>
+      <c r="B480" s="1" t="s">
         <v>1171</v>
       </c>
-      <c r="C478" s="8"/>
-    </row>
-    <row r="479" spans="1:3" ht="64">
-      <c r="A479" s="1" t="s">
-        <v>1145</v>
-      </c>
-      <c r="B479" s="1" t="s">
+      <c r="C480" s="8" t="s">
+        <v>1129</v>
+      </c>
+    </row>
+    <row r="481" spans="1:3" ht="30">
+      <c r="A481" s="1" t="s">
         <v>1162</v>
       </c>
-      <c r="C479" s="8" t="s">
-        <v>1129</v>
-      </c>
-    </row>
-    <row r="480" spans="1:3" ht="96">
-      <c r="A480" s="1" t="s">
+      <c r="B481" s="1" t="s">
+        <v>1170</v>
+      </c>
+      <c r="C481" s="8"/>
+    </row>
+    <row r="482" spans="1:3" ht="45">
+      <c r="A482" s="1" t="s">
         <v>1146</v>
       </c>
-      <c r="B480" s="1" t="s">
+      <c r="B482" s="1" t="s">
+        <v>1203</v>
+      </c>
+      <c r="C482" s="8"/>
+    </row>
+    <row r="483" spans="1:3" ht="135">
+      <c r="A483" s="1" t="s">
+        <v>1151</v>
+      </c>
+      <c r="B483" s="1" t="s">
         <v>1172</v>
       </c>
-      <c r="C480" s="8" t="s">
-        <v>1130</v>
-      </c>
-    </row>
-    <row r="481" spans="1:3" ht="32">
-      <c r="A481" s="1" t="s">
+      <c r="C483" s="8"/>
+    </row>
+    <row r="484" spans="1:3" ht="30">
+      <c r="A484" s="1" t="s">
         <v>1163</v>
       </c>
-      <c r="B481" s="1" t="s">
-        <v>1171</v>
-      </c>
-      <c r="C481" s="8"/>
-    </row>
-    <row r="482" spans="1:3" ht="48">
-      <c r="A482" s="1" t="s">
+      <c r="B484" s="1" t="s">
+        <v>1173</v>
+      </c>
+      <c r="C484" s="8"/>
+    </row>
+    <row r="485" spans="1:3" ht="60">
+      <c r="A485" s="1" t="s">
         <v>1147</v>
       </c>
-      <c r="B482" s="1" t="s">
+      <c r="B485" s="1" t="s">
         <v>1204</v>
       </c>
-      <c r="C482" s="8"/>
-    </row>
-    <row r="483" spans="1:3" ht="144">
-      <c r="A483" s="1" t="s">
+      <c r="C485" s="8"/>
+    </row>
+    <row r="486" spans="1:3" ht="90">
+      <c r="A486" s="1" t="s">
         <v>1152</v>
       </c>
-      <c r="B483" s="1" t="s">
+      <c r="B486" s="1" t="s">
+        <v>1176</v>
+      </c>
+      <c r="C486" s="8"/>
+    </row>
+    <row r="487" spans="1:3" ht="30">
+      <c r="A487" s="1" t="s">
+        <v>1164</v>
+      </c>
+      <c r="B487" s="1" t="s">
         <v>1173</v>
       </c>
-      <c r="C483" s="8"/>
-    </row>
-    <row r="484" spans="1:3" ht="32">
-      <c r="A484" s="1" t="s">
-        <v>1164</v>
-      </c>
-      <c r="B484" s="1" t="s">
+      <c r="C487" s="8"/>
+    </row>
+    <row r="488" spans="1:3" ht="30">
+      <c r="A488" s="1" t="s">
+        <v>1148</v>
+      </c>
+      <c r="B488" s="1" t="s">
+        <v>1177</v>
+      </c>
+      <c r="C488" s="8"/>
+    </row>
+    <row r="489" spans="1:3" ht="135">
+      <c r="A489" s="1" t="s">
+        <v>1153</v>
+      </c>
+      <c r="B489" s="1" t="s">
         <v>1174</v>
-      </c>
-      <c r="C484" s="8"/>
-    </row>
-    <row r="485" spans="1:3" ht="64">
-      <c r="A485" s="1" t="s">
-        <v>1148</v>
-      </c>
-      <c r="B485" s="1" t="s">
-        <v>1205</v>
-      </c>
-      <c r="C485" s="8"/>
-    </row>
-    <row r="486" spans="1:3" ht="96">
-      <c r="A486" s="1" t="s">
-        <v>1153</v>
-      </c>
-      <c r="B486" s="1" t="s">
-        <v>1177</v>
-      </c>
-      <c r="C486" s="8"/>
-    </row>
-    <row r="487" spans="1:3" ht="32">
-      <c r="A487" s="1" t="s">
-        <v>1165</v>
-      </c>
-      <c r="B487" s="1" t="s">
-        <v>1174</v>
-      </c>
-      <c r="C487" s="8"/>
-    </row>
-    <row r="488" spans="1:3" ht="32">
-      <c r="A488" s="1" t="s">
-        <v>1149</v>
-      </c>
-      <c r="B488" s="1" t="s">
-        <v>1178</v>
-      </c>
-      <c r="C488" s="8"/>
-    </row>
-    <row r="489" spans="1:3" ht="144">
-      <c r="A489" s="1" t="s">
-        <v>1154</v>
-      </c>
-      <c r="B489" s="1" t="s">
-        <v>1175</v>
       </c>
       <c r="C489" s="8"/>
     </row>
     <row r="490" spans="1:3">
       <c r="A490" s="1" t="s">
-        <v>1166</v>
+        <v>1165</v>
       </c>
       <c r="B490" s="1" t="s">
+        <v>1178</v>
+      </c>
+      <c r="C490" s="8"/>
+    </row>
+    <row r="491" spans="1:3" ht="30">
+      <c r="A491" s="1" t="s">
+        <v>1149</v>
+      </c>
+      <c r="B491" s="1" t="s">
         <v>1179</v>
       </c>
-      <c r="C490" s="8"/>
-    </row>
-    <row r="491" spans="1:3" ht="32">
-      <c r="A491" s="1" t="s">
-        <v>1150</v>
-      </c>
-      <c r="B491" s="1" t="s">
-        <v>1180</v>
-      </c>
       <c r="C491" s="8"/>
     </row>
-    <row r="492" spans="1:3" ht="96">
+    <row r="492" spans="1:3" ht="90">
       <c r="A492" s="1" t="s">
-        <v>1155</v>
+        <v>1154</v>
       </c>
       <c r="B492" s="1" t="s">
-        <v>1176</v>
+        <v>1175</v>
       </c>
       <c r="C492" s="8"/>
     </row>
     <row r="493" spans="1:3">
       <c r="A493" s="1" t="s">
-        <v>1167</v>
+        <v>1166</v>
       </c>
       <c r="B493" s="1" t="s">
-        <v>1179</v>
+        <v>1178</v>
       </c>
       <c r="C493" s="8"/>
     </row>
-    <row r="494" spans="1:3" ht="48">
+    <row r="494" spans="1:3" ht="45">
       <c r="A494" s="1" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="B494" s="1" t="s">
-        <v>1188</v>
+        <v>1187</v>
       </c>
       <c r="C494" s="8"/>
     </row>
-    <row r="495" spans="1:3" ht="64">
+    <row r="495" spans="1:3" ht="60">
       <c r="A495" s="1" t="s">
-        <v>1156</v>
+        <v>1155</v>
       </c>
       <c r="B495" s="1" t="s">
-        <v>1191</v>
+        <v>1190</v>
       </c>
       <c r="C495" s="8"/>
     </row>
     <row r="496" spans="1:3">
       <c r="A496" s="1" t="s">
-        <v>1168</v>
+        <v>1167</v>
       </c>
       <c r="B496" s="1" t="s">
+        <v>1180</v>
+      </c>
+      <c r="C496" s="8"/>
+    </row>
+    <row r="497" spans="1:3" ht="45">
+      <c r="A497" s="1" t="s">
+        <v>1156</v>
+      </c>
+      <c r="B497" s="1" t="s">
+        <v>1188</v>
+      </c>
+      <c r="C497" s="8"/>
+    </row>
+    <row r="498" spans="1:3" ht="75">
+      <c r="A498" s="1" t="s">
+        <v>1157</v>
+      </c>
+      <c r="B498" s="1" t="s">
         <v>1181</v>
-      </c>
-      <c r="C496" s="8"/>
-    </row>
-    <row r="497" spans="1:3" ht="48">
-      <c r="A497" s="1" t="s">
-        <v>1157</v>
-      </c>
-      <c r="B497" s="1" t="s">
-        <v>1189</v>
-      </c>
-      <c r="C497" s="8"/>
-    </row>
-    <row r="498" spans="1:3" ht="80">
-      <c r="A498" s="1" t="s">
-        <v>1158</v>
-      </c>
-      <c r="B498" s="1" t="s">
-        <v>1182</v>
       </c>
       <c r="C498" s="8"/>
     </row>
     <row r="499" spans="1:3">
       <c r="A499" s="1" t="s">
-        <v>1169</v>
+        <v>1168</v>
       </c>
       <c r="B499" s="1" t="s">
-        <v>1181</v>
+        <v>1180</v>
       </c>
       <c r="C499" s="8"/>
     </row>
     <row r="500" spans="1:3">
       <c r="A500" s="1" t="s">
-        <v>1159</v>
+        <v>1158</v>
       </c>
       <c r="B500" s="1" t="s">
-        <v>1190</v>
+        <v>1189</v>
       </c>
       <c r="C500" s="8"/>
     </row>
-    <row r="501" spans="1:3" ht="48">
+    <row r="501" spans="1:3" ht="45">
       <c r="A501" s="1" t="s">
+        <v>1183</v>
+      </c>
+      <c r="B501" s="1" t="s">
+        <v>1185</v>
+      </c>
+      <c r="C501" s="8"/>
+    </row>
+    <row r="502" spans="1:3" ht="75">
+      <c r="A502" s="1" t="s">
         <v>1184</v>
       </c>
-      <c r="B501" s="1" t="s">
+      <c r="B502" s="1" t="s">
         <v>1186</v>
-      </c>
-      <c r="C501" s="8"/>
-    </row>
-    <row r="502" spans="1:3" ht="80">
-      <c r="A502" s="1" t="s">
-        <v>1185</v>
-      </c>
-      <c r="B502" s="1" t="s">
-        <v>1187</v>
       </c>
       <c r="C502" s="8"/>
     </row>
     <row r="503" spans="1:3">
       <c r="A503" s="1" t="s">
-        <v>1170</v>
+        <v>1169</v>
       </c>
       <c r="B503" s="1" t="s">
-        <v>1183</v>
+        <v>1182</v>
       </c>
       <c r="C503" s="8"/>
     </row>
-    <row r="504" spans="1:3" ht="64">
+    <row r="504" spans="1:3" ht="75">
       <c r="A504" s="1" t="s">
+        <v>1159</v>
+      </c>
+      <c r="B504" s="1" t="s">
+        <v>1224</v>
+      </c>
+      <c r="C504" s="8"/>
+    </row>
+    <row r="505" spans="1:3" ht="60">
+      <c r="A505" s="1" t="s">
+        <v>1223</v>
+      </c>
+      <c r="B505" s="1" t="s">
+        <v>1225</v>
+      </c>
+      <c r="C505" s="8"/>
+    </row>
+    <row r="506" spans="1:3" ht="90">
+      <c r="A506" s="1" t="s">
         <v>1160</v>
       </c>
-      <c r="B504" s="1" t="s">
-        <v>1225</v>
-      </c>
-      <c r="C504" s="8"/>
-    </row>
-    <row r="505" spans="1:3" ht="64">
-      <c r="A505" s="1" t="s">
-        <v>1224</v>
-      </c>
-      <c r="B505" s="1" t="s">
+      <c r="B506" s="1" t="s">
         <v>1226</v>
       </c>
-      <c r="C505" s="8"/>
-    </row>
-    <row r="506" spans="1:3" ht="96">
-      <c r="A506" s="1" t="s">
-        <v>1161</v>
-      </c>
-      <c r="B506" s="1" t="s">
+      <c r="C506" s="8"/>
+    </row>
+    <row r="507" spans="1:3" ht="30">
+      <c r="A507" s="1" t="s">
         <v>1227</v>
       </c>
-      <c r="C506" s="8"/>
-    </row>
-    <row r="507" spans="1:3" ht="32">
-      <c r="A507" s="1" t="s">
+      <c r="B507" s="1" t="s">
+        <v>1239</v>
+      </c>
+      <c r="C507" s="8"/>
+    </row>
+    <row r="508" spans="1:3" ht="45">
+      <c r="A508" s="1" t="s">
         <v>1228</v>
       </c>
-      <c r="B507" s="1" t="s">
+      <c r="B508" s="1" t="s">
+        <v>1241</v>
+      </c>
+      <c r="C508" s="8"/>
+    </row>
+    <row r="509" spans="1:3" ht="60">
+      <c r="A509" s="1" t="s">
+        <v>1229</v>
+      </c>
+      <c r="B509" s="1" t="s">
+        <v>1242</v>
+      </c>
+      <c r="C509" s="8"/>
+    </row>
+    <row r="510" spans="1:3" ht="30">
+      <c r="A510" s="1" t="s">
+        <v>1230</v>
+      </c>
+      <c r="B510" s="1" t="s">
         <v>1240</v>
       </c>
-      <c r="C507" s="8"/>
-    </row>
-    <row r="508" spans="1:3" ht="48">
-      <c r="A508" s="1" t="s">
-        <v>1229</v>
-      </c>
-      <c r="B508" s="1" t="s">
-        <v>1242</v>
-      </c>
-      <c r="C508" s="8"/>
-    </row>
-    <row r="509" spans="1:3" ht="64">
-      <c r="A509" s="1" t="s">
-        <v>1230</v>
-      </c>
-      <c r="B509" s="1" t="s">
+      <c r="C510" s="8"/>
+    </row>
+    <row r="511" spans="1:3" ht="45">
+      <c r="A511" s="1" t="s">
+        <v>1231</v>
+      </c>
+      <c r="B511" s="1" t="s">
         <v>1243</v>
       </c>
-      <c r="C509" s="8"/>
-    </row>
-    <row r="510" spans="1:3" ht="32">
-      <c r="A510" s="1" t="s">
-        <v>1231</v>
-      </c>
-      <c r="B510" s="1" t="s">
-        <v>1241</v>
-      </c>
-      <c r="C510" s="8"/>
-    </row>
-    <row r="511" spans="1:3" ht="48">
-      <c r="A511" s="1" t="s">
+      <c r="C511" s="8"/>
+    </row>
+    <row r="512" spans="1:3" ht="60">
+      <c r="A512" s="1" t="s">
         <v>1232</v>
       </c>
-      <c r="B511" s="1" t="s">
+      <c r="B512" s="1" t="s">
         <v>1244</v>
       </c>
-      <c r="C511" s="8"/>
-    </row>
-    <row r="512" spans="1:3" ht="64">
-      <c r="A512" s="1" t="s">
+      <c r="C512" s="8"/>
+    </row>
+    <row r="513" spans="1:3" ht="30">
+      <c r="A513" s="1" t="s">
         <v>1233</v>
       </c>
-      <c r="B512" s="1" t="s">
+      <c r="B513" s="1" t="s">
         <v>1245</v>
       </c>
-      <c r="C512" s="8"/>
-    </row>
-    <row r="513" spans="1:3" ht="32">
-      <c r="A513" s="1" t="s">
+      <c r="C513" s="8"/>
+    </row>
+    <row r="514" spans="1:3" ht="30">
+      <c r="A514" s="1" t="s">
         <v>1234</v>
       </c>
-      <c r="B513" s="1" t="s">
+      <c r="B514" s="1" t="s">
         <v>1246</v>
       </c>
-      <c r="C513" s="8"/>
-    </row>
-    <row r="514" spans="1:3" ht="32">
-      <c r="A514" s="1" t="s">
+      <c r="C514" s="8"/>
+    </row>
+    <row r="515" spans="1:3" ht="75">
+      <c r="A515" s="1" t="s">
         <v>1235</v>
       </c>
-      <c r="B514" s="1" t="s">
+      <c r="B515" s="1" t="s">
         <v>1247</v>
       </c>
-      <c r="C514" s="8"/>
-    </row>
-    <row r="515" spans="1:3" ht="80">
-      <c r="A515" s="1" t="s">
+      <c r="C515" s="8"/>
+    </row>
+    <row r="516" spans="1:3" ht="30">
+      <c r="A516" s="1" t="s">
+        <v>1253</v>
+      </c>
+      <c r="B516" s="1" t="s">
+        <v>1248</v>
+      </c>
+      <c r="C516" s="8"/>
+    </row>
+    <row r="517" spans="1:3" ht="90">
+      <c r="A517" s="1" t="s">
+        <v>1255</v>
+      </c>
+      <c r="B517" s="1" t="s">
+        <v>1259</v>
+      </c>
+      <c r="C517" s="8"/>
+    </row>
+    <row r="518" spans="1:3" ht="105">
+      <c r="A518" s="1" t="s">
+        <v>1256</v>
+      </c>
+      <c r="B518" s="1" t="s">
+        <v>1261</v>
+      </c>
+      <c r="C518" s="8"/>
+    </row>
+    <row r="519" spans="1:3" ht="30">
+      <c r="A519" s="1" t="s">
+        <v>1254</v>
+      </c>
+      <c r="B519" s="1" t="s">
+        <v>1248</v>
+      </c>
+      <c r="C519" s="8"/>
+    </row>
+    <row r="520" spans="1:3" ht="105">
+      <c r="A520" s="1" t="s">
+        <v>1257</v>
+      </c>
+      <c r="B520" s="1" t="s">
+        <v>1260</v>
+      </c>
+      <c r="C520" s="8"/>
+    </row>
+    <row r="521" spans="1:3" ht="105">
+      <c r="A521" s="1" t="s">
+        <v>1258</v>
+      </c>
+      <c r="B521" s="1" t="s">
+        <v>1249</v>
+      </c>
+      <c r="C521" s="8"/>
+    </row>
+    <row r="522" spans="1:3" ht="30">
+      <c r="A522" s="1" t="s">
         <v>1236</v>
       </c>
-      <c r="B515" s="1" t="s">
-        <v>1248</v>
-      </c>
-      <c r="C515" s="8"/>
-    </row>
-    <row r="516" spans="1:3" ht="32">
-      <c r="A516" s="1" t="s">
-        <v>1254</v>
-      </c>
-      <c r="B516" s="1" t="s">
-        <v>1249</v>
-      </c>
-      <c r="C516" s="8"/>
-    </row>
-    <row r="517" spans="1:3" ht="96">
-      <c r="A517" s="1" t="s">
-        <v>1256</v>
-      </c>
-      <c r="B517" s="1" t="s">
-        <v>1260</v>
-      </c>
-      <c r="C517" s="8"/>
-    </row>
-    <row r="518" spans="1:3" ht="112">
-      <c r="A518" s="1" t="s">
-        <v>1257</v>
-      </c>
-      <c r="B518" s="1" t="s">
-        <v>1262</v>
-      </c>
-      <c r="C518" s="8"/>
-    </row>
-    <row r="519" spans="1:3" ht="32">
-      <c r="A519" s="1" t="s">
-        <v>1255</v>
-      </c>
-      <c r="B519" s="1" t="s">
-        <v>1249</v>
-      </c>
-      <c r="C519" s="8"/>
-    </row>
-    <row r="520" spans="1:3" ht="112">
-      <c r="A520" s="1" t="s">
-        <v>1258</v>
-      </c>
-      <c r="B520" s="1" t="s">
-        <v>1261</v>
-      </c>
-      <c r="C520" s="8"/>
-    </row>
-    <row r="521" spans="1:3" ht="112">
-      <c r="A521" s="1" t="s">
-        <v>1259</v>
-      </c>
-      <c r="B521" s="1" t="s">
+      <c r="B522" s="1" t="s">
         <v>1250</v>
       </c>
-      <c r="C521" s="8"/>
-    </row>
-    <row r="522" spans="1:3" ht="32">
-      <c r="A522" s="1" t="s">
+      <c r="C522" s="8"/>
+    </row>
+    <row r="523" spans="1:3" ht="90">
+      <c r="A523" s="1" t="s">
         <v>1237</v>
       </c>
-      <c r="B522" s="1" t="s">
+      <c r="B523" s="1" t="s">
         <v>1251</v>
       </c>
-      <c r="C522" s="8"/>
-    </row>
-    <row r="523" spans="1:3" ht="96">
-      <c r="A523" s="1" t="s">
+      <c r="C523" s="8"/>
+    </row>
+    <row r="524" spans="1:3" ht="75">
+      <c r="A524" s="1" t="s">
         <v>1238</v>
       </c>
-      <c r="B523" s="1" t="s">
+      <c r="B524" s="1" t="s">
         <v>1252</v>
-      </c>
-      <c r="C523" s="8"/>
-    </row>
-    <row r="524" spans="1:3" ht="80">
-      <c r="A524" s="1" t="s">
-        <v>1239</v>
-      </c>
-      <c r="B524" s="1" t="s">
-        <v>1253</v>
       </c>
       <c r="C524" s="8"/>
     </row>
     <row r="525" spans="1:3">
       <c r="A525" s="1" t="s">
+        <v>1192</v>
+      </c>
+      <c r="B525" s="1" t="s">
+        <v>1191</v>
+      </c>
+      <c r="C525" s="8"/>
+    </row>
+    <row r="526" spans="1:3" ht="60">
+      <c r="A526" s="1" t="s">
         <v>1193</v>
       </c>
-      <c r="B525" s="1" t="s">
-        <v>1192</v>
-      </c>
-      <c r="C525" s="8"/>
-    </row>
-    <row r="526" spans="1:3" ht="64">
-      <c r="A526" s="1" t="s">
+      <c r="B526" s="1" t="s">
+        <v>1198</v>
+      </c>
+      <c r="C526" s="8"/>
+    </row>
+    <row r="527" spans="1:3" ht="90">
+      <c r="A527" s="1" t="s">
         <v>1194</v>
       </c>
-      <c r="B526" s="1" t="s">
+      <c r="B527" s="1" t="s">
         <v>1199</v>
-      </c>
-      <c r="C526" s="8"/>
-    </row>
-    <row r="527" spans="1:3" ht="96">
-      <c r="A527" s="1" t="s">
-        <v>1195</v>
-      </c>
-      <c r="B527" s="1" t="s">
-        <v>1200</v>
       </c>
       <c r="C527" s="8"/>
     </row>
     <row r="528" spans="1:3">
       <c r="A528" s="1" t="s">
+        <v>1195</v>
+      </c>
+      <c r="B528" s="1" t="s">
+        <v>1200</v>
+      </c>
+      <c r="C528" s="8"/>
+    </row>
+    <row r="529" spans="1:7" ht="60">
+      <c r="A529" s="1" t="s">
         <v>1196</v>
       </c>
-      <c r="B528" s="1" t="s">
+      <c r="B529" s="1" t="s">
         <v>1201</v>
       </c>
-      <c r="C528" s="8"/>
-    </row>
-    <row r="529" spans="1:7" ht="64">
-      <c r="A529" s="1" t="s">
+      <c r="C529" s="8"/>
+    </row>
+    <row r="530" spans="1:7" ht="90">
+      <c r="A530" s="1" t="s">
         <v>1197</v>
       </c>
-      <c r="B529" s="1" t="s">
+      <c r="B530" s="1" t="s">
         <v>1202</v>
-      </c>
-      <c r="C529" s="8"/>
-    </row>
-    <row r="530" spans="1:7" ht="96">
-      <c r="A530" s="1" t="s">
-        <v>1198</v>
-      </c>
-      <c r="B530" s="1" t="s">
-        <v>1203</v>
       </c>
       <c r="C530" s="8"/>
     </row>
     <row r="531" spans="1:7">
       <c r="A531" s="1" t="s">
+        <v>1205</v>
+      </c>
+      <c r="B531" s="1" t="s">
+        <v>1214</v>
+      </c>
+      <c r="C531" s="8"/>
+    </row>
+    <row r="532" spans="1:7" ht="45">
+      <c r="A532" s="1" t="s">
         <v>1206</v>
       </c>
-      <c r="B531" s="1" t="s">
+      <c r="B532" s="1" t="s">
         <v>1215</v>
       </c>
-      <c r="C531" s="8"/>
-    </row>
-    <row r="532" spans="1:7" ht="48">
-      <c r="A532" s="1" t="s">
+      <c r="C532" s="8"/>
+    </row>
+    <row r="533" spans="1:7" ht="60">
+      <c r="A533" s="1" t="s">
         <v>1207</v>
       </c>
-      <c r="B532" s="1" t="s">
+      <c r="B533" s="1" t="s">
         <v>1216</v>
-      </c>
-      <c r="C532" s="8"/>
-    </row>
-    <row r="533" spans="1:7" ht="64">
-      <c r="A533" s="1" t="s">
-        <v>1208</v>
-      </c>
-      <c r="B533" s="1" t="s">
-        <v>1217</v>
       </c>
       <c r="C533" s="8"/>
     </row>
     <row r="534" spans="1:7">
       <c r="A534" s="1" t="s">
+        <v>1208</v>
+      </c>
+      <c r="B534" s="1" t="s">
+        <v>1217</v>
+      </c>
+      <c r="C534" s="8"/>
+    </row>
+    <row r="535" spans="1:7" ht="30">
+      <c r="A535" s="1" t="s">
         <v>1209</v>
       </c>
-      <c r="B534" s="1" t="s">
+      <c r="B535" s="1" t="s">
         <v>1218</v>
       </c>
-      <c r="C534" s="8"/>
-    </row>
-    <row r="535" spans="1:7" ht="32">
-      <c r="A535" s="1" t="s">
+      <c r="C535" s="8"/>
+    </row>
+    <row r="536" spans="1:7" ht="45">
+      <c r="A536" s="1" t="s">
         <v>1210</v>
       </c>
-      <c r="B535" s="1" t="s">
+      <c r="B536" s="1" t="s">
         <v>1219</v>
-      </c>
-      <c r="C535" s="8"/>
-    </row>
-    <row r="536" spans="1:7" ht="48">
-      <c r="A536" s="1" t="s">
-        <v>1211</v>
-      </c>
-      <c r="B536" s="1" t="s">
-        <v>1220</v>
       </c>
       <c r="C536" s="8"/>
     </row>
     <row r="537" spans="1:7">
       <c r="A537" s="1" t="s">
+        <v>1211</v>
+      </c>
+      <c r="B537" s="1" t="s">
+        <v>1220</v>
+      </c>
+      <c r="C537" s="8"/>
+    </row>
+    <row r="538" spans="1:7" ht="30">
+      <c r="A538" s="1" t="s">
         <v>1212</v>
       </c>
-      <c r="B537" s="1" t="s">
+      <c r="B538" s="1" t="s">
         <v>1221</v>
       </c>
-      <c r="C537" s="8"/>
-    </row>
-    <row r="538" spans="1:7" ht="32">
-      <c r="A538" s="1" t="s">
+      <c r="C538" s="8"/>
+    </row>
+    <row r="539" spans="1:7" ht="45">
+      <c r="A539" s="1" t="s">
         <v>1213</v>
       </c>
-      <c r="B538" s="1" t="s">
+      <c r="B539" s="1" t="s">
         <v>1222</v>
-      </c>
-      <c r="C538" s="8"/>
-    </row>
-    <row r="539" spans="1:7" ht="48">
-      <c r="A539" s="1" t="s">
-        <v>1214</v>
-      </c>
-      <c r="B539" s="1" t="s">
-        <v>1223</v>
       </c>
       <c r="C539" s="8"/>
     </row>
     <row r="540" spans="1:7">
       <c r="A540" t="s">
-        <v>1263</v>
+        <v>1262</v>
       </c>
       <c r="B540" s="1" t="s">
-        <v>1268</v>
+        <v>1267</v>
       </c>
       <c r="C540" s="1" t="s">
-        <v>968</v>
+        <v>967</v>
       </c>
     </row>
     <row r="541" spans="1:7">
       <c r="A541" t="s">
-        <v>1264</v>
+        <v>1263</v>
       </c>
       <c r="B541" s="1" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
       <c r="C541" s="1" t="s">
-        <v>965</v>
+        <v>964</v>
       </c>
     </row>
     <row r="542" spans="1:7">
       <c r="A542" t="s">
-        <v>1265</v>
+        <v>1264</v>
       </c>
       <c r="B542" s="1" t="s">
-        <v>1269</v>
+        <v>1268</v>
       </c>
       <c r="C542" s="1" t="s">
-        <v>1271</v>
+        <v>1270</v>
       </c>
     </row>
     <row r="543" spans="1:7">
       <c r="A543" t="s">
-        <v>1266</v>
+        <v>1265</v>
       </c>
       <c r="B543" s="1" t="s">
-        <v>1270</v>
+        <v>1269</v>
       </c>
       <c r="C543" s="1" t="s">
-        <v>1272</v>
+        <v>1271</v>
       </c>
     </row>
     <row r="544" spans="1:7">
       <c r="A544" t="s">
-        <v>1267</v>
+        <v>1266</v>
       </c>
       <c r="B544" s="4" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
       <c r="C544" s="4" t="s">
-        <v>1273</v>
+        <v>1272</v>
       </c>
       <c r="D544" s="4"/>
       <c r="E544" s="4"/>

</xml_diff>

<commit_message>
WTF? Fixing 6969 certificate number
</commit_message>
<xml_diff>
--- a/config/i18n/i18n.xlsx
+++ b/config/i18n/i18n.xlsx
@@ -3925,9 +3925,6 @@
     <t>1662</t>
   </si>
   <si>
-    <t>6969</t>
-  </si>
-  <si>
     <t>document_certified_notice_business_business</t>
   </si>
   <si>
@@ -3967,34 +3964,37 @@
     <t>Issued by certified program nr. 1662/AT - TOConline</t>
   </si>
   <si>
-    <t>Processado por programa certificado nº 6969/AT - Cloudware.business</t>
-  </si>
-  <si>
-    <t>Processed by certified program nr. 6969/AT - Cloudware.business</t>
-  </si>
-  <si>
-    <t>Emitido por programa certificado nº 6969/AT - Cloudware.business</t>
-  </si>
-  <si>
-    <t>Issued by certified program nr. 6969/AT - Cloudware.business</t>
-  </si>
-  <si>
-    <t>Processado por programa certificado nº 6969/AT - M Fatura (Powered by Cloudware.business)</t>
-  </si>
-  <si>
-    <t>Processed by certified program nr. 6969/AT - M Fatura (Powered by Cloudware.business)</t>
-  </si>
-  <si>
-    <t>Emitido por programa certificado nº 6969/AT - M Fatura (Powered by Cloudware.business)</t>
-  </si>
-  <si>
-    <t>Issued by certified program nr. 6969/AT - M Fatura (Powered by Cloudware.business)</t>
-  </si>
-  <si>
     <t>document_certified_number_toconline</t>
   </si>
   <si>
     <t>document_certified_number_business</t>
+  </si>
+  <si>
+    <t>2397</t>
+  </si>
+  <si>
+    <t>Processado por programa certificado nº 2397/AT - Cloudware.business</t>
+  </si>
+  <si>
+    <t>Emitido por programa certificado nº 2397/AT - Cloudware.business</t>
+  </si>
+  <si>
+    <t>Processado por programa certificado nº 2397/AT - M Fatura (Powered by Cloudware.business)</t>
+  </si>
+  <si>
+    <t>Emitido por programa certificado nº 2397/AT - M Fatura (Powered by Cloudware.business)</t>
+  </si>
+  <si>
+    <t>Issued by certified program nr. 2397/AT - M Fatura (Powered by Cloudware.business)</t>
+  </si>
+  <si>
+    <t>Processed by certified program nr. 2397/AT - M Fatura (Powered by Cloudware.business)</t>
+  </si>
+  <si>
+    <t>Issued by certified program nr. 2397/AT - Cloudware.business</t>
+  </si>
+  <si>
+    <t>Processed by certified program nr. 2397/AT - Cloudware.business</t>
   </si>
 </sst>
 </file>
@@ -4584,7 +4584,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -4594,8 +4594,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G561"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A543" workbookViewId="0">
-      <selection activeCell="I548" sqref="I548"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -9504,7 +9504,7 @@
         <v>1214</v>
       </c>
       <c r="B500" s="1" t="s">
-        <v>1290</v>
+        <v>1289</v>
       </c>
       <c r="C500" s="8"/>
     </row>
@@ -9933,10 +9933,10 @@
         <v>1277</v>
       </c>
       <c r="B545" s="7" t="s">
-        <v>1291</v>
+        <v>1290</v>
       </c>
       <c r="C545" s="7" t="s">
-        <v>1293</v>
+        <v>1292</v>
       </c>
       <c r="D545" s="7"/>
       <c r="E545" s="7"/>
@@ -9948,10 +9948,10 @@
         <v>1278</v>
       </c>
       <c r="B546" s="14" t="s">
-        <v>1292</v>
+        <v>1291</v>
       </c>
       <c r="C546" s="14" t="s">
-        <v>1294</v>
+        <v>1293</v>
       </c>
       <c r="D546" s="14"/>
       <c r="E546" s="14"/>
@@ -9975,7 +9975,7 @@
     </row>
     <row r="548" spans="1:7">
       <c r="A548" t="s">
-        <v>1303</v>
+        <v>1294</v>
       </c>
       <c r="B548" s="16" t="s">
         <v>1280</v>
@@ -9986,24 +9986,24 @@
     </row>
     <row r="549" spans="1:7">
       <c r="A549" t="s">
-        <v>1304</v>
+        <v>1295</v>
       </c>
       <c r="B549" s="16" t="s">
-        <v>1281</v>
+        <v>1296</v>
       </c>
       <c r="C549" s="16" t="s">
-        <v>1281</v>
+        <v>1296</v>
       </c>
     </row>
     <row r="550" spans="1:7" ht="30">
       <c r="A550" s="11" t="s">
-        <v>1282</v>
+        <v>1281</v>
       </c>
       <c r="B550" s="7" t="s">
-        <v>1295</v>
+        <v>1297</v>
       </c>
       <c r="C550" s="7" t="s">
-        <v>1296</v>
+        <v>1304</v>
       </c>
       <c r="D550" s="4"/>
       <c r="E550" s="4"/>
@@ -10012,57 +10012,57 @@
     </row>
     <row r="551" spans="1:7" ht="30">
       <c r="A551" s="13" t="s">
-        <v>1283</v>
+        <v>1282</v>
       </c>
       <c r="B551" s="14" t="s">
-        <v>1297</v>
+        <v>1298</v>
       </c>
       <c r="C551" s="14" t="s">
-        <v>1298</v>
+        <v>1303</v>
       </c>
     </row>
     <row r="552" spans="1:7" ht="30">
       <c r="A552" s="11" t="s">
-        <v>1284</v>
+        <v>1283</v>
       </c>
       <c r="B552" s="1" t="s">
         <v>1272</v>
       </c>
       <c r="C552" s="1" t="s">
-        <v>1285</v>
+        <v>1284</v>
       </c>
     </row>
     <row r="553" spans="1:7" ht="30">
       <c r="A553" s="11" t="s">
-        <v>1286</v>
+        <v>1285</v>
       </c>
       <c r="B553" s="7" t="s">
         <v>1299</v>
       </c>
       <c r="C553" s="7" t="s">
-        <v>1300</v>
+        <v>1302</v>
       </c>
     </row>
     <row r="554" spans="1:7" ht="30">
       <c r="A554" s="13" t="s">
-        <v>1287</v>
+        <v>1286</v>
       </c>
       <c r="B554" s="14" t="s">
+        <v>1300</v>
+      </c>
+      <c r="C554" s="14" t="s">
         <v>1301</v>
-      </c>
-      <c r="C554" s="14" t="s">
-        <v>1302</v>
       </c>
     </row>
     <row r="555" spans="1:7" ht="45">
       <c r="A555" s="11" t="s">
-        <v>1288</v>
+        <v>1287</v>
       </c>
       <c r="B555" s="1" t="s">
         <v>1274</v>
       </c>
       <c r="C555" s="1" t="s">
-        <v>1289</v>
+        <v>1288</v>
       </c>
     </row>
     <row r="561" spans="1:7">

</xml_diff>

<commit_message>
Add non-branded certified notices to the i18n resources (to allow for use both inside and outside "platform")
</commit_message>
<xml_diff>
--- a/config/i18n/i18n.xlsx
+++ b/config/i18n/i18n.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1362" uniqueCount="1305">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1375" uniqueCount="1310">
   <si>
     <t>key</t>
   </si>
@@ -3996,6 +3996,21 @@
   <si>
     <t>Processed by certified program nr. 2397/AT - Cloudware.business</t>
   </si>
+  <si>
+    <t>certified_software_notice</t>
+  </si>
+  <si>
+    <t>document_certified_number</t>
+  </si>
+  <si>
+    <t>document_certified_notice</t>
+  </si>
+  <si>
+    <t>document_certified_notice_non_hashed</t>
+  </si>
+  <si>
+    <t>document_certified_notice_short</t>
+  </si>
 </sst>
 </file>
 
@@ -4007,7 +4022,6 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -4314,8 +4328,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="i18n" displayName="i18n" ref="A1:G555" totalsRowShown="0" headerRowDxfId="6">
-  <autoFilter ref="A1:G555"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="i18n" displayName="i18n" ref="A1:G560" totalsRowShown="0" headerRowDxfId="6">
+  <autoFilter ref="A1:G560"/>
   <tableColumns count="7">
     <tableColumn id="1" name="key"/>
     <tableColumn id="2" name="pt" dataDxfId="5"/>
@@ -4584,7 +4598,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -4594,8 +4608,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G561"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A547" workbookViewId="0">
+      <selection activeCell="A559" sqref="A559"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -10063,6 +10077,58 @@
       </c>
       <c r="C555" s="1" t="s">
         <v>1288</v>
+      </c>
+    </row>
+    <row r="556" spans="1:7">
+      <c r="A556" s="1" t="s">
+        <v>1305</v>
+      </c>
+      <c r="B556" s="1" t="s">
+        <v>522</v>
+      </c>
+      <c r="C556" s="1" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="557" spans="1:7">
+      <c r="A557" s="1" t="s">
+        <v>1306</v>
+      </c>
+      <c r="B557" s="1">
+        <v>1662</v>
+      </c>
+    </row>
+    <row r="558" spans="1:7" ht="30">
+      <c r="A558" s="1" t="s">
+        <v>1307</v>
+      </c>
+      <c r="B558" s="1" t="s">
+        <v>1290</v>
+      </c>
+      <c r="C558" s="1" t="s">
+        <v>1292</v>
+      </c>
+    </row>
+    <row r="559" spans="1:7" ht="30">
+      <c r="A559" s="1" t="s">
+        <v>1308</v>
+      </c>
+      <c r="B559" s="1" t="s">
+        <v>1291</v>
+      </c>
+      <c r="C559" s="1" t="s">
+        <v>1293</v>
+      </c>
+    </row>
+    <row r="560" spans="1:7">
+      <c r="A560" s="1" t="s">
+        <v>1309</v>
+      </c>
+      <c r="B560" s="1" t="s">
+        <v>522</v>
+      </c>
+      <c r="C560" s="1" t="s">
+        <v>602</v>
       </c>
     </row>
     <row r="561" spans="1:7">

</xml_diff>

<commit_message>
Set business url as app.cloudware.pt.
</commit_message>
<xml_diff>
--- a/config/i18n/i18n.xlsx
+++ b/config/i18n/i18n.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11208"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/josepacheco/cldware_work/sp-duh/config/i18n/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91189D1A-90F1-0247-B3DA-42B9093C71D9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{857BC1A7-8FDA-2947-9540-DC15192D0DEB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3892,21 +3892,9 @@
     <t>certified_software_notice_business_business</t>
   </si>
   <si>
-    <t>Emitido por Cloudware.business - https://cloudware.pt/cloudwarebiz/</t>
-  </si>
-  <si>
     <t>certified_software_notice_business_mbcp</t>
   </si>
   <si>
-    <t>Emitido por M Fatura (Powered by Cloudware.business - https://cloudware.pt/cloudwarebiz/)</t>
-  </si>
-  <si>
-    <t>Created by M Fatura (Powered by Cloudware.business - https://cloudware.pt/cloudwarebiz/)</t>
-  </si>
-  <si>
-    <t>Created by Cloudware.business - https://cloudware.pt/cloudwarebiz/</t>
-  </si>
-  <si>
     <t>document_certified_notice_toconline_toconline</t>
   </si>
   <si>
@@ -3928,9 +3916,6 @@
     <t>document_certified_notice_short_business_business</t>
   </si>
   <si>
-    <t>Processed by Cloudware.business - https://cloudware.pt/cloudwarebiz/</t>
-  </si>
-  <si>
     <t>document_certified_notice_business_mbcp</t>
   </si>
   <si>
@@ -3940,9 +3925,6 @@
     <t>document_certified_notice_short_business_mbcp</t>
   </si>
   <si>
-    <t>Processed by M Fatura (Powered by Cloudware.business - https://cloudware.pt/cloudwarebiz/)</t>
-  </si>
-  <si>
     <t>Os saldos de abertura devem ser coincidentes com os saldos finais do exercício anterior. Não nos foi possível efetuar este teste uma vez que não existe exercício do ano {0}.</t>
   </si>
   <si>
@@ -4016,6 +3998,24 @@
   </si>
   <si>
     <t>Recebemos até esta data {4} {0}  a quantia de {1} ({2}) para a liquidação do documento {3}. {5}</t>
+  </si>
+  <si>
+    <t>Emitido por Cloudware.business - https://app.cloudware.pt</t>
+  </si>
+  <si>
+    <t>Created by Cloudware.business - https://app.cloudware.pt</t>
+  </si>
+  <si>
+    <t>Emitido por M Fatura (Powered by Cloudware.business - https://app.cloudware.pt)</t>
+  </si>
+  <si>
+    <t>Created by M Fatura (Powered by Cloudware.business - https://app.cloudware.pt)</t>
+  </si>
+  <si>
+    <t>Processed by Cloudware.business - https://app.cloudware.pt</t>
+  </si>
+  <si>
+    <t>Processed by M Fatura (Powered by Cloudware.business - https://app.cloudware.pt)</t>
   </si>
 </sst>
 </file>
@@ -4335,7 +4335,6 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="i18n" displayName="i18n" ref="A1:G560" totalsRowShown="0" headerRowDxfId="6">
-  <autoFilter ref="A1:G560" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="key"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="pt" dataDxfId="5"/>
@@ -4614,8 +4613,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G561"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A311" workbookViewId="0">
-      <selection activeCell="B324" sqref="B324"/>
+    <sheetView tabSelected="1" topLeftCell="A545" workbookViewId="0">
+      <selection activeCell="C555" sqref="C555"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7432,10 +7431,10 @@
         <v>846</v>
       </c>
       <c r="B322" s="1" t="s">
-        <v>1307</v>
+        <v>1301</v>
       </c>
       <c r="C322" s="1" t="s">
-        <v>1306</v>
+        <v>1300</v>
       </c>
     </row>
     <row r="323" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -7443,10 +7442,10 @@
         <v>847</v>
       </c>
       <c r="B323" s="1" t="s">
-        <v>1309</v>
+        <v>1303</v>
       </c>
       <c r="C323" s="1" t="s">
-        <v>1308</v>
+        <v>1302</v>
       </c>
     </row>
     <row r="324" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -9524,7 +9523,7 @@
         <v>1210</v>
       </c>
       <c r="B500" s="1" t="s">
-        <v>1285</v>
+        <v>1279</v>
       </c>
       <c r="C500" s="8"/>
     </row>
@@ -9931,32 +9930,32 @@
         <v>1267</v>
       </c>
       <c r="B543" s="1" t="s">
-        <v>1268</v>
+        <v>1304</v>
       </c>
       <c r="C543" s="1" t="s">
-        <v>1272</v>
+        <v>1305</v>
       </c>
     </row>
     <row r="544" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A544" s="1" t="s">
-        <v>1269</v>
+        <v>1268</v>
       </c>
       <c r="B544" s="1" t="s">
-        <v>1270</v>
+        <v>1306</v>
       </c>
       <c r="C544" s="1" t="s">
-        <v>1271</v>
+        <v>1307</v>
       </c>
     </row>
     <row r="545" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A545" s="11" t="s">
-        <v>1273</v>
+        <v>1269</v>
       </c>
       <c r="B545" s="7" t="s">
-        <v>1286</v>
+        <v>1280</v>
       </c>
       <c r="C545" s="7" t="s">
-        <v>1288</v>
+        <v>1282</v>
       </c>
       <c r="D545" s="7"/>
       <c r="E545" s="7"/>
@@ -9965,13 +9964,13 @@
     </row>
     <row r="546" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A546" s="13" t="s">
-        <v>1274</v>
+        <v>1270</v>
       </c>
       <c r="B546" s="14" t="s">
-        <v>1287</v>
+        <v>1281</v>
       </c>
       <c r="C546" s="14" t="s">
-        <v>1289</v>
+        <v>1283</v>
       </c>
       <c r="D546" s="14"/>
       <c r="E546" s="14"/>
@@ -9980,7 +9979,7 @@
     </row>
     <row r="547" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A547" s="11" t="s">
-        <v>1275</v>
+        <v>1271</v>
       </c>
       <c r="B547" s="7" t="s">
         <v>522</v>
@@ -9995,35 +9994,35 @@
     </row>
     <row r="548" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A548" t="s">
-        <v>1290</v>
+        <v>1284</v>
       </c>
       <c r="B548" s="16" t="s">
-        <v>1276</v>
+        <v>1272</v>
       </c>
       <c r="C548" s="16" t="s">
-        <v>1276</v>
+        <v>1272</v>
       </c>
     </row>
     <row r="549" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A549" t="s">
-        <v>1291</v>
+        <v>1285</v>
       </c>
       <c r="B549" s="16" t="s">
-        <v>1292</v>
+        <v>1286</v>
       </c>
       <c r="C549" s="16" t="s">
-        <v>1292</v>
+        <v>1286</v>
       </c>
     </row>
     <row r="550" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A550" s="11" t="s">
-        <v>1277</v>
+        <v>1273</v>
       </c>
       <c r="B550" s="7" t="s">
-        <v>1293</v>
+        <v>1287</v>
       </c>
       <c r="C550" s="7" t="s">
-        <v>1300</v>
+        <v>1294</v>
       </c>
       <c r="D550" s="4"/>
       <c r="E550" s="4"/>
@@ -10032,62 +10031,62 @@
     </row>
     <row r="551" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A551" s="13" t="s">
-        <v>1278</v>
+        <v>1274</v>
       </c>
       <c r="B551" s="14" t="s">
-        <v>1294</v>
+        <v>1288</v>
       </c>
       <c r="C551" s="14" t="s">
-        <v>1299</v>
+        <v>1293</v>
       </c>
     </row>
     <row r="552" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A552" s="11" t="s">
-        <v>1279</v>
+        <v>1275</v>
       </c>
       <c r="B552" s="1" t="s">
-        <v>1268</v>
+        <v>1304</v>
       </c>
       <c r="C552" s="1" t="s">
-        <v>1280</v>
+        <v>1308</v>
       </c>
     </row>
     <row r="553" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A553" s="11" t="s">
-        <v>1281</v>
+        <v>1276</v>
       </c>
       <c r="B553" s="7" t="s">
-        <v>1295</v>
+        <v>1289</v>
       </c>
       <c r="C553" s="7" t="s">
-        <v>1298</v>
+        <v>1292</v>
       </c>
     </row>
     <row r="554" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A554" s="13" t="s">
-        <v>1282</v>
+        <v>1277</v>
       </c>
       <c r="B554" s="14" t="s">
-        <v>1296</v>
+        <v>1290</v>
       </c>
       <c r="C554" s="14" t="s">
-        <v>1297</v>
+        <v>1291</v>
       </c>
     </row>
     <row r="555" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A555" s="11" t="s">
-        <v>1283</v>
+        <v>1278</v>
       </c>
       <c r="B555" s="1" t="s">
-        <v>1270</v>
+        <v>1306</v>
       </c>
       <c r="C555" s="1" t="s">
-        <v>1284</v>
+        <v>1309</v>
       </c>
     </row>
     <row r="556" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A556" s="1" t="s">
-        <v>1301</v>
+        <v>1295</v>
       </c>
       <c r="B556" s="1" t="s">
         <v>522</v>
@@ -10098,7 +10097,7 @@
     </row>
     <row r="557" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A557" s="1" t="s">
-        <v>1302</v>
+        <v>1296</v>
       </c>
       <c r="B557" s="1">
         <v>1662</v>
@@ -10106,29 +10105,29 @@
     </row>
     <row r="558" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A558" s="1" t="s">
-        <v>1303</v>
+        <v>1297</v>
       </c>
       <c r="B558" s="1" t="s">
-        <v>1286</v>
+        <v>1280</v>
       </c>
       <c r="C558" s="1" t="s">
-        <v>1288</v>
+        <v>1282</v>
       </c>
     </row>
     <row r="559" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A559" s="1" t="s">
-        <v>1304</v>
+        <v>1298</v>
       </c>
       <c r="B559" s="1" t="s">
-        <v>1287</v>
+        <v>1281</v>
       </c>
       <c r="C559" s="1" t="s">
-        <v>1289</v>
+        <v>1283</v>
       </c>
     </row>
     <row r="560" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A560" s="1" t="s">
-        <v>1305</v>
+        <v>1299</v>
       </c>
       <c r="B560" s="1" t="s">
         <v>522</v>

</xml_diff>

<commit_message>
Added svat_t41* and svat_t42*
</commit_message>
<xml_diff>
--- a/config/i18n/i18n.xlsx
+++ b/config/i18n/i18n.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11208"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10113"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/josepacheco/cldware_work/sp-duh/config/i18n/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joana/work/sp-duh/config/i18n/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{857BC1A7-8FDA-2947-9540-DC15192D0DEB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41CACF5C-9E02-0E40-97CE-4E48B462BAF8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1375" uniqueCount="1310">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1387" uniqueCount="1322">
   <si>
     <t>key</t>
   </si>
@@ -4016,6 +4016,42 @@
   </si>
   <si>
     <t>Processed by M Fatura (Powered by Cloudware.business - https://app.cloudware.pt)</t>
+  </si>
+  <si>
+    <t>Teste à contabilização de documentos emitidos em faturação</t>
+  </si>
+  <si>
+    <t>Teste à contabilização de outros documentos comerciais</t>
+  </si>
+  <si>
+    <t>Verificamos que todos os documentos emitidos em faturação têm movimento finalizado. Sem exceções.</t>
+  </si>
+  <si>
+    <t>Verificamos que faltam movimentos para documentos emitidos em faturação:</t>
+  </si>
+  <si>
+    <t>Verificamos que todos os documentos dos módulos de Vendas e Compras têm movimento finalizado. Sem exceções.</t>
+  </si>
+  <si>
+    <t>Verificamos que faltam movimentos para documentos comerciais:</t>
+  </si>
+  <si>
+    <t>svat_t41</t>
+  </si>
+  <si>
+    <t>svat_t41_ok</t>
+  </si>
+  <si>
+    <t>svat_t41_nok</t>
+  </si>
+  <si>
+    <t>svat_t42</t>
+  </si>
+  <si>
+    <t>svat_t42_ok</t>
+  </si>
+  <si>
+    <t>svat_t42_nok</t>
   </si>
 </sst>
 </file>
@@ -4334,7 +4370,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="i18n" displayName="i18n" ref="A1:G560" totalsRowShown="0" headerRowDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="i18n" displayName="i18n" ref="A1:G566" totalsRowShown="0" headerRowDxfId="6">
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="key"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="pt" dataDxfId="5"/>
@@ -4611,10 +4647,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G561"/>
+  <dimension ref="A1:G567"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A545" workbookViewId="0">
-      <selection activeCell="C555" sqref="C555"/>
+    <sheetView tabSelected="1" topLeftCell="A524" workbookViewId="0">
+      <selection activeCell="A541" sqref="A541"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9779,7 +9815,7 @@
       </c>
       <c r="C528" s="8"/>
     </row>
-    <row r="529" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="529" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A529" s="1" t="s">
         <v>1195</v>
       </c>
@@ -9788,7 +9824,7 @@
       </c>
       <c r="C529" s="8"/>
     </row>
-    <row r="530" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+    <row r="530" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A530" s="1" t="s">
         <v>1196</v>
       </c>
@@ -9797,7 +9833,7 @@
       </c>
       <c r="C530" s="8"/>
     </row>
-    <row r="531" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+    <row r="531" spans="1:3" ht="51" x14ac:dyDescent="0.2">
       <c r="A531" s="1" t="s">
         <v>1197</v>
       </c>
@@ -9806,7 +9842,7 @@
       </c>
       <c r="C531" s="8"/>
     </row>
-    <row r="532" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="532" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A532" s="1" t="s">
         <v>1198</v>
       </c>
@@ -9815,7 +9851,7 @@
       </c>
       <c r="C532" s="8"/>
     </row>
-    <row r="533" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+    <row r="533" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A533" s="1" t="s">
         <v>1199</v>
       </c>
@@ -9824,7 +9860,7 @@
       </c>
       <c r="C533" s="8"/>
     </row>
-    <row r="534" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+    <row r="534" spans="1:3" ht="51" x14ac:dyDescent="0.2">
       <c r="A534" s="1" t="s">
         <v>1200</v>
       </c>
@@ -9833,317 +9869,371 @@
       </c>
       <c r="C534" s="8"/>
     </row>
-    <row r="535" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="535" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A535" s="1" t="s">
+        <v>1316</v>
+      </c>
+      <c r="B535" s="1" t="s">
+        <v>1310</v>
+      </c>
+      <c r="C535" s="8"/>
+    </row>
+    <row r="536" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+      <c r="A536" s="1" t="s">
+        <v>1317</v>
+      </c>
+      <c r="B536" s="1" t="s">
+        <v>1312</v>
+      </c>
+      <c r="C536" s="8"/>
+    </row>
+    <row r="537" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A537" s="1" t="s">
+        <v>1318</v>
+      </c>
+      <c r="B537" s="1" t="s">
+        <v>1313</v>
+      </c>
+      <c r="C537" s="8"/>
+    </row>
+    <row r="538" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A538" s="1" t="s">
+        <v>1319</v>
+      </c>
+      <c r="B538" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="C538" s="8"/>
+    </row>
+    <row r="539" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+      <c r="A539" s="1" t="s">
+        <v>1320</v>
+      </c>
+      <c r="B539" s="1" t="s">
+        <v>1314</v>
+      </c>
+      <c r="C539" s="8"/>
+    </row>
+    <row r="540" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A540" s="1" t="s">
+        <v>1321</v>
+      </c>
+      <c r="B540" s="1" t="s">
+        <v>1315</v>
+      </c>
+      <c r="C540" s="8"/>
+    </row>
+    <row r="541" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A541" s="1" t="s">
         <v>1260</v>
       </c>
-      <c r="B535" s="1" t="s">
+      <c r="B541" s="1" t="s">
         <v>1261</v>
       </c>
-      <c r="C535" s="9" t="s">
+      <c r="C541" s="9" t="s">
         <v>1262</v>
       </c>
     </row>
-    <row r="536" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A536" s="1" t="s">
+    <row r="542" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A542" s="1" t="s">
         <v>1263</v>
       </c>
-      <c r="B536" s="1" t="s">
+      <c r="B542" s="1" t="s">
         <v>1264</v>
       </c>
-      <c r="C536" s="9" t="s">
+      <c r="C542" s="9" t="s">
         <v>1265</v>
       </c>
     </row>
-    <row r="537" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A537" t="s">
+    <row r="543" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A543" t="s">
         <v>1248</v>
       </c>
-      <c r="B537" s="1" t="s">
+      <c r="B543" s="1" t="s">
         <v>1253</v>
       </c>
-      <c r="C537" s="1" t="s">
+      <c r="C543" s="1" t="s">
         <v>956</v>
       </c>
     </row>
-    <row r="538" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A538" t="s">
+    <row r="544" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A544" t="s">
         <v>1249</v>
       </c>
-      <c r="B538" s="1" t="s">
+      <c r="B544" s="1" t="s">
         <v>958</v>
       </c>
-      <c r="C538" s="1" t="s">
+      <c r="C544" s="1" t="s">
         <v>953</v>
       </c>
     </row>
-    <row r="539" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A539" t="s">
+    <row r="545" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A545" t="s">
         <v>1250</v>
       </c>
-      <c r="B539" s="1" t="s">
+      <c r="B545" s="1" t="s">
         <v>1254</v>
       </c>
-      <c r="C539" s="1" t="s">
+      <c r="C545" s="1" t="s">
         <v>1256</v>
       </c>
     </row>
-    <row r="540" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A540" t="s">
+    <row r="546" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A546" t="s">
         <v>1251</v>
       </c>
-      <c r="B540" s="1" t="s">
+      <c r="B546" s="1" t="s">
         <v>1255</v>
       </c>
-      <c r="C540" s="1" t="s">
+      <c r="C546" s="1" t="s">
         <v>1257</v>
       </c>
     </row>
-    <row r="541" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A541" t="s">
+    <row r="547" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A547" t="s">
         <v>1252</v>
       </c>
-      <c r="B541" s="4" t="s">
+      <c r="B547" s="4" t="s">
         <v>1046</v>
       </c>
-      <c r="C541" s="4" t="s">
+      <c r="C547" s="4" t="s">
         <v>1258</v>
       </c>
-      <c r="D541" s="4"/>
-      <c r="E541" s="4"/>
-      <c r="F541" s="4"/>
-      <c r="G541" s="4"/>
-    </row>
-    <row r="542" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A542" s="1" t="s">
+      <c r="D547" s="4"/>
+      <c r="E547" s="4"/>
+      <c r="F547" s="4"/>
+      <c r="G547" s="4"/>
+    </row>
+    <row r="548" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A548" s="1" t="s">
         <v>1266</v>
       </c>
-      <c r="B542" s="1" t="s">
+      <c r="B548" s="1" t="s">
         <v>522</v>
       </c>
-      <c r="C542" s="1" t="s">
+      <c r="C548" s="1" t="s">
         <v>523</v>
       </c>
     </row>
-    <row r="543" spans="1:7" ht="34" x14ac:dyDescent="0.2">
-      <c r="A543" s="1" t="s">
+    <row r="549" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="A549" s="1" t="s">
         <v>1267</v>
       </c>
-      <c r="B543" s="1" t="s">
+      <c r="B549" s="1" t="s">
         <v>1304</v>
       </c>
-      <c r="C543" s="1" t="s">
+      <c r="C549" s="1" t="s">
         <v>1305</v>
       </c>
     </row>
-    <row r="544" spans="1:7" ht="51" x14ac:dyDescent="0.2">
-      <c r="A544" s="1" t="s">
+    <row r="550" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+      <c r="A550" s="1" t="s">
         <v>1268</v>
       </c>
-      <c r="B544" s="1" t="s">
+      <c r="B550" s="1" t="s">
         <v>1306</v>
       </c>
-      <c r="C544" s="1" t="s">
+      <c r="C550" s="1" t="s">
         <v>1307</v>
       </c>
     </row>
-    <row r="545" spans="1:7" ht="34" x14ac:dyDescent="0.2">
-      <c r="A545" s="11" t="s">
+    <row r="551" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="A551" s="11" t="s">
         <v>1269</v>
       </c>
-      <c r="B545" s="7" t="s">
+      <c r="B551" s="7" t="s">
         <v>1280</v>
       </c>
-      <c r="C545" s="7" t="s">
+      <c r="C551" s="7" t="s">
         <v>1282</v>
       </c>
-      <c r="D545" s="7"/>
-      <c r="E545" s="7"/>
-      <c r="F545" s="7"/>
-      <c r="G545" s="12"/>
-    </row>
-    <row r="546" spans="1:7" ht="34" x14ac:dyDescent="0.2">
-      <c r="A546" s="13" t="s">
+      <c r="D551" s="7"/>
+      <c r="E551" s="7"/>
+      <c r="F551" s="7"/>
+      <c r="G551" s="12"/>
+    </row>
+    <row r="552" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="A552" s="13" t="s">
         <v>1270</v>
       </c>
-      <c r="B546" s="14" t="s">
+      <c r="B552" s="14" t="s">
         <v>1281</v>
       </c>
-      <c r="C546" s="14" t="s">
+      <c r="C552" s="14" t="s">
         <v>1283</v>
       </c>
-      <c r="D546" s="14"/>
-      <c r="E546" s="14"/>
-      <c r="F546" s="14"/>
-      <c r="G546" s="15"/>
-    </row>
-    <row r="547" spans="1:7" ht="34" x14ac:dyDescent="0.2">
-      <c r="A547" s="11" t="s">
-        <v>1271</v>
-      </c>
-      <c r="B547" s="7" t="s">
-        <v>522</v>
-      </c>
-      <c r="C547" s="7" t="s">
-        <v>602</v>
-      </c>
-      <c r="D547" s="7"/>
-      <c r="E547" s="7"/>
-      <c r="F547" s="7"/>
-      <c r="G547" s="12"/>
-    </row>
-    <row r="548" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A548" t="s">
-        <v>1284</v>
-      </c>
-      <c r="B548" s="16" t="s">
-        <v>1272</v>
-      </c>
-      <c r="C548" s="16" t="s">
-        <v>1272</v>
-      </c>
-    </row>
-    <row r="549" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A549" t="s">
-        <v>1285</v>
-      </c>
-      <c r="B549" s="16" t="s">
-        <v>1286</v>
-      </c>
-      <c r="C549" s="16" t="s">
-        <v>1286</v>
-      </c>
-    </row>
-    <row r="550" spans="1:7" ht="34" x14ac:dyDescent="0.2">
-      <c r="A550" s="11" t="s">
-        <v>1273</v>
-      </c>
-      <c r="B550" s="7" t="s">
-        <v>1287</v>
-      </c>
-      <c r="C550" s="7" t="s">
-        <v>1294</v>
-      </c>
-      <c r="D550" s="4"/>
-      <c r="E550" s="4"/>
-      <c r="F550" s="4"/>
-      <c r="G550" s="4"/>
-    </row>
-    <row r="551" spans="1:7" ht="34" x14ac:dyDescent="0.2">
-      <c r="A551" s="13" t="s">
-        <v>1274</v>
-      </c>
-      <c r="B551" s="14" t="s">
-        <v>1288</v>
-      </c>
-      <c r="C551" s="14" t="s">
-        <v>1293</v>
-      </c>
-    </row>
-    <row r="552" spans="1:7" ht="34" x14ac:dyDescent="0.2">
-      <c r="A552" s="11" t="s">
-        <v>1275</v>
-      </c>
-      <c r="B552" s="1" t="s">
-        <v>1304</v>
-      </c>
-      <c r="C552" s="1" t="s">
-        <v>1308</v>
-      </c>
+      <c r="D552" s="14"/>
+      <c r="E552" s="14"/>
+      <c r="F552" s="14"/>
+      <c r="G552" s="15"/>
     </row>
     <row r="553" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A553" s="11" t="s">
+        <v>1271</v>
+      </c>
+      <c r="B553" s="7" t="s">
+        <v>522</v>
+      </c>
+      <c r="C553" s="7" t="s">
+        <v>602</v>
+      </c>
+      <c r="D553" s="7"/>
+      <c r="E553" s="7"/>
+      <c r="F553" s="7"/>
+      <c r="G553" s="12"/>
+    </row>
+    <row r="554" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A554" t="s">
+        <v>1284</v>
+      </c>
+      <c r="B554" s="16" t="s">
+        <v>1272</v>
+      </c>
+      <c r="C554" s="16" t="s">
+        <v>1272</v>
+      </c>
+    </row>
+    <row r="555" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A555" t="s">
+        <v>1285</v>
+      </c>
+      <c r="B555" s="16" t="s">
+        <v>1286</v>
+      </c>
+      <c r="C555" s="16" t="s">
+        <v>1286</v>
+      </c>
+    </row>
+    <row r="556" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="A556" s="11" t="s">
+        <v>1273</v>
+      </c>
+      <c r="B556" s="7" t="s">
+        <v>1287</v>
+      </c>
+      <c r="C556" s="7" t="s">
+        <v>1294</v>
+      </c>
+      <c r="D556" s="4"/>
+      <c r="E556" s="4"/>
+      <c r="F556" s="4"/>
+      <c r="G556" s="4"/>
+    </row>
+    <row r="557" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="A557" s="13" t="s">
+        <v>1274</v>
+      </c>
+      <c r="B557" s="14" t="s">
+        <v>1288</v>
+      </c>
+      <c r="C557" s="14" t="s">
+        <v>1293</v>
+      </c>
+    </row>
+    <row r="558" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="A558" s="11" t="s">
+        <v>1275</v>
+      </c>
+      <c r="B558" s="1" t="s">
+        <v>1304</v>
+      </c>
+      <c r="C558" s="1" t="s">
+        <v>1308</v>
+      </c>
+    </row>
+    <row r="559" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="A559" s="11" t="s">
         <v>1276</v>
       </c>
-      <c r="B553" s="7" t="s">
+      <c r="B559" s="7" t="s">
         <v>1289</v>
       </c>
-      <c r="C553" s="7" t="s">
+      <c r="C559" s="7" t="s">
         <v>1292</v>
       </c>
     </row>
-    <row r="554" spans="1:7" ht="34" x14ac:dyDescent="0.2">
-      <c r="A554" s="13" t="s">
+    <row r="560" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="A560" s="13" t="s">
         <v>1277</v>
       </c>
-      <c r="B554" s="14" t="s">
+      <c r="B560" s="14" t="s">
         <v>1290</v>
       </c>
-      <c r="C554" s="14" t="s">
+      <c r="C560" s="14" t="s">
         <v>1291</v>
       </c>
     </row>
-    <row r="555" spans="1:7" ht="51" x14ac:dyDescent="0.2">
-      <c r="A555" s="11" t="s">
+    <row r="561" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+      <c r="A561" s="11" t="s">
         <v>1278</v>
       </c>
-      <c r="B555" s="1" t="s">
+      <c r="B561" s="1" t="s">
         <v>1306</v>
       </c>
-      <c r="C555" s="1" t="s">
+      <c r="C561" s="1" t="s">
         <v>1309</v>
       </c>
     </row>
-    <row r="556" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A556" s="1" t="s">
+    <row r="562" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A562" s="1" t="s">
         <v>1295</v>
       </c>
-      <c r="B556" s="1" t="s">
+      <c r="B562" s="1" t="s">
         <v>522</v>
       </c>
-      <c r="C556" s="1" t="s">
+      <c r="C562" s="1" t="s">
         <v>523</v>
       </c>
     </row>
-    <row r="557" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A557" s="1" t="s">
+    <row r="563" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A563" s="1" t="s">
         <v>1296</v>
       </c>
-      <c r="B557" s="1">
+      <c r="B563" s="1">
         <v>1662</v>
       </c>
     </row>
-    <row r="558" spans="1:7" ht="34" x14ac:dyDescent="0.2">
-      <c r="A558" s="1" t="s">
+    <row r="564" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="A564" s="1" t="s">
         <v>1297</v>
       </c>
-      <c r="B558" s="1" t="s">
+      <c r="B564" s="1" t="s">
         <v>1280</v>
       </c>
-      <c r="C558" s="1" t="s">
+      <c r="C564" s="1" t="s">
         <v>1282</v>
       </c>
     </row>
-    <row r="559" spans="1:7" ht="34" x14ac:dyDescent="0.2">
-      <c r="A559" s="1" t="s">
+    <row r="565" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="A565" s="1" t="s">
         <v>1298</v>
       </c>
-      <c r="B559" s="1" t="s">
+      <c r="B565" s="1" t="s">
         <v>1281</v>
       </c>
-      <c r="C559" s="1" t="s">
+      <c r="C565" s="1" t="s">
         <v>1283</v>
       </c>
     </row>
-    <row r="560" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A560" s="1" t="s">
+    <row r="566" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A566" s="1" t="s">
         <v>1299</v>
       </c>
-      <c r="B560" s="1" t="s">
+      <c r="B566" s="1" t="s">
         <v>522</v>
       </c>
-      <c r="C560" s="1" t="s">
+      <c r="C566" s="1" t="s">
         <v>602</v>
       </c>
     </row>
-    <row r="561" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A561" s="10"/>
-      <c r="B561" s="4"/>
-      <c r="C561" s="4"/>
-      <c r="D561" s="4"/>
-      <c r="E561" s="4"/>
-      <c r="F561" s="4"/>
-      <c r="G561" s="4"/>
+    <row r="567" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A567" s="10"/>
+      <c r="B567" s="4"/>
+      <c r="C567" s="4"/>
+      <c r="D567" s="4"/>
+      <c r="E567" s="4"/>
+      <c r="F567" s="4"/>
+      <c r="G567" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Adding keys for 'suggestion' transaction status
</commit_message>
<xml_diff>
--- a/config/i18n/i18n.xlsx
+++ b/config/i18n/i18n.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10209"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joana/work/sp-duh/config/i18n/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41CACF5C-9E02-0E40-97CE-4E48B462BAF8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{936C0947-39B2-C14F-81BB-178572CA6D9C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1387" uniqueCount="1322">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1390" uniqueCount="1325">
   <si>
     <t>key</t>
   </si>
@@ -4052,6 +4052,15 @@
   </si>
   <si>
     <t>svat_t42_nok</t>
+  </si>
+  <si>
+    <t>Sugestão</t>
+  </si>
+  <si>
+    <t>transaction_suggestion</t>
+  </si>
+  <si>
+    <t>Suggestion</t>
   </si>
 </sst>
 </file>
@@ -4370,7 +4379,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="i18n" displayName="i18n" ref="A1:G566" totalsRowShown="0" headerRowDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="i18n" displayName="i18n" ref="A1:G567" totalsRowShown="0" headerRowDxfId="6">
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="key"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="pt" dataDxfId="5"/>
@@ -4647,10 +4656,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G567"/>
+  <dimension ref="A1:G568"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A524" workbookViewId="0">
-      <selection activeCell="A541" sqref="A541"/>
+    <sheetView tabSelected="1" topLeftCell="A421" workbookViewId="0">
+      <selection activeCell="C429" sqref="C429"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8809,50 +8818,46 @@
     </row>
     <row r="429" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A429" t="s">
-        <v>954</v>
+        <v>1323</v>
       </c>
       <c r="B429" s="1" t="s">
-        <v>955</v>
+        <v>1322</v>
       </c>
       <c r="C429" s="1" t="s">
-        <v>956</v>
+        <v>1324</v>
       </c>
     </row>
     <row r="430" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A430" t="s">
+        <v>954</v>
+      </c>
+      <c r="B430" s="1" t="s">
+        <v>955</v>
+      </c>
+      <c r="C430" s="1" t="s">
+        <v>956</v>
+      </c>
+    </row>
+    <row r="431" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A431" t="s">
         <v>957</v>
       </c>
-      <c r="B430" s="1" t="s">
+      <c r="B431" s="1" t="s">
         <v>1046</v>
       </c>
-      <c r="C430" s="1" t="s">
+      <c r="C431" s="1" t="s">
         <v>959</v>
       </c>
-    </row>
-    <row r="431" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A431" s="1" t="s">
-        <v>963</v>
-      </c>
-      <c r="B431" s="1" t="s">
-        <v>966</v>
-      </c>
-      <c r="C431" s="1" t="s">
-        <v>969</v>
-      </c>
-      <c r="D431" s="4"/>
-      <c r="E431" s="4"/>
-      <c r="F431" s="4"/>
-      <c r="G431" s="4"/>
     </row>
     <row r="432" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A432" s="1" t="s">
-        <v>964</v>
+        <v>963</v>
       </c>
       <c r="B432" s="1" t="s">
-        <v>967</v>
+        <v>966</v>
       </c>
       <c r="C432" s="1" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
       <c r="D432" s="4"/>
       <c r="E432" s="4"/>
@@ -8861,1379 +8866,1394 @@
     </row>
     <row r="433" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A433" s="1" t="s">
-        <v>965</v>
+        <v>964</v>
       </c>
       <c r="B433" s="1" t="s">
-        <v>968</v>
+        <v>967</v>
       </c>
       <c r="C433" s="1" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
       <c r="D433" s="4"/>
       <c r="E433" s="4"/>
       <c r="F433" s="4"/>
       <c r="G433" s="4"/>
     </row>
-    <row r="434" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+    <row r="434" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A434" s="1" t="s">
-        <v>974</v>
+        <v>965</v>
       </c>
       <c r="B434" s="1" t="s">
-        <v>975</v>
+        <v>968</v>
       </c>
       <c r="C434" s="1" t="s">
-        <v>976</v>
+        <v>971</v>
       </c>
       <c r="D434" s="4"/>
       <c r="E434" s="4"/>
       <c r="F434" s="4"/>
       <c r="G434" s="4"/>
     </row>
-    <row r="435" spans="1:7" ht="170" x14ac:dyDescent="0.2">
+    <row r="435" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A435" s="1" t="s">
+        <v>974</v>
+      </c>
+      <c r="B435" s="1" t="s">
+        <v>975</v>
+      </c>
+      <c r="C435" s="1" t="s">
+        <v>976</v>
+      </c>
+      <c r="D435" s="4"/>
+      <c r="E435" s="4"/>
+      <c r="F435" s="4"/>
+      <c r="G435" s="4"/>
+    </row>
+    <row r="436" spans="1:7" ht="170" x14ac:dyDescent="0.2">
+      <c r="A436" s="1" t="s">
         <v>977</v>
       </c>
-      <c r="B435" s="1" t="s">
+      <c r="B436" s="1" t="s">
         <v>978</v>
       </c>
-      <c r="C435" s="1" t="s">
+      <c r="C436" s="1" t="s">
         <v>979</v>
       </c>
     </row>
-    <row r="436" spans="1:7" ht="187" x14ac:dyDescent="0.2">
-      <c r="A436" s="1" t="s">
+    <row r="437" spans="1:7" ht="187" x14ac:dyDescent="0.2">
+      <c r="A437" s="1" t="s">
         <v>980</v>
       </c>
-      <c r="B436" s="1" t="s">
+      <c r="B437" s="1" t="s">
         <v>981</v>
       </c>
-      <c r="C436" s="1" t="s">
+      <c r="C437" s="1" t="s">
         <v>982</v>
       </c>
     </row>
-    <row r="437" spans="1:7" ht="34" x14ac:dyDescent="0.2">
-      <c r="A437" s="1" t="s">
+    <row r="438" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="A438" s="1" t="s">
         <v>983</v>
       </c>
-      <c r="B437" s="1" t="s">
+      <c r="B438" s="1" t="s">
         <v>984</v>
       </c>
-      <c r="C437" s="1" t="s">
+      <c r="C438" s="1" t="s">
         <v>985</v>
       </c>
     </row>
-    <row r="438" spans="1:7" ht="102" x14ac:dyDescent="0.2">
-      <c r="A438" s="1" t="s">
+    <row r="439" spans="1:7" ht="102" x14ac:dyDescent="0.2">
+      <c r="A439" s="1" t="s">
         <v>986</v>
       </c>
-      <c r="B438" s="1" t="s">
+      <c r="B439" s="1" t="s">
         <v>987</v>
       </c>
-      <c r="C438" s="1" t="s">
+      <c r="C439" s="1" t="s">
         <v>988</v>
       </c>
     </row>
-    <row r="439" spans="1:7" ht="68" x14ac:dyDescent="0.2">
-      <c r="A439" s="1" t="s">
+    <row r="440" spans="1:7" ht="68" x14ac:dyDescent="0.2">
+      <c r="A440" s="1" t="s">
         <v>989</v>
       </c>
-      <c r="B439" s="1" t="s">
+      <c r="B440" s="1" t="s">
         <v>990</v>
       </c>
-      <c r="C439" s="1" t="s">
+      <c r="C440" s="1" t="s">
         <v>991</v>
       </c>
     </row>
-    <row r="440" spans="1:7" ht="34" x14ac:dyDescent="0.2">
-      <c r="A440" s="1" t="s">
+    <row r="441" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="A441" s="1" t="s">
         <v>992</v>
       </c>
-      <c r="B440" s="1" t="s">
+      <c r="B441" s="1" t="s">
         <v>993</v>
       </c>
-      <c r="C440" s="1" t="s">
+      <c r="C441" s="1" t="s">
         <v>994</v>
       </c>
     </row>
-    <row r="441" spans="1:7" ht="119" x14ac:dyDescent="0.2">
-      <c r="A441" s="1" t="s">
+    <row r="442" spans="1:7" ht="119" x14ac:dyDescent="0.2">
+      <c r="A442" s="1" t="s">
         <v>995</v>
       </c>
-      <c r="B441" s="1" t="s">
+      <c r="B442" s="1" t="s">
         <v>996</v>
       </c>
-      <c r="C441" s="1" t="s">
+      <c r="C442" s="1" t="s">
         <v>997</v>
       </c>
     </row>
-    <row r="442" spans="1:7" ht="153" x14ac:dyDescent="0.2">
-      <c r="A442" s="1" t="s">
+    <row r="443" spans="1:7" ht="153" x14ac:dyDescent="0.2">
+      <c r="A443" s="1" t="s">
         <v>998</v>
       </c>
-      <c r="B442" s="1" t="s">
+      <c r="B443" s="1" t="s">
         <v>999</v>
       </c>
-      <c r="C442" s="7" t="s">
+      <c r="C443" s="7" t="s">
         <v>1000</v>
       </c>
     </row>
-    <row r="443" spans="1:7" ht="34" x14ac:dyDescent="0.2">
-      <c r="A443" s="1" t="s">
+    <row r="444" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="A444" s="1" t="s">
         <v>1001</v>
       </c>
-      <c r="B443" s="1" t="s">
+      <c r="B444" s="1" t="s">
         <v>1002</v>
       </c>
-      <c r="C443" s="1" t="s">
+      <c r="C444" s="1" t="s">
         <v>1003</v>
       </c>
     </row>
-    <row r="444" spans="1:7" ht="68" x14ac:dyDescent="0.2">
-      <c r="A444" s="1" t="s">
+    <row r="445" spans="1:7" ht="68" x14ac:dyDescent="0.2">
+      <c r="A445" s="1" t="s">
         <v>1004</v>
       </c>
-      <c r="B444" s="1" t="s">
+      <c r="B445" s="1" t="s">
         <v>1005</v>
       </c>
-      <c r="C444" s="1" t="s">
+      <c r="C445" s="1" t="s">
         <v>1006</v>
       </c>
     </row>
-    <row r="445" spans="1:7" ht="85" x14ac:dyDescent="0.2">
-      <c r="A445" s="1" t="s">
+    <row r="446" spans="1:7" ht="85" x14ac:dyDescent="0.2">
+      <c r="A446" s="1" t="s">
         <v>1007</v>
       </c>
-      <c r="B445" s="1" t="s">
+      <c r="B446" s="1" t="s">
         <v>1008</v>
       </c>
-      <c r="C445" s="1" t="s">
+      <c r="C446" s="1" t="s">
         <v>1009</v>
       </c>
     </row>
-    <row r="446" spans="1:7" ht="51" x14ac:dyDescent="0.2">
-      <c r="A446" s="1" t="s">
+    <row r="447" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+      <c r="A447" s="1" t="s">
         <v>1010</v>
       </c>
-      <c r="B446" s="1" t="s">
+      <c r="B447" s="1" t="s">
         <v>1011</v>
       </c>
-      <c r="C446" s="1" t="s">
+      <c r="C447" s="1" t="s">
         <v>1012</v>
       </c>
     </row>
-    <row r="447" spans="1:7" ht="136" x14ac:dyDescent="0.2">
-      <c r="A447" s="1" t="s">
+    <row r="448" spans="1:7" ht="136" x14ac:dyDescent="0.2">
+      <c r="A448" s="1" t="s">
         <v>1013</v>
       </c>
-      <c r="B447" s="1" t="s">
+      <c r="B448" s="1" t="s">
         <v>1014</v>
       </c>
-      <c r="C447" s="1" t="s">
+      <c r="C448" s="1" t="s">
         <v>1015</v>
       </c>
     </row>
-    <row r="448" spans="1:7" ht="153" x14ac:dyDescent="0.2">
-      <c r="A448" s="1" t="s">
+    <row r="449" spans="1:3" ht="153" x14ac:dyDescent="0.2">
+      <c r="A449" s="1" t="s">
         <v>1016</v>
       </c>
-      <c r="B448" s="1" t="s">
+      <c r="B449" s="1" t="s">
         <v>1017</v>
       </c>
-      <c r="C448" s="1" t="s">
+      <c r="C449" s="1" t="s">
         <v>1018</v>
       </c>
     </row>
-    <row r="449" spans="1:3" ht="51" x14ac:dyDescent="0.2">
-      <c r="A449" s="1" t="s">
+    <row r="450" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+      <c r="A450" s="1" t="s">
         <v>1019</v>
       </c>
-      <c r="B449" s="1" t="s">
+      <c r="B450" s="1" t="s">
         <v>1020</v>
       </c>
-      <c r="C449" s="7" t="s">
+      <c r="C450" s="7" t="s">
         <v>1021</v>
       </c>
     </row>
-    <row r="450" spans="1:3" ht="136" x14ac:dyDescent="0.2">
-      <c r="A450" s="1" t="s">
+    <row r="451" spans="1:3" ht="136" x14ac:dyDescent="0.2">
+      <c r="A451" s="1" t="s">
         <v>1022</v>
       </c>
-      <c r="B450" s="1" t="s">
+      <c r="B451" s="1" t="s">
         <v>1023</v>
       </c>
-      <c r="C450" s="7" t="s">
+      <c r="C451" s="7" t="s">
         <v>1024</v>
       </c>
     </row>
-    <row r="451" spans="1:3" ht="153" x14ac:dyDescent="0.2">
-      <c r="A451" s="1" t="s">
+    <row r="452" spans="1:3" ht="153" x14ac:dyDescent="0.2">
+      <c r="A452" s="1" t="s">
         <v>1025</v>
       </c>
-      <c r="B451" s="1" t="s">
+      <c r="B452" s="1" t="s">
         <v>1026</v>
       </c>
-      <c r="C451" s="7" t="s">
+      <c r="C452" s="7" t="s">
         <v>1027</v>
       </c>
     </row>
-    <row r="452" spans="1:3" ht="51" x14ac:dyDescent="0.2">
-      <c r="A452" s="1" t="s">
+    <row r="453" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+      <c r="A453" s="1" t="s">
         <v>1028</v>
       </c>
-      <c r="B452" s="1" t="s">
+      <c r="B453" s="1" t="s">
         <v>1029</v>
       </c>
-      <c r="C452" s="7" t="s">
+      <c r="C453" s="7" t="s">
         <v>1030</v>
       </c>
     </row>
-    <row r="453" spans="1:3" ht="119" x14ac:dyDescent="0.2">
-      <c r="A453" s="1" t="s">
+    <row r="454" spans="1:3" ht="119" x14ac:dyDescent="0.2">
+      <c r="A454" s="1" t="s">
         <v>1031</v>
       </c>
-      <c r="B453" s="1" t="s">
+      <c r="B454" s="1" t="s">
         <v>1032</v>
       </c>
-      <c r="C453" s="7" t="s">
+      <c r="C454" s="7" t="s">
         <v>1033</v>
       </c>
     </row>
-    <row r="454" spans="1:3" ht="153" x14ac:dyDescent="0.2">
-      <c r="A454" s="1" t="s">
+    <row r="455" spans="1:3" ht="153" x14ac:dyDescent="0.2">
+      <c r="A455" s="1" t="s">
         <v>1034</v>
       </c>
-      <c r="B454" s="1" t="s">
+      <c r="B455" s="1" t="s">
         <v>1035</v>
       </c>
-      <c r="C454" s="7" t="s">
+      <c r="C455" s="7" t="s">
         <v>1036</v>
       </c>
     </row>
-    <row r="455" spans="1:3" ht="51" x14ac:dyDescent="0.2">
-      <c r="A455" s="1" t="s">
+    <row r="456" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+      <c r="A456" s="1" t="s">
         <v>1037</v>
       </c>
-      <c r="B455" s="1" t="s">
+      <c r="B456" s="1" t="s">
         <v>1038</v>
       </c>
-      <c r="C455" s="7" t="s">
+      <c r="C456" s="7" t="s">
         <v>1039</v>
       </c>
     </row>
-    <row r="456" spans="1:3" ht="136" x14ac:dyDescent="0.2">
-      <c r="A456" s="1" t="s">
+    <row r="457" spans="1:3" ht="136" x14ac:dyDescent="0.2">
+      <c r="A457" s="1" t="s">
         <v>1040</v>
       </c>
-      <c r="B456" s="1" t="s">
+      <c r="B457" s="1" t="s">
         <v>1041</v>
       </c>
-      <c r="C456" s="7" t="s">
+      <c r="C457" s="7" t="s">
         <v>1042</v>
       </c>
     </row>
-    <row r="457" spans="1:3" ht="153" x14ac:dyDescent="0.2">
-      <c r="A457" s="1" t="s">
+    <row r="458" spans="1:3" ht="153" x14ac:dyDescent="0.2">
+      <c r="A458" s="1" t="s">
         <v>1043</v>
       </c>
-      <c r="B457" s="1" t="s">
+      <c r="B458" s="1" t="s">
         <v>1044</v>
       </c>
-      <c r="C457" s="7" t="s">
+      <c r="C458" s="7" t="s">
         <v>1045</v>
-      </c>
-    </row>
-    <row r="458" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A458" s="1" t="s">
-        <v>1074</v>
-      </c>
-      <c r="B458" s="1" t="s">
-        <v>1086</v>
-      </c>
-      <c r="C458" s="8" t="s">
-        <v>1087</v>
       </c>
     </row>
     <row r="459" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A459" s="1" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
       <c r="B459" s="1" t="s">
-        <v>1099</v>
+        <v>1086</v>
       </c>
       <c r="C459" s="8" t="s">
-        <v>1088</v>
+        <v>1087</v>
       </c>
     </row>
     <row r="460" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A460" s="1" t="s">
-        <v>1076</v>
+        <v>1075</v>
       </c>
       <c r="B460" s="1" t="s">
-        <v>1100</v>
+        <v>1099</v>
       </c>
       <c r="C460" s="8" t="s">
-        <v>1089</v>
+        <v>1088</v>
       </c>
     </row>
     <row r="461" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A461" s="1" t="s">
-        <v>1077</v>
+        <v>1076</v>
       </c>
       <c r="B461" s="1" t="s">
-        <v>1101</v>
+        <v>1100</v>
       </c>
       <c r="C461" s="8" t="s">
-        <v>1090</v>
+        <v>1089</v>
       </c>
     </row>
     <row r="462" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A462" s="1" t="s">
-        <v>1078</v>
+        <v>1077</v>
       </c>
       <c r="B462" s="1" t="s">
-        <v>1102</v>
+        <v>1101</v>
       </c>
       <c r="C462" s="8" t="s">
-        <v>1091</v>
+        <v>1090</v>
       </c>
     </row>
     <row r="463" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A463" s="1" t="s">
-        <v>1079</v>
+        <v>1078</v>
       </c>
       <c r="B463" s="1" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
       <c r="C463" s="8" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
     </row>
     <row r="464" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A464" s="1" t="s">
-        <v>1080</v>
+        <v>1079</v>
       </c>
       <c r="B464" s="1" t="s">
-        <v>1104</v>
+        <v>1103</v>
       </c>
       <c r="C464" s="8" t="s">
-        <v>1093</v>
+        <v>1092</v>
       </c>
     </row>
     <row r="465" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A465" s="1" t="s">
-        <v>1081</v>
+        <v>1080</v>
       </c>
       <c r="B465" s="1" t="s">
-        <v>1105</v>
+        <v>1104</v>
       </c>
       <c r="C465" s="8" t="s">
-        <v>1094</v>
+        <v>1093</v>
       </c>
     </row>
     <row r="466" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A466" s="1" t="s">
-        <v>1082</v>
+        <v>1081</v>
       </c>
       <c r="B466" s="1" t="s">
-        <v>1106</v>
+        <v>1105</v>
       </c>
       <c r="C466" s="8" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
     </row>
     <row r="467" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A467" s="1" t="s">
-        <v>1083</v>
+        <v>1082</v>
       </c>
       <c r="B467" s="1" t="s">
-        <v>1107</v>
+        <v>1106</v>
       </c>
       <c r="C467" s="8" t="s">
-        <v>1096</v>
+        <v>1095</v>
       </c>
     </row>
     <row r="468" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A468" s="1" t="s">
-        <v>1084</v>
+        <v>1083</v>
       </c>
       <c r="B468" s="1" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
       <c r="C468" s="8" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
     </row>
     <row r="469" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A469" s="1" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
       <c r="B469" s="1" t="s">
-        <v>1109</v>
+        <v>1108</v>
       </c>
       <c r="C469" s="8" t="s">
-        <v>1098</v>
+        <v>1097</v>
       </c>
     </row>
     <row r="470" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A470" s="1" t="s">
+        <v>1085</v>
+      </c>
+      <c r="B470" s="1" t="s">
+        <v>1109</v>
+      </c>
+      <c r="C470" s="8" t="s">
+        <v>1098</v>
+      </c>
+    </row>
+    <row r="471" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A471" s="1" t="s">
         <v>1110</v>
       </c>
-      <c r="B470" s="1" t="s">
+      <c r="B471" s="1" t="s">
         <v>1113</v>
       </c>
-      <c r="C470" s="1" t="s">
+      <c r="C471" s="1" t="s">
         <v>1114</v>
-      </c>
-    </row>
-    <row r="471" spans="1:3" ht="51" x14ac:dyDescent="0.2">
-      <c r="A471" s="1" t="s">
-        <v>1111</v>
-      </c>
-      <c r="B471" s="1" t="s">
-        <v>1117</v>
-      </c>
-      <c r="C471" s="8" t="s">
-        <v>1115</v>
       </c>
     </row>
     <row r="472" spans="1:3" ht="51" x14ac:dyDescent="0.2">
       <c r="A472" s="1" t="s">
+        <v>1111</v>
+      </c>
+      <c r="B472" s="1" t="s">
+        <v>1117</v>
+      </c>
+      <c r="C472" s="8" t="s">
+        <v>1115</v>
+      </c>
+    </row>
+    <row r="473" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+      <c r="A473" s="1" t="s">
         <v>1112</v>
       </c>
-      <c r="B472" s="1" t="s">
+      <c r="B473" s="1" t="s">
         <v>1118</v>
       </c>
-      <c r="C472" s="8" t="s">
+      <c r="C473" s="8" t="s">
         <v>1116</v>
       </c>
     </row>
-    <row r="473" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A473" s="1" t="s">
+    <row r="474" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A474" s="1" t="s">
         <v>1130</v>
       </c>
-      <c r="B473" s="1" t="s">
+      <c r="B474" s="1" t="s">
         <v>1157</v>
       </c>
-      <c r="C473" s="8"/>
-    </row>
-    <row r="474" spans="1:3" ht="68" x14ac:dyDescent="0.2">
-      <c r="A474" s="1" t="s">
+      <c r="C474" s="8"/>
+    </row>
+    <row r="475" spans="1:3" ht="68" x14ac:dyDescent="0.2">
+      <c r="A475" s="1" t="s">
         <v>1131</v>
       </c>
-      <c r="B474" s="1" t="s">
+      <c r="B475" s="1" t="s">
         <v>1148</v>
       </c>
-      <c r="C474" s="8" t="s">
+      <c r="C475" s="8" t="s">
         <v>1115</v>
       </c>
     </row>
-    <row r="475" spans="1:3" ht="119" x14ac:dyDescent="0.2">
-      <c r="A475" s="1" t="s">
+    <row r="476" spans="1:3" ht="119" x14ac:dyDescent="0.2">
+      <c r="A476" s="1" t="s">
         <v>1132</v>
       </c>
-      <c r="B475" s="1" t="s">
+      <c r="B476" s="1" t="s">
         <v>1158</v>
       </c>
-      <c r="C475" s="8" t="s">
+      <c r="C476" s="8" t="s">
         <v>1116</v>
       </c>
     </row>
-    <row r="476" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A476" s="1" t="s">
+    <row r="477" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A477" s="1" t="s">
         <v>1149</v>
       </c>
-      <c r="B476" s="1" t="s">
+      <c r="B477" s="1" t="s">
         <v>1157</v>
       </c>
-      <c r="C476" s="8"/>
-    </row>
-    <row r="477" spans="1:3" ht="51" x14ac:dyDescent="0.2">
-      <c r="A477" s="1" t="s">
+      <c r="C477" s="8"/>
+    </row>
+    <row r="478" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+      <c r="A478" s="1" t="s">
         <v>1133</v>
       </c>
-      <c r="B477" s="1" t="s">
+      <c r="B478" s="1" t="s">
         <v>1190</v>
       </c>
-      <c r="C477" s="8"/>
-    </row>
-    <row r="478" spans="1:3" ht="153" x14ac:dyDescent="0.2">
-      <c r="A478" s="1" t="s">
+      <c r="C478" s="8"/>
+    </row>
+    <row r="479" spans="1:3" ht="153" x14ac:dyDescent="0.2">
+      <c r="A479" s="1" t="s">
         <v>1138</v>
       </c>
-      <c r="B478" s="1" t="s">
+      <c r="B479" s="1" t="s">
         <v>1159</v>
       </c>
-      <c r="C478" s="8"/>
-    </row>
-    <row r="479" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A479" s="1" t="s">
+      <c r="C479" s="8"/>
+    </row>
+    <row r="480" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A480" s="1" t="s">
         <v>1150</v>
       </c>
-      <c r="B479" s="1" t="s">
+      <c r="B480" s="1" t="s">
         <v>1160</v>
       </c>
-      <c r="C479" s="8"/>
-    </row>
-    <row r="480" spans="1:3" ht="68" x14ac:dyDescent="0.2">
-      <c r="A480" s="1" t="s">
+      <c r="C480" s="8"/>
+    </row>
+    <row r="481" spans="1:3" ht="68" x14ac:dyDescent="0.2">
+      <c r="A481" s="1" t="s">
         <v>1134</v>
       </c>
-      <c r="B480" s="1" t="s">
+      <c r="B481" s="1" t="s">
         <v>1191</v>
       </c>
-      <c r="C480" s="8"/>
-    </row>
-    <row r="481" spans="1:3" ht="102" x14ac:dyDescent="0.2">
-      <c r="A481" s="1" t="s">
+      <c r="C481" s="8"/>
+    </row>
+    <row r="482" spans="1:3" ht="102" x14ac:dyDescent="0.2">
+      <c r="A482" s="1" t="s">
         <v>1139</v>
       </c>
-      <c r="B481" s="1" t="s">
+      <c r="B482" s="1" t="s">
         <v>1163</v>
-      </c>
-      <c r="C481" s="8"/>
-    </row>
-    <row r="482" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A482" s="1" t="s">
-        <v>1151</v>
-      </c>
-      <c r="B482" s="1" t="s">
-        <v>1160</v>
       </c>
       <c r="C482" s="8"/>
     </row>
     <row r="483" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A483" s="1" t="s">
+        <v>1151</v>
+      </c>
+      <c r="B483" s="1" t="s">
+        <v>1160</v>
+      </c>
+      <c r="C483" s="8"/>
+    </row>
+    <row r="484" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A484" s="1" t="s">
         <v>1135</v>
       </c>
-      <c r="B483" s="1" t="s">
+      <c r="B484" s="1" t="s">
         <v>1164</v>
       </c>
-      <c r="C483" s="8"/>
-    </row>
-    <row r="484" spans="1:3" ht="153" x14ac:dyDescent="0.2">
-      <c r="A484" s="1" t="s">
+      <c r="C484" s="8"/>
+    </row>
+    <row r="485" spans="1:3" ht="153" x14ac:dyDescent="0.2">
+      <c r="A485" s="1" t="s">
         <v>1140</v>
       </c>
-      <c r="B484" s="1" t="s">
+      <c r="B485" s="1" t="s">
         <v>1161</v>
       </c>
-      <c r="C484" s="8"/>
-    </row>
-    <row r="485" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A485" s="1" t="s">
+      <c r="C485" s="8"/>
+    </row>
+    <row r="486" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A486" s="1" t="s">
         <v>1152</v>
       </c>
-      <c r="B485" s="1" t="s">
+      <c r="B486" s="1" t="s">
         <v>1165</v>
       </c>
-      <c r="C485" s="8"/>
-    </row>
-    <row r="486" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A486" s="1" t="s">
+      <c r="C486" s="8"/>
+    </row>
+    <row r="487" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A487" s="1" t="s">
         <v>1136</v>
       </c>
-      <c r="B486" s="1" t="s">
+      <c r="B487" s="1" t="s">
         <v>1166</v>
       </c>
-      <c r="C486" s="8"/>
-    </row>
-    <row r="487" spans="1:3" ht="102" x14ac:dyDescent="0.2">
-      <c r="A487" s="1" t="s">
+      <c r="C487" s="8"/>
+    </row>
+    <row r="488" spans="1:3" ht="102" x14ac:dyDescent="0.2">
+      <c r="A488" s="1" t="s">
         <v>1141</v>
       </c>
-      <c r="B487" s="1" t="s">
+      <c r="B488" s="1" t="s">
         <v>1162</v>
       </c>
-      <c r="C487" s="8"/>
-    </row>
-    <row r="488" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A488" s="1" t="s">
+      <c r="C488" s="8"/>
+    </row>
+    <row r="489" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A489" s="1" t="s">
         <v>1153</v>
       </c>
-      <c r="B488" s="1" t="s">
+      <c r="B489" s="1" t="s">
         <v>1165</v>
       </c>
-      <c r="C488" s="8"/>
-    </row>
-    <row r="489" spans="1:3" ht="51" x14ac:dyDescent="0.2">
-      <c r="A489" s="1" t="s">
+      <c r="C489" s="8"/>
+    </row>
+    <row r="490" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+      <c r="A490" s="1" t="s">
         <v>1137</v>
       </c>
-      <c r="B489" s="1" t="s">
+      <c r="B490" s="1" t="s">
         <v>1174</v>
       </c>
-      <c r="C489" s="8"/>
-    </row>
-    <row r="490" spans="1:3" ht="68" x14ac:dyDescent="0.2">
-      <c r="A490" s="1" t="s">
+      <c r="C490" s="8"/>
+    </row>
+    <row r="491" spans="1:3" ht="68" x14ac:dyDescent="0.2">
+      <c r="A491" s="1" t="s">
         <v>1142</v>
       </c>
-      <c r="B490" s="1" t="s">
+      <c r="B491" s="1" t="s">
         <v>1177</v>
       </c>
-      <c r="C490" s="8"/>
-    </row>
-    <row r="491" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A491" s="1" t="s">
+      <c r="C491" s="8"/>
+    </row>
+    <row r="492" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A492" s="1" t="s">
         <v>1154</v>
       </c>
-      <c r="B491" s="1" t="s">
+      <c r="B492" s="1" t="s">
         <v>1167</v>
       </c>
-      <c r="C491" s="8"/>
-    </row>
-    <row r="492" spans="1:3" ht="51" x14ac:dyDescent="0.2">
-      <c r="A492" s="1" t="s">
+      <c r="C492" s="8"/>
+    </row>
+    <row r="493" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+      <c r="A493" s="1" t="s">
         <v>1143</v>
       </c>
-      <c r="B492" s="1" t="s">
+      <c r="B493" s="1" t="s">
         <v>1175</v>
       </c>
-      <c r="C492" s="8"/>
-    </row>
-    <row r="493" spans="1:3" ht="102" x14ac:dyDescent="0.2">
-      <c r="A493" s="1" t="s">
+      <c r="C493" s="8"/>
+    </row>
+    <row r="494" spans="1:3" ht="102" x14ac:dyDescent="0.2">
+      <c r="A494" s="1" t="s">
         <v>1144</v>
       </c>
-      <c r="B493" s="1" t="s">
+      <c r="B494" s="1" t="s">
         <v>1168</v>
-      </c>
-      <c r="C493" s="8"/>
-    </row>
-    <row r="494" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A494" s="1" t="s">
-        <v>1155</v>
-      </c>
-      <c r="B494" s="1" t="s">
-        <v>1167</v>
       </c>
       <c r="C494" s="8"/>
     </row>
     <row r="495" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A495" s="1" t="s">
+        <v>1155</v>
+      </c>
+      <c r="B495" s="1" t="s">
+        <v>1167</v>
+      </c>
+      <c r="C495" s="8"/>
+    </row>
+    <row r="496" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A496" s="1" t="s">
         <v>1145</v>
       </c>
-      <c r="B495" s="1" t="s">
+      <c r="B496" s="1" t="s">
         <v>1176</v>
       </c>
-      <c r="C495" s="8"/>
-    </row>
-    <row r="496" spans="1:3" ht="51" x14ac:dyDescent="0.2">
-      <c r="A496" s="1" t="s">
+      <c r="C496" s="8"/>
+    </row>
+    <row r="497" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+      <c r="A497" s="1" t="s">
         <v>1170</v>
       </c>
-      <c r="B496" s="1" t="s">
+      <c r="B497" s="1" t="s">
         <v>1172</v>
       </c>
-      <c r="C496" s="8"/>
-    </row>
-    <row r="497" spans="1:3" ht="85" x14ac:dyDescent="0.2">
-      <c r="A497" s="1" t="s">
+      <c r="C497" s="8"/>
+    </row>
+    <row r="498" spans="1:3" ht="85" x14ac:dyDescent="0.2">
+      <c r="A498" s="1" t="s">
         <v>1171</v>
       </c>
-      <c r="B497" s="1" t="s">
+      <c r="B498" s="1" t="s">
         <v>1173</v>
       </c>
-      <c r="C497" s="8"/>
-    </row>
-    <row r="498" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A498" s="1" t="s">
+      <c r="C498" s="8"/>
+    </row>
+    <row r="499" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A499" s="1" t="s">
         <v>1156</v>
       </c>
-      <c r="B498" s="1" t="s">
+      <c r="B499" s="1" t="s">
         <v>1169</v>
       </c>
-      <c r="C498" s="8"/>
-    </row>
-    <row r="499" spans="1:3" ht="85" x14ac:dyDescent="0.2">
-      <c r="A499" s="1" t="s">
+      <c r="C499" s="8"/>
+    </row>
+    <row r="500" spans="1:3" ht="85" x14ac:dyDescent="0.2">
+      <c r="A500" s="1" t="s">
         <v>1146</v>
       </c>
-      <c r="B499" s="1" t="s">
+      <c r="B500" s="1" t="s">
         <v>1211</v>
       </c>
-      <c r="C499" s="8"/>
-    </row>
-    <row r="500" spans="1:3" ht="68" x14ac:dyDescent="0.2">
-      <c r="A500" s="1" t="s">
+      <c r="C500" s="8"/>
+    </row>
+    <row r="501" spans="1:3" ht="68" x14ac:dyDescent="0.2">
+      <c r="A501" s="1" t="s">
         <v>1210</v>
       </c>
-      <c r="B500" s="1" t="s">
+      <c r="B501" s="1" t="s">
         <v>1279</v>
       </c>
-      <c r="C500" s="8"/>
-    </row>
-    <row r="501" spans="1:3" ht="102" x14ac:dyDescent="0.2">
-      <c r="A501" s="1" t="s">
+      <c r="C501" s="8"/>
+    </row>
+    <row r="502" spans="1:3" ht="102" x14ac:dyDescent="0.2">
+      <c r="A502" s="1" t="s">
         <v>1147</v>
       </c>
-      <c r="B501" s="1" t="s">
+      <c r="B502" s="1" t="s">
         <v>1212</v>
       </c>
-      <c r="C501" s="8"/>
-    </row>
-    <row r="502" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A502" s="1" t="s">
+      <c r="C502" s="8"/>
+    </row>
+    <row r="503" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A503" s="1" t="s">
         <v>1213</v>
       </c>
-      <c r="B502" s="1" t="s">
+      <c r="B503" s="1" t="s">
         <v>1225</v>
       </c>
-      <c r="C502" s="8"/>
-    </row>
-    <row r="503" spans="1:3" ht="51" x14ac:dyDescent="0.2">
-      <c r="A503" s="1" t="s">
+      <c r="C503" s="8"/>
+    </row>
+    <row r="504" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+      <c r="A504" s="1" t="s">
         <v>1214</v>
       </c>
-      <c r="B503" s="1" t="s">
+      <c r="B504" s="1" t="s">
         <v>1227</v>
       </c>
-      <c r="C503" s="8"/>
-    </row>
-    <row r="504" spans="1:3" ht="68" x14ac:dyDescent="0.2">
-      <c r="A504" s="1" t="s">
+      <c r="C504" s="8"/>
+    </row>
+    <row r="505" spans="1:3" ht="68" x14ac:dyDescent="0.2">
+      <c r="A505" s="1" t="s">
         <v>1215</v>
       </c>
-      <c r="B504" s="1" t="s">
+      <c r="B505" s="1" t="s">
         <v>1228</v>
       </c>
-      <c r="C504" s="8"/>
-    </row>
-    <row r="505" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A505" s="1" t="s">
+      <c r="C505" s="8"/>
+    </row>
+    <row r="506" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A506" s="1" t="s">
         <v>1216</v>
       </c>
-      <c r="B505" s="1" t="s">
+      <c r="B506" s="1" t="s">
         <v>1226</v>
       </c>
-      <c r="C505" s="8"/>
-    </row>
-    <row r="506" spans="1:3" ht="51" x14ac:dyDescent="0.2">
-      <c r="A506" s="1" t="s">
+      <c r="C506" s="8"/>
+    </row>
+    <row r="507" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+      <c r="A507" s="1" t="s">
         <v>1217</v>
       </c>
-      <c r="B506" s="1" t="s">
+      <c r="B507" s="1" t="s">
         <v>1229</v>
       </c>
-      <c r="C506" s="8"/>
-    </row>
-    <row r="507" spans="1:3" ht="68" x14ac:dyDescent="0.2">
-      <c r="A507" s="1" t="s">
+      <c r="C507" s="8"/>
+    </row>
+    <row r="508" spans="1:3" ht="68" x14ac:dyDescent="0.2">
+      <c r="A508" s="1" t="s">
         <v>1218</v>
       </c>
-      <c r="B507" s="1" t="s">
+      <c r="B508" s="1" t="s">
         <v>1230</v>
-      </c>
-      <c r="C507" s="8"/>
-    </row>
-    <row r="508" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A508" s="1" t="s">
-        <v>1219</v>
-      </c>
-      <c r="B508" s="1" t="s">
-        <v>1231</v>
       </c>
       <c r="C508" s="8"/>
     </row>
     <row r="509" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A509" s="1" t="s">
+        <v>1219</v>
+      </c>
+      <c r="B509" s="1" t="s">
+        <v>1231</v>
+      </c>
+      <c r="C509" s="8"/>
+    </row>
+    <row r="510" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A510" s="1" t="s">
         <v>1220</v>
       </c>
-      <c r="B509" s="1" t="s">
+      <c r="B510" s="1" t="s">
         <v>1232</v>
       </c>
-      <c r="C509" s="8"/>
-    </row>
-    <row r="510" spans="1:3" ht="85" x14ac:dyDescent="0.2">
-      <c r="A510" s="1" t="s">
+      <c r="C510" s="8"/>
+    </row>
+    <row r="511" spans="1:3" ht="85" x14ac:dyDescent="0.2">
+      <c r="A511" s="1" t="s">
         <v>1221</v>
       </c>
-      <c r="B510" s="1" t="s">
+      <c r="B511" s="1" t="s">
         <v>1233</v>
       </c>
-      <c r="C510" s="8"/>
-    </row>
-    <row r="511" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A511" s="1" t="s">
+      <c r="C511" s="8"/>
+    </row>
+    <row r="512" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A512" s="1" t="s">
         <v>1239</v>
       </c>
-      <c r="B511" s="1" t="s">
+      <c r="B512" s="1" t="s">
         <v>1234</v>
       </c>
-      <c r="C511" s="8"/>
-    </row>
-    <row r="512" spans="1:3" ht="102" x14ac:dyDescent="0.2">
-      <c r="A512" s="1" t="s">
+      <c r="C512" s="8"/>
+    </row>
+    <row r="513" spans="1:3" ht="102" x14ac:dyDescent="0.2">
+      <c r="A513" s="1" t="s">
         <v>1241</v>
       </c>
-      <c r="B512" s="1" t="s">
+      <c r="B513" s="1" t="s">
         <v>1245</v>
       </c>
-      <c r="C512" s="8"/>
-    </row>
-    <row r="513" spans="1:3" ht="119" x14ac:dyDescent="0.2">
-      <c r="A513" s="1" t="s">
+      <c r="C513" s="8"/>
+    </row>
+    <row r="514" spans="1:3" ht="119" x14ac:dyDescent="0.2">
+      <c r="A514" s="1" t="s">
         <v>1242</v>
       </c>
-      <c r="B513" s="1" t="s">
+      <c r="B514" s="1" t="s">
         <v>1247</v>
       </c>
-      <c r="C513" s="8"/>
-    </row>
-    <row r="514" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A514" s="1" t="s">
+      <c r="C514" s="8"/>
+    </row>
+    <row r="515" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A515" s="1" t="s">
         <v>1240</v>
       </c>
-      <c r="B514" s="1" t="s">
+      <c r="B515" s="1" t="s">
         <v>1234</v>
-      </c>
-      <c r="C514" s="8"/>
-    </row>
-    <row r="515" spans="1:3" ht="119" x14ac:dyDescent="0.2">
-      <c r="A515" s="1" t="s">
-        <v>1243</v>
-      </c>
-      <c r="B515" s="1" t="s">
-        <v>1246</v>
       </c>
       <c r="C515" s="8"/>
     </row>
     <row r="516" spans="1:3" ht="119" x14ac:dyDescent="0.2">
       <c r="A516" s="1" t="s">
+        <v>1243</v>
+      </c>
+      <c r="B516" s="1" t="s">
+        <v>1246</v>
+      </c>
+      <c r="C516" s="8"/>
+    </row>
+    <row r="517" spans="1:3" ht="119" x14ac:dyDescent="0.2">
+      <c r="A517" s="1" t="s">
         <v>1244</v>
       </c>
-      <c r="B516" s="1" t="s">
+      <c r="B517" s="1" t="s">
         <v>1235</v>
       </c>
-      <c r="C516" s="8"/>
-    </row>
-    <row r="517" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A517" s="1" t="s">
+      <c r="C517" s="8"/>
+    </row>
+    <row r="518" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A518" s="1" t="s">
         <v>1222</v>
       </c>
-      <c r="B517" s="1" t="s">
+      <c r="B518" s="1" t="s">
         <v>1236</v>
       </c>
-      <c r="C517" s="8"/>
-    </row>
-    <row r="518" spans="1:3" ht="102" x14ac:dyDescent="0.2">
-      <c r="A518" s="1" t="s">
+      <c r="C518" s="8"/>
+    </row>
+    <row r="519" spans="1:3" ht="102" x14ac:dyDescent="0.2">
+      <c r="A519" s="1" t="s">
         <v>1223</v>
       </c>
-      <c r="B518" s="1" t="s">
+      <c r="B519" s="1" t="s">
         <v>1237</v>
       </c>
-      <c r="C518" s="8"/>
-    </row>
-    <row r="519" spans="1:3" ht="85" x14ac:dyDescent="0.2">
-      <c r="A519" s="1" t="s">
+      <c r="C519" s="8"/>
+    </row>
+    <row r="520" spans="1:3" ht="85" x14ac:dyDescent="0.2">
+      <c r="A520" s="1" t="s">
         <v>1224</v>
       </c>
-      <c r="B519" s="1" t="s">
+      <c r="B520" s="1" t="s">
         <v>1238</v>
       </c>
-      <c r="C519" s="8"/>
-    </row>
-    <row r="520" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A520" s="1" t="s">
+      <c r="C520" s="8"/>
+    </row>
+    <row r="521" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A521" s="1" t="s">
         <v>1179</v>
       </c>
-      <c r="B520" s="1" t="s">
+      <c r="B521" s="1" t="s">
         <v>1178</v>
       </c>
-      <c r="C520" s="8"/>
-    </row>
-    <row r="521" spans="1:3" ht="68" x14ac:dyDescent="0.2">
-      <c r="A521" s="1" t="s">
+      <c r="C521" s="8"/>
+    </row>
+    <row r="522" spans="1:3" ht="68" x14ac:dyDescent="0.2">
+      <c r="A522" s="1" t="s">
         <v>1180</v>
       </c>
-      <c r="B521" s="1" t="s">
+      <c r="B522" s="1" t="s">
         <v>1185</v>
       </c>
-      <c r="C521" s="8"/>
-    </row>
-    <row r="522" spans="1:3" ht="102" x14ac:dyDescent="0.2">
-      <c r="A522" s="1" t="s">
+      <c r="C522" s="8"/>
+    </row>
+    <row r="523" spans="1:3" ht="102" x14ac:dyDescent="0.2">
+      <c r="A523" s="1" t="s">
         <v>1181</v>
       </c>
-      <c r="B522" s="1" t="s">
+      <c r="B523" s="1" t="s">
         <v>1186</v>
       </c>
-      <c r="C522" s="8"/>
-    </row>
-    <row r="523" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A523" s="1" t="s">
+      <c r="C523" s="8"/>
+    </row>
+    <row r="524" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A524" s="1" t="s">
         <v>1182</v>
       </c>
-      <c r="B523" s="1" t="s">
+      <c r="B524" s="1" t="s">
         <v>1187</v>
       </c>
-      <c r="C523" s="8"/>
-    </row>
-    <row r="524" spans="1:3" ht="68" x14ac:dyDescent="0.2">
-      <c r="A524" s="1" t="s">
+      <c r="C524" s="8"/>
+    </row>
+    <row r="525" spans="1:3" ht="68" x14ac:dyDescent="0.2">
+      <c r="A525" s="1" t="s">
         <v>1183</v>
       </c>
-      <c r="B524" s="1" t="s">
+      <c r="B525" s="1" t="s">
         <v>1188</v>
       </c>
-      <c r="C524" s="8"/>
-    </row>
-    <row r="525" spans="1:3" ht="102" x14ac:dyDescent="0.2">
-      <c r="A525" s="1" t="s">
+      <c r="C525" s="8"/>
+    </row>
+    <row r="526" spans="1:3" ht="102" x14ac:dyDescent="0.2">
+      <c r="A526" s="1" t="s">
         <v>1184</v>
       </c>
-      <c r="B525" s="1" t="s">
+      <c r="B526" s="1" t="s">
         <v>1189</v>
       </c>
-      <c r="C525" s="8"/>
-    </row>
-    <row r="526" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A526" s="1" t="s">
+      <c r="C526" s="8"/>
+    </row>
+    <row r="527" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A527" s="1" t="s">
         <v>1192</v>
       </c>
-      <c r="B526" s="1" t="s">
+      <c r="B527" s="1" t="s">
         <v>1201</v>
-      </c>
-      <c r="C526" s="8"/>
-    </row>
-    <row r="527" spans="1:3" ht="68" x14ac:dyDescent="0.2">
-      <c r="A527" s="1" t="s">
-        <v>1193</v>
-      </c>
-      <c r="B527" s="1" t="s">
-        <v>1202</v>
       </c>
       <c r="C527" s="8"/>
     </row>
     <row r="528" spans="1:3" ht="68" x14ac:dyDescent="0.2">
       <c r="A528" s="1" t="s">
+        <v>1193</v>
+      </c>
+      <c r="B528" s="1" t="s">
+        <v>1202</v>
+      </c>
+      <c r="C528" s="8"/>
+    </row>
+    <row r="529" spans="1:3" ht="68" x14ac:dyDescent="0.2">
+      <c r="A529" s="1" t="s">
         <v>1194</v>
       </c>
-      <c r="B528" s="1" t="s">
+      <c r="B529" s="1" t="s">
         <v>1203</v>
       </c>
-      <c r="C528" s="8"/>
-    </row>
-    <row r="529" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A529" s="1" t="s">
+      <c r="C529" s="8"/>
+    </row>
+    <row r="530" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A530" s="1" t="s">
         <v>1195</v>
       </c>
-      <c r="B529" s="1" t="s">
+      <c r="B530" s="1" t="s">
         <v>1204</v>
       </c>
-      <c r="C529" s="8"/>
-    </row>
-    <row r="530" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A530" s="1" t="s">
+      <c r="C530" s="8"/>
+    </row>
+    <row r="531" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A531" s="1" t="s">
         <v>1196</v>
       </c>
-      <c r="B530" s="1" t="s">
+      <c r="B531" s="1" t="s">
         <v>1205</v>
       </c>
-      <c r="C530" s="8"/>
-    </row>
-    <row r="531" spans="1:3" ht="51" x14ac:dyDescent="0.2">
-      <c r="A531" s="1" t="s">
+      <c r="C531" s="8"/>
+    </row>
+    <row r="532" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+      <c r="A532" s="1" t="s">
         <v>1197</v>
       </c>
-      <c r="B531" s="1" t="s">
+      <c r="B532" s="1" t="s">
         <v>1206</v>
       </c>
-      <c r="C531" s="8"/>
-    </row>
-    <row r="532" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A532" s="1" t="s">
+      <c r="C532" s="8"/>
+    </row>
+    <row r="533" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A533" s="1" t="s">
         <v>1198</v>
       </c>
-      <c r="B532" s="1" t="s">
+      <c r="B533" s="1" t="s">
         <v>1207</v>
       </c>
-      <c r="C532" s="8"/>
-    </row>
-    <row r="533" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A533" s="1" t="s">
+      <c r="C533" s="8"/>
+    </row>
+    <row r="534" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A534" s="1" t="s">
         <v>1199</v>
       </c>
-      <c r="B533" s="1" t="s">
+      <c r="B534" s="1" t="s">
         <v>1208</v>
       </c>
-      <c r="C533" s="8"/>
-    </row>
-    <row r="534" spans="1:3" ht="51" x14ac:dyDescent="0.2">
-      <c r="A534" s="1" t="s">
+      <c r="C534" s="8"/>
+    </row>
+    <row r="535" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+      <c r="A535" s="1" t="s">
         <v>1200</v>
       </c>
-      <c r="B534" s="1" t="s">
+      <c r="B535" s="1" t="s">
         <v>1209</v>
       </c>
-      <c r="C534" s="8"/>
-    </row>
-    <row r="535" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A535" s="1" t="s">
+      <c r="C535" s="8"/>
+    </row>
+    <row r="536" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A536" s="1" t="s">
         <v>1316</v>
       </c>
-      <c r="B535" s="1" t="s">
+      <c r="B536" s="1" t="s">
         <v>1310</v>
       </c>
-      <c r="C535" s="8"/>
-    </row>
-    <row r="536" spans="1:3" ht="51" x14ac:dyDescent="0.2">
-      <c r="A536" s="1" t="s">
+      <c r="C536" s="8"/>
+    </row>
+    <row r="537" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+      <c r="A537" s="1" t="s">
         <v>1317</v>
       </c>
-      <c r="B536" s="1" t="s">
+      <c r="B537" s="1" t="s">
         <v>1312</v>
-      </c>
-      <c r="C536" s="8"/>
-    </row>
-    <row r="537" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A537" s="1" t="s">
-        <v>1318</v>
-      </c>
-      <c r="B537" s="1" t="s">
-        <v>1313</v>
       </c>
       <c r="C537" s="8"/>
     </row>
     <row r="538" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A538" s="1" t="s">
+        <v>1318</v>
+      </c>
+      <c r="B538" s="1" t="s">
+        <v>1313</v>
+      </c>
+      <c r="C538" s="8"/>
+    </row>
+    <row r="539" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A539" s="1" t="s">
         <v>1319</v>
       </c>
-      <c r="B538" s="1" t="s">
+      <c r="B539" s="1" t="s">
         <v>1311</v>
       </c>
-      <c r="C538" s="8"/>
-    </row>
-    <row r="539" spans="1:3" ht="51" x14ac:dyDescent="0.2">
-      <c r="A539" s="1" t="s">
+      <c r="C539" s="8"/>
+    </row>
+    <row r="540" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+      <c r="A540" s="1" t="s">
         <v>1320</v>
       </c>
-      <c r="B539" s="1" t="s">
+      <c r="B540" s="1" t="s">
         <v>1314</v>
       </c>
-      <c r="C539" s="8"/>
-    </row>
-    <row r="540" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A540" s="1" t="s">
+      <c r="C540" s="8"/>
+    </row>
+    <row r="541" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A541" s="1" t="s">
         <v>1321</v>
       </c>
-      <c r="B540" s="1" t="s">
+      <c r="B541" s="1" t="s">
         <v>1315</v>
       </c>
-      <c r="C540" s="8"/>
-    </row>
-    <row r="541" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A541" s="1" t="s">
-        <v>1260</v>
-      </c>
-      <c r="B541" s="1" t="s">
-        <v>1261</v>
-      </c>
-      <c r="C541" s="9" t="s">
-        <v>1262</v>
-      </c>
+      <c r="C541" s="8"/>
     </row>
     <row r="542" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A542" s="1" t="s">
+        <v>1260</v>
+      </c>
+      <c r="B542" s="1" t="s">
+        <v>1261</v>
+      </c>
+      <c r="C542" s="9" t="s">
+        <v>1262</v>
+      </c>
+    </row>
+    <row r="543" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A543" s="1" t="s">
         <v>1263</v>
       </c>
-      <c r="B542" s="1" t="s">
+      <c r="B543" s="1" t="s">
         <v>1264</v>
       </c>
-      <c r="C542" s="9" t="s">
+      <c r="C543" s="9" t="s">
         <v>1265</v>
-      </c>
-    </row>
-    <row r="543" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A543" t="s">
-        <v>1248</v>
-      </c>
-      <c r="B543" s="1" t="s">
-        <v>1253</v>
-      </c>
-      <c r="C543" s="1" t="s">
-        <v>956</v>
       </c>
     </row>
     <row r="544" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A544" t="s">
-        <v>1249</v>
+        <v>1248</v>
       </c>
       <c r="B544" s="1" t="s">
-        <v>958</v>
+        <v>1253</v>
       </c>
       <c r="C544" s="1" t="s">
-        <v>953</v>
+        <v>956</v>
       </c>
     </row>
     <row r="545" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A545" t="s">
-        <v>1250</v>
+        <v>1249</v>
       </c>
       <c r="B545" s="1" t="s">
-        <v>1254</v>
+        <v>958</v>
       </c>
       <c r="C545" s="1" t="s">
-        <v>1256</v>
+        <v>953</v>
       </c>
     </row>
     <row r="546" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A546" t="s">
-        <v>1251</v>
+        <v>1250</v>
       </c>
       <c r="B546" s="1" t="s">
-        <v>1255</v>
+        <v>1254</v>
       </c>
       <c r="C546" s="1" t="s">
-        <v>1257</v>
+        <v>1256</v>
       </c>
     </row>
     <row r="547" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A547" t="s">
+        <v>1251</v>
+      </c>
+      <c r="B547" s="1" t="s">
+        <v>1255</v>
+      </c>
+      <c r="C547" s="1" t="s">
+        <v>1257</v>
+      </c>
+    </row>
+    <row r="548" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A548" t="s">
         <v>1252</v>
       </c>
-      <c r="B547" s="4" t="s">
+      <c r="B548" s="4" t="s">
         <v>1046</v>
       </c>
-      <c r="C547" s="4" t="s">
+      <c r="C548" s="4" t="s">
         <v>1258</v>
       </c>
-      <c r="D547" s="4"/>
-      <c r="E547" s="4"/>
-      <c r="F547" s="4"/>
-      <c r="G547" s="4"/>
-    </row>
-    <row r="548" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A548" s="1" t="s">
+      <c r="D548" s="4"/>
+      <c r="E548" s="4"/>
+      <c r="F548" s="4"/>
+      <c r="G548" s="4"/>
+    </row>
+    <row r="549" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A549" s="1" t="s">
         <v>1266</v>
       </c>
-      <c r="B548" s="1" t="s">
+      <c r="B549" s="1" t="s">
         <v>522</v>
       </c>
-      <c r="C548" s="1" t="s">
+      <c r="C549" s="1" t="s">
         <v>523</v>
       </c>
     </row>
-    <row r="549" spans="1:7" ht="34" x14ac:dyDescent="0.2">
-      <c r="A549" s="1" t="s">
+    <row r="550" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="A550" s="1" t="s">
         <v>1267</v>
       </c>
-      <c r="B549" s="1" t="s">
+      <c r="B550" s="1" t="s">
         <v>1304</v>
       </c>
-      <c r="C549" s="1" t="s">
+      <c r="C550" s="1" t="s">
         <v>1305</v>
       </c>
     </row>
-    <row r="550" spans="1:7" ht="51" x14ac:dyDescent="0.2">
-      <c r="A550" s="1" t="s">
+    <row r="551" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="A551" s="1" t="s">
         <v>1268</v>
       </c>
-      <c r="B550" s="1" t="s">
+      <c r="B551" s="1" t="s">
         <v>1306</v>
       </c>
-      <c r="C550" s="1" t="s">
+      <c r="C551" s="1" t="s">
         <v>1307</v>
       </c>
     </row>
-    <row r="551" spans="1:7" ht="34" x14ac:dyDescent="0.2">
-      <c r="A551" s="11" t="s">
+    <row r="552" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="A552" s="11" t="s">
         <v>1269</v>
       </c>
-      <c r="B551" s="7" t="s">
+      <c r="B552" s="7" t="s">
         <v>1280</v>
       </c>
-      <c r="C551" s="7" t="s">
+      <c r="C552" s="7" t="s">
         <v>1282</v>
       </c>
-      <c r="D551" s="7"/>
-      <c r="E551" s="7"/>
-      <c r="F551" s="7"/>
-      <c r="G551" s="12"/>
-    </row>
-    <row r="552" spans="1:7" ht="34" x14ac:dyDescent="0.2">
-      <c r="A552" s="13" t="s">
+      <c r="D552" s="7"/>
+      <c r="E552" s="7"/>
+      <c r="F552" s="7"/>
+      <c r="G552" s="12"/>
+    </row>
+    <row r="553" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="A553" s="13" t="s">
         <v>1270</v>
       </c>
-      <c r="B552" s="14" t="s">
+      <c r="B553" s="14" t="s">
         <v>1281</v>
       </c>
-      <c r="C552" s="14" t="s">
+      <c r="C553" s="14" t="s">
         <v>1283</v>
       </c>
-      <c r="D552" s="14"/>
-      <c r="E552" s="14"/>
-      <c r="F552" s="14"/>
-      <c r="G552" s="15"/>
-    </row>
-    <row r="553" spans="1:7" ht="34" x14ac:dyDescent="0.2">
-      <c r="A553" s="11" t="s">
+      <c r="D553" s="14"/>
+      <c r="E553" s="14"/>
+      <c r="F553" s="14"/>
+      <c r="G553" s="15"/>
+    </row>
+    <row r="554" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="A554" s="11" t="s">
         <v>1271</v>
       </c>
-      <c r="B553" s="7" t="s">
+      <c r="B554" s="7" t="s">
         <v>522</v>
       </c>
-      <c r="C553" s="7" t="s">
+      <c r="C554" s="7" t="s">
         <v>602</v>
       </c>
-      <c r="D553" s="7"/>
-      <c r="E553" s="7"/>
-      <c r="F553" s="7"/>
-      <c r="G553" s="12"/>
-    </row>
-    <row r="554" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A554" t="s">
-        <v>1284</v>
-      </c>
-      <c r="B554" s="16" t="s">
-        <v>1272</v>
-      </c>
-      <c r="C554" s="16" t="s">
-        <v>1272</v>
-      </c>
+      <c r="D554" s="7"/>
+      <c r="E554" s="7"/>
+      <c r="F554" s="7"/>
+      <c r="G554" s="12"/>
     </row>
     <row r="555" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A555" t="s">
+        <v>1284</v>
+      </c>
+      <c r="B555" s="16" t="s">
+        <v>1272</v>
+      </c>
+      <c r="C555" s="16" t="s">
+        <v>1272</v>
+      </c>
+    </row>
+    <row r="556" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A556" t="s">
         <v>1285</v>
       </c>
-      <c r="B555" s="16" t="s">
+      <c r="B556" s="16" t="s">
         <v>1286</v>
       </c>
-      <c r="C555" s="16" t="s">
+      <c r="C556" s="16" t="s">
         <v>1286</v>
       </c>
     </row>
-    <row r="556" spans="1:7" ht="34" x14ac:dyDescent="0.2">
-      <c r="A556" s="11" t="s">
+    <row r="557" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="A557" s="11" t="s">
         <v>1273</v>
       </c>
-      <c r="B556" s="7" t="s">
+      <c r="B557" s="7" t="s">
         <v>1287</v>
       </c>
-      <c r="C556" s="7" t="s">
+      <c r="C557" s="7" t="s">
         <v>1294</v>
       </c>
-      <c r="D556" s="4"/>
-      <c r="E556" s="4"/>
-      <c r="F556" s="4"/>
-      <c r="G556" s="4"/>
-    </row>
-    <row r="557" spans="1:7" ht="34" x14ac:dyDescent="0.2">
-      <c r="A557" s="13" t="s">
+      <c r="D557" s="4"/>
+      <c r="E557" s="4"/>
+      <c r="F557" s="4"/>
+      <c r="G557" s="4"/>
+    </row>
+    <row r="558" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="A558" s="13" t="s">
         <v>1274</v>
       </c>
-      <c r="B557" s="14" t="s">
+      <c r="B558" s="14" t="s">
         <v>1288</v>
       </c>
-      <c r="C557" s="14" t="s">
+      <c r="C558" s="14" t="s">
         <v>1293</v>
-      </c>
-    </row>
-    <row r="558" spans="1:7" ht="34" x14ac:dyDescent="0.2">
-      <c r="A558" s="11" t="s">
-        <v>1275</v>
-      </c>
-      <c r="B558" s="1" t="s">
-        <v>1304</v>
-      </c>
-      <c r="C558" s="1" t="s">
-        <v>1308</v>
       </c>
     </row>
     <row r="559" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A559" s="11" t="s">
+        <v>1275</v>
+      </c>
+      <c r="B559" s="1" t="s">
+        <v>1304</v>
+      </c>
+      <c r="C559" s="1" t="s">
+        <v>1308</v>
+      </c>
+    </row>
+    <row r="560" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="A560" s="11" t="s">
         <v>1276</v>
       </c>
-      <c r="B559" s="7" t="s">
+      <c r="B560" s="7" t="s">
         <v>1289</v>
       </c>
-      <c r="C559" s="7" t="s">
+      <c r="C560" s="7" t="s">
         <v>1292</v>
       </c>
     </row>
-    <row r="560" spans="1:7" ht="34" x14ac:dyDescent="0.2">
-      <c r="A560" s="13" t="s">
+    <row r="561" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="A561" s="13" t="s">
         <v>1277</v>
       </c>
-      <c r="B560" s="14" t="s">
+      <c r="B561" s="14" t="s">
         <v>1290</v>
       </c>
-      <c r="C560" s="14" t="s">
+      <c r="C561" s="14" t="s">
         <v>1291</v>
       </c>
     </row>
-    <row r="561" spans="1:7" ht="51" x14ac:dyDescent="0.2">
-      <c r="A561" s="11" t="s">
+    <row r="562" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="A562" s="11" t="s">
         <v>1278</v>
       </c>
-      <c r="B561" s="1" t="s">
+      <c r="B562" s="1" t="s">
         <v>1306</v>
       </c>
-      <c r="C561" s="1" t="s">
+      <c r="C562" s="1" t="s">
         <v>1309</v>
-      </c>
-    </row>
-    <row r="562" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A562" s="1" t="s">
-        <v>1295</v>
-      </c>
-      <c r="B562" s="1" t="s">
-        <v>522</v>
-      </c>
-      <c r="C562" s="1" t="s">
-        <v>523</v>
       </c>
     </row>
     <row r="563" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A563" s="1" t="s">
+        <v>1295</v>
+      </c>
+      <c r="B563" s="1" t="s">
+        <v>522</v>
+      </c>
+      <c r="C563" s="1" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="564" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A564" s="1" t="s">
         <v>1296</v>
       </c>
-      <c r="B563" s="1">
+      <c r="B564" s="1">
         <v>1662</v>
-      </c>
-    </row>
-    <row r="564" spans="1:7" ht="34" x14ac:dyDescent="0.2">
-      <c r="A564" s="1" t="s">
-        <v>1297</v>
-      </c>
-      <c r="B564" s="1" t="s">
-        <v>1280</v>
-      </c>
-      <c r="C564" s="1" t="s">
-        <v>1282</v>
       </c>
     </row>
     <row r="565" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A565" s="1" t="s">
+        <v>1297</v>
+      </c>
+      <c r="B565" s="1" t="s">
+        <v>1280</v>
+      </c>
+      <c r="C565" s="1" t="s">
+        <v>1282</v>
+      </c>
+    </row>
+    <row r="566" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="A566" s="1" t="s">
         <v>1298</v>
       </c>
-      <c r="B565" s="1" t="s">
+      <c r="B566" s="1" t="s">
         <v>1281</v>
       </c>
-      <c r="C565" s="1" t="s">
+      <c r="C566" s="1" t="s">
         <v>1283</v>
       </c>
     </row>
-    <row r="566" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A566" s="1" t="s">
+    <row r="567" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A567" s="1" t="s">
         <v>1299</v>
       </c>
-      <c r="B566" s="1" t="s">
+      <c r="B567" s="1" t="s">
         <v>522</v>
       </c>
-      <c r="C566" s="1" t="s">
+      <c r="C567" s="1" t="s">
         <v>602</v>
       </c>
     </row>
-    <row r="567" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A567" s="10"/>
-      <c r="B567" s="4"/>
-      <c r="C567" s="4"/>
-      <c r="D567" s="4"/>
-      <c r="E567" s="4"/>
-      <c r="F567" s="4"/>
-      <c r="G567" s="4"/>
+    <row r="568" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A568" s="10"/>
+      <c r="B568" s="4"/>
+      <c r="C568" s="4"/>
+      <c r="D568" s="4"/>
+      <c r="E568" s="4"/>
+      <c r="F568" s="4"/>
+      <c r="G568" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Adding svat_ok_activity_start to i18n
</commit_message>
<xml_diff>
--- a/config/i18n/i18n.xlsx
+++ b/config/i18n/i18n.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joana/work/sp-duh/config/i18n/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{936C0947-39B2-C14F-81BB-178572CA6D9C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F06894E5-4D67-7A41-9507-F8B02B33B67E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1390" uniqueCount="1325">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1392" uniqueCount="1327">
   <si>
     <t>key</t>
   </si>
@@ -4061,6 +4061,12 @@
   </si>
   <si>
     <t>Suggestion</t>
+  </si>
+  <si>
+    <t>svat_ok_activity_start</t>
+  </si>
+  <si>
+    <t>Não foi efetuado este teste uma vez que a empresa teve o início de atividade em {0}.</t>
   </si>
 </sst>
 </file>
@@ -4379,7 +4385,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="i18n" displayName="i18n" ref="A1:G567" totalsRowShown="0" headerRowDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="i18n" displayName="i18n" ref="A1:G568" totalsRowShown="0" headerRowDxfId="6">
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="key"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="pt" dataDxfId="5"/>
@@ -4656,10 +4662,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G568"/>
+  <dimension ref="A1:G569"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A421" workbookViewId="0">
-      <selection activeCell="C429" sqref="C429"/>
+    <sheetView tabSelected="1" topLeftCell="A528" workbookViewId="0">
+      <selection activeCell="A543" sqref="A543"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9943,317 +9949,326 @@
       </c>
       <c r="C541" s="8"/>
     </row>
-    <row r="542" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="542" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A542" s="1" t="s">
-        <v>1260</v>
+        <v>1325</v>
       </c>
       <c r="B542" s="1" t="s">
-        <v>1261</v>
-      </c>
-      <c r="C542" s="9" t="s">
-        <v>1262</v>
-      </c>
+        <v>1326</v>
+      </c>
+      <c r="C542" s="8"/>
     </row>
     <row r="543" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A543" s="1" t="s">
+        <v>1260</v>
+      </c>
+      <c r="B543" s="1" t="s">
+        <v>1261</v>
+      </c>
+      <c r="C543" s="9" t="s">
+        <v>1262</v>
+      </c>
+    </row>
+    <row r="544" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A544" s="1" t="s">
         <v>1263</v>
       </c>
-      <c r="B543" s="1" t="s">
+      <c r="B544" s="1" t="s">
         <v>1264</v>
       </c>
-      <c r="C543" s="9" t="s">
+      <c r="C544" s="9" t="s">
         <v>1265</v>
-      </c>
-    </row>
-    <row r="544" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A544" t="s">
-        <v>1248</v>
-      </c>
-      <c r="B544" s="1" t="s">
-        <v>1253</v>
-      </c>
-      <c r="C544" s="1" t="s">
-        <v>956</v>
       </c>
     </row>
     <row r="545" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A545" t="s">
-        <v>1249</v>
+        <v>1248</v>
       </c>
       <c r="B545" s="1" t="s">
-        <v>958</v>
+        <v>1253</v>
       </c>
       <c r="C545" s="1" t="s">
-        <v>953</v>
+        <v>956</v>
       </c>
     </row>
     <row r="546" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A546" t="s">
-        <v>1250</v>
+        <v>1249</v>
       </c>
       <c r="B546" s="1" t="s">
-        <v>1254</v>
+        <v>958</v>
       </c>
       <c r="C546" s="1" t="s">
-        <v>1256</v>
+        <v>953</v>
       </c>
     </row>
     <row r="547" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A547" t="s">
-        <v>1251</v>
+        <v>1250</v>
       </c>
       <c r="B547" s="1" t="s">
-        <v>1255</v>
+        <v>1254</v>
       </c>
       <c r="C547" s="1" t="s">
-        <v>1257</v>
+        <v>1256</v>
       </c>
     </row>
     <row r="548" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A548" t="s">
+        <v>1251</v>
+      </c>
+      <c r="B548" s="1" t="s">
+        <v>1255</v>
+      </c>
+      <c r="C548" s="1" t="s">
+        <v>1257</v>
+      </c>
+    </row>
+    <row r="549" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A549" t="s">
         <v>1252</v>
       </c>
-      <c r="B548" s="4" t="s">
+      <c r="B549" s="4" t="s">
         <v>1046</v>
       </c>
-      <c r="C548" s="4" t="s">
+      <c r="C549" s="4" t="s">
         <v>1258</v>
       </c>
-      <c r="D548" s="4"/>
-      <c r="E548" s="4"/>
-      <c r="F548" s="4"/>
-      <c r="G548" s="4"/>
-    </row>
-    <row r="549" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A549" s="1" t="s">
+      <c r="D549" s="4"/>
+      <c r="E549" s="4"/>
+      <c r="F549" s="4"/>
+      <c r="G549" s="4"/>
+    </row>
+    <row r="550" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A550" s="1" t="s">
         <v>1266</v>
       </c>
-      <c r="B549" s="1" t="s">
+      <c r="B550" s="1" t="s">
         <v>522</v>
       </c>
-      <c r="C549" s="1" t="s">
+      <c r="C550" s="1" t="s">
         <v>523</v>
-      </c>
-    </row>
-    <row r="550" spans="1:7" ht="34" x14ac:dyDescent="0.2">
-      <c r="A550" s="1" t="s">
-        <v>1267</v>
-      </c>
-      <c r="B550" s="1" t="s">
-        <v>1304</v>
-      </c>
-      <c r="C550" s="1" t="s">
-        <v>1305</v>
       </c>
     </row>
     <row r="551" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A551" s="1" t="s">
+        <v>1267</v>
+      </c>
+      <c r="B551" s="1" t="s">
+        <v>1304</v>
+      </c>
+      <c r="C551" s="1" t="s">
+        <v>1305</v>
+      </c>
+    </row>
+    <row r="552" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="A552" s="1" t="s">
         <v>1268</v>
       </c>
-      <c r="B551" s="1" t="s">
+      <c r="B552" s="1" t="s">
         <v>1306</v>
       </c>
-      <c r="C551" s="1" t="s">
+      <c r="C552" s="1" t="s">
         <v>1307</v>
       </c>
     </row>
-    <row r="552" spans="1:7" ht="34" x14ac:dyDescent="0.2">
-      <c r="A552" s="11" t="s">
+    <row r="553" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="A553" s="11" t="s">
         <v>1269</v>
       </c>
-      <c r="B552" s="7" t="s">
+      <c r="B553" s="7" t="s">
         <v>1280</v>
       </c>
-      <c r="C552" s="7" t="s">
+      <c r="C553" s="7" t="s">
         <v>1282</v>
       </c>
-      <c r="D552" s="7"/>
-      <c r="E552" s="7"/>
-      <c r="F552" s="7"/>
-      <c r="G552" s="12"/>
-    </row>
-    <row r="553" spans="1:7" ht="34" x14ac:dyDescent="0.2">
-      <c r="A553" s="13" t="s">
+      <c r="D553" s="7"/>
+      <c r="E553" s="7"/>
+      <c r="F553" s="7"/>
+      <c r="G553" s="12"/>
+    </row>
+    <row r="554" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="A554" s="13" t="s">
         <v>1270</v>
       </c>
-      <c r="B553" s="14" t="s">
+      <c r="B554" s="14" t="s">
         <v>1281</v>
       </c>
-      <c r="C553" s="14" t="s">
+      <c r="C554" s="14" t="s">
         <v>1283</v>
       </c>
-      <c r="D553" s="14"/>
-      <c r="E553" s="14"/>
-      <c r="F553" s="14"/>
-      <c r="G553" s="15"/>
-    </row>
-    <row r="554" spans="1:7" ht="34" x14ac:dyDescent="0.2">
-      <c r="A554" s="11" t="s">
+      <c r="D554" s="14"/>
+      <c r="E554" s="14"/>
+      <c r="F554" s="14"/>
+      <c r="G554" s="15"/>
+    </row>
+    <row r="555" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="A555" s="11" t="s">
         <v>1271</v>
       </c>
-      <c r="B554" s="7" t="s">
+      <c r="B555" s="7" t="s">
         <v>522</v>
       </c>
-      <c r="C554" s="7" t="s">
+      <c r="C555" s="7" t="s">
         <v>602</v>
       </c>
-      <c r="D554" s="7"/>
-      <c r="E554" s="7"/>
-      <c r="F554" s="7"/>
-      <c r="G554" s="12"/>
-    </row>
-    <row r="555" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A555" t="s">
-        <v>1284</v>
-      </c>
-      <c r="B555" s="16" t="s">
-        <v>1272</v>
-      </c>
-      <c r="C555" s="16" t="s">
-        <v>1272</v>
-      </c>
+      <c r="D555" s="7"/>
+      <c r="E555" s="7"/>
+      <c r="F555" s="7"/>
+      <c r="G555" s="12"/>
     </row>
     <row r="556" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A556" t="s">
+        <v>1284</v>
+      </c>
+      <c r="B556" s="16" t="s">
+        <v>1272</v>
+      </c>
+      <c r="C556" s="16" t="s">
+        <v>1272</v>
+      </c>
+    </row>
+    <row r="557" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A557" t="s">
         <v>1285</v>
       </c>
-      <c r="B556" s="16" t="s">
+      <c r="B557" s="16" t="s">
         <v>1286</v>
       </c>
-      <c r="C556" s="16" t="s">
+      <c r="C557" s="16" t="s">
         <v>1286</v>
       </c>
     </row>
-    <row r="557" spans="1:7" ht="34" x14ac:dyDescent="0.2">
-      <c r="A557" s="11" t="s">
+    <row r="558" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="A558" s="11" t="s">
         <v>1273</v>
       </c>
-      <c r="B557" s="7" t="s">
+      <c r="B558" s="7" t="s">
         <v>1287</v>
       </c>
-      <c r="C557" s="7" t="s">
+      <c r="C558" s="7" t="s">
         <v>1294</v>
       </c>
-      <c r="D557" s="4"/>
-      <c r="E557" s="4"/>
-      <c r="F557" s="4"/>
-      <c r="G557" s="4"/>
-    </row>
-    <row r="558" spans="1:7" ht="34" x14ac:dyDescent="0.2">
-      <c r="A558" s="13" t="s">
+      <c r="D558" s="4"/>
+      <c r="E558" s="4"/>
+      <c r="F558" s="4"/>
+      <c r="G558" s="4"/>
+    </row>
+    <row r="559" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="A559" s="13" t="s">
         <v>1274</v>
       </c>
-      <c r="B558" s="14" t="s">
+      <c r="B559" s="14" t="s">
         <v>1288</v>
       </c>
-      <c r="C558" s="14" t="s">
+      <c r="C559" s="14" t="s">
         <v>1293</v>
-      </c>
-    </row>
-    <row r="559" spans="1:7" ht="34" x14ac:dyDescent="0.2">
-      <c r="A559" s="11" t="s">
-        <v>1275</v>
-      </c>
-      <c r="B559" s="1" t="s">
-        <v>1304</v>
-      </c>
-      <c r="C559" s="1" t="s">
-        <v>1308</v>
       </c>
     </row>
     <row r="560" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A560" s="11" t="s">
+        <v>1275</v>
+      </c>
+      <c r="B560" s="1" t="s">
+        <v>1304</v>
+      </c>
+      <c r="C560" s="1" t="s">
+        <v>1308</v>
+      </c>
+    </row>
+    <row r="561" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="A561" s="11" t="s">
         <v>1276</v>
       </c>
-      <c r="B560" s="7" t="s">
+      <c r="B561" s="7" t="s">
         <v>1289</v>
       </c>
-      <c r="C560" s="7" t="s">
+      <c r="C561" s="7" t="s">
         <v>1292</v>
       </c>
     </row>
-    <row r="561" spans="1:7" ht="34" x14ac:dyDescent="0.2">
-      <c r="A561" s="13" t="s">
+    <row r="562" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="A562" s="13" t="s">
         <v>1277</v>
       </c>
-      <c r="B561" s="14" t="s">
+      <c r="B562" s="14" t="s">
         <v>1290</v>
       </c>
-      <c r="C561" s="14" t="s">
+      <c r="C562" s="14" t="s">
         <v>1291</v>
       </c>
     </row>
-    <row r="562" spans="1:7" ht="34" x14ac:dyDescent="0.2">
-      <c r="A562" s="11" t="s">
+    <row r="563" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="A563" s="11" t="s">
         <v>1278</v>
       </c>
-      <c r="B562" s="1" t="s">
+      <c r="B563" s="1" t="s">
         <v>1306</v>
       </c>
-      <c r="C562" s="1" t="s">
+      <c r="C563" s="1" t="s">
         <v>1309</v>
-      </c>
-    </row>
-    <row r="563" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A563" s="1" t="s">
-        <v>1295</v>
-      </c>
-      <c r="B563" s="1" t="s">
-        <v>522</v>
-      </c>
-      <c r="C563" s="1" t="s">
-        <v>523</v>
       </c>
     </row>
     <row r="564" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A564" s="1" t="s">
+        <v>1295</v>
+      </c>
+      <c r="B564" s="1" t="s">
+        <v>522</v>
+      </c>
+      <c r="C564" s="1" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="565" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A565" s="1" t="s">
         <v>1296</v>
       </c>
-      <c r="B564" s="1">
+      <c r="B565" s="1">
         <v>1662</v>
-      </c>
-    </row>
-    <row r="565" spans="1:7" ht="34" x14ac:dyDescent="0.2">
-      <c r="A565" s="1" t="s">
-        <v>1297</v>
-      </c>
-      <c r="B565" s="1" t="s">
-        <v>1280</v>
-      </c>
-      <c r="C565" s="1" t="s">
-        <v>1282</v>
       </c>
     </row>
     <row r="566" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A566" s="1" t="s">
+        <v>1297</v>
+      </c>
+      <c r="B566" s="1" t="s">
+        <v>1280</v>
+      </c>
+      <c r="C566" s="1" t="s">
+        <v>1282</v>
+      </c>
+    </row>
+    <row r="567" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="A567" s="1" t="s">
         <v>1298</v>
       </c>
-      <c r="B566" s="1" t="s">
+      <c r="B567" s="1" t="s">
         <v>1281</v>
       </c>
-      <c r="C566" s="1" t="s">
+      <c r="C567" s="1" t="s">
         <v>1283</v>
       </c>
     </row>
-    <row r="567" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A567" s="1" t="s">
+    <row r="568" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A568" s="1" t="s">
         <v>1299</v>
       </c>
-      <c r="B567" s="1" t="s">
+      <c r="B568" s="1" t="s">
         <v>522</v>
       </c>
-      <c r="C567" s="1" t="s">
+      <c r="C568" s="1" t="s">
         <v>602</v>
       </c>
     </row>
-    <row r="568" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A568" s="10"/>
-      <c r="B568" s="4"/>
-      <c r="C568" s="4"/>
-      <c r="D568" s="4"/>
-      <c r="E568" s="4"/>
-      <c r="F568" s="4"/>
-      <c r="G568" s="4"/>
+    <row r="569" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A569" s="10"/>
+      <c r="B569" s="4"/>
+      <c r="C569" s="4"/>
+      <c r="D569" s="4"/>
+      <c r="E569" s="4"/>
+      <c r="F569" s="4"/>
+      <c r="G569" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added translations for suggestion_type
</commit_message>
<xml_diff>
--- a/config/i18n/i18n.xlsx
+++ b/config/i18n/i18n.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10309"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joana/work/sp-duh/config/i18n/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/falves/work/sp-duh/config/i18n/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F06894E5-4D67-7A41-9507-F8B02B33B67E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3D66D9A-C068-0E48-8244-0831413D8DF1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-660" yWindow="-21600" windowWidth="38400" windowHeight="21600" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1392" uniqueCount="1327">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1422" uniqueCount="1355">
   <si>
     <t>key</t>
   </si>
@@ -4067,6 +4067,90 @@
   </si>
   <si>
     <t>Não foi efetuado este teste uma vez que a empresa teve o início de atividade em {0}.</t>
+  </si>
+  <si>
+    <t>accounting_suggestion_type_manual</t>
+  </si>
+  <si>
+    <t>accounting_suggestion_type_reverse</t>
+  </si>
+  <si>
+    <t>accounting_suggestion_type_sales</t>
+  </si>
+  <si>
+    <t>accounting_suggestion_type_purchases</t>
+  </si>
+  <si>
+    <t>accounting_suggestion_type_banks</t>
+  </si>
+  <si>
+    <t>accounting_suggestion_type_payrolls</t>
+  </si>
+  <si>
+    <t>accounting_suggestion_type_fixedassets</t>
+  </si>
+  <si>
+    <t>accounting_suggestion_type_stocks</t>
+  </si>
+  <si>
+    <t>accounting_suggestion_type_opening</t>
+  </si>
+  <si>
+    <t>accounting_suggestion_type_automatic_balance</t>
+  </si>
+  <si>
+    <t>Manual</t>
+  </si>
+  <si>
+    <t>Estorno</t>
+  </si>
+  <si>
+    <t>Vendas</t>
+  </si>
+  <si>
+    <t>Compras</t>
+  </si>
+  <si>
+    <t>Bancos</t>
+  </si>
+  <si>
+    <t>Salários</t>
+  </si>
+  <si>
+    <t>Ativos</t>
+  </si>
+  <si>
+    <t>Stocks</t>
+  </si>
+  <si>
+    <t>Abertura</t>
+  </si>
+  <si>
+    <t>Apuramento e Fecho</t>
+  </si>
+  <si>
+    <t>Reverse</t>
+  </si>
+  <si>
+    <t>Sales</t>
+  </si>
+  <si>
+    <t>Purchases</t>
+  </si>
+  <si>
+    <t>Banks</t>
+  </si>
+  <si>
+    <t>Payrolls</t>
+  </si>
+  <si>
+    <t>Fixed Assets</t>
+  </si>
+  <si>
+    <t>Opening</t>
+  </si>
+  <si>
+    <t>Automatic Balance</t>
   </si>
 </sst>
 </file>
@@ -4385,7 +4469,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="i18n" displayName="i18n" ref="A1:G568" totalsRowShown="0" headerRowDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="i18n" displayName="i18n" ref="A1:G578" totalsRowShown="0" headerRowDxfId="6">
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="key"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="pt" dataDxfId="5"/>
@@ -4662,10 +4746,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G569"/>
+  <dimension ref="A1:G578"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A528" workbookViewId="0">
-      <selection activeCell="A543" sqref="A543"/>
+    <sheetView tabSelected="1" topLeftCell="A558" workbookViewId="0">
+      <selection activeCell="A579" sqref="A579"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10261,14 +10345,119 @@
         <v>602</v>
       </c>
     </row>
-    <row r="569" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A569" s="10"/>
-      <c r="B569" s="4"/>
-      <c r="C569" s="4"/>
+    <row r="569" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A569" s="10" t="s">
+        <v>1327</v>
+      </c>
+      <c r="B569" s="4" t="s">
+        <v>1337</v>
+      </c>
+      <c r="C569" s="4" t="s">
+        <v>1337</v>
+      </c>
       <c r="D569" s="4"/>
       <c r="E569" s="4"/>
       <c r="F569" s="4"/>
       <c r="G569" s="4"/>
+    </row>
+    <row r="570" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A570" t="s">
+        <v>1328</v>
+      </c>
+      <c r="B570" s="1" t="s">
+        <v>1338</v>
+      </c>
+      <c r="C570" s="1" t="s">
+        <v>1347</v>
+      </c>
+    </row>
+    <row r="571" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A571" t="s">
+        <v>1329</v>
+      </c>
+      <c r="B571" s="1" t="s">
+        <v>1339</v>
+      </c>
+      <c r="C571" s="1" t="s">
+        <v>1348</v>
+      </c>
+    </row>
+    <row r="572" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A572" t="s">
+        <v>1330</v>
+      </c>
+      <c r="B572" s="1" t="s">
+        <v>1340</v>
+      </c>
+      <c r="C572" s="1" t="s">
+        <v>1349</v>
+      </c>
+    </row>
+    <row r="573" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A573" t="s">
+        <v>1331</v>
+      </c>
+      <c r="B573" s="1" t="s">
+        <v>1341</v>
+      </c>
+      <c r="C573" s="1" t="s">
+        <v>1350</v>
+      </c>
+    </row>
+    <row r="574" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A574" t="s">
+        <v>1332</v>
+      </c>
+      <c r="B574" s="1" t="s">
+        <v>1342</v>
+      </c>
+      <c r="C574" s="1" t="s">
+        <v>1351</v>
+      </c>
+    </row>
+    <row r="575" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A575" t="s">
+        <v>1333</v>
+      </c>
+      <c r="B575" s="1" t="s">
+        <v>1343</v>
+      </c>
+      <c r="C575" s="1" t="s">
+        <v>1352</v>
+      </c>
+    </row>
+    <row r="576" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A576" t="s">
+        <v>1334</v>
+      </c>
+      <c r="B576" s="1" t="s">
+        <v>1344</v>
+      </c>
+      <c r="C576" s="1" t="s">
+        <v>1344</v>
+      </c>
+    </row>
+    <row r="577" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A577" t="s">
+        <v>1335</v>
+      </c>
+      <c r="B577" s="1" t="s">
+        <v>1345</v>
+      </c>
+      <c r="C577" s="1" t="s">
+        <v>1353</v>
+      </c>
+    </row>
+    <row r="578" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A578" t="s">
+        <v>1336</v>
+      </c>
+      <c r="B578" s="1" t="s">
+        <v>1346</v>
+      </c>
+      <c r="C578" s="1" t="s">
+        <v>1354</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Fixing description for rules related with activity start Luisa & JAN
</commit_message>
<xml_diff>
--- a/config/i18n/i18n.xlsx
+++ b/config/i18n/i18n.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10309"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10209"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/falves/work/sp-duh/config/i18n/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joana/work/sp-duh/config/i18n/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3D66D9A-C068-0E48-8244-0831413D8DF1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E13A870B-0098-0443-9C8B-DC2C7FB64A68}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-660" yWindow="-21600" windowWidth="38400" windowHeight="21600" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-620" yWindow="-30800" windowWidth="38360" windowHeight="30800" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -3574,9 +3574,6 @@
     <t>Verificamos que não existe nenhum movimento de apuramento de resultado líquido, ou se existir não está registado no diário correto. Por favor verifique se deve fazer este movimento ou se deve registar o mesmo no diário correto de apuramento de resultados. Alertamos para a FAQ 15-2887, que refere que em entidades com atividade, este movimento tem sempre de existir, ainda que tenha valor "0,00" (zero)</t>
   </si>
   <si>
-    <t>Verificamos que não existe nenhum movimento de aplicação de resultados. Confirme por favor se não deverá efetuar esse movimento. Alertamos para a FAQ 14-2886, que refere que em entidades com atividade, este movimento tem sempre de existir, ainda que tenha valor "0,00" (zero)</t>
-  </si>
-  <si>
     <t>O movimento de apuramento de resultado líquido tem de ser efetuado em diário próprio, para uma correta identificação no ficheiro SAF-T (PT). Verificamos que os seguintes lançamentos estão registados em diário tipificado como apuramento e movimentam contas não expectáveis:</t>
   </si>
   <si>
@@ -3607,9 +3604,6 @@
     <t xml:space="preserve">Verificamos que existe mais do que um movimento de abertura. Por favor verifique se os seguintes registos estão corretos: </t>
   </si>
   <si>
-    <t>Verificamos que não existe nenhum movimento de abertura, ou se existir não está registado no diário correto. Por favor verifique se deve fazer este movimento ou se deve registar o mesmo em outro diário.</t>
-  </si>
-  <si>
     <t>Verificamos que o movimento de aplicação de resultados foi registado até 31 de Março {0}. Teste realizado com sucesso.</t>
   </si>
   <si>
@@ -4066,9 +4060,6 @@
     <t>svat_ok_activity_start</t>
   </si>
   <si>
-    <t>Não foi efetuado este teste uma vez que a empresa teve o início de atividade em {0}.</t>
-  </si>
-  <si>
     <t>accounting_suggestion_type_manual</t>
   </si>
   <si>
@@ -4151,6 +4142,15 @@
   </si>
   <si>
     <t>Automatic Balance</t>
+  </si>
+  <si>
+    <t>Não foi efetuado este teste, uma vez que está definido na ficha da empresa que data de início de atividade da entidade é {0}.</t>
+  </si>
+  <si>
+    <t>Verificamos que não existe nenhum movimento de aplicação de resultados. Confirme por favor se não deverá efetuar esse movimento. Alertamos para a FAQ no portal das finanças que refere que em entidades com atividade, este movimento tem sempre de existir, ainda que tenha valor “0,00” (zero). Poderá ainda definir na ficha da empresa informação sobre a data de início de atividade.</t>
+  </si>
+  <si>
+    <t>Verificamos que não existe nenhum movimento de abertura, ou se existir não está registado no diário correto. Por favor verifique se deve fazer este movimento ou se deve registar o mesmo em outro diário. Poderá ainda definir na ficha da empresa informação sobre a data de início de atividade.</t>
   </si>
 </sst>
 </file>
@@ -4748,8 +4748,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G578"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A558" workbookViewId="0">
-      <selection activeCell="A579" sqref="A579"/>
+    <sheetView tabSelected="1" topLeftCell="A479" workbookViewId="0">
+      <selection activeCell="B498" sqref="B498"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7525,7 +7525,7 @@
         <v>832</v>
       </c>
       <c r="C318" s="1" t="s">
-        <v>1259</v>
+        <v>1257</v>
       </c>
     </row>
     <row r="319" spans="1:3" ht="68" x14ac:dyDescent="0.2">
@@ -7566,10 +7566,10 @@
         <v>846</v>
       </c>
       <c r="B322" s="1" t="s">
-        <v>1301</v>
+        <v>1299</v>
       </c>
       <c r="C322" s="1" t="s">
-        <v>1300</v>
+        <v>1298</v>
       </c>
     </row>
     <row r="323" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -7577,10 +7577,10 @@
         <v>847</v>
       </c>
       <c r="B323" s="1" t="s">
-        <v>1303</v>
+        <v>1301</v>
       </c>
       <c r="C323" s="1" t="s">
-        <v>1302</v>
+        <v>1300</v>
       </c>
     </row>
     <row r="324" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -8908,13 +8908,13 @@
     </row>
     <row r="429" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A429" t="s">
-        <v>1323</v>
+        <v>1321</v>
       </c>
       <c r="B429" s="1" t="s">
+        <v>1320</v>
+      </c>
+      <c r="C429" s="1" t="s">
         <v>1322</v>
-      </c>
-      <c r="C429" s="1" t="s">
-        <v>1324</v>
       </c>
     </row>
     <row r="430" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -9462,7 +9462,7 @@
         <v>1133</v>
       </c>
       <c r="B478" s="1" t="s">
-        <v>1190</v>
+        <v>1188</v>
       </c>
       <c r="C478" s="8"/>
     </row>
@@ -9489,7 +9489,7 @@
         <v>1134</v>
       </c>
       <c r="B481" s="1" t="s">
-        <v>1191</v>
+        <v>1189</v>
       </c>
       <c r="C481" s="8"/>
     </row>
@@ -9498,7 +9498,7 @@
         <v>1139</v>
       </c>
       <c r="B482" s="1" t="s">
-        <v>1163</v>
+        <v>1162</v>
       </c>
       <c r="C482" s="8"/>
     </row>
@@ -9516,7 +9516,7 @@
         <v>1135</v>
       </c>
       <c r="B484" s="1" t="s">
-        <v>1164</v>
+        <v>1163</v>
       </c>
       <c r="C484" s="8"/>
     </row>
@@ -9534,7 +9534,7 @@
         <v>1152</v>
       </c>
       <c r="B486" s="1" t="s">
-        <v>1165</v>
+        <v>1164</v>
       </c>
       <c r="C486" s="8"/>
     </row>
@@ -9543,25 +9543,25 @@
         <v>1136</v>
       </c>
       <c r="B487" s="1" t="s">
-        <v>1166</v>
+        <v>1165</v>
       </c>
       <c r="C487" s="8"/>
     </row>
-    <row r="488" spans="1:3" ht="102" x14ac:dyDescent="0.2">
+    <row r="488" spans="1:3" ht="136" x14ac:dyDescent="0.2">
       <c r="A488" s="1" t="s">
         <v>1141</v>
       </c>
       <c r="B488" s="1" t="s">
-        <v>1162</v>
-      </c>
-      <c r="C488" s="8"/>
+        <v>1353</v>
+      </c>
+      <c r="C488" s="9"/>
     </row>
     <row r="489" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A489" s="1" t="s">
         <v>1153</v>
       </c>
       <c r="B489" s="1" t="s">
-        <v>1165</v>
+        <v>1164</v>
       </c>
       <c r="C489" s="8"/>
     </row>
@@ -9570,7 +9570,7 @@
         <v>1137</v>
       </c>
       <c r="B490" s="1" t="s">
-        <v>1174</v>
+        <v>1172</v>
       </c>
       <c r="C490" s="8"/>
     </row>
@@ -9579,7 +9579,7 @@
         <v>1142</v>
       </c>
       <c r="B491" s="1" t="s">
-        <v>1177</v>
+        <v>1175</v>
       </c>
       <c r="C491" s="8"/>
     </row>
@@ -9588,7 +9588,7 @@
         <v>1154</v>
       </c>
       <c r="B492" s="1" t="s">
-        <v>1167</v>
+        <v>1166</v>
       </c>
       <c r="C492" s="8"/>
     </row>
@@ -9597,7 +9597,7 @@
         <v>1143</v>
       </c>
       <c r="B493" s="1" t="s">
-        <v>1175</v>
+        <v>1173</v>
       </c>
       <c r="C493" s="8"/>
     </row>
@@ -9606,7 +9606,7 @@
         <v>1144</v>
       </c>
       <c r="B494" s="1" t="s">
-        <v>1168</v>
+        <v>1167</v>
       </c>
       <c r="C494" s="8"/>
     </row>
@@ -9615,7 +9615,7 @@
         <v>1155</v>
       </c>
       <c r="B495" s="1" t="s">
-        <v>1167</v>
+        <v>1166</v>
       </c>
       <c r="C495" s="8"/>
     </row>
@@ -9624,34 +9624,34 @@
         <v>1145</v>
       </c>
       <c r="B496" s="1" t="s">
-        <v>1176</v>
+        <v>1174</v>
       </c>
       <c r="C496" s="8"/>
     </row>
     <row r="497" spans="1:3" ht="51" x14ac:dyDescent="0.2">
       <c r="A497" s="1" t="s">
+        <v>1169</v>
+      </c>
+      <c r="B497" s="1" t="s">
+        <v>1171</v>
+      </c>
+      <c r="C497" s="8"/>
+    </row>
+    <row r="498" spans="1:3" ht="102" x14ac:dyDescent="0.2">
+      <c r="A498" s="1" t="s">
         <v>1170</v>
       </c>
-      <c r="B497" s="1" t="s">
-        <v>1172</v>
-      </c>
-      <c r="C497" s="8"/>
-    </row>
-    <row r="498" spans="1:3" ht="85" x14ac:dyDescent="0.2">
-      <c r="A498" s="1" t="s">
-        <v>1171</v>
-      </c>
       <c r="B498" s="1" t="s">
-        <v>1173</v>
-      </c>
-      <c r="C498" s="8"/>
+        <v>1354</v>
+      </c>
+      <c r="C498" s="9"/>
     </row>
     <row r="499" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A499" s="1" t="s">
         <v>1156</v>
       </c>
       <c r="B499" s="1" t="s">
-        <v>1169</v>
+        <v>1168</v>
       </c>
       <c r="C499" s="8"/>
     </row>
@@ -9660,16 +9660,16 @@
         <v>1146</v>
       </c>
       <c r="B500" s="1" t="s">
-        <v>1211</v>
+        <v>1209</v>
       </c>
       <c r="C500" s="8"/>
     </row>
     <row r="501" spans="1:3" ht="68" x14ac:dyDescent="0.2">
       <c r="A501" s="1" t="s">
-        <v>1210</v>
+        <v>1208</v>
       </c>
       <c r="B501" s="1" t="s">
-        <v>1279</v>
+        <v>1277</v>
       </c>
       <c r="C501" s="8"/>
     </row>
@@ -9678,398 +9678,398 @@
         <v>1147</v>
       </c>
       <c r="B502" s="1" t="s">
-        <v>1212</v>
+        <v>1210</v>
       </c>
       <c r="C502" s="8"/>
     </row>
     <row r="503" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A503" s="1" t="s">
-        <v>1213</v>
+        <v>1211</v>
       </c>
       <c r="B503" s="1" t="s">
-        <v>1225</v>
+        <v>1223</v>
       </c>
       <c r="C503" s="8"/>
     </row>
     <row r="504" spans="1:3" ht="51" x14ac:dyDescent="0.2">
       <c r="A504" s="1" t="s">
-        <v>1214</v>
+        <v>1212</v>
       </c>
       <c r="B504" s="1" t="s">
-        <v>1227</v>
+        <v>1225</v>
       </c>
       <c r="C504" s="8"/>
     </row>
     <row r="505" spans="1:3" ht="68" x14ac:dyDescent="0.2">
       <c r="A505" s="1" t="s">
-        <v>1215</v>
+        <v>1213</v>
       </c>
       <c r="B505" s="1" t="s">
-        <v>1228</v>
+        <v>1226</v>
       </c>
       <c r="C505" s="8"/>
     </row>
     <row r="506" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A506" s="1" t="s">
-        <v>1216</v>
+        <v>1214</v>
       </c>
       <c r="B506" s="1" t="s">
-        <v>1226</v>
+        <v>1224</v>
       </c>
       <c r="C506" s="8"/>
     </row>
     <row r="507" spans="1:3" ht="51" x14ac:dyDescent="0.2">
       <c r="A507" s="1" t="s">
-        <v>1217</v>
+        <v>1215</v>
       </c>
       <c r="B507" s="1" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="C507" s="8"/>
     </row>
     <row r="508" spans="1:3" ht="68" x14ac:dyDescent="0.2">
       <c r="A508" s="1" t="s">
-        <v>1218</v>
+        <v>1216</v>
       </c>
       <c r="B508" s="1" t="s">
-        <v>1230</v>
+        <v>1228</v>
       </c>
       <c r="C508" s="8"/>
     </row>
     <row r="509" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A509" s="1" t="s">
-        <v>1219</v>
+        <v>1217</v>
       </c>
       <c r="B509" s="1" t="s">
-        <v>1231</v>
+        <v>1229</v>
       </c>
       <c r="C509" s="8"/>
     </row>
     <row r="510" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A510" s="1" t="s">
-        <v>1220</v>
+        <v>1218</v>
       </c>
       <c r="B510" s="1" t="s">
-        <v>1232</v>
+        <v>1230</v>
       </c>
       <c r="C510" s="8"/>
     </row>
     <row r="511" spans="1:3" ht="85" x14ac:dyDescent="0.2">
       <c r="A511" s="1" t="s">
-        <v>1221</v>
+        <v>1219</v>
       </c>
       <c r="B511" s="1" t="s">
-        <v>1233</v>
+        <v>1231</v>
       </c>
       <c r="C511" s="8"/>
     </row>
     <row r="512" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A512" s="1" t="s">
-        <v>1239</v>
+        <v>1237</v>
       </c>
       <c r="B512" s="1" t="s">
-        <v>1234</v>
+        <v>1232</v>
       </c>
       <c r="C512" s="8"/>
     </row>
     <row r="513" spans="1:3" ht="102" x14ac:dyDescent="0.2">
       <c r="A513" s="1" t="s">
-        <v>1241</v>
+        <v>1239</v>
       </c>
       <c r="B513" s="1" t="s">
-        <v>1245</v>
+        <v>1243</v>
       </c>
       <c r="C513" s="8"/>
     </row>
     <row r="514" spans="1:3" ht="119" x14ac:dyDescent="0.2">
       <c r="A514" s="1" t="s">
-        <v>1242</v>
+        <v>1240</v>
       </c>
       <c r="B514" s="1" t="s">
-        <v>1247</v>
+        <v>1245</v>
       </c>
       <c r="C514" s="8"/>
     </row>
     <row r="515" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A515" s="1" t="s">
-        <v>1240</v>
+        <v>1238</v>
       </c>
       <c r="B515" s="1" t="s">
-        <v>1234</v>
+        <v>1232</v>
       </c>
       <c r="C515" s="8"/>
     </row>
     <row r="516" spans="1:3" ht="119" x14ac:dyDescent="0.2">
       <c r="A516" s="1" t="s">
-        <v>1243</v>
+        <v>1241</v>
       </c>
       <c r="B516" s="1" t="s">
-        <v>1246</v>
+        <v>1244</v>
       </c>
       <c r="C516" s="8"/>
     </row>
     <row r="517" spans="1:3" ht="119" x14ac:dyDescent="0.2">
       <c r="A517" s="1" t="s">
-        <v>1244</v>
+        <v>1242</v>
       </c>
       <c r="B517" s="1" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
       <c r="C517" s="8"/>
     </row>
     <row r="518" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A518" s="1" t="s">
-        <v>1222</v>
+        <v>1220</v>
       </c>
       <c r="B518" s="1" t="s">
-        <v>1236</v>
+        <v>1234</v>
       </c>
       <c r="C518" s="8"/>
     </row>
     <row r="519" spans="1:3" ht="102" x14ac:dyDescent="0.2">
       <c r="A519" s="1" t="s">
-        <v>1223</v>
+        <v>1221</v>
       </c>
       <c r="B519" s="1" t="s">
-        <v>1237</v>
+        <v>1235</v>
       </c>
       <c r="C519" s="8"/>
     </row>
     <row r="520" spans="1:3" ht="85" x14ac:dyDescent="0.2">
       <c r="A520" s="1" t="s">
-        <v>1224</v>
+        <v>1222</v>
       </c>
       <c r="B520" s="1" t="s">
-        <v>1238</v>
+        <v>1236</v>
       </c>
       <c r="C520" s="8"/>
     </row>
     <row r="521" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A521" s="1" t="s">
-        <v>1179</v>
+        <v>1177</v>
       </c>
       <c r="B521" s="1" t="s">
-        <v>1178</v>
+        <v>1176</v>
       </c>
       <c r="C521" s="8"/>
     </row>
     <row r="522" spans="1:3" ht="68" x14ac:dyDescent="0.2">
       <c r="A522" s="1" t="s">
-        <v>1180</v>
+        <v>1178</v>
       </c>
       <c r="B522" s="1" t="s">
-        <v>1185</v>
+        <v>1183</v>
       </c>
       <c r="C522" s="8"/>
     </row>
     <row r="523" spans="1:3" ht="102" x14ac:dyDescent="0.2">
       <c r="A523" s="1" t="s">
-        <v>1181</v>
+        <v>1179</v>
       </c>
       <c r="B523" s="1" t="s">
-        <v>1186</v>
+        <v>1184</v>
       </c>
       <c r="C523" s="8"/>
     </row>
     <row r="524" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A524" s="1" t="s">
-        <v>1182</v>
+        <v>1180</v>
       </c>
       <c r="B524" s="1" t="s">
-        <v>1187</v>
+        <v>1185</v>
       </c>
       <c r="C524" s="8"/>
     </row>
     <row r="525" spans="1:3" ht="68" x14ac:dyDescent="0.2">
       <c r="A525" s="1" t="s">
-        <v>1183</v>
+        <v>1181</v>
       </c>
       <c r="B525" s="1" t="s">
-        <v>1188</v>
+        <v>1186</v>
       </c>
       <c r="C525" s="8"/>
     </row>
     <row r="526" spans="1:3" ht="102" x14ac:dyDescent="0.2">
       <c r="A526" s="1" t="s">
-        <v>1184</v>
+        <v>1182</v>
       </c>
       <c r="B526" s="1" t="s">
-        <v>1189</v>
+        <v>1187</v>
       </c>
       <c r="C526" s="8"/>
     </row>
     <row r="527" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A527" s="1" t="s">
-        <v>1192</v>
+        <v>1190</v>
       </c>
       <c r="B527" s="1" t="s">
-        <v>1201</v>
+        <v>1199</v>
       </c>
       <c r="C527" s="8"/>
     </row>
     <row r="528" spans="1:3" ht="68" x14ac:dyDescent="0.2">
       <c r="A528" s="1" t="s">
-        <v>1193</v>
+        <v>1191</v>
       </c>
       <c r="B528" s="1" t="s">
-        <v>1202</v>
+        <v>1200</v>
       </c>
       <c r="C528" s="8"/>
     </row>
     <row r="529" spans="1:3" ht="68" x14ac:dyDescent="0.2">
       <c r="A529" s="1" t="s">
-        <v>1194</v>
+        <v>1192</v>
       </c>
       <c r="B529" s="1" t="s">
-        <v>1203</v>
+        <v>1201</v>
       </c>
       <c r="C529" s="8"/>
     </row>
     <row r="530" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A530" s="1" t="s">
-        <v>1195</v>
+        <v>1193</v>
       </c>
       <c r="B530" s="1" t="s">
-        <v>1204</v>
+        <v>1202</v>
       </c>
       <c r="C530" s="8"/>
     </row>
     <row r="531" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A531" s="1" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="B531" s="1" t="s">
-        <v>1205</v>
+        <v>1203</v>
       </c>
       <c r="C531" s="8"/>
     </row>
     <row r="532" spans="1:3" ht="51" x14ac:dyDescent="0.2">
       <c r="A532" s="1" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="B532" s="1" t="s">
-        <v>1206</v>
+        <v>1204</v>
       </c>
       <c r="C532" s="8"/>
     </row>
     <row r="533" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A533" s="1" t="s">
-        <v>1198</v>
+        <v>1196</v>
       </c>
       <c r="B533" s="1" t="s">
-        <v>1207</v>
+        <v>1205</v>
       </c>
       <c r="C533" s="8"/>
     </row>
     <row r="534" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A534" s="1" t="s">
-        <v>1199</v>
+        <v>1197</v>
       </c>
       <c r="B534" s="1" t="s">
-        <v>1208</v>
+        <v>1206</v>
       </c>
       <c r="C534" s="8"/>
     </row>
     <row r="535" spans="1:3" ht="51" x14ac:dyDescent="0.2">
       <c r="A535" s="1" t="s">
-        <v>1200</v>
+        <v>1198</v>
       </c>
       <c r="B535" s="1" t="s">
-        <v>1209</v>
+        <v>1207</v>
       </c>
       <c r="C535" s="8"/>
     </row>
     <row r="536" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A536" s="1" t="s">
-        <v>1316</v>
+        <v>1314</v>
       </c>
       <c r="B536" s="1" t="s">
-        <v>1310</v>
+        <v>1308</v>
       </c>
       <c r="C536" s="8"/>
     </row>
     <row r="537" spans="1:3" ht="51" x14ac:dyDescent="0.2">
       <c r="A537" s="1" t="s">
-        <v>1317</v>
+        <v>1315</v>
       </c>
       <c r="B537" s="1" t="s">
-        <v>1312</v>
+        <v>1310</v>
       </c>
       <c r="C537" s="8"/>
     </row>
     <row r="538" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A538" s="1" t="s">
-        <v>1318</v>
+        <v>1316</v>
       </c>
       <c r="B538" s="1" t="s">
-        <v>1313</v>
+        <v>1311</v>
       </c>
       <c r="C538" s="8"/>
     </row>
     <row r="539" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A539" s="1" t="s">
-        <v>1319</v>
+        <v>1317</v>
       </c>
       <c r="B539" s="1" t="s">
-        <v>1311</v>
+        <v>1309</v>
       </c>
       <c r="C539" s="8"/>
     </row>
     <row r="540" spans="1:3" ht="51" x14ac:dyDescent="0.2">
       <c r="A540" s="1" t="s">
-        <v>1320</v>
+        <v>1318</v>
       </c>
       <c r="B540" s="1" t="s">
-        <v>1314</v>
+        <v>1312</v>
       </c>
       <c r="C540" s="8"/>
     </row>
     <row r="541" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A541" s="1" t="s">
-        <v>1321</v>
+        <v>1319</v>
       </c>
       <c r="B541" s="1" t="s">
-        <v>1315</v>
+        <v>1313</v>
       </c>
       <c r="C541" s="8"/>
     </row>
-    <row r="542" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+    <row r="542" spans="1:3" ht="51" x14ac:dyDescent="0.2">
       <c r="A542" s="1" t="s">
-        <v>1325</v>
+        <v>1323</v>
       </c>
       <c r="B542" s="1" t="s">
-        <v>1326</v>
+        <v>1352</v>
       </c>
       <c r="C542" s="8"/>
     </row>
     <row r="543" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A543" s="1" t="s">
+        <v>1258</v>
+      </c>
+      <c r="B543" s="1" t="s">
+        <v>1259</v>
+      </c>
+      <c r="C543" s="9" t="s">
         <v>1260</v>
-      </c>
-      <c r="B543" s="1" t="s">
-        <v>1261</v>
-      </c>
-      <c r="C543" s="9" t="s">
-        <v>1262</v>
       </c>
     </row>
     <row r="544" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A544" s="1" t="s">
+        <v>1261</v>
+      </c>
+      <c r="B544" s="1" t="s">
+        <v>1262</v>
+      </c>
+      <c r="C544" s="9" t="s">
         <v>1263</v>
-      </c>
-      <c r="B544" s="1" t="s">
-        <v>1264</v>
-      </c>
-      <c r="C544" s="9" t="s">
-        <v>1265</v>
       </c>
     </row>
     <row r="545" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A545" t="s">
-        <v>1248</v>
+        <v>1246</v>
       </c>
       <c r="B545" s="1" t="s">
-        <v>1253</v>
+        <v>1251</v>
       </c>
       <c r="C545" s="1" t="s">
         <v>956</v>
@@ -10077,7 +10077,7 @@
     </row>
     <row r="546" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A546" t="s">
-        <v>1249</v>
+        <v>1247</v>
       </c>
       <c r="B546" s="1" t="s">
         <v>958</v>
@@ -10088,35 +10088,35 @@
     </row>
     <row r="547" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A547" t="s">
-        <v>1250</v>
+        <v>1248</v>
       </c>
       <c r="B547" s="1" t="s">
+        <v>1252</v>
+      </c>
+      <c r="C547" s="1" t="s">
         <v>1254</v>
-      </c>
-      <c r="C547" s="1" t="s">
-        <v>1256</v>
       </c>
     </row>
     <row r="548" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A548" t="s">
-        <v>1251</v>
+        <v>1249</v>
       </c>
       <c r="B548" s="1" t="s">
+        <v>1253</v>
+      </c>
+      <c r="C548" s="1" t="s">
         <v>1255</v>
-      </c>
-      <c r="C548" s="1" t="s">
-        <v>1257</v>
       </c>
     </row>
     <row r="549" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A549" t="s">
-        <v>1252</v>
+        <v>1250</v>
       </c>
       <c r="B549" s="4" t="s">
         <v>1046</v>
       </c>
       <c r="C549" s="4" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
       <c r="D549" s="4"/>
       <c r="E549" s="4"/>
@@ -10125,7 +10125,7 @@
     </row>
     <row r="550" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A550" s="1" t="s">
-        <v>1266</v>
+        <v>1264</v>
       </c>
       <c r="B550" s="1" t="s">
         <v>522</v>
@@ -10136,35 +10136,35 @@
     </row>
     <row r="551" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A551" s="1" t="s">
-        <v>1267</v>
+        <v>1265</v>
       </c>
       <c r="B551" s="1" t="s">
-        <v>1304</v>
+        <v>1302</v>
       </c>
       <c r="C551" s="1" t="s">
-        <v>1305</v>
+        <v>1303</v>
       </c>
     </row>
     <row r="552" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A552" s="1" t="s">
-        <v>1268</v>
+        <v>1266</v>
       </c>
       <c r="B552" s="1" t="s">
-        <v>1306</v>
+        <v>1304</v>
       </c>
       <c r="C552" s="1" t="s">
-        <v>1307</v>
+        <v>1305</v>
       </c>
     </row>
     <row r="553" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A553" s="11" t="s">
-        <v>1269</v>
+        <v>1267</v>
       </c>
       <c r="B553" s="7" t="s">
+        <v>1278</v>
+      </c>
+      <c r="C553" s="7" t="s">
         <v>1280</v>
-      </c>
-      <c r="C553" s="7" t="s">
-        <v>1282</v>
       </c>
       <c r="D553" s="7"/>
       <c r="E553" s="7"/>
@@ -10173,13 +10173,13 @@
     </row>
     <row r="554" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A554" s="13" t="s">
-        <v>1270</v>
+        <v>1268</v>
       </c>
       <c r="B554" s="14" t="s">
+        <v>1279</v>
+      </c>
+      <c r="C554" s="14" t="s">
         <v>1281</v>
-      </c>
-      <c r="C554" s="14" t="s">
-        <v>1283</v>
       </c>
       <c r="D554" s="14"/>
       <c r="E554" s="14"/>
@@ -10188,7 +10188,7 @@
     </row>
     <row r="555" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A555" s="11" t="s">
-        <v>1271</v>
+        <v>1269</v>
       </c>
       <c r="B555" s="7" t="s">
         <v>522</v>
@@ -10203,35 +10203,35 @@
     </row>
     <row r="556" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A556" t="s">
-        <v>1284</v>
+        <v>1282</v>
       </c>
       <c r="B556" s="16" t="s">
-        <v>1272</v>
+        <v>1270</v>
       </c>
       <c r="C556" s="16" t="s">
-        <v>1272</v>
+        <v>1270</v>
       </c>
     </row>
     <row r="557" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A557" t="s">
-        <v>1285</v>
+        <v>1283</v>
       </c>
       <c r="B557" s="16" t="s">
-        <v>1286</v>
+        <v>1284</v>
       </c>
       <c r="C557" s="16" t="s">
-        <v>1286</v>
+        <v>1284</v>
       </c>
     </row>
     <row r="558" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A558" s="11" t="s">
-        <v>1273</v>
+        <v>1271</v>
       </c>
       <c r="B558" s="7" t="s">
-        <v>1287</v>
+        <v>1285</v>
       </c>
       <c r="C558" s="7" t="s">
-        <v>1294</v>
+        <v>1292</v>
       </c>
       <c r="D558" s="4"/>
       <c r="E558" s="4"/>
@@ -10240,62 +10240,62 @@
     </row>
     <row r="559" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A559" s="13" t="s">
-        <v>1274</v>
+        <v>1272</v>
       </c>
       <c r="B559" s="14" t="s">
-        <v>1288</v>
+        <v>1286</v>
       </c>
       <c r="C559" s="14" t="s">
-        <v>1293</v>
+        <v>1291</v>
       </c>
     </row>
     <row r="560" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A560" s="11" t="s">
-        <v>1275</v>
+        <v>1273</v>
       </c>
       <c r="B560" s="1" t="s">
-        <v>1304</v>
+        <v>1302</v>
       </c>
       <c r="C560" s="1" t="s">
-        <v>1308</v>
+        <v>1306</v>
       </c>
     </row>
     <row r="561" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A561" s="11" t="s">
-        <v>1276</v>
+        <v>1274</v>
       </c>
       <c r="B561" s="7" t="s">
-        <v>1289</v>
+        <v>1287</v>
       </c>
       <c r="C561" s="7" t="s">
-        <v>1292</v>
+        <v>1290</v>
       </c>
     </row>
     <row r="562" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A562" s="13" t="s">
-        <v>1277</v>
+        <v>1275</v>
       </c>
       <c r="B562" s="14" t="s">
-        <v>1290</v>
+        <v>1288</v>
       </c>
       <c r="C562" s="14" t="s">
-        <v>1291</v>
+        <v>1289</v>
       </c>
     </row>
     <row r="563" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A563" s="11" t="s">
-        <v>1278</v>
+        <v>1276</v>
       </c>
       <c r="B563" s="1" t="s">
-        <v>1306</v>
+        <v>1304</v>
       </c>
       <c r="C563" s="1" t="s">
-        <v>1309</v>
+        <v>1307</v>
       </c>
     </row>
     <row r="564" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A564" s="1" t="s">
-        <v>1295</v>
+        <v>1293</v>
       </c>
       <c r="B564" s="1" t="s">
         <v>522</v>
@@ -10306,7 +10306,7 @@
     </row>
     <row r="565" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A565" s="1" t="s">
-        <v>1296</v>
+        <v>1294</v>
       </c>
       <c r="B565" s="1">
         <v>1662</v>
@@ -10314,29 +10314,29 @@
     </row>
     <row r="566" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A566" s="1" t="s">
-        <v>1297</v>
+        <v>1295</v>
       </c>
       <c r="B566" s="1" t="s">
+        <v>1278</v>
+      </c>
+      <c r="C566" s="1" t="s">
         <v>1280</v>
-      </c>
-      <c r="C566" s="1" t="s">
-        <v>1282</v>
       </c>
     </row>
     <row r="567" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A567" s="1" t="s">
-        <v>1298</v>
+        <v>1296</v>
       </c>
       <c r="B567" s="1" t="s">
+        <v>1279</v>
+      </c>
+      <c r="C567" s="1" t="s">
         <v>1281</v>
-      </c>
-      <c r="C567" s="1" t="s">
-        <v>1283</v>
       </c>
     </row>
     <row r="568" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A568" s="1" t="s">
-        <v>1299</v>
+        <v>1297</v>
       </c>
       <c r="B568" s="1" t="s">
         <v>522</v>
@@ -10347,13 +10347,13 @@
     </row>
     <row r="569" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A569" s="10" t="s">
-        <v>1327</v>
+        <v>1324</v>
       </c>
       <c r="B569" s="4" t="s">
-        <v>1337</v>
+        <v>1334</v>
       </c>
       <c r="C569" s="4" t="s">
-        <v>1337</v>
+        <v>1334</v>
       </c>
       <c r="D569" s="4"/>
       <c r="E569" s="4"/>
@@ -10362,101 +10362,101 @@
     </row>
     <row r="570" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A570" t="s">
-        <v>1328</v>
+        <v>1325</v>
       </c>
       <c r="B570" s="1" t="s">
-        <v>1338</v>
+        <v>1335</v>
       </c>
       <c r="C570" s="1" t="s">
-        <v>1347</v>
+        <v>1344</v>
       </c>
     </row>
     <row r="571" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A571" t="s">
-        <v>1329</v>
+        <v>1326</v>
       </c>
       <c r="B571" s="1" t="s">
-        <v>1339</v>
+        <v>1336</v>
       </c>
       <c r="C571" s="1" t="s">
-        <v>1348</v>
+        <v>1345</v>
       </c>
     </row>
     <row r="572" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A572" t="s">
-        <v>1330</v>
+        <v>1327</v>
       </c>
       <c r="B572" s="1" t="s">
-        <v>1340</v>
+        <v>1337</v>
       </c>
       <c r="C572" s="1" t="s">
-        <v>1349</v>
+        <v>1346</v>
       </c>
     </row>
     <row r="573" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A573" t="s">
-        <v>1331</v>
+        <v>1328</v>
       </c>
       <c r="B573" s="1" t="s">
-        <v>1341</v>
+        <v>1338</v>
       </c>
       <c r="C573" s="1" t="s">
-        <v>1350</v>
+        <v>1347</v>
       </c>
     </row>
     <row r="574" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A574" t="s">
-        <v>1332</v>
+        <v>1329</v>
       </c>
       <c r="B574" s="1" t="s">
-        <v>1342</v>
+        <v>1339</v>
       </c>
       <c r="C574" s="1" t="s">
-        <v>1351</v>
+        <v>1348</v>
       </c>
     </row>
     <row r="575" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A575" t="s">
-        <v>1333</v>
+        <v>1330</v>
       </c>
       <c r="B575" s="1" t="s">
-        <v>1343</v>
+        <v>1340</v>
       </c>
       <c r="C575" s="1" t="s">
-        <v>1352</v>
+        <v>1349</v>
       </c>
     </row>
     <row r="576" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A576" t="s">
-        <v>1334</v>
+        <v>1331</v>
       </c>
       <c r="B576" s="1" t="s">
-        <v>1344</v>
+        <v>1341</v>
       </c>
       <c r="C576" s="1" t="s">
-        <v>1344</v>
+        <v>1341</v>
       </c>
     </row>
     <row r="577" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A577" t="s">
-        <v>1335</v>
+        <v>1332</v>
       </c>
       <c r="B577" s="1" t="s">
-        <v>1345</v>
+        <v>1342</v>
       </c>
       <c r="C577" s="1" t="s">
-        <v>1353</v>
+        <v>1350</v>
       </c>
     </row>
     <row r="578" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A578" t="s">
-        <v>1336</v>
+        <v>1333</v>
       </c>
       <c r="B578" s="1" t="s">
-        <v>1346</v>
+        <v>1343</v>
       </c>
       <c r="C578" s="1" t="s">
-        <v>1354</v>
+        <v>1351</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add to i18n the product name
</commit_message>
<xml_diff>
--- a/config/i18n/i18n.xlsx
+++ b/config/i18n/i18n.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10810"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joana/work/sp-duh/config/i18n/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tiagodias/work/sp-duh/config/i18n/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E13A870B-0098-0443-9C8B-DC2C7FB64A68}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B053FA1-2F3E-F54A-ADE3-8F3E33CC2B26}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-620" yWindow="-30800" windowWidth="38360" windowHeight="30800" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1422" uniqueCount="1355">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1428" uniqueCount="1359">
   <si>
     <t>key</t>
   </si>
@@ -4152,6 +4152,18 @@
   <si>
     <t>Verificamos que não existe nenhum movimento de abertura, ou se existir não está registado no diário correto. Por favor verifique se deve fazer este movimento ou se deve registar o mesmo em outro diário. Poderá ainda definir na ficha da empresa informação sobre a data de início de atividade.</t>
   </si>
+  <si>
+    <t>product_name_toconline</t>
+  </si>
+  <si>
+    <t>product_name_business</t>
+  </si>
+  <si>
+    <t>TOConline</t>
+  </si>
+  <si>
+    <t>Cloudware.business</t>
+  </si>
 </sst>
 </file>
 
@@ -4185,6 +4197,7 @@
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -4469,7 +4482,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="i18n" displayName="i18n" ref="A1:G578" totalsRowShown="0" headerRowDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="i18n" displayName="i18n" ref="A1:G580" totalsRowShown="0" headerRowDxfId="6">
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="key"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="pt" dataDxfId="5"/>
@@ -4746,10 +4759,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G578"/>
+  <dimension ref="A1:G580"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A479" workbookViewId="0">
-      <selection activeCell="B498" sqref="B498"/>
+    <sheetView tabSelected="1" topLeftCell="A551" workbookViewId="0">
+      <selection activeCell="B566" sqref="B566"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10457,6 +10470,28 @@
       </c>
       <c r="C578" s="1" t="s">
         <v>1351</v>
+      </c>
+    </row>
+    <row r="579" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A579" t="s">
+        <v>1355</v>
+      </c>
+      <c r="B579" s="1" t="s">
+        <v>1357</v>
+      </c>
+      <c r="C579" s="1" t="s">
+        <v>1357</v>
+      </c>
+    </row>
+    <row r="580" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A580" t="s">
+        <v>1356</v>
+      </c>
+      <c r="B580" s="1" t="s">
+        <v>1358</v>
+      </c>
+      <c r="C580" s="1" t="s">
+        <v>1358</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding messages for svat_unbalanced and svat_unbalanced_nok
</commit_message>
<xml_diff>
--- a/config/i18n/i18n.xlsx
+++ b/config/i18n/i18n.xlsx
@@ -5,12 +5,12 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tiagodias/work/sp-duh/config/i18n/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joana/work/sp-duh/config/i18n/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B053FA1-2F3E-F54A-ADE3-8F3E33CC2B26}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88BF3707-FC8D-844E-919C-D7ABF222650C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19620" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1428" uniqueCount="1359">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1432" uniqueCount="1363">
   <si>
     <t>key</t>
   </si>
@@ -4163,6 +4163,18 @@
   </si>
   <si>
     <t>Cloudware.business</t>
+  </si>
+  <si>
+    <t>svat_unbalanced</t>
+  </si>
+  <si>
+    <t>svat_unbalanced_nok</t>
+  </si>
+  <si>
+    <t>Teste a movimentos finalizados em moeda estrangeira</t>
+  </si>
+  <si>
+    <t>Verificamos que alguns movimentos efectuados em moeda estrangeira não estão consistentes, por favor reabra e corrija os seguintes movimentos:</t>
   </si>
 </sst>
 </file>
@@ -4482,7 +4494,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="i18n" displayName="i18n" ref="A1:G580" totalsRowShown="0" headerRowDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="i18n" displayName="i18n" ref="A1:G582" totalsRowShown="0" headerRowDxfId="6">
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="key"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="pt" dataDxfId="5"/>
@@ -4759,10 +4771,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G580"/>
+  <dimension ref="A1:G582"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A551" workbookViewId="0">
-      <selection activeCell="B566" sqref="B566"/>
+    <sheetView tabSelected="1" topLeftCell="A530" workbookViewId="0">
+      <selection activeCell="B543" sqref="B543"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10046,451 +10058,469 @@
       </c>
       <c r="C541" s="8"/>
     </row>
-    <row r="542" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+    <row r="542" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A542" s="1" t="s">
+        <v>1359</v>
+      </c>
+      <c r="B542" s="1" t="s">
+        <v>1361</v>
+      </c>
+      <c r="C542" s="8"/>
+    </row>
+    <row r="543" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+      <c r="A543" s="1" t="s">
+        <v>1360</v>
+      </c>
+      <c r="B543" s="1" t="s">
+        <v>1362</v>
+      </c>
+      <c r="C543" s="8"/>
+    </row>
+    <row r="544" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+      <c r="A544" s="1" t="s">
         <v>1323</v>
       </c>
-      <c r="B542" s="1" t="s">
+      <c r="B544" s="1" t="s">
         <v>1352</v>
       </c>
-      <c r="C542" s="8"/>
-    </row>
-    <row r="543" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A543" s="1" t="s">
+      <c r="C544" s="8"/>
+    </row>
+    <row r="545" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A545" s="1" t="s">
         <v>1258</v>
       </c>
-      <c r="B543" s="1" t="s">
+      <c r="B545" s="1" t="s">
         <v>1259</v>
       </c>
-      <c r="C543" s="9" t="s">
+      <c r="C545" s="9" t="s">
         <v>1260</v>
       </c>
     </row>
-    <row r="544" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A544" s="1" t="s">
+    <row r="546" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A546" s="1" t="s">
         <v>1261</v>
       </c>
-      <c r="B544" s="1" t="s">
+      <c r="B546" s="1" t="s">
         <v>1262</v>
       </c>
-      <c r="C544" s="9" t="s">
+      <c r="C546" s="9" t="s">
         <v>1263</v>
-      </c>
-    </row>
-    <row r="545" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A545" t="s">
-        <v>1246</v>
-      </c>
-      <c r="B545" s="1" t="s">
-        <v>1251</v>
-      </c>
-      <c r="C545" s="1" t="s">
-        <v>956</v>
-      </c>
-    </row>
-    <row r="546" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A546" t="s">
-        <v>1247</v>
-      </c>
-      <c r="B546" s="1" t="s">
-        <v>958</v>
-      </c>
-      <c r="C546" s="1" t="s">
-        <v>953</v>
       </c>
     </row>
     <row r="547" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A547" t="s">
-        <v>1248</v>
+        <v>1246</v>
       </c>
       <c r="B547" s="1" t="s">
-        <v>1252</v>
+        <v>1251</v>
       </c>
       <c r="C547" s="1" t="s">
-        <v>1254</v>
+        <v>956</v>
       </c>
     </row>
     <row r="548" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A548" t="s">
-        <v>1249</v>
+        <v>1247</v>
       </c>
       <c r="B548" s="1" t="s">
-        <v>1253</v>
+        <v>958</v>
       </c>
       <c r="C548" s="1" t="s">
-        <v>1255</v>
+        <v>953</v>
       </c>
     </row>
     <row r="549" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A549" t="s">
+        <v>1248</v>
+      </c>
+      <c r="B549" s="1" t="s">
+        <v>1252</v>
+      </c>
+      <c r="C549" s="1" t="s">
+        <v>1254</v>
+      </c>
+    </row>
+    <row r="550" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A550" t="s">
+        <v>1249</v>
+      </c>
+      <c r="B550" s="1" t="s">
+        <v>1253</v>
+      </c>
+      <c r="C550" s="1" t="s">
+        <v>1255</v>
+      </c>
+    </row>
+    <row r="551" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A551" t="s">
         <v>1250</v>
       </c>
-      <c r="B549" s="4" t="s">
+      <c r="B551" s="4" t="s">
         <v>1046</v>
       </c>
-      <c r="C549" s="4" t="s">
+      <c r="C551" s="4" t="s">
         <v>1256</v>
       </c>
-      <c r="D549" s="4"/>
-      <c r="E549" s="4"/>
-      <c r="F549" s="4"/>
-      <c r="G549" s="4"/>
-    </row>
-    <row r="550" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A550" s="1" t="s">
+      <c r="D551" s="4"/>
+      <c r="E551" s="4"/>
+      <c r="F551" s="4"/>
+      <c r="G551" s="4"/>
+    </row>
+    <row r="552" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A552" s="1" t="s">
         <v>1264</v>
       </c>
-      <c r="B550" s="1" t="s">
+      <c r="B552" s="1" t="s">
         <v>522</v>
       </c>
-      <c r="C550" s="1" t="s">
+      <c r="C552" s="1" t="s">
         <v>523</v>
       </c>
     </row>
-    <row r="551" spans="1:7" ht="34" x14ac:dyDescent="0.2">
-      <c r="A551" s="1" t="s">
+    <row r="553" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="A553" s="1" t="s">
         <v>1265</v>
       </c>
-      <c r="B551" s="1" t="s">
+      <c r="B553" s="1" t="s">
         <v>1302</v>
       </c>
-      <c r="C551" s="1" t="s">
+      <c r="C553" s="1" t="s">
         <v>1303</v>
       </c>
     </row>
-    <row r="552" spans="1:7" ht="34" x14ac:dyDescent="0.2">
-      <c r="A552" s="1" t="s">
+    <row r="554" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="A554" s="1" t="s">
         <v>1266</v>
       </c>
-      <c r="B552" s="1" t="s">
+      <c r="B554" s="1" t="s">
         <v>1304</v>
       </c>
-      <c r="C552" s="1" t="s">
+      <c r="C554" s="1" t="s">
         <v>1305</v>
       </c>
-    </row>
-    <row r="553" spans="1:7" ht="34" x14ac:dyDescent="0.2">
-      <c r="A553" s="11" t="s">
-        <v>1267</v>
-      </c>
-      <c r="B553" s="7" t="s">
-        <v>1278</v>
-      </c>
-      <c r="C553" s="7" t="s">
-        <v>1280</v>
-      </c>
-      <c r="D553" s="7"/>
-      <c r="E553" s="7"/>
-      <c r="F553" s="7"/>
-      <c r="G553" s="12"/>
-    </row>
-    <row r="554" spans="1:7" ht="34" x14ac:dyDescent="0.2">
-      <c r="A554" s="13" t="s">
-        <v>1268</v>
-      </c>
-      <c r="B554" s="14" t="s">
-        <v>1279</v>
-      </c>
-      <c r="C554" s="14" t="s">
-        <v>1281</v>
-      </c>
-      <c r="D554" s="14"/>
-      <c r="E554" s="14"/>
-      <c r="F554" s="14"/>
-      <c r="G554" s="15"/>
     </row>
     <row r="555" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A555" s="11" t="s">
-        <v>1269</v>
+        <v>1267</v>
       </c>
       <c r="B555" s="7" t="s">
-        <v>522</v>
+        <v>1278</v>
       </c>
       <c r="C555" s="7" t="s">
-        <v>602</v>
+        <v>1280</v>
       </c>
       <c r="D555" s="7"/>
       <c r="E555" s="7"/>
       <c r="F555" s="7"/>
       <c r="G555" s="12"/>
     </row>
-    <row r="556" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A556" t="s">
+    <row r="556" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="A556" s="13" t="s">
+        <v>1268</v>
+      </c>
+      <c r="B556" s="14" t="s">
+        <v>1279</v>
+      </c>
+      <c r="C556" s="14" t="s">
+        <v>1281</v>
+      </c>
+      <c r="D556" s="14"/>
+      <c r="E556" s="14"/>
+      <c r="F556" s="14"/>
+      <c r="G556" s="15"/>
+    </row>
+    <row r="557" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="A557" s="11" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B557" s="7" t="s">
+        <v>522</v>
+      </c>
+      <c r="C557" s="7" t="s">
+        <v>602</v>
+      </c>
+      <c r="D557" s="7"/>
+      <c r="E557" s="7"/>
+      <c r="F557" s="7"/>
+      <c r="G557" s="12"/>
+    </row>
+    <row r="558" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A558" t="s">
         <v>1282</v>
       </c>
-      <c r="B556" s="16" t="s">
+      <c r="B558" s="16" t="s">
         <v>1270</v>
       </c>
-      <c r="C556" s="16" t="s">
+      <c r="C558" s="16" t="s">
         <v>1270</v>
       </c>
     </row>
-    <row r="557" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A557" t="s">
+    <row r="559" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A559" t="s">
         <v>1283</v>
       </c>
-      <c r="B557" s="16" t="s">
+      <c r="B559" s="16" t="s">
         <v>1284</v>
       </c>
-      <c r="C557" s="16" t="s">
+      <c r="C559" s="16" t="s">
         <v>1284</v>
-      </c>
-    </row>
-    <row r="558" spans="1:7" ht="34" x14ac:dyDescent="0.2">
-      <c r="A558" s="11" t="s">
-        <v>1271</v>
-      </c>
-      <c r="B558" s="7" t="s">
-        <v>1285</v>
-      </c>
-      <c r="C558" s="7" t="s">
-        <v>1292</v>
-      </c>
-      <c r="D558" s="4"/>
-      <c r="E558" s="4"/>
-      <c r="F558" s="4"/>
-      <c r="G558" s="4"/>
-    </row>
-    <row r="559" spans="1:7" ht="34" x14ac:dyDescent="0.2">
-      <c r="A559" s="13" t="s">
-        <v>1272</v>
-      </c>
-      <c r="B559" s="14" t="s">
-        <v>1286</v>
-      </c>
-      <c r="C559" s="14" t="s">
-        <v>1291</v>
       </c>
     </row>
     <row r="560" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A560" s="11" t="s">
+        <v>1271</v>
+      </c>
+      <c r="B560" s="7" t="s">
+        <v>1285</v>
+      </c>
+      <c r="C560" s="7" t="s">
+        <v>1292</v>
+      </c>
+      <c r="D560" s="4"/>
+      <c r="E560" s="4"/>
+      <c r="F560" s="4"/>
+      <c r="G560" s="4"/>
+    </row>
+    <row r="561" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="A561" s="13" t="s">
+        <v>1272</v>
+      </c>
+      <c r="B561" s="14" t="s">
+        <v>1286</v>
+      </c>
+      <c r="C561" s="14" t="s">
+        <v>1291</v>
+      </c>
+    </row>
+    <row r="562" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="A562" s="11" t="s">
         <v>1273</v>
       </c>
-      <c r="B560" s="1" t="s">
+      <c r="B562" s="1" t="s">
         <v>1302</v>
       </c>
-      <c r="C560" s="1" t="s">
+      <c r="C562" s="1" t="s">
         <v>1306</v>
-      </c>
-    </row>
-    <row r="561" spans="1:7" ht="34" x14ac:dyDescent="0.2">
-      <c r="A561" s="11" t="s">
-        <v>1274</v>
-      </c>
-      <c r="B561" s="7" t="s">
-        <v>1287</v>
-      </c>
-      <c r="C561" s="7" t="s">
-        <v>1290</v>
-      </c>
-    </row>
-    <row r="562" spans="1:7" ht="34" x14ac:dyDescent="0.2">
-      <c r="A562" s="13" t="s">
-        <v>1275</v>
-      </c>
-      <c r="B562" s="14" t="s">
-        <v>1288</v>
-      </c>
-      <c r="C562" s="14" t="s">
-        <v>1289</v>
       </c>
     </row>
     <row r="563" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A563" s="11" t="s">
+        <v>1274</v>
+      </c>
+      <c r="B563" s="7" t="s">
+        <v>1287</v>
+      </c>
+      <c r="C563" s="7" t="s">
+        <v>1290</v>
+      </c>
+    </row>
+    <row r="564" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="A564" s="13" t="s">
+        <v>1275</v>
+      </c>
+      <c r="B564" s="14" t="s">
+        <v>1288</v>
+      </c>
+      <c r="C564" s="14" t="s">
+        <v>1289</v>
+      </c>
+    </row>
+    <row r="565" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="A565" s="11" t="s">
         <v>1276</v>
       </c>
-      <c r="B563" s="1" t="s">
+      <c r="B565" s="1" t="s">
         <v>1304</v>
       </c>
-      <c r="C563" s="1" t="s">
+      <c r="C565" s="1" t="s">
         <v>1307</v>
       </c>
     </row>
-    <row r="564" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A564" s="1" t="s">
+    <row r="566" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A566" s="1" t="s">
         <v>1293</v>
       </c>
-      <c r="B564" s="1" t="s">
+      <c r="B566" s="1" t="s">
         <v>522</v>
       </c>
-      <c r="C564" s="1" t="s">
+      <c r="C566" s="1" t="s">
         <v>523</v>
       </c>
     </row>
-    <row r="565" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A565" s="1" t="s">
+    <row r="567" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A567" s="1" t="s">
         <v>1294</v>
       </c>
-      <c r="B565" s="1">
+      <c r="B567" s="1">
         <v>1662</v>
       </c>
     </row>
-    <row r="566" spans="1:7" ht="34" x14ac:dyDescent="0.2">
-      <c r="A566" s="1" t="s">
+    <row r="568" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="A568" s="1" t="s">
         <v>1295</v>
       </c>
-      <c r="B566" s="1" t="s">
+      <c r="B568" s="1" t="s">
         <v>1278</v>
       </c>
-      <c r="C566" s="1" t="s">
+      <c r="C568" s="1" t="s">
         <v>1280</v>
       </c>
     </row>
-    <row r="567" spans="1:7" ht="34" x14ac:dyDescent="0.2">
-      <c r="A567" s="1" t="s">
+    <row r="569" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="A569" s="1" t="s">
         <v>1296</v>
       </c>
-      <c r="B567" s="1" t="s">
+      <c r="B569" s="1" t="s">
         <v>1279</v>
       </c>
-      <c r="C567" s="1" t="s">
+      <c r="C569" s="1" t="s">
         <v>1281</v>
       </c>
     </row>
-    <row r="568" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A568" s="1" t="s">
+    <row r="570" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A570" s="1" t="s">
         <v>1297</v>
       </c>
-      <c r="B568" s="1" t="s">
+      <c r="B570" s="1" t="s">
         <v>522</v>
       </c>
-      <c r="C568" s="1" t="s">
+      <c r="C570" s="1" t="s">
         <v>602</v>
       </c>
     </row>
-    <row r="569" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A569" s="10" t="s">
+    <row r="571" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A571" s="10" t="s">
         <v>1324</v>
       </c>
-      <c r="B569" s="4" t="s">
+      <c r="B571" s="4" t="s">
         <v>1334</v>
       </c>
-      <c r="C569" s="4" t="s">
+      <c r="C571" s="4" t="s">
         <v>1334</v>
       </c>
-      <c r="D569" s="4"/>
-      <c r="E569" s="4"/>
-      <c r="F569" s="4"/>
-      <c r="G569" s="4"/>
-    </row>
-    <row r="570" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A570" t="s">
-        <v>1325</v>
-      </c>
-      <c r="B570" s="1" t="s">
-        <v>1335</v>
-      </c>
-      <c r="C570" s="1" t="s">
-        <v>1344</v>
-      </c>
-    </row>
-    <row r="571" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A571" t="s">
-        <v>1326</v>
-      </c>
-      <c r="B571" s="1" t="s">
-        <v>1336</v>
-      </c>
-      <c r="C571" s="1" t="s">
-        <v>1345</v>
-      </c>
+      <c r="D571" s="4"/>
+      <c r="E571" s="4"/>
+      <c r="F571" s="4"/>
+      <c r="G571" s="4"/>
     </row>
     <row r="572" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A572" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="B572" s="1" t="s">
-        <v>1337</v>
+        <v>1335</v>
       </c>
       <c r="C572" s="1" t="s">
-        <v>1346</v>
+        <v>1344</v>
       </c>
     </row>
     <row r="573" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A573" t="s">
-        <v>1328</v>
+        <v>1326</v>
       </c>
       <c r="B573" s="1" t="s">
-        <v>1338</v>
+        <v>1336</v>
       </c>
       <c r="C573" s="1" t="s">
-        <v>1347</v>
+        <v>1345</v>
       </c>
     </row>
     <row r="574" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A574" t="s">
-        <v>1329</v>
+        <v>1327</v>
       </c>
       <c r="B574" s="1" t="s">
-        <v>1339</v>
+        <v>1337</v>
       </c>
       <c r="C574" s="1" t="s">
-        <v>1348</v>
+        <v>1346</v>
       </c>
     </row>
     <row r="575" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A575" t="s">
-        <v>1330</v>
+        <v>1328</v>
       </c>
       <c r="B575" s="1" t="s">
-        <v>1340</v>
+        <v>1338</v>
       </c>
       <c r="C575" s="1" t="s">
-        <v>1349</v>
+        <v>1347</v>
       </c>
     </row>
     <row r="576" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A576" t="s">
-        <v>1331</v>
+        <v>1329</v>
       </c>
       <c r="B576" s="1" t="s">
-        <v>1341</v>
+        <v>1339</v>
       </c>
       <c r="C576" s="1" t="s">
-        <v>1341</v>
+        <v>1348</v>
       </c>
     </row>
     <row r="577" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A577" t="s">
-        <v>1332</v>
+        <v>1330</v>
       </c>
       <c r="B577" s="1" t="s">
-        <v>1342</v>
+        <v>1340</v>
       </c>
       <c r="C577" s="1" t="s">
-        <v>1350</v>
+        <v>1349</v>
       </c>
     </row>
     <row r="578" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A578" t="s">
-        <v>1333</v>
+        <v>1331</v>
       </c>
       <c r="B578" s="1" t="s">
-        <v>1343</v>
+        <v>1341</v>
       </c>
       <c r="C578" s="1" t="s">
-        <v>1351</v>
+        <v>1341</v>
       </c>
     </row>
     <row r="579" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A579" t="s">
-        <v>1355</v>
+        <v>1332</v>
       </c>
       <c r="B579" s="1" t="s">
-        <v>1357</v>
+        <v>1342</v>
       </c>
       <c r="C579" s="1" t="s">
-        <v>1357</v>
+        <v>1350</v>
       </c>
     </row>
     <row r="580" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A580" t="s">
+        <v>1333</v>
+      </c>
+      <c r="B580" s="1" t="s">
+        <v>1343</v>
+      </c>
+      <c r="C580" s="1" t="s">
+        <v>1351</v>
+      </c>
+    </row>
+    <row r="581" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A581" t="s">
+        <v>1355</v>
+      </c>
+      <c r="B581" s="1" t="s">
+        <v>1357</v>
+      </c>
+      <c r="C581" s="1" t="s">
+        <v>1357</v>
+      </c>
+    </row>
+    <row r="582" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A582" t="s">
         <v>1356</v>
       </c>
-      <c r="B580" s="1" t="s">
+      <c r="B582" s="1" t="s">
         <v>1358</v>
       </c>
-      <c r="C580" s="1" t="s">
+      <c r="C582" s="1" t="s">
         <v>1358</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Adding more messages related with svat_unbalanced
</commit_message>
<xml_diff>
--- a/config/i18n/i18n.xlsx
+++ b/config/i18n/i18n.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joana/work/sp-duh/config/i18n/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88BF3707-FC8D-844E-919C-D7ABF222650C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32D6A10E-E9C0-1B40-AB77-B75BD4D46B26}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19620" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1432" uniqueCount="1363">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1438" uniqueCount="1369">
   <si>
     <t>key</t>
   </si>
@@ -4174,7 +4174,27 @@
     <t>Teste a movimentos finalizados em moeda estrangeira</t>
   </si>
   <si>
-    <t>Verificamos que alguns movimentos efectuados em moeda estrangeira não estão consistentes, por favor reabra e corrija os seguintes movimentos:</t>
+    <t>svat_unbalanced_ok</t>
+  </si>
+  <si>
+    <t>Verificamos que existem {0} movimentos efectuados em moeda estrangeira que não estão consistentes e impedem a exportação do SAF-T.
+Por favor consulte estes movimentos no relatório de conformidade e efectue as devidas correcções.</t>
+  </si>
+  <si>
+    <t>Verificamos que alguns movimentos efetuados em moeda estrangeira não estão consistentes, por favor reabra e corrija os seguintes movimentos:</t>
+  </si>
+  <si>
+    <t>Verificamos que os movimentos efetuados em moeda estrangeira estão consistentes.</t>
+  </si>
+  <si>
+    <t>svat_unbalanced_saft_many</t>
+  </si>
+  <si>
+    <t>svat_unbalanced_saft_single</t>
+  </si>
+  <si>
+    <t>Verificamos que existe 1 movimento em moeda estrangeira que não está consistente e impede a exportação do SAF-T.
+Por favor efectue as correcções necessárias no movimento {0}.</t>
   </si>
 </sst>
 </file>
@@ -4494,7 +4514,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="i18n" displayName="i18n" ref="A1:G582" totalsRowShown="0" headerRowDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="i18n" displayName="i18n" ref="A1:G585" totalsRowShown="0" headerRowDxfId="6">
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="key"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="pt" dataDxfId="5"/>
@@ -4771,10 +4791,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G582"/>
+  <dimension ref="A1:G585"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A530" workbookViewId="0">
-      <selection activeCell="B543" sqref="B543"/>
+    <sheetView tabSelected="1" topLeftCell="A532" workbookViewId="0">
+      <selection activeCell="A543" sqref="A543:A546"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10072,455 +10092,482 @@
         <v>1360</v>
       </c>
       <c r="B543" s="1" t="s">
+        <v>1364</v>
+      </c>
+      <c r="C543" s="8"/>
+    </row>
+    <row r="544" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A544" s="1" t="s">
         <v>1362</v>
       </c>
-      <c r="C543" s="8"/>
-    </row>
-    <row r="544" spans="1:3" ht="51" x14ac:dyDescent="0.2">
-      <c r="A544" s="1" t="s">
+      <c r="B544" s="1" t="s">
+        <v>1365</v>
+      </c>
+      <c r="C544" s="8"/>
+    </row>
+    <row r="545" spans="1:7" ht="85" x14ac:dyDescent="0.2">
+      <c r="A545" s="1" t="s">
+        <v>1367</v>
+      </c>
+      <c r="B545" s="1" t="s">
+        <v>1368</v>
+      </c>
+      <c r="C545" s="8"/>
+    </row>
+    <row r="546" spans="1:7" ht="85" x14ac:dyDescent="0.2">
+      <c r="A546" s="1" t="s">
+        <v>1366</v>
+      </c>
+      <c r="B546" s="1" t="s">
+        <v>1363</v>
+      </c>
+      <c r="C546" s="8"/>
+    </row>
+    <row r="547" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+      <c r="A547" s="1" t="s">
         <v>1323</v>
       </c>
-      <c r="B544" s="1" t="s">
+      <c r="B547" s="1" t="s">
         <v>1352</v>
       </c>
-      <c r="C544" s="8"/>
-    </row>
-    <row r="545" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A545" s="1" t="s">
+      <c r="C547" s="8"/>
+    </row>
+    <row r="548" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A548" s="1" t="s">
         <v>1258</v>
       </c>
-      <c r="B545" s="1" t="s">
+      <c r="B548" s="1" t="s">
         <v>1259</v>
       </c>
-      <c r="C545" s="9" t="s">
+      <c r="C548" s="9" t="s">
         <v>1260</v>
       </c>
     </row>
-    <row r="546" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A546" s="1" t="s">
+    <row r="549" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A549" s="1" t="s">
         <v>1261</v>
       </c>
-      <c r="B546" s="1" t="s">
+      <c r="B549" s="1" t="s">
         <v>1262</v>
       </c>
-      <c r="C546" s="9" t="s">
+      <c r="C549" s="9" t="s">
         <v>1263</v>
-      </c>
-    </row>
-    <row r="547" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A547" t="s">
-        <v>1246</v>
-      </c>
-      <c r="B547" s="1" t="s">
-        <v>1251</v>
-      </c>
-      <c r="C547" s="1" t="s">
-        <v>956</v>
-      </c>
-    </row>
-    <row r="548" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A548" t="s">
-        <v>1247</v>
-      </c>
-      <c r="B548" s="1" t="s">
-        <v>958</v>
-      </c>
-      <c r="C548" s="1" t="s">
-        <v>953</v>
-      </c>
-    </row>
-    <row r="549" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A549" t="s">
-        <v>1248</v>
-      </c>
-      <c r="B549" s="1" t="s">
-        <v>1252</v>
-      </c>
-      <c r="C549" s="1" t="s">
-        <v>1254</v>
       </c>
     </row>
     <row r="550" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A550" t="s">
-        <v>1249</v>
+        <v>1246</v>
       </c>
       <c r="B550" s="1" t="s">
-        <v>1253</v>
+        <v>1251</v>
       </c>
       <c r="C550" s="1" t="s">
-        <v>1255</v>
+        <v>956</v>
       </c>
     </row>
     <row r="551" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A551" t="s">
+        <v>1247</v>
+      </c>
+      <c r="B551" s="1" t="s">
+        <v>958</v>
+      </c>
+      <c r="C551" s="1" t="s">
+        <v>953</v>
+      </c>
+    </row>
+    <row r="552" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A552" t="s">
+        <v>1248</v>
+      </c>
+      <c r="B552" s="1" t="s">
+        <v>1252</v>
+      </c>
+      <c r="C552" s="1" t="s">
+        <v>1254</v>
+      </c>
+    </row>
+    <row r="553" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A553" t="s">
+        <v>1249</v>
+      </c>
+      <c r="B553" s="1" t="s">
+        <v>1253</v>
+      </c>
+      <c r="C553" s="1" t="s">
+        <v>1255</v>
+      </c>
+    </row>
+    <row r="554" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A554" t="s">
         <v>1250</v>
       </c>
-      <c r="B551" s="4" t="s">
+      <c r="B554" s="4" t="s">
         <v>1046</v>
       </c>
-      <c r="C551" s="4" t="s">
+      <c r="C554" s="4" t="s">
         <v>1256</v>
       </c>
-      <c r="D551" s="4"/>
-      <c r="E551" s="4"/>
-      <c r="F551" s="4"/>
-      <c r="G551" s="4"/>
-    </row>
-    <row r="552" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A552" s="1" t="s">
+      <c r="D554" s="4"/>
+      <c r="E554" s="4"/>
+      <c r="F554" s="4"/>
+      <c r="G554" s="4"/>
+    </row>
+    <row r="555" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A555" s="1" t="s">
         <v>1264</v>
       </c>
-      <c r="B552" s="1" t="s">
+      <c r="B555" s="1" t="s">
         <v>522</v>
       </c>
-      <c r="C552" s="1" t="s">
+      <c r="C555" s="1" t="s">
         <v>523</v>
       </c>
     </row>
-    <row r="553" spans="1:7" ht="34" x14ac:dyDescent="0.2">
-      <c r="A553" s="1" t="s">
+    <row r="556" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="A556" s="1" t="s">
         <v>1265</v>
       </c>
-      <c r="B553" s="1" t="s">
+      <c r="B556" s="1" t="s">
         <v>1302</v>
       </c>
-      <c r="C553" s="1" t="s">
+      <c r="C556" s="1" t="s">
         <v>1303</v>
       </c>
     </row>
-    <row r="554" spans="1:7" ht="34" x14ac:dyDescent="0.2">
-      <c r="A554" s="1" t="s">
+    <row r="557" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="A557" s="1" t="s">
         <v>1266</v>
       </c>
-      <c r="B554" s="1" t="s">
+      <c r="B557" s="1" t="s">
         <v>1304</v>
       </c>
-      <c r="C554" s="1" t="s">
+      <c r="C557" s="1" t="s">
         <v>1305</v>
       </c>
     </row>
-    <row r="555" spans="1:7" ht="34" x14ac:dyDescent="0.2">
-      <c r="A555" s="11" t="s">
+    <row r="558" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="A558" s="11" t="s">
         <v>1267</v>
       </c>
-      <c r="B555" s="7" t="s">
+      <c r="B558" s="7" t="s">
         <v>1278</v>
       </c>
-      <c r="C555" s="7" t="s">
+      <c r="C558" s="7" t="s">
         <v>1280</v>
       </c>
-      <c r="D555" s="7"/>
-      <c r="E555" s="7"/>
-      <c r="F555" s="7"/>
-      <c r="G555" s="12"/>
-    </row>
-    <row r="556" spans="1:7" ht="34" x14ac:dyDescent="0.2">
-      <c r="A556" s="13" t="s">
+      <c r="D558" s="7"/>
+      <c r="E558" s="7"/>
+      <c r="F558" s="7"/>
+      <c r="G558" s="12"/>
+    </row>
+    <row r="559" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="A559" s="13" t="s">
         <v>1268</v>
       </c>
-      <c r="B556" s="14" t="s">
+      <c r="B559" s="14" t="s">
         <v>1279</v>
       </c>
-      <c r="C556" s="14" t="s">
+      <c r="C559" s="14" t="s">
         <v>1281</v>
       </c>
-      <c r="D556" s="14"/>
-      <c r="E556" s="14"/>
-      <c r="F556" s="14"/>
-      <c r="G556" s="15"/>
-    </row>
-    <row r="557" spans="1:7" ht="34" x14ac:dyDescent="0.2">
-      <c r="A557" s="11" t="s">
-        <v>1269</v>
-      </c>
-      <c r="B557" s="7" t="s">
-        <v>522</v>
-      </c>
-      <c r="C557" s="7" t="s">
-        <v>602</v>
-      </c>
-      <c r="D557" s="7"/>
-      <c r="E557" s="7"/>
-      <c r="F557" s="7"/>
-      <c r="G557" s="12"/>
-    </row>
-    <row r="558" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A558" t="s">
-        <v>1282</v>
-      </c>
-      <c r="B558" s="16" t="s">
-        <v>1270</v>
-      </c>
-      <c r="C558" s="16" t="s">
-        <v>1270</v>
-      </c>
-    </row>
-    <row r="559" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A559" t="s">
-        <v>1283</v>
-      </c>
-      <c r="B559" s="16" t="s">
-        <v>1284</v>
-      </c>
-      <c r="C559" s="16" t="s">
-        <v>1284</v>
-      </c>
+      <c r="D559" s="14"/>
+      <c r="E559" s="14"/>
+      <c r="F559" s="14"/>
+      <c r="G559" s="15"/>
     </row>
     <row r="560" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A560" s="11" t="s">
-        <v>1271</v>
+        <v>1269</v>
       </c>
       <c r="B560" s="7" t="s">
-        <v>1285</v>
+        <v>522</v>
       </c>
       <c r="C560" s="7" t="s">
-        <v>1292</v>
-      </c>
-      <c r="D560" s="4"/>
-      <c r="E560" s="4"/>
-      <c r="F560" s="4"/>
-      <c r="G560" s="4"/>
-    </row>
-    <row r="561" spans="1:7" ht="34" x14ac:dyDescent="0.2">
-      <c r="A561" s="13" t="s">
-        <v>1272</v>
-      </c>
-      <c r="B561" s="14" t="s">
-        <v>1286</v>
-      </c>
-      <c r="C561" s="14" t="s">
-        <v>1291</v>
-      </c>
-    </row>
-    <row r="562" spans="1:7" ht="34" x14ac:dyDescent="0.2">
-      <c r="A562" s="11" t="s">
-        <v>1273</v>
-      </c>
-      <c r="B562" s="1" t="s">
-        <v>1302</v>
-      </c>
-      <c r="C562" s="1" t="s">
-        <v>1306</v>
+        <v>602</v>
+      </c>
+      <c r="D560" s="7"/>
+      <c r="E560" s="7"/>
+      <c r="F560" s="7"/>
+      <c r="G560" s="12"/>
+    </row>
+    <row r="561" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A561" t="s">
+        <v>1282</v>
+      </c>
+      <c r="B561" s="16" t="s">
+        <v>1270</v>
+      </c>
+      <c r="C561" s="16" t="s">
+        <v>1270</v>
+      </c>
+    </row>
+    <row r="562" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A562" t="s">
+        <v>1283</v>
+      </c>
+      <c r="B562" s="16" t="s">
+        <v>1284</v>
+      </c>
+      <c r="C562" s="16" t="s">
+        <v>1284</v>
       </c>
     </row>
     <row r="563" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A563" s="11" t="s">
-        <v>1274</v>
+        <v>1271</v>
       </c>
       <c r="B563" s="7" t="s">
-        <v>1287</v>
+        <v>1285</v>
       </c>
       <c r="C563" s="7" t="s">
-        <v>1290</v>
-      </c>
+        <v>1292</v>
+      </c>
+      <c r="D563" s="4"/>
+      <c r="E563" s="4"/>
+      <c r="F563" s="4"/>
+      <c r="G563" s="4"/>
     </row>
     <row r="564" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A564" s="13" t="s">
-        <v>1275</v>
+        <v>1272</v>
       </c>
       <c r="B564" s="14" t="s">
-        <v>1288</v>
+        <v>1286</v>
       </c>
       <c r="C564" s="14" t="s">
-        <v>1289</v>
+        <v>1291</v>
       </c>
     </row>
     <row r="565" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A565" s="11" t="s">
+        <v>1273</v>
+      </c>
+      <c r="B565" s="1" t="s">
+        <v>1302</v>
+      </c>
+      <c r="C565" s="1" t="s">
+        <v>1306</v>
+      </c>
+    </row>
+    <row r="566" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="A566" s="11" t="s">
+        <v>1274</v>
+      </c>
+      <c r="B566" s="7" t="s">
+        <v>1287</v>
+      </c>
+      <c r="C566" s="7" t="s">
+        <v>1290</v>
+      </c>
+    </row>
+    <row r="567" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="A567" s="13" t="s">
+        <v>1275</v>
+      </c>
+      <c r="B567" s="14" t="s">
+        <v>1288</v>
+      </c>
+      <c r="C567" s="14" t="s">
+        <v>1289</v>
+      </c>
+    </row>
+    <row r="568" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="A568" s="11" t="s">
         <v>1276</v>
       </c>
-      <c r="B565" s="1" t="s">
+      <c r="B568" s="1" t="s">
         <v>1304</v>
       </c>
-      <c r="C565" s="1" t="s">
+      <c r="C568" s="1" t="s">
         <v>1307</v>
       </c>
     </row>
-    <row r="566" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A566" s="1" t="s">
+    <row r="569" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A569" s="1" t="s">
         <v>1293</v>
       </c>
-      <c r="B566" s="1" t="s">
+      <c r="B569" s="1" t="s">
         <v>522</v>
       </c>
-      <c r="C566" s="1" t="s">
+      <c r="C569" s="1" t="s">
         <v>523</v>
-      </c>
-    </row>
-    <row r="567" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A567" s="1" t="s">
-        <v>1294</v>
-      </c>
-      <c r="B567" s="1">
-        <v>1662</v>
-      </c>
-    </row>
-    <row r="568" spans="1:7" ht="34" x14ac:dyDescent="0.2">
-      <c r="A568" s="1" t="s">
-        <v>1295</v>
-      </c>
-      <c r="B568" s="1" t="s">
-        <v>1278</v>
-      </c>
-      <c r="C568" s="1" t="s">
-        <v>1280</v>
-      </c>
-    </row>
-    <row r="569" spans="1:7" ht="34" x14ac:dyDescent="0.2">
-      <c r="A569" s="1" t="s">
-        <v>1296</v>
-      </c>
-      <c r="B569" s="1" t="s">
-        <v>1279</v>
-      </c>
-      <c r="C569" s="1" t="s">
-        <v>1281</v>
       </c>
     </row>
     <row r="570" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A570" s="1" t="s">
+        <v>1294</v>
+      </c>
+      <c r="B570" s="1">
+        <v>1662</v>
+      </c>
+    </row>
+    <row r="571" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="A571" s="1" t="s">
+        <v>1295</v>
+      </c>
+      <c r="B571" s="1" t="s">
+        <v>1278</v>
+      </c>
+      <c r="C571" s="1" t="s">
+        <v>1280</v>
+      </c>
+    </row>
+    <row r="572" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="A572" s="1" t="s">
+        <v>1296</v>
+      </c>
+      <c r="B572" s="1" t="s">
+        <v>1279</v>
+      </c>
+      <c r="C572" s="1" t="s">
+        <v>1281</v>
+      </c>
+    </row>
+    <row r="573" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A573" s="1" t="s">
         <v>1297</v>
       </c>
-      <c r="B570" s="1" t="s">
+      <c r="B573" s="1" t="s">
         <v>522</v>
       </c>
-      <c r="C570" s="1" t="s">
+      <c r="C573" s="1" t="s">
         <v>602</v>
       </c>
     </row>
-    <row r="571" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A571" s="10" t="s">
+    <row r="574" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A574" s="10" t="s">
         <v>1324</v>
       </c>
-      <c r="B571" s="4" t="s">
+      <c r="B574" s="4" t="s">
         <v>1334</v>
       </c>
-      <c r="C571" s="4" t="s">
+      <c r="C574" s="4" t="s">
         <v>1334</v>
       </c>
-      <c r="D571" s="4"/>
-      <c r="E571" s="4"/>
-      <c r="F571" s="4"/>
-      <c r="G571" s="4"/>
-    </row>
-    <row r="572" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A572" t="s">
-        <v>1325</v>
-      </c>
-      <c r="B572" s="1" t="s">
-        <v>1335</v>
-      </c>
-      <c r="C572" s="1" t="s">
-        <v>1344</v>
-      </c>
-    </row>
-    <row r="573" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A573" t="s">
-        <v>1326</v>
-      </c>
-      <c r="B573" s="1" t="s">
-        <v>1336</v>
-      </c>
-      <c r="C573" s="1" t="s">
-        <v>1345</v>
-      </c>
-    </row>
-    <row r="574" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A574" t="s">
-        <v>1327</v>
-      </c>
-      <c r="B574" s="1" t="s">
-        <v>1337</v>
-      </c>
-      <c r="C574" s="1" t="s">
-        <v>1346</v>
-      </c>
+      <c r="D574" s="4"/>
+      <c r="E574" s="4"/>
+      <c r="F574" s="4"/>
+      <c r="G574" s="4"/>
     </row>
     <row r="575" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A575" t="s">
-        <v>1328</v>
+        <v>1325</v>
       </c>
       <c r="B575" s="1" t="s">
-        <v>1338</v>
+        <v>1335</v>
       </c>
       <c r="C575" s="1" t="s">
-        <v>1347</v>
+        <v>1344</v>
       </c>
     </row>
     <row r="576" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A576" t="s">
-        <v>1329</v>
+        <v>1326</v>
       </c>
       <c r="B576" s="1" t="s">
-        <v>1339</v>
+        <v>1336</v>
       </c>
       <c r="C576" s="1" t="s">
-        <v>1348</v>
+        <v>1345</v>
       </c>
     </row>
     <row r="577" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A577" t="s">
-        <v>1330</v>
+        <v>1327</v>
       </c>
       <c r="B577" s="1" t="s">
-        <v>1340</v>
+        <v>1337</v>
       </c>
       <c r="C577" s="1" t="s">
-        <v>1349</v>
+        <v>1346</v>
       </c>
     </row>
     <row r="578" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A578" t="s">
-        <v>1331</v>
+        <v>1328</v>
       </c>
       <c r="B578" s="1" t="s">
-        <v>1341</v>
+        <v>1338</v>
       </c>
       <c r="C578" s="1" t="s">
-        <v>1341</v>
+        <v>1347</v>
       </c>
     </row>
     <row r="579" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A579" t="s">
-        <v>1332</v>
+        <v>1329</v>
       </c>
       <c r="B579" s="1" t="s">
-        <v>1342</v>
+        <v>1339</v>
       </c>
       <c r="C579" s="1" t="s">
-        <v>1350</v>
+        <v>1348</v>
       </c>
     </row>
     <row r="580" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A580" t="s">
-        <v>1333</v>
+        <v>1330</v>
       </c>
       <c r="B580" s="1" t="s">
-        <v>1343</v>
+        <v>1340</v>
       </c>
       <c r="C580" s="1" t="s">
-        <v>1351</v>
+        <v>1349</v>
       </c>
     </row>
     <row r="581" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A581" t="s">
-        <v>1355</v>
+        <v>1331</v>
       </c>
       <c r="B581" s="1" t="s">
-        <v>1357</v>
+        <v>1341</v>
       </c>
       <c r="C581" s="1" t="s">
-        <v>1357</v>
+        <v>1341</v>
       </c>
     </row>
     <row r="582" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A582" t="s">
+        <v>1332</v>
+      </c>
+      <c r="B582" s="1" t="s">
+        <v>1342</v>
+      </c>
+      <c r="C582" s="1" t="s">
+        <v>1350</v>
+      </c>
+    </row>
+    <row r="583" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A583" t="s">
+        <v>1333</v>
+      </c>
+      <c r="B583" s="1" t="s">
+        <v>1343</v>
+      </c>
+      <c r="C583" s="1" t="s">
+        <v>1351</v>
+      </c>
+    </row>
+    <row r="584" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A584" t="s">
+        <v>1355</v>
+      </c>
+      <c r="B584" s="1" t="s">
+        <v>1357</v>
+      </c>
+      <c r="C584" s="1" t="s">
+        <v>1357</v>
+      </c>
+    </row>
+    <row r="585" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A585" t="s">
         <v>1356</v>
       </c>
-      <c r="B582" s="1" t="s">
+      <c r="B585" s="1" t="s">
         <v>1358</v>
       </c>
-      <c r="C582" s="1" t="s">
+      <c r="C585" s="1" t="s">
         <v>1358</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Adding SVAT 43 and 44 rules JAN (& Rita)
</commit_message>
<xml_diff>
--- a/config/i18n/i18n.xlsx
+++ b/config/i18n/i18n.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10810"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11011"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joana/work/sp-duh/config/i18n/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32D6A10E-E9C0-1B40-AB77-B75BD4D46B26}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6A003EC-466A-5644-B292-C375DC195265}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19620" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-3560" yWindow="-19180" windowWidth="33600" windowHeight="18420" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1438" uniqueCount="1369">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1450" uniqueCount="1381">
   <si>
     <t>key</t>
   </si>
@@ -4195,6 +4195,44 @@
   <si>
     <t>Verificamos que existe 1 movimento em moeda estrangeira que não está consistente e impede a exportação do SAF-T.
 Por favor efectue as correcções necessárias no movimento {0}.</t>
+  </si>
+  <si>
+    <t>svat_t43</t>
+  </si>
+  <si>
+    <t>svat_t44</t>
+  </si>
+  <si>
+    <t>svat_t43_ok</t>
+  </si>
+  <si>
+    <t>svat_t43_nok</t>
+  </si>
+  <si>
+    <t>svat_t44_ok</t>
+  </si>
+  <si>
+    <t>svat_t44_nok</t>
+  </si>
+  <si>
+    <t>Teste à contabilização de documentos anulados emitidos em faturação</t>
+  </si>
+  <si>
+    <t>Teste à contabilização de outros documentos anulados na comercial</t>
+  </si>
+  <si>
+    <t>Verificamos que existem movimentos contabilísticos no estado finalizado para documentos comerciais anulados, sem que exista o respetivo estorno na contabilidade. Verifique no menu de contabilidade a sugestão de estorno, caso não encontre o lançamento de estorno, gere novamente as sugestões.
+Verifique os movovimentos dos seguintes documentos comerciais:</t>
+  </si>
+  <si>
+    <t>Verificamos que existem movimentos contabilísticos no estado finalizado para documentos comerciais anulados, sem que exista o respetivo estorno na contabilidade. Verifique no menu de contabilidade a sugestão de estorno, caso não encontre o lançamento de estorno, gere novamente as sugestões.
+Verifique os movovimentos dos seguintes documentos emitidos em faturação:</t>
+  </si>
+  <si>
+    <t>Verificamos que não existem movimentos contabilísticos no estado finalizado para documentos emitidos em faturação, ou que existe o respetivo estorno na contabilidade. Sem exceções.</t>
+  </si>
+  <si>
+    <t>Verificamos que não existem movimentos contabilísticos no estado finalizado para documentos comerciais anulados, ou que existe o respetivo estorno na contabilidade. Sem exceções.</t>
   </si>
 </sst>
 </file>
@@ -4514,7 +4552,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="i18n" displayName="i18n" ref="A1:G585" totalsRowShown="0" headerRowDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="i18n" displayName="i18n" ref="A1:G591" totalsRowShown="0" headerRowDxfId="6">
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="key"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="pt" dataDxfId="5"/>
@@ -4791,10 +4829,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G585"/>
+  <dimension ref="A1:G591"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A532" workbookViewId="0">
-      <selection activeCell="A543" sqref="A543:A546"/>
+    <sheetView tabSelected="1" topLeftCell="A541" workbookViewId="0">
+      <selection activeCell="B547" sqref="B547"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10080,494 +10118,548 @@
     </row>
     <row r="542" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A542" s="1" t="s">
+        <v>1369</v>
+      </c>
+      <c r="B542" s="1" t="s">
+        <v>1375</v>
+      </c>
+      <c r="C542" s="8"/>
+    </row>
+    <row r="543" spans="1:3" ht="85" x14ac:dyDescent="0.2">
+      <c r="A543" s="1" t="s">
+        <v>1371</v>
+      </c>
+      <c r="B543" s="1" t="s">
+        <v>1379</v>
+      </c>
+      <c r="C543" s="8"/>
+    </row>
+    <row r="544" spans="1:3" ht="153" x14ac:dyDescent="0.2">
+      <c r="A544" s="1" t="s">
+        <v>1372</v>
+      </c>
+      <c r="B544" s="1" t="s">
+        <v>1378</v>
+      </c>
+      <c r="C544" s="8"/>
+    </row>
+    <row r="545" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="A545" s="1" t="s">
+        <v>1370</v>
+      </c>
+      <c r="B545" s="1" t="s">
+        <v>1376</v>
+      </c>
+      <c r="C545" s="8"/>
+    </row>
+    <row r="546" spans="1:7" ht="68" x14ac:dyDescent="0.2">
+      <c r="A546" s="1" t="s">
+        <v>1373</v>
+      </c>
+      <c r="B546" s="1" t="s">
+        <v>1380</v>
+      </c>
+      <c r="C546" s="8"/>
+    </row>
+    <row r="547" spans="1:7" ht="153" x14ac:dyDescent="0.2">
+      <c r="A547" s="1" t="s">
+        <v>1374</v>
+      </c>
+      <c r="B547" s="1" t="s">
+        <v>1377</v>
+      </c>
+      <c r="C547" s="8"/>
+    </row>
+    <row r="548" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="A548" s="1" t="s">
         <v>1359</v>
       </c>
-      <c r="B542" s="1" t="s">
+      <c r="B548" s="1" t="s">
         <v>1361</v>
       </c>
-      <c r="C542" s="8"/>
-    </row>
-    <row r="543" spans="1:3" ht="51" x14ac:dyDescent="0.2">
-      <c r="A543" s="1" t="s">
+      <c r="C548" s="8"/>
+    </row>
+    <row r="549" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+      <c r="A549" s="1" t="s">
         <v>1360</v>
       </c>
-      <c r="B543" s="1" t="s">
+      <c r="B549" s="1" t="s">
         <v>1364</v>
       </c>
-      <c r="C543" s="8"/>
-    </row>
-    <row r="544" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A544" s="1" t="s">
+      <c r="C549" s="8"/>
+    </row>
+    <row r="550" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="A550" s="1" t="s">
         <v>1362</v>
       </c>
-      <c r="B544" s="1" t="s">
+      <c r="B550" s="1" t="s">
         <v>1365</v>
       </c>
-      <c r="C544" s="8"/>
-    </row>
-    <row r="545" spans="1:7" ht="85" x14ac:dyDescent="0.2">
-      <c r="A545" s="1" t="s">
+      <c r="C550" s="8"/>
+    </row>
+    <row r="551" spans="1:7" ht="85" x14ac:dyDescent="0.2">
+      <c r="A551" s="1" t="s">
         <v>1367</v>
       </c>
-      <c r="B545" s="1" t="s">
+      <c r="B551" s="1" t="s">
         <v>1368</v>
       </c>
-      <c r="C545" s="8"/>
-    </row>
-    <row r="546" spans="1:7" ht="85" x14ac:dyDescent="0.2">
-      <c r="A546" s="1" t="s">
+      <c r="C551" s="8"/>
+    </row>
+    <row r="552" spans="1:7" ht="85" x14ac:dyDescent="0.2">
+      <c r="A552" s="1" t="s">
         <v>1366</v>
       </c>
-      <c r="B546" s="1" t="s">
+      <c r="B552" s="1" t="s">
         <v>1363</v>
       </c>
-      <c r="C546" s="8"/>
-    </row>
-    <row r="547" spans="1:7" ht="51" x14ac:dyDescent="0.2">
-      <c r="A547" s="1" t="s">
+      <c r="C552" s="8"/>
+    </row>
+    <row r="553" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+      <c r="A553" s="1" t="s">
         <v>1323</v>
       </c>
-      <c r="B547" s="1" t="s">
+      <c r="B553" s="1" t="s">
         <v>1352</v>
       </c>
-      <c r="C547" s="8"/>
-    </row>
-    <row r="548" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A548" s="1" t="s">
+      <c r="C553" s="8"/>
+    </row>
+    <row r="554" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A554" s="1" t="s">
         <v>1258</v>
       </c>
-      <c r="B548" s="1" t="s">
+      <c r="B554" s="1" t="s">
         <v>1259</v>
       </c>
-      <c r="C548" s="9" t="s">
+      <c r="C554" s="9" t="s">
         <v>1260</v>
       </c>
-    </row>
-    <row r="549" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A549" s="1" t="s">
-        <v>1261</v>
-      </c>
-      <c r="B549" s="1" t="s">
-        <v>1262</v>
-      </c>
-      <c r="C549" s="9" t="s">
-        <v>1263</v>
-      </c>
-    </row>
-    <row r="550" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A550" t="s">
-        <v>1246</v>
-      </c>
-      <c r="B550" s="1" t="s">
-        <v>1251</v>
-      </c>
-      <c r="C550" s="1" t="s">
-        <v>956</v>
-      </c>
-    </row>
-    <row r="551" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A551" t="s">
-        <v>1247</v>
-      </c>
-      <c r="B551" s="1" t="s">
-        <v>958</v>
-      </c>
-      <c r="C551" s="1" t="s">
-        <v>953</v>
-      </c>
-    </row>
-    <row r="552" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A552" t="s">
-        <v>1248</v>
-      </c>
-      <c r="B552" s="1" t="s">
-        <v>1252</v>
-      </c>
-      <c r="C552" s="1" t="s">
-        <v>1254</v>
-      </c>
-    </row>
-    <row r="553" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A553" t="s">
-        <v>1249</v>
-      </c>
-      <c r="B553" s="1" t="s">
-        <v>1253</v>
-      </c>
-      <c r="C553" s="1" t="s">
-        <v>1255</v>
-      </c>
-    </row>
-    <row r="554" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A554" t="s">
-        <v>1250</v>
-      </c>
-      <c r="B554" s="4" t="s">
-        <v>1046</v>
-      </c>
-      <c r="C554" s="4" t="s">
-        <v>1256</v>
-      </c>
-      <c r="D554" s="4"/>
-      <c r="E554" s="4"/>
-      <c r="F554" s="4"/>
-      <c r="G554" s="4"/>
     </row>
     <row r="555" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A555" s="1" t="s">
+        <v>1261</v>
+      </c>
+      <c r="B555" s="1" t="s">
+        <v>1262</v>
+      </c>
+      <c r="C555" s="9" t="s">
+        <v>1263</v>
+      </c>
+    </row>
+    <row r="556" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A556" t="s">
+        <v>1246</v>
+      </c>
+      <c r="B556" s="1" t="s">
+        <v>1251</v>
+      </c>
+      <c r="C556" s="1" t="s">
+        <v>956</v>
+      </c>
+    </row>
+    <row r="557" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A557" t="s">
+        <v>1247</v>
+      </c>
+      <c r="B557" s="1" t="s">
+        <v>958</v>
+      </c>
+      <c r="C557" s="1" t="s">
+        <v>953</v>
+      </c>
+    </row>
+    <row r="558" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A558" t="s">
+        <v>1248</v>
+      </c>
+      <c r="B558" s="1" t="s">
+        <v>1252</v>
+      </c>
+      <c r="C558" s="1" t="s">
+        <v>1254</v>
+      </c>
+    </row>
+    <row r="559" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A559" t="s">
+        <v>1249</v>
+      </c>
+      <c r="B559" s="1" t="s">
+        <v>1253</v>
+      </c>
+      <c r="C559" s="1" t="s">
+        <v>1255</v>
+      </c>
+    </row>
+    <row r="560" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A560" t="s">
+        <v>1250</v>
+      </c>
+      <c r="B560" s="4" t="s">
+        <v>1046</v>
+      </c>
+      <c r="C560" s="4" t="s">
+        <v>1256</v>
+      </c>
+      <c r="D560" s="4"/>
+      <c r="E560" s="4"/>
+      <c r="F560" s="4"/>
+      <c r="G560" s="4"/>
+    </row>
+    <row r="561" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A561" s="1" t="s">
         <v>1264</v>
       </c>
-      <c r="B555" s="1" t="s">
+      <c r="B561" s="1" t="s">
         <v>522</v>
       </c>
-      <c r="C555" s="1" t="s">
+      <c r="C561" s="1" t="s">
         <v>523</v>
       </c>
     </row>
-    <row r="556" spans="1:7" ht="34" x14ac:dyDescent="0.2">
-      <c r="A556" s="1" t="s">
+    <row r="562" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="A562" s="1" t="s">
         <v>1265</v>
       </c>
-      <c r="B556" s="1" t="s">
+      <c r="B562" s="1" t="s">
         <v>1302</v>
       </c>
-      <c r="C556" s="1" t="s">
+      <c r="C562" s="1" t="s">
         <v>1303</v>
       </c>
     </row>
-    <row r="557" spans="1:7" ht="34" x14ac:dyDescent="0.2">
-      <c r="A557" s="1" t="s">
+    <row r="563" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="A563" s="1" t="s">
         <v>1266</v>
       </c>
-      <c r="B557" s="1" t="s">
+      <c r="B563" s="1" t="s">
         <v>1304</v>
       </c>
-      <c r="C557" s="1" t="s">
+      <c r="C563" s="1" t="s">
         <v>1305</v>
       </c>
     </row>
-    <row r="558" spans="1:7" ht="34" x14ac:dyDescent="0.2">
-      <c r="A558" s="11" t="s">
+    <row r="564" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="A564" s="11" t="s">
         <v>1267</v>
       </c>
-      <c r="B558" s="7" t="s">
+      <c r="B564" s="7" t="s">
         <v>1278</v>
       </c>
-      <c r="C558" s="7" t="s">
+      <c r="C564" s="7" t="s">
         <v>1280</v>
       </c>
-      <c r="D558" s="7"/>
-      <c r="E558" s="7"/>
-      <c r="F558" s="7"/>
-      <c r="G558" s="12"/>
-    </row>
-    <row r="559" spans="1:7" ht="34" x14ac:dyDescent="0.2">
-      <c r="A559" s="13" t="s">
+      <c r="D564" s="7"/>
+      <c r="E564" s="7"/>
+      <c r="F564" s="7"/>
+      <c r="G564" s="12"/>
+    </row>
+    <row r="565" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="A565" s="13" t="s">
         <v>1268</v>
       </c>
-      <c r="B559" s="14" t="s">
+      <c r="B565" s="14" t="s">
         <v>1279</v>
       </c>
-      <c r="C559" s="14" t="s">
+      <c r="C565" s="14" t="s">
         <v>1281</v>
       </c>
-      <c r="D559" s="14"/>
-      <c r="E559" s="14"/>
-      <c r="F559" s="14"/>
-      <c r="G559" s="15"/>
-    </row>
-    <row r="560" spans="1:7" ht="34" x14ac:dyDescent="0.2">
-      <c r="A560" s="11" t="s">
-        <v>1269</v>
-      </c>
-      <c r="B560" s="7" t="s">
-        <v>522</v>
-      </c>
-      <c r="C560" s="7" t="s">
-        <v>602</v>
-      </c>
-      <c r="D560" s="7"/>
-      <c r="E560" s="7"/>
-      <c r="F560" s="7"/>
-      <c r="G560" s="12"/>
-    </row>
-    <row r="561" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A561" t="s">
-        <v>1282</v>
-      </c>
-      <c r="B561" s="16" t="s">
-        <v>1270</v>
-      </c>
-      <c r="C561" s="16" t="s">
-        <v>1270</v>
-      </c>
-    </row>
-    <row r="562" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A562" t="s">
-        <v>1283</v>
-      </c>
-      <c r="B562" s="16" t="s">
-        <v>1284</v>
-      </c>
-      <c r="C562" s="16" t="s">
-        <v>1284</v>
-      </c>
-    </row>
-    <row r="563" spans="1:7" ht="34" x14ac:dyDescent="0.2">
-      <c r="A563" s="11" t="s">
-        <v>1271</v>
-      </c>
-      <c r="B563" s="7" t="s">
-        <v>1285</v>
-      </c>
-      <c r="C563" s="7" t="s">
-        <v>1292</v>
-      </c>
-      <c r="D563" s="4"/>
-      <c r="E563" s="4"/>
-      <c r="F563" s="4"/>
-      <c r="G563" s="4"/>
-    </row>
-    <row r="564" spans="1:7" ht="34" x14ac:dyDescent="0.2">
-      <c r="A564" s="13" t="s">
-        <v>1272</v>
-      </c>
-      <c r="B564" s="14" t="s">
-        <v>1286</v>
-      </c>
-      <c r="C564" s="14" t="s">
-        <v>1291</v>
-      </c>
-    </row>
-    <row r="565" spans="1:7" ht="34" x14ac:dyDescent="0.2">
-      <c r="A565" s="11" t="s">
-        <v>1273</v>
-      </c>
-      <c r="B565" s="1" t="s">
-        <v>1302</v>
-      </c>
-      <c r="C565" s="1" t="s">
-        <v>1306</v>
-      </c>
+      <c r="D565" s="14"/>
+      <c r="E565" s="14"/>
+      <c r="F565" s="14"/>
+      <c r="G565" s="15"/>
     </row>
     <row r="566" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A566" s="11" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B566" s="7" t="s">
+        <v>522</v>
+      </c>
+      <c r="C566" s="7" t="s">
+        <v>602</v>
+      </c>
+      <c r="D566" s="7"/>
+      <c r="E566" s="7"/>
+      <c r="F566" s="7"/>
+      <c r="G566" s="12"/>
+    </row>
+    <row r="567" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A567" t="s">
+        <v>1282</v>
+      </c>
+      <c r="B567" s="16" t="s">
+        <v>1270</v>
+      </c>
+      <c r="C567" s="16" t="s">
+        <v>1270</v>
+      </c>
+    </row>
+    <row r="568" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A568" t="s">
+        <v>1283</v>
+      </c>
+      <c r="B568" s="16" t="s">
+        <v>1284</v>
+      </c>
+      <c r="C568" s="16" t="s">
+        <v>1284</v>
+      </c>
+    </row>
+    <row r="569" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="A569" s="11" t="s">
+        <v>1271</v>
+      </c>
+      <c r="B569" s="7" t="s">
+        <v>1285</v>
+      </c>
+      <c r="C569" s="7" t="s">
+        <v>1292</v>
+      </c>
+      <c r="D569" s="4"/>
+      <c r="E569" s="4"/>
+      <c r="F569" s="4"/>
+      <c r="G569" s="4"/>
+    </row>
+    <row r="570" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="A570" s="13" t="s">
+        <v>1272</v>
+      </c>
+      <c r="B570" s="14" t="s">
+        <v>1286</v>
+      </c>
+      <c r="C570" s="14" t="s">
+        <v>1291</v>
+      </c>
+    </row>
+    <row r="571" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="A571" s="11" t="s">
+        <v>1273</v>
+      </c>
+      <c r="B571" s="1" t="s">
+        <v>1302</v>
+      </c>
+      <c r="C571" s="1" t="s">
+        <v>1306</v>
+      </c>
+    </row>
+    <row r="572" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="A572" s="11" t="s">
         <v>1274</v>
       </c>
-      <c r="B566" s="7" t="s">
+      <c r="B572" s="7" t="s">
         <v>1287</v>
       </c>
-      <c r="C566" s="7" t="s">
+      <c r="C572" s="7" t="s">
         <v>1290</v>
       </c>
     </row>
-    <row r="567" spans="1:7" ht="34" x14ac:dyDescent="0.2">
-      <c r="A567" s="13" t="s">
+    <row r="573" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="A573" s="13" t="s">
         <v>1275</v>
       </c>
-      <c r="B567" s="14" t="s">
+      <c r="B573" s="14" t="s">
         <v>1288</v>
       </c>
-      <c r="C567" s="14" t="s">
+      <c r="C573" s="14" t="s">
         <v>1289</v>
       </c>
     </row>
-    <row r="568" spans="1:7" ht="34" x14ac:dyDescent="0.2">
-      <c r="A568" s="11" t="s">
+    <row r="574" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="A574" s="11" t="s">
         <v>1276</v>
       </c>
-      <c r="B568" s="1" t="s">
+      <c r="B574" s="1" t="s">
         <v>1304</v>
       </c>
-      <c r="C568" s="1" t="s">
+      <c r="C574" s="1" t="s">
         <v>1307</v>
       </c>
     </row>
-    <row r="569" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A569" s="1" t="s">
+    <row r="575" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A575" s="1" t="s">
         <v>1293</v>
       </c>
-      <c r="B569" s="1" t="s">
+      <c r="B575" s="1" t="s">
         <v>522</v>
       </c>
-      <c r="C569" s="1" t="s">
+      <c r="C575" s="1" t="s">
         <v>523</v>
       </c>
     </row>
-    <row r="570" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A570" s="1" t="s">
+    <row r="576" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A576" s="1" t="s">
         <v>1294</v>
       </c>
-      <c r="B570" s="1">
+      <c r="B576" s="1">
         <v>1662</v>
       </c>
     </row>
-    <row r="571" spans="1:7" ht="34" x14ac:dyDescent="0.2">
-      <c r="A571" s="1" t="s">
+    <row r="577" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="A577" s="1" t="s">
         <v>1295</v>
       </c>
-      <c r="B571" s="1" t="s">
+      <c r="B577" s="1" t="s">
         <v>1278</v>
       </c>
-      <c r="C571" s="1" t="s">
+      <c r="C577" s="1" t="s">
         <v>1280</v>
       </c>
     </row>
-    <row r="572" spans="1:7" ht="34" x14ac:dyDescent="0.2">
-      <c r="A572" s="1" t="s">
+    <row r="578" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="A578" s="1" t="s">
         <v>1296</v>
       </c>
-      <c r="B572" s="1" t="s">
+      <c r="B578" s="1" t="s">
         <v>1279</v>
       </c>
-      <c r="C572" s="1" t="s">
+      <c r="C578" s="1" t="s">
         <v>1281</v>
       </c>
     </row>
-    <row r="573" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A573" s="1" t="s">
+    <row r="579" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A579" s="1" t="s">
         <v>1297</v>
       </c>
-      <c r="B573" s="1" t="s">
+      <c r="B579" s="1" t="s">
         <v>522</v>
       </c>
-      <c r="C573" s="1" t="s">
+      <c r="C579" s="1" t="s">
         <v>602</v>
       </c>
     </row>
-    <row r="574" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A574" s="10" t="s">
+    <row r="580" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A580" s="10" t="s">
         <v>1324</v>
       </c>
-      <c r="B574" s="4" t="s">
+      <c r="B580" s="4" t="s">
         <v>1334</v>
       </c>
-      <c r="C574" s="4" t="s">
+      <c r="C580" s="4" t="s">
         <v>1334</v>
       </c>
-      <c r="D574" s="4"/>
-      <c r="E574" s="4"/>
-      <c r="F574" s="4"/>
-      <c r="G574" s="4"/>
-    </row>
-    <row r="575" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A575" t="s">
+      <c r="D580" s="4"/>
+      <c r="E580" s="4"/>
+      <c r="F580" s="4"/>
+      <c r="G580" s="4"/>
+    </row>
+    <row r="581" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A581" t="s">
         <v>1325</v>
       </c>
-      <c r="B575" s="1" t="s">
+      <c r="B581" s="1" t="s">
         <v>1335</v>
       </c>
-      <c r="C575" s="1" t="s">
+      <c r="C581" s="1" t="s">
         <v>1344</v>
       </c>
     </row>
-    <row r="576" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A576" t="s">
+    <row r="582" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A582" t="s">
         <v>1326</v>
       </c>
-      <c r="B576" s="1" t="s">
+      <c r="B582" s="1" t="s">
         <v>1336</v>
       </c>
-      <c r="C576" s="1" t="s">
+      <c r="C582" s="1" t="s">
         <v>1345</v>
       </c>
     </row>
-    <row r="577" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A577" t="s">
+    <row r="583" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A583" t="s">
         <v>1327</v>
       </c>
-      <c r="B577" s="1" t="s">
+      <c r="B583" s="1" t="s">
         <v>1337</v>
       </c>
-      <c r="C577" s="1" t="s">
+      <c r="C583" s="1" t="s">
         <v>1346</v>
       </c>
     </row>
-    <row r="578" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A578" t="s">
+    <row r="584" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A584" t="s">
         <v>1328</v>
       </c>
-      <c r="B578" s="1" t="s">
+      <c r="B584" s="1" t="s">
         <v>1338</v>
       </c>
-      <c r="C578" s="1" t="s">
+      <c r="C584" s="1" t="s">
         <v>1347</v>
       </c>
     </row>
-    <row r="579" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A579" t="s">
+    <row r="585" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A585" t="s">
         <v>1329</v>
       </c>
-      <c r="B579" s="1" t="s">
+      <c r="B585" s="1" t="s">
         <v>1339</v>
       </c>
-      <c r="C579" s="1" t="s">
+      <c r="C585" s="1" t="s">
         <v>1348</v>
       </c>
     </row>
-    <row r="580" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A580" t="s">
+    <row r="586" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A586" t="s">
         <v>1330</v>
       </c>
-      <c r="B580" s="1" t="s">
+      <c r="B586" s="1" t="s">
         <v>1340</v>
       </c>
-      <c r="C580" s="1" t="s">
+      <c r="C586" s="1" t="s">
         <v>1349</v>
       </c>
     </row>
-    <row r="581" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A581" t="s">
+    <row r="587" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A587" t="s">
         <v>1331</v>
       </c>
-      <c r="B581" s="1" t="s">
+      <c r="B587" s="1" t="s">
         <v>1341</v>
       </c>
-      <c r="C581" s="1" t="s">
+      <c r="C587" s="1" t="s">
         <v>1341</v>
       </c>
     </row>
-    <row r="582" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A582" t="s">
+    <row r="588" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A588" t="s">
         <v>1332</v>
       </c>
-      <c r="B582" s="1" t="s">
+      <c r="B588" s="1" t="s">
         <v>1342</v>
       </c>
-      <c r="C582" s="1" t="s">
+      <c r="C588" s="1" t="s">
         <v>1350</v>
       </c>
     </row>
-    <row r="583" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A583" t="s">
+    <row r="589" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A589" t="s">
         <v>1333</v>
       </c>
-      <c r="B583" s="1" t="s">
+      <c r="B589" s="1" t="s">
         <v>1343</v>
       </c>
-      <c r="C583" s="1" t="s">
+      <c r="C589" s="1" t="s">
         <v>1351</v>
       </c>
     </row>
-    <row r="584" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A584" t="s">
+    <row r="590" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A590" t="s">
         <v>1355</v>
       </c>
-      <c r="B584" s="1" t="s">
+      <c r="B590" s="1" t="s">
         <v>1357</v>
       </c>
-      <c r="C584" s="1" t="s">
+      <c r="C590" s="1" t="s">
         <v>1357</v>
       </c>
     </row>
-    <row r="585" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A585" t="s">
+    <row r="591" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A591" t="s">
         <v>1356</v>
       </c>
-      <c r="B585" s="1" t="s">
+      <c r="B591" s="1" t="s">
         <v>1358</v>
       </c>
-      <c r="C585" s="1" t="s">
+      <c r="C591" s="1" t="s">
         <v>1358</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixing typo on SVAT 43 and 44 rules
</commit_message>
<xml_diff>
--- a/config/i18n/i18n.xlsx
+++ b/config/i18n/i18n.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joana/work/sp-duh/config/i18n/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6A003EC-466A-5644-B292-C375DC195265}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58623789-3C8B-1A4E-B4CC-842147E2A05C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-3560" yWindow="-19180" windowWidth="33600" windowHeight="18420" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1450" uniqueCount="1381">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1450" uniqueCount="1380">
   <si>
     <t>key</t>
   </si>
@@ -4221,18 +4221,13 @@
     <t>Teste à contabilização de outros documentos anulados na comercial</t>
   </si>
   <si>
-    <t>Verificamos que existem movimentos contabilísticos no estado finalizado para documentos comerciais anulados, sem que exista o respetivo estorno na contabilidade. Verifique no menu de contabilidade a sugestão de estorno, caso não encontre o lançamento de estorno, gere novamente as sugestões.
-Verifique os movovimentos dos seguintes documentos comerciais:</t>
-  </si>
-  <si>
-    <t>Verificamos que existem movimentos contabilísticos no estado finalizado para documentos comerciais anulados, sem que exista o respetivo estorno na contabilidade. Verifique no menu de contabilidade a sugestão de estorno, caso não encontre o lançamento de estorno, gere novamente as sugestões.
-Verifique os movovimentos dos seguintes documentos emitidos em faturação:</t>
-  </si>
-  <si>
     <t>Verificamos que não existem movimentos contabilísticos no estado finalizado para documentos emitidos em faturação, ou que existe o respetivo estorno na contabilidade. Sem exceções.</t>
   </si>
   <si>
     <t>Verificamos que não existem movimentos contabilísticos no estado finalizado para documentos comerciais anulados, ou que existe o respetivo estorno na contabilidade. Sem exceções.</t>
+  </si>
+  <si>
+    <t>Verificamos que existem movimentos contabilísticos no estado finalizado para documentos comerciais anulados, sem que exista o respetivo estorno na contabilidade. Verifique no menu de contabilidade a sugestão de estorno, caso não encontre o lançamento de estorno, gere novamente as sugestões.</t>
   </si>
 </sst>
 </file>
@@ -4831,8 +4826,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G591"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A541" workbookViewId="0">
-      <selection activeCell="B547" sqref="B547"/>
+    <sheetView tabSelected="1" topLeftCell="A538" workbookViewId="0">
+      <selection activeCell="B548" sqref="B548"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10125,21 +10120,21 @@
       </c>
       <c r="C542" s="8"/>
     </row>
-    <row r="543" spans="1:3" ht="85" x14ac:dyDescent="0.2">
+    <row r="543" spans="1:3" ht="66" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A543" s="1" t="s">
         <v>1371</v>
       </c>
       <c r="B543" s="1" t="s">
-        <v>1379</v>
+        <v>1377</v>
       </c>
       <c r="C543" s="8"/>
     </row>
-    <row r="544" spans="1:3" ht="153" x14ac:dyDescent="0.2">
+    <row r="544" spans="1:3" ht="119" x14ac:dyDescent="0.2">
       <c r="A544" s="1" t="s">
         <v>1372</v>
       </c>
       <c r="B544" s="1" t="s">
-        <v>1378</v>
+        <v>1379</v>
       </c>
       <c r="C544" s="8"/>
     </row>
@@ -10157,16 +10152,16 @@
         <v>1373</v>
       </c>
       <c r="B546" s="1" t="s">
-        <v>1380</v>
+        <v>1378</v>
       </c>
       <c r="C546" s="8"/>
     </row>
-    <row r="547" spans="1:7" ht="153" x14ac:dyDescent="0.2">
+    <row r="547" spans="1:7" ht="119" x14ac:dyDescent="0.2">
       <c r="A547" s="1" t="s">
         <v>1374</v>
       </c>
       <c r="B547" s="1" t="s">
-        <v>1377</v>
+        <v>1379</v>
       </c>
       <c r="C547" s="8"/>
     </row>

</xml_diff>

<commit_message>
adding notices for ensino
</commit_message>
<xml_diff>
--- a/config/i18n/i18n.xlsx
+++ b/config/i18n/i18n.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10111"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joana/work/sp-duh/config/i18n/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emi/work/sp-duh/config/i18n/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58623789-3C8B-1A4E-B4CC-842147E2A05C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03470317-4EA8-D041-B642-2259CB492055}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-3560" yWindow="-19180" windowWidth="33600" windowHeight="18420" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="67200" windowHeight="37300" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1450" uniqueCount="1380">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1462" uniqueCount="1384">
   <si>
     <t>key</t>
   </si>
@@ -4228,6 +4228,18 @@
   </si>
   <si>
     <t>Verificamos que existem movimentos contabilísticos no estado finalizado para documentos comerciais anulados, sem que exista o respetivo estorno na contabilidade. Verifique no menu de contabilidade a sugestão de estorno, caso não encontre o lançamento de estorno, gere novamente as sugestões.</t>
+  </si>
+  <si>
+    <t>certified_software_notice_toconline_ensino</t>
+  </si>
+  <si>
+    <t>document_certified_notice_toconline_ensino</t>
+  </si>
+  <si>
+    <t>document_certified_notice_short_toconline_ensino</t>
+  </si>
+  <si>
+    <t>document_certified_notice_non_hashed_toconline_ensino</t>
   </si>
 </sst>
 </file>
@@ -4547,7 +4559,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="i18n" displayName="i18n" ref="A1:G591" totalsRowShown="0" headerRowDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="i18n" displayName="i18n" ref="A1:G595" totalsRowShown="0" headerRowDxfId="6">
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="key"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="pt" dataDxfId="5"/>
@@ -4824,10 +4836,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G591"/>
+  <dimension ref="A1:G595"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A538" workbookViewId="0">
-      <selection activeCell="B548" sqref="B548"/>
+    <sheetView tabSelected="1" topLeftCell="A551" workbookViewId="0">
+      <selection activeCell="J595" sqref="J595"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10311,350 +10323,406 @@
         <v>523</v>
       </c>
     </row>
-    <row r="562" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+    <row r="562" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A562" s="1" t="s">
-        <v>1265</v>
+        <v>1380</v>
       </c>
       <c r="B562" s="1" t="s">
-        <v>1302</v>
+        <v>522</v>
       </c>
       <c r="C562" s="1" t="s">
-        <v>1303</v>
+        <v>523</v>
       </c>
     </row>
     <row r="563" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A563" s="1" t="s">
+        <v>1265</v>
+      </c>
+      <c r="B563" s="1" t="s">
+        <v>1302</v>
+      </c>
+      <c r="C563" s="1" t="s">
+        <v>1303</v>
+      </c>
+    </row>
+    <row r="564" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="A564" s="1" t="s">
         <v>1266</v>
       </c>
-      <c r="B563" s="1" t="s">
+      <c r="B564" s="1" t="s">
         <v>1304</v>
       </c>
-      <c r="C563" s="1" t="s">
+      <c r="C564" s="1" t="s">
         <v>1305</v>
       </c>
     </row>
-    <row r="564" spans="1:7" ht="34" x14ac:dyDescent="0.2">
-      <c r="A564" s="11" t="s">
+    <row r="565" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="A565" s="11" t="s">
         <v>1267</v>
       </c>
-      <c r="B564" s="7" t="s">
+      <c r="B565" s="7" t="s">
         <v>1278</v>
       </c>
-      <c r="C564" s="7" t="s">
+      <c r="C565" s="7" t="s">
         <v>1280</v>
       </c>
-      <c r="D564" s="7"/>
-      <c r="E564" s="7"/>
-      <c r="F564" s="7"/>
-      <c r="G564" s="12"/>
-    </row>
-    <row r="565" spans="1:7" ht="34" x14ac:dyDescent="0.2">
-      <c r="A565" s="13" t="s">
-        <v>1268</v>
-      </c>
-      <c r="B565" s="14" t="s">
-        <v>1279</v>
-      </c>
-      <c r="C565" s="14" t="s">
-        <v>1281</v>
-      </c>
-      <c r="D565" s="14"/>
-      <c r="E565" s="14"/>
-      <c r="F565" s="14"/>
-      <c r="G565" s="15"/>
+      <c r="D565" s="7"/>
+      <c r="E565" s="7"/>
+      <c r="F565" s="7"/>
+      <c r="G565" s="12"/>
     </row>
     <row r="566" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A566" s="11" t="s">
-        <v>1269</v>
+        <v>1381</v>
       </c>
       <c r="B566" s="7" t="s">
-        <v>522</v>
+        <v>1278</v>
       </c>
       <c r="C566" s="7" t="s">
-        <v>602</v>
+        <v>1280</v>
       </c>
       <c r="D566" s="7"/>
       <c r="E566" s="7"/>
       <c r="F566" s="7"/>
       <c r="G566" s="12"/>
     </row>
-    <row r="567" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A567" t="s">
-        <v>1282</v>
-      </c>
-      <c r="B567" s="16" t="s">
-        <v>1270</v>
-      </c>
-      <c r="C567" s="16" t="s">
-        <v>1270</v>
-      </c>
-    </row>
-    <row r="568" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A568" t="s">
-        <v>1283</v>
-      </c>
-      <c r="B568" s="16" t="s">
-        <v>1284</v>
-      </c>
-      <c r="C568" s="16" t="s">
-        <v>1284</v>
-      </c>
+    <row r="567" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="A567" s="13" t="s">
+        <v>1268</v>
+      </c>
+      <c r="B567" s="14" t="s">
+        <v>1279</v>
+      </c>
+      <c r="C567" s="14" t="s">
+        <v>1281</v>
+      </c>
+      <c r="D567" s="14"/>
+      <c r="E567" s="14"/>
+      <c r="F567" s="14"/>
+      <c r="G567" s="15"/>
+    </row>
+    <row r="568" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="A568" s="13" t="s">
+        <v>1383</v>
+      </c>
+      <c r="B568" s="14" t="s">
+        <v>1279</v>
+      </c>
+      <c r="C568" s="14" t="s">
+        <v>1281</v>
+      </c>
+      <c r="D568" s="14"/>
+      <c r="E568" s="14"/>
+      <c r="F568" s="14"/>
+      <c r="G568" s="15"/>
     </row>
     <row r="569" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A569" s="11" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B569" s="7" t="s">
+        <v>522</v>
+      </c>
+      <c r="C569" s="7" t="s">
+        <v>602</v>
+      </c>
+      <c r="D569" s="7"/>
+      <c r="E569" s="7"/>
+      <c r="F569" s="7"/>
+      <c r="G569" s="12"/>
+    </row>
+    <row r="570" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="A570" s="11" t="s">
+        <v>1382</v>
+      </c>
+      <c r="B570" s="7" t="s">
+        <v>522</v>
+      </c>
+      <c r="C570" s="7" t="s">
+        <v>602</v>
+      </c>
+      <c r="D570" s="8"/>
+      <c r="E570" s="8"/>
+      <c r="F570" s="8"/>
+      <c r="G570" s="8"/>
+    </row>
+    <row r="571" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A571" t="s">
+        <v>1282</v>
+      </c>
+      <c r="B571" s="16" t="s">
+        <v>1270</v>
+      </c>
+      <c r="C571" s="16" t="s">
+        <v>1270</v>
+      </c>
+    </row>
+    <row r="572" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A572" t="s">
+        <v>1283</v>
+      </c>
+      <c r="B572" s="16" t="s">
+        <v>1284</v>
+      </c>
+      <c r="C572" s="16" t="s">
+        <v>1284</v>
+      </c>
+    </row>
+    <row r="573" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="A573" s="11" t="s">
         <v>1271</v>
       </c>
-      <c r="B569" s="7" t="s">
+      <c r="B573" s="7" t="s">
         <v>1285</v>
       </c>
-      <c r="C569" s="7" t="s">
+      <c r="C573" s="7" t="s">
         <v>1292</v>
       </c>
-      <c r="D569" s="4"/>
-      <c r="E569" s="4"/>
-      <c r="F569" s="4"/>
-      <c r="G569" s="4"/>
-    </row>
-    <row r="570" spans="1:7" ht="34" x14ac:dyDescent="0.2">
-      <c r="A570" s="13" t="s">
+      <c r="D573" s="4"/>
+      <c r="E573" s="4"/>
+      <c r="F573" s="4"/>
+      <c r="G573" s="4"/>
+    </row>
+    <row r="574" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="A574" s="13" t="s">
         <v>1272</v>
       </c>
-      <c r="B570" s="14" t="s">
+      <c r="B574" s="14" t="s">
         <v>1286</v>
       </c>
-      <c r="C570" s="14" t="s">
+      <c r="C574" s="14" t="s">
         <v>1291</v>
       </c>
     </row>
-    <row r="571" spans="1:7" ht="34" x14ac:dyDescent="0.2">
-      <c r="A571" s="11" t="s">
+    <row r="575" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="A575" s="11" t="s">
         <v>1273</v>
       </c>
-      <c r="B571" s="1" t="s">
+      <c r="B575" s="1" t="s">
         <v>1302</v>
       </c>
-      <c r="C571" s="1" t="s">
+      <c r="C575" s="1" t="s">
         <v>1306</v>
       </c>
     </row>
-    <row r="572" spans="1:7" ht="34" x14ac:dyDescent="0.2">
-      <c r="A572" s="11" t="s">
+    <row r="576" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="A576" s="11" t="s">
         <v>1274</v>
       </c>
-      <c r="B572" s="7" t="s">
+      <c r="B576" s="7" t="s">
         <v>1287</v>
       </c>
-      <c r="C572" s="7" t="s">
+      <c r="C576" s="7" t="s">
         <v>1290</v>
       </c>
     </row>
-    <row r="573" spans="1:7" ht="34" x14ac:dyDescent="0.2">
-      <c r="A573" s="13" t="s">
+    <row r="577" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="A577" s="13" t="s">
         <v>1275</v>
       </c>
-      <c r="B573" s="14" t="s">
+      <c r="B577" s="14" t="s">
         <v>1288</v>
       </c>
-      <c r="C573" s="14" t="s">
+      <c r="C577" s="14" t="s">
         <v>1289</v>
       </c>
     </row>
-    <row r="574" spans="1:7" ht="34" x14ac:dyDescent="0.2">
-      <c r="A574" s="11" t="s">
+    <row r="578" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="A578" s="11" t="s">
         <v>1276</v>
       </c>
-      <c r="B574" s="1" t="s">
+      <c r="B578" s="1" t="s">
         <v>1304</v>
       </c>
-      <c r="C574" s="1" t="s">
+      <c r="C578" s="1" t="s">
         <v>1307</v>
-      </c>
-    </row>
-    <row r="575" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A575" s="1" t="s">
-        <v>1293</v>
-      </c>
-      <c r="B575" s="1" t="s">
-        <v>522</v>
-      </c>
-      <c r="C575" s="1" t="s">
-        <v>523</v>
-      </c>
-    </row>
-    <row r="576" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A576" s="1" t="s">
-        <v>1294</v>
-      </c>
-      <c r="B576" s="1">
-        <v>1662</v>
-      </c>
-    </row>
-    <row r="577" spans="1:7" ht="34" x14ac:dyDescent="0.2">
-      <c r="A577" s="1" t="s">
-        <v>1295</v>
-      </c>
-      <c r="B577" s="1" t="s">
-        <v>1278</v>
-      </c>
-      <c r="C577" s="1" t="s">
-        <v>1280</v>
-      </c>
-    </row>
-    <row r="578" spans="1:7" ht="34" x14ac:dyDescent="0.2">
-      <c r="A578" s="1" t="s">
-        <v>1296</v>
-      </c>
-      <c r="B578" s="1" t="s">
-        <v>1279</v>
-      </c>
-      <c r="C578" s="1" t="s">
-        <v>1281</v>
       </c>
     </row>
     <row r="579" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A579" s="1" t="s">
-        <v>1297</v>
+        <v>1293</v>
       </c>
       <c r="B579" s="1" t="s">
         <v>522</v>
       </c>
       <c r="C579" s="1" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="580" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A580" s="1" t="s">
+        <v>1294</v>
+      </c>
+      <c r="B580" s="1">
+        <v>1662</v>
+      </c>
+    </row>
+    <row r="581" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="A581" s="1" t="s">
+        <v>1295</v>
+      </c>
+      <c r="B581" s="1" t="s">
+        <v>1278</v>
+      </c>
+      <c r="C581" s="1" t="s">
+        <v>1280</v>
+      </c>
+    </row>
+    <row r="582" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="A582" s="1" t="s">
+        <v>1296</v>
+      </c>
+      <c r="B582" s="1" t="s">
+        <v>1279</v>
+      </c>
+      <c r="C582" s="1" t="s">
+        <v>1281</v>
+      </c>
+    </row>
+    <row r="583" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A583" s="1" t="s">
+        <v>1297</v>
+      </c>
+      <c r="B583" s="1" t="s">
+        <v>522</v>
+      </c>
+      <c r="C583" s="1" t="s">
         <v>602</v>
       </c>
     </row>
-    <row r="580" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A580" s="10" t="s">
+    <row r="584" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A584" s="10" t="s">
         <v>1324</v>
       </c>
-      <c r="B580" s="4" t="s">
+      <c r="B584" s="4" t="s">
         <v>1334</v>
       </c>
-      <c r="C580" s="4" t="s">
+      <c r="C584" s="4" t="s">
         <v>1334</v>
       </c>
-      <c r="D580" s="4"/>
-      <c r="E580" s="4"/>
-      <c r="F580" s="4"/>
-      <c r="G580" s="4"/>
-    </row>
-    <row r="581" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A581" t="s">
-        <v>1325</v>
-      </c>
-      <c r="B581" s="1" t="s">
-        <v>1335</v>
-      </c>
-      <c r="C581" s="1" t="s">
-        <v>1344</v>
-      </c>
-    </row>
-    <row r="582" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A582" t="s">
-        <v>1326</v>
-      </c>
-      <c r="B582" s="1" t="s">
-        <v>1336</v>
-      </c>
-      <c r="C582" s="1" t="s">
-        <v>1345</v>
-      </c>
-    </row>
-    <row r="583" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A583" t="s">
-        <v>1327</v>
-      </c>
-      <c r="B583" s="1" t="s">
-        <v>1337</v>
-      </c>
-      <c r="C583" s="1" t="s">
-        <v>1346</v>
-      </c>
-    </row>
-    <row r="584" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A584" t="s">
-        <v>1328</v>
-      </c>
-      <c r="B584" s="1" t="s">
-        <v>1338</v>
-      </c>
-      <c r="C584" s="1" t="s">
-        <v>1347</v>
-      </c>
+      <c r="D584" s="4"/>
+      <c r="E584" s="4"/>
+      <c r="F584" s="4"/>
+      <c r="G584" s="4"/>
     </row>
     <row r="585" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A585" t="s">
-        <v>1329</v>
+        <v>1325</v>
       </c>
       <c r="B585" s="1" t="s">
-        <v>1339</v>
+        <v>1335</v>
       </c>
       <c r="C585" s="1" t="s">
-        <v>1348</v>
+        <v>1344</v>
       </c>
     </row>
     <row r="586" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A586" t="s">
-        <v>1330</v>
+        <v>1326</v>
       </c>
       <c r="B586" s="1" t="s">
-        <v>1340</v>
+        <v>1336</v>
       </c>
       <c r="C586" s="1" t="s">
-        <v>1349</v>
+        <v>1345</v>
       </c>
     </row>
     <row r="587" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A587" t="s">
-        <v>1331</v>
+        <v>1327</v>
       </c>
       <c r="B587" s="1" t="s">
-        <v>1341</v>
+        <v>1337</v>
       </c>
       <c r="C587" s="1" t="s">
-        <v>1341</v>
+        <v>1346</v>
       </c>
     </row>
     <row r="588" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A588" t="s">
-        <v>1332</v>
+        <v>1328</v>
       </c>
       <c r="B588" s="1" t="s">
-        <v>1342</v>
+        <v>1338</v>
       </c>
       <c r="C588" s="1" t="s">
-        <v>1350</v>
+        <v>1347</v>
       </c>
     </row>
     <row r="589" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A589" t="s">
-        <v>1333</v>
+        <v>1329</v>
       </c>
       <c r="B589" s="1" t="s">
-        <v>1343</v>
+        <v>1339</v>
       </c>
       <c r="C589" s="1" t="s">
-        <v>1351</v>
+        <v>1348</v>
       </c>
     </row>
     <row r="590" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A590" t="s">
-        <v>1355</v>
+        <v>1330</v>
       </c>
       <c r="B590" s="1" t="s">
-        <v>1357</v>
+        <v>1340</v>
       </c>
       <c r="C590" s="1" t="s">
-        <v>1357</v>
+        <v>1349</v>
       </c>
     </row>
     <row r="591" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A591" t="s">
+        <v>1331</v>
+      </c>
+      <c r="B591" s="1" t="s">
+        <v>1341</v>
+      </c>
+      <c r="C591" s="1" t="s">
+        <v>1341</v>
+      </c>
+    </row>
+    <row r="592" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A592" t="s">
+        <v>1332</v>
+      </c>
+      <c r="B592" s="1" t="s">
+        <v>1342</v>
+      </c>
+      <c r="C592" s="1" t="s">
+        <v>1350</v>
+      </c>
+    </row>
+    <row r="593" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A593" t="s">
+        <v>1333</v>
+      </c>
+      <c r="B593" s="1" t="s">
+        <v>1343</v>
+      </c>
+      <c r="C593" s="1" t="s">
+        <v>1351</v>
+      </c>
+    </row>
+    <row r="594" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A594" t="s">
+        <v>1355</v>
+      </c>
+      <c r="B594" s="1" t="s">
+        <v>1357</v>
+      </c>
+      <c r="C594" s="1" t="s">
+        <v>1357</v>
+      </c>
+    </row>
+    <row r="595" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A595" t="s">
         <v>1356</v>
       </c>
-      <c r="B591" s="1" t="s">
+      <c r="B595" s="1" t="s">
         <v>1358</v>
       </c>
-      <c r="C591" s="1" t="s">
+      <c r="C595" s="1" t="s">
         <v>1358</v>
       </c>
     </row>

</xml_diff>

<commit_message>
changing notices from mbcp to iziBizi
</commit_message>
<xml_diff>
--- a/config/i18n/i18n.xlsx
+++ b/config/i18n/i18n.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10711"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10111"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jpacheco/work/sp-duh/config/i18n/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emi/work/sp-duh/config/i18n/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96F9FCB2-D488-2641-83F2-3E8F7B334C59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CFC5BD1-D4E9-8A4F-956D-0D9400CCD927}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="680" yWindow="500" windowWidth="21040" windowHeight="21900" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5760" yWindow="2220" windowWidth="38120" windowHeight="27540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1462" uniqueCount="1391">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1462" uniqueCount="1392">
   <si>
     <t>key</t>
   </si>
@@ -3880,9 +3880,6 @@
     <t>certified_software_notice_business_business</t>
   </si>
   <si>
-    <t>certified_software_notice_business_mbcp</t>
-  </si>
-  <si>
     <t>document_certified_notice_toconline_toconline</t>
   </si>
   <si>
@@ -3904,15 +3901,6 @@
     <t>document_certified_notice_short_business_business</t>
   </si>
   <si>
-    <t>document_certified_notice_business_mbcp</t>
-  </si>
-  <si>
-    <t>document_certified_notice_non_hashed_business_mbcp</t>
-  </si>
-  <si>
-    <t>document_certified_notice_short_business_mbcp</t>
-  </si>
-  <si>
     <t>Os saldos de abertura devem ser coincidentes com os saldos finais do exercício anterior. Não nos foi possível efetuar este teste uma vez que não existe exercício do ano {0}.</t>
   </si>
   <si>
@@ -3943,18 +3931,6 @@
     <t>Emitido por programa certificado nº 2397/AT - Cloudware.business</t>
   </si>
   <si>
-    <t>Processado por programa certificado nº 2397/AT - M Fatura (Powered by Cloudware.business)</t>
-  </si>
-  <si>
-    <t>Emitido por programa certificado nº 2397/AT - M Fatura (Powered by Cloudware.business)</t>
-  </si>
-  <si>
-    <t>Issued by certified program nr. 2397/AT - M Fatura (Powered by Cloudware.business)</t>
-  </si>
-  <si>
-    <t>Processed by certified program nr. 2397/AT - M Fatura (Powered by Cloudware.business)</t>
-  </si>
-  <si>
     <t>Issued by certified program nr. 2397/AT - Cloudware.business</t>
   </si>
   <si>
@@ -3994,16 +3970,7 @@
     <t>Created by Cloudware.business - https://app.cloudware.pt</t>
   </si>
   <si>
-    <t>Emitido por M Fatura (Powered by Cloudware.business - https://app.cloudware.pt)</t>
-  </si>
-  <si>
-    <t>Created by M Fatura (Powered by Cloudware.business - https://app.cloudware.pt)</t>
-  </si>
-  <si>
     <t>Processed by Cloudware.business - https://app.cloudware.pt</t>
-  </si>
-  <si>
-    <t>Processed by M Fatura (Powered by Cloudware.business - https://app.cloudware.pt)</t>
   </si>
   <si>
     <t>Teste à contabilização de documentos emitidos em faturação</t>
@@ -4261,6 +4228,42 @@
   </si>
   <si>
     <t>libras esterlinas</t>
+  </si>
+  <si>
+    <t>document_certified_notice_business_izibizi</t>
+  </si>
+  <si>
+    <t>document_certified_notice_non_hashed_business_izibizi</t>
+  </si>
+  <si>
+    <t>document_certified_notice_short_business_izibizi</t>
+  </si>
+  <si>
+    <t>Processado por programa certificado nº 2397/AT - iziBizi (Powered by Cloudware.business)</t>
+  </si>
+  <si>
+    <t>Emitido por programa certificado nº 2397/AT - iziBizi (Powered by Cloudware.business)</t>
+  </si>
+  <si>
+    <t>Emitido por iziBizi (Powered by Cloudware.business - https://app.izibizi.pt)</t>
+  </si>
+  <si>
+    <t>Processed by certified program nr. 2397/AT - iziBizi (Powered by Cloudware.business)</t>
+  </si>
+  <si>
+    <t>Issued by certified program nr. 2397/AT - iziBizi (Powered by Cloudware.business)</t>
+  </si>
+  <si>
+    <t>Processed by iziBizi (Powered by Cloudware.business - https://app.cloudware.pt)</t>
+  </si>
+  <si>
+    <t>certified_software_notice_business_izibizi</t>
+  </si>
+  <si>
+    <t>Emitido por iziBizi (Powered by Cloudware.business - https://app.cloudware.pt)</t>
+  </si>
+  <si>
+    <t>Created by iziBizi (Powered by Cloudware.business - https://app.cloudware.pt)</t>
   </si>
 </sst>
 </file>
@@ -4862,14 +4865,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G595"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A228" workbookViewId="0">
-      <selection activeCell="B253" sqref="B253"/>
+    <sheetView tabSelected="1" topLeftCell="A548" workbookViewId="0">
+      <selection activeCell="A577" sqref="A577"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="41.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="44.33203125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="64.6640625" customWidth="1"/>
+    <col min="2" max="2" width="61.5" style="1" customWidth="1"/>
+    <col min="3" max="3" width="44.33203125" style="1" customWidth="1"/>
     <col min="4" max="7" width="8" style="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -6913,7 +6917,7 @@
         <v>510</v>
       </c>
       <c r="B252" s="1" t="s">
-        <v>1389</v>
+        <v>1378</v>
       </c>
       <c r="C252" s="1" t="s">
         <v>511</v>
@@ -6924,7 +6928,7 @@
         <v>512</v>
       </c>
       <c r="B253" s="1" t="s">
-        <v>1390</v>
+        <v>1379</v>
       </c>
       <c r="C253" s="1" t="s">
         <v>513</v>
@@ -7680,10 +7684,10 @@
         <v>844</v>
       </c>
       <c r="B322" s="1" t="s">
-        <v>1297</v>
+        <v>1289</v>
       </c>
       <c r="C322" s="1" t="s">
-        <v>1296</v>
+        <v>1288</v>
       </c>
     </row>
     <row r="323" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -7691,10 +7695,10 @@
         <v>845</v>
       </c>
       <c r="B323" s="1" t="s">
-        <v>1299</v>
+        <v>1291</v>
       </c>
       <c r="C323" s="1" t="s">
-        <v>1298</v>
+        <v>1290</v>
       </c>
     </row>
     <row r="324" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -9022,13 +9026,13 @@
     </row>
     <row r="429" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A429" t="s">
-        <v>1319</v>
+        <v>1308</v>
       </c>
       <c r="B429" s="1" t="s">
-        <v>1318</v>
+        <v>1307</v>
       </c>
       <c r="C429" s="1" t="s">
-        <v>1320</v>
+        <v>1309</v>
       </c>
     </row>
     <row r="430" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -9666,7 +9670,7 @@
         <v>1139</v>
       </c>
       <c r="B488" s="1" t="s">
-        <v>1351</v>
+        <v>1340</v>
       </c>
       <c r="C488" s="9"/>
     </row>
@@ -9756,7 +9760,7 @@
         <v>1168</v>
       </c>
       <c r="B498" s="1" t="s">
-        <v>1352</v>
+        <v>1341</v>
       </c>
       <c r="C498" s="9"/>
     </row>
@@ -9783,7 +9787,7 @@
         <v>1206</v>
       </c>
       <c r="B501" s="1" t="s">
-        <v>1275</v>
+        <v>1271</v>
       </c>
       <c r="C501" s="8"/>
     </row>
@@ -10095,163 +10099,163 @@
     </row>
     <row r="536" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A536" s="1" t="s">
-        <v>1312</v>
+        <v>1301</v>
       </c>
       <c r="B536" s="1" t="s">
-        <v>1306</v>
+        <v>1295</v>
       </c>
       <c r="C536" s="8"/>
     </row>
     <row r="537" spans="1:3" ht="51" x14ac:dyDescent="0.2">
       <c r="A537" s="1" t="s">
-        <v>1313</v>
+        <v>1302</v>
       </c>
       <c r="B537" s="1" t="s">
-        <v>1308</v>
+        <v>1297</v>
       </c>
       <c r="C537" s="8"/>
     </row>
     <row r="538" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A538" s="1" t="s">
-        <v>1314</v>
+        <v>1303</v>
       </c>
       <c r="B538" s="1" t="s">
-        <v>1309</v>
+        <v>1298</v>
       </c>
       <c r="C538" s="8"/>
     </row>
     <row r="539" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A539" s="1" t="s">
-        <v>1315</v>
+        <v>1304</v>
       </c>
       <c r="B539" s="1" t="s">
-        <v>1307</v>
+        <v>1296</v>
       </c>
       <c r="C539" s="8"/>
     </row>
     <row r="540" spans="1:3" ht="51" x14ac:dyDescent="0.2">
       <c r="A540" s="1" t="s">
-        <v>1316</v>
+        <v>1305</v>
       </c>
       <c r="B540" s="1" t="s">
-        <v>1310</v>
+        <v>1299</v>
       </c>
       <c r="C540" s="8"/>
     </row>
     <row r="541" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A541" s="1" t="s">
-        <v>1317</v>
+        <v>1306</v>
       </c>
       <c r="B541" s="1" t="s">
-        <v>1311</v>
+        <v>1300</v>
       </c>
       <c r="C541" s="8"/>
     </row>
     <row r="542" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A542" s="1" t="s">
-        <v>1367</v>
+        <v>1356</v>
       </c>
       <c r="B542" s="1" t="s">
-        <v>1373</v>
+        <v>1362</v>
       </c>
       <c r="C542" s="8"/>
     </row>
     <row r="543" spans="1:3" ht="66" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A543" s="1" t="s">
-        <v>1369</v>
+        <v>1358</v>
       </c>
       <c r="B543" s="1" t="s">
-        <v>1375</v>
+        <v>1364</v>
       </c>
       <c r="C543" s="8"/>
     </row>
     <row r="544" spans="1:3" ht="119" x14ac:dyDescent="0.2">
       <c r="A544" s="1" t="s">
-        <v>1370</v>
+        <v>1359</v>
       </c>
       <c r="B544" s="1" t="s">
-        <v>1377</v>
+        <v>1366</v>
       </c>
       <c r="C544" s="8"/>
     </row>
     <row r="545" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A545" s="1" t="s">
-        <v>1368</v>
+        <v>1357</v>
       </c>
       <c r="B545" s="1" t="s">
-        <v>1374</v>
+        <v>1363</v>
       </c>
       <c r="C545" s="8"/>
     </row>
     <row r="546" spans="1:7" ht="68" x14ac:dyDescent="0.2">
       <c r="A546" s="1" t="s">
-        <v>1371</v>
+        <v>1360</v>
       </c>
       <c r="B546" s="1" t="s">
-        <v>1376</v>
+        <v>1365</v>
       </c>
       <c r="C546" s="8"/>
     </row>
     <row r="547" spans="1:7" ht="119" x14ac:dyDescent="0.2">
       <c r="A547" s="1" t="s">
-        <v>1372</v>
+        <v>1361</v>
       </c>
       <c r="B547" s="1" t="s">
-        <v>1377</v>
+        <v>1366</v>
       </c>
       <c r="C547" s="8"/>
     </row>
     <row r="548" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A548" s="1" t="s">
-        <v>1357</v>
+        <v>1346</v>
       </c>
       <c r="B548" s="1" t="s">
-        <v>1359</v>
+        <v>1348</v>
       </c>
       <c r="C548" s="8"/>
     </row>
     <row r="549" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A549" s="1" t="s">
-        <v>1358</v>
+        <v>1347</v>
       </c>
       <c r="B549" s="1" t="s">
-        <v>1362</v>
+        <v>1351</v>
       </c>
       <c r="C549" s="8"/>
     </row>
     <row r="550" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A550" s="1" t="s">
-        <v>1360</v>
+        <v>1349</v>
       </c>
       <c r="B550" s="1" t="s">
-        <v>1363</v>
+        <v>1352</v>
       </c>
       <c r="C550" s="8"/>
     </row>
     <row r="551" spans="1:7" ht="85" x14ac:dyDescent="0.2">
       <c r="A551" s="1" t="s">
-        <v>1365</v>
+        <v>1354</v>
       </c>
       <c r="B551" s="1" t="s">
-        <v>1366</v>
+        <v>1355</v>
       </c>
       <c r="C551" s="8"/>
     </row>
     <row r="552" spans="1:7" ht="85" x14ac:dyDescent="0.2">
       <c r="A552" s="1" t="s">
-        <v>1364</v>
+        <v>1353</v>
       </c>
       <c r="B552" s="1" t="s">
-        <v>1361</v>
+        <v>1350</v>
       </c>
       <c r="C552" s="8"/>
     </row>
     <row r="553" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A553" s="1" t="s">
-        <v>1321</v>
+        <v>1310</v>
       </c>
       <c r="B553" s="1" t="s">
-        <v>1350</v>
+        <v>1339</v>
       </c>
       <c r="C553" s="8"/>
     </row>
@@ -10349,13 +10353,13 @@
     </row>
     <row r="562" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A562" s="17" t="s">
-        <v>1378</v>
+        <v>1367</v>
       </c>
       <c r="B562" s="17" t="s">
-        <v>1382</v>
+        <v>1371</v>
       </c>
       <c r="C562" s="17" t="s">
-        <v>1383</v>
+        <v>1372</v>
       </c>
     </row>
     <row r="563" spans="1:7" ht="34" x14ac:dyDescent="0.2">
@@ -10363,32 +10367,32 @@
         <v>1263</v>
       </c>
       <c r="B563" s="1" t="s">
-        <v>1300</v>
+        <v>1292</v>
       </c>
       <c r="C563" s="1" t="s">
-        <v>1301</v>
+        <v>1293</v>
       </c>
     </row>
     <row r="564" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A564" s="1" t="s">
-        <v>1264</v>
+        <v>1389</v>
       </c>
       <c r="B564" s="1" t="s">
-        <v>1302</v>
+        <v>1390</v>
       </c>
       <c r="C564" s="1" t="s">
-        <v>1303</v>
+        <v>1391</v>
       </c>
     </row>
     <row r="565" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A565" s="11" t="s">
-        <v>1265</v>
+        <v>1264</v>
       </c>
       <c r="B565" s="7" t="s">
-        <v>1276</v>
+        <v>1272</v>
       </c>
       <c r="C565" s="7" t="s">
-        <v>1278</v>
+        <v>1274</v>
       </c>
       <c r="D565" s="7"/>
       <c r="E565" s="7"/>
@@ -10397,13 +10401,13 @@
     </row>
     <row r="566" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A566" s="11" t="s">
-        <v>1379</v>
+        <v>1368</v>
       </c>
       <c r="B566" s="7" t="s">
-        <v>1384</v>
+        <v>1373</v>
       </c>
       <c r="C566" s="7" t="s">
-        <v>1385</v>
+        <v>1374</v>
       </c>
       <c r="D566" s="7"/>
       <c r="E566" s="7"/>
@@ -10412,13 +10416,13 @@
     </row>
     <row r="567" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A567" s="13" t="s">
-        <v>1266</v>
+        <v>1265</v>
       </c>
       <c r="B567" s="14" t="s">
-        <v>1277</v>
+        <v>1273</v>
       </c>
       <c r="C567" s="14" t="s">
-        <v>1279</v>
+        <v>1275</v>
       </c>
       <c r="D567" s="14"/>
       <c r="E567" s="14"/>
@@ -10427,13 +10431,13 @@
     </row>
     <row r="568" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A568" s="13" t="s">
-        <v>1381</v>
+        <v>1370</v>
       </c>
       <c r="B568" s="14" t="s">
-        <v>1386</v>
+        <v>1375</v>
       </c>
       <c r="C568" s="14" t="s">
-        <v>1387</v>
+        <v>1376</v>
       </c>
       <c r="D568" s="14"/>
       <c r="E568" s="14"/>
@@ -10442,7 +10446,7 @@
     </row>
     <row r="569" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A569" s="11" t="s">
-        <v>1267</v>
+        <v>1266</v>
       </c>
       <c r="B569" s="7" t="s">
         <v>520</v>
@@ -10457,13 +10461,13 @@
     </row>
     <row r="570" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A570" s="11" t="s">
-        <v>1380</v>
+        <v>1369</v>
       </c>
       <c r="B570" s="7" t="s">
-        <v>1382</v>
+        <v>1371</v>
       </c>
       <c r="C570" s="7" t="s">
-        <v>1388</v>
+        <v>1377</v>
       </c>
       <c r="D570" s="8"/>
       <c r="E570" s="8"/>
@@ -10472,35 +10476,35 @@
     </row>
     <row r="571" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A571" t="s">
-        <v>1280</v>
+        <v>1276</v>
       </c>
       <c r="B571" s="16" t="s">
-        <v>1268</v>
+        <v>1267</v>
       </c>
       <c r="C571" s="16" t="s">
-        <v>1268</v>
+        <v>1267</v>
       </c>
     </row>
     <row r="572" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A572" t="s">
-        <v>1281</v>
+        <v>1277</v>
       </c>
       <c r="B572" s="16" t="s">
-        <v>1282</v>
+        <v>1278</v>
       </c>
       <c r="C572" s="16" t="s">
-        <v>1282</v>
+        <v>1278</v>
       </c>
     </row>
     <row r="573" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A573" s="11" t="s">
-        <v>1269</v>
+        <v>1268</v>
       </c>
       <c r="B573" s="7" t="s">
-        <v>1283</v>
+        <v>1279</v>
       </c>
       <c r="C573" s="7" t="s">
-        <v>1290</v>
+        <v>1282</v>
       </c>
       <c r="D573" s="4"/>
       <c r="E573" s="4"/>
@@ -10509,62 +10513,62 @@
     </row>
     <row r="574" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A574" s="13" t="s">
-        <v>1270</v>
+        <v>1269</v>
       </c>
       <c r="B574" s="14" t="s">
-        <v>1284</v>
+        <v>1280</v>
       </c>
       <c r="C574" s="14" t="s">
-        <v>1289</v>
+        <v>1281</v>
       </c>
     </row>
     <row r="575" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A575" s="11" t="s">
-        <v>1271</v>
+        <v>1270</v>
       </c>
       <c r="B575" s="1" t="s">
-        <v>1300</v>
+        <v>1292</v>
       </c>
       <c r="C575" s="1" t="s">
-        <v>1304</v>
+        <v>1294</v>
       </c>
     </row>
     <row r="576" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A576" s="11" t="s">
-        <v>1272</v>
+        <v>1380</v>
       </c>
       <c r="B576" s="7" t="s">
-        <v>1285</v>
+        <v>1383</v>
       </c>
       <c r="C576" s="7" t="s">
-        <v>1288</v>
+        <v>1386</v>
       </c>
     </row>
     <row r="577" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A577" s="13" t="s">
-        <v>1273</v>
+        <v>1381</v>
       </c>
       <c r="B577" s="14" t="s">
-        <v>1286</v>
+        <v>1384</v>
       </c>
       <c r="C577" s="14" t="s">
-        <v>1287</v>
+        <v>1387</v>
       </c>
     </row>
     <row r="578" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A578" s="11" t="s">
-        <v>1274</v>
+        <v>1382</v>
       </c>
       <c r="B578" s="1" t="s">
-        <v>1302</v>
+        <v>1385</v>
       </c>
       <c r="C578" s="1" t="s">
-        <v>1305</v>
+        <v>1388</v>
       </c>
     </row>
     <row r="579" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A579" s="1" t="s">
-        <v>1291</v>
+        <v>1283</v>
       </c>
       <c r="B579" s="1" t="s">
         <v>520</v>
@@ -10575,7 +10579,7 @@
     </row>
     <row r="580" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A580" s="1" t="s">
-        <v>1292</v>
+        <v>1284</v>
       </c>
       <c r="B580" s="1">
         <v>1662</v>
@@ -10583,29 +10587,29 @@
     </row>
     <row r="581" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A581" s="1" t="s">
-        <v>1293</v>
+        <v>1285</v>
       </c>
       <c r="B581" s="1" t="s">
-        <v>1276</v>
+        <v>1272</v>
       </c>
       <c r="C581" s="1" t="s">
-        <v>1278</v>
+        <v>1274</v>
       </c>
     </row>
     <row r="582" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A582" s="1" t="s">
-        <v>1294</v>
+        <v>1286</v>
       </c>
       <c r="B582" s="1" t="s">
-        <v>1277</v>
+        <v>1273</v>
       </c>
       <c r="C582" s="1" t="s">
-        <v>1279</v>
+        <v>1275</v>
       </c>
     </row>
     <row r="583" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A583" s="1" t="s">
-        <v>1295</v>
+        <v>1287</v>
       </c>
       <c r="B583" s="1" t="s">
         <v>520</v>
@@ -10616,13 +10620,13 @@
     </row>
     <row r="584" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A584" s="10" t="s">
-        <v>1322</v>
+        <v>1311</v>
       </c>
       <c r="B584" s="4" t="s">
-        <v>1332</v>
+        <v>1321</v>
       </c>
       <c r="C584" s="4" t="s">
-        <v>1332</v>
+        <v>1321</v>
       </c>
       <c r="D584" s="4"/>
       <c r="E584" s="4"/>
@@ -10631,123 +10635,123 @@
     </row>
     <row r="585" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A585" t="s">
-        <v>1323</v>
+        <v>1312</v>
       </c>
       <c r="B585" s="1" t="s">
-        <v>1333</v>
+        <v>1322</v>
       </c>
       <c r="C585" s="1" t="s">
-        <v>1342</v>
+        <v>1331</v>
       </c>
     </row>
     <row r="586" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A586" t="s">
-        <v>1324</v>
+        <v>1313</v>
       </c>
       <c r="B586" s="1" t="s">
-        <v>1334</v>
+        <v>1323</v>
       </c>
       <c r="C586" s="1" t="s">
-        <v>1343</v>
+        <v>1332</v>
       </c>
     </row>
     <row r="587" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A587" t="s">
-        <v>1325</v>
+        <v>1314</v>
       </c>
       <c r="B587" s="1" t="s">
-        <v>1335</v>
+        <v>1324</v>
       </c>
       <c r="C587" s="1" t="s">
-        <v>1344</v>
+        <v>1333</v>
       </c>
     </row>
     <row r="588" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A588" t="s">
-        <v>1326</v>
+        <v>1315</v>
       </c>
       <c r="B588" s="1" t="s">
-        <v>1336</v>
+        <v>1325</v>
       </c>
       <c r="C588" s="1" t="s">
-        <v>1345</v>
+        <v>1334</v>
       </c>
     </row>
     <row r="589" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A589" t="s">
-        <v>1327</v>
+        <v>1316</v>
       </c>
       <c r="B589" s="1" t="s">
-        <v>1337</v>
+        <v>1326</v>
       </c>
       <c r="C589" s="1" t="s">
-        <v>1346</v>
+        <v>1335</v>
       </c>
     </row>
     <row r="590" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A590" t="s">
-        <v>1328</v>
+        <v>1317</v>
       </c>
       <c r="B590" s="1" t="s">
-        <v>1338</v>
+        <v>1327</v>
       </c>
       <c r="C590" s="1" t="s">
-        <v>1347</v>
+        <v>1336</v>
       </c>
     </row>
     <row r="591" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A591" t="s">
-        <v>1329</v>
+        <v>1318</v>
       </c>
       <c r="B591" s="1" t="s">
-        <v>1339</v>
+        <v>1328</v>
       </c>
       <c r="C591" s="1" t="s">
-        <v>1339</v>
+        <v>1328</v>
       </c>
     </row>
     <row r="592" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A592" t="s">
-        <v>1330</v>
+        <v>1319</v>
       </c>
       <c r="B592" s="1" t="s">
-        <v>1340</v>
+        <v>1329</v>
       </c>
       <c r="C592" s="1" t="s">
-        <v>1348</v>
+        <v>1337</v>
       </c>
     </row>
     <row r="593" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A593" t="s">
-        <v>1331</v>
+        <v>1320</v>
       </c>
       <c r="B593" s="1" t="s">
-        <v>1341</v>
+        <v>1330</v>
       </c>
       <c r="C593" s="1" t="s">
-        <v>1349</v>
+        <v>1338</v>
       </c>
     </row>
     <row r="594" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A594" t="s">
-        <v>1353</v>
+        <v>1342</v>
       </c>
       <c r="B594" s="1" t="s">
-        <v>1355</v>
+        <v>1344</v>
       </c>
       <c r="C594" s="1" t="s">
-        <v>1355</v>
+        <v>1344</v>
       </c>
     </row>
     <row r="595" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A595" t="s">
-        <v>1354</v>
+        <v>1343</v>
       </c>
       <c r="B595" s="1" t="s">
-        <v>1356</v>
+        <v>1345</v>
       </c>
       <c r="C595" s="1" t="s">
-        <v>1356</v>
+        <v>1345</v>
       </c>
     </row>
   </sheetData>

</xml_diff>